<commit_message>
GearSwap v0.800 - A NEW HOPE
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variables.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variables.xlsx
@@ -570,9 +570,6 @@
     <t>aftercast</t>
   </si>
   <si>
-    <t>buff_change(name,gain_or_loss)</t>
-  </si>
-  <si>
     <t>pet_aftercast(spell,{type=Magic_or_Ability)</t>
   </si>
   <si>
@@ -591,9 +588,6 @@
     <t>self_command(command)</t>
   </si>
   <si>
-    <t>Passes the new buff name and whether it was gained or lost.</t>
-  </si>
-  <si>
     <t>Passes any self commands, which are triggered by //gs c &lt;command&gt;</t>
   </si>
   <si>
@@ -1900,18 +1894,6 @@
   </si>
   <si>
     <t>pretarget(spell,{type=Magic_or_Ability})</t>
-  </si>
-  <si>
-    <t>Passes the resources line for the spell with a few modifications. Occurs when the command text hits the outgoing text buffer.</t>
-  </si>
-  <si>
-    <t>Passes the resources line for the spell with a few modifications. Occurs when the outgoing action packet is cued.</t>
-  </si>
-  <si>
-    <t>Passes the resources line for the spell with a few modifications. Occurs when the "readies" action packet is received.</t>
-  </si>
-  <si>
-    <t>Passes the resources line for the spell with a few modifications. Occurs when the "result" action packet is received.</t>
   </si>
   <si>
     <t>Passes the resources line for the spell with a few modifications. Occurs when the "readies" action packet is received for your pet.</t>
@@ -1959,6 +1941,24 @@
   </si>
   <si>
     <t>Returns true or false based on whether or not you are in the middle of an action. True between precast and aftercast. Will not be accurate if packets are dropped.</t>
+  </si>
+  <si>
+    <t>buff_change(name,gain)</t>
+  </si>
+  <si>
+    <t>Passes the new buff name and a boolean that indicates whether it was gained (true) or lost (false).</t>
+  </si>
+  <si>
+    <t>Passes the resources line for the spell with a few modifications. Occurs when the "readies" action packet is received from the server.</t>
+  </si>
+  <si>
+    <t>Passes the resources line for the spell with a few modifications. Occurs when the "result" action packet is received from the server.</t>
+  </si>
+  <si>
+    <t>Passes the resources line for the spell with a few modifications. Occurs when the command text hits the outgoing text buffer. Does not occur for some rare actions that bypass the outgoing text buffer (like using a HELM item from the menu). cancel_spell() and change_target() are implemented in this phase.</t>
+  </si>
+  <si>
+    <t>Passes the resources line for the spell with a few modifications. Occurs when the outgoing action packet is cued. verify_equip(), force_send(), and cast_delay() are implemented in this phase. cancel_spell() is also implemented in this phase.</t>
   </si>
 </sst>
 </file>
@@ -2354,8 +2354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F310"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="F264" sqref="F264"/>
+    <sheetView tabSelected="1" topLeftCell="F262" workbookViewId="0">
+      <selection activeCell="F270" sqref="F270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2369,14 +2369,14 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25.95" x14ac:dyDescent="0.5">
       <c r="B1" s="6" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>148</v>
@@ -2411,7 +2411,7 @@
         <v>140</v>
       </c>
       <c r="F4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2426,7 +2426,7 @@
         <v>142</v>
       </c>
       <c r="F5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2441,7 +2441,7 @@
         <v>140</v>
       </c>
       <c r="F6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2456,7 +2456,7 @@
         <v>140</v>
       </c>
       <c r="F7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2468,10 +2468,10 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F8" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2483,10 +2483,10 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2501,7 +2501,7 @@
         <v>140</v>
       </c>
       <c r="F10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2513,10 +2513,10 @@
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2528,46 +2528,46 @@
         <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F12" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="D13" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E13" t="s">
         <v>140</v>
       </c>
       <c r="F13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="D14" t="s">
+        <v>251</v>
+      </c>
+      <c r="E14" t="s">
+        <v>140</v>
+      </c>
+      <c r="F14" t="s">
         <v>253</v>
-      </c>
-      <c r="E14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F14" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="D15" t="s">
+        <v>252</v>
+      </c>
+      <c r="E15" t="s">
+        <v>140</v>
+      </c>
+      <c r="F15" t="s">
         <v>254</v>
-      </c>
-      <c r="E15" t="s">
-        <v>140</v>
-      </c>
-      <c r="F15" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2578,7 +2578,7 @@
     </row>
     <row r="18" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B18" t="s">
         <v>72</v>
@@ -2590,7 +2590,7 @@
         <v>140</v>
       </c>
       <c r="F18" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2605,7 +2605,7 @@
         <v>140</v>
       </c>
       <c r="F19" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2620,7 +2620,7 @@
         <v>140</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2632,10 +2632,10 @@
         <v>79</v>
       </c>
       <c r="E21" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F21" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2647,10 +2647,10 @@
         <v>81</v>
       </c>
       <c r="E22" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F22" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2662,231 +2662,231 @@
         <v>83</v>
       </c>
       <c r="E23" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F23" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12"/>
       <c r="D24" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E24" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F24" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12"/>
       <c r="D25" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E25" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F25" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12"/>
       <c r="D26" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E26" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F26" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12"/>
       <c r="D27" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="E27" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F27" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
       <c r="D28" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="E28" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F28" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="12"/>
       <c r="D29" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E29" t="s">
         <v>140</v>
       </c>
       <c r="F29" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12"/>
       <c r="D30" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E30" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F30" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="12"/>
       <c r="D31" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E31" t="s">
         <v>140</v>
       </c>
       <c r="F31" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12"/>
       <c r="D32" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E32" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F32" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="12"/>
       <c r="D33" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E33" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F33" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="12"/>
       <c r="D34" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E34" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F34" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12"/>
       <c r="D35" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="E35" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F35" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="12"/>
       <c r="D36" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E36" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F36" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12"/>
       <c r="D37" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="E37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F37" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="12"/>
       <c r="D38" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E38" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F38" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="12"/>
       <c r="D39" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E39" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F39" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="12"/>
       <c r="D40" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="E40" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F40" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="12"/>
       <c r="D41" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E41" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F41" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B44" t="s">
         <v>21</v>
@@ -2898,7 +2898,7 @@
         <v>140</v>
       </c>
       <c r="F44" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2913,7 +2913,7 @@
         <v>140</v>
       </c>
       <c r="F45" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2925,10 +2925,10 @@
         <v>27</v>
       </c>
       <c r="E46" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F46" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2940,10 +2940,10 @@
         <v>29</v>
       </c>
       <c r="E47" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F47" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2955,10 +2955,10 @@
         <v>31</v>
       </c>
       <c r="E48" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F48" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2970,10 +2970,10 @@
         <v>34</v>
       </c>
       <c r="E49" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F49" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2985,10 +2985,10 @@
         <v>35</v>
       </c>
       <c r="E50" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F50" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3000,10 +3000,10 @@
         <v>37</v>
       </c>
       <c r="E51" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F51" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3015,22 +3015,22 @@
         <v>39</v>
       </c>
       <c r="E52" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F52" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="12"/>
       <c r="D53" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E53" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F53" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3045,19 +3045,19 @@
         <v>140</v>
       </c>
       <c r="F54" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="12"/>
       <c r="D55" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E55" t="s">
         <v>140</v>
       </c>
       <c r="F55" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3069,22 +3069,22 @@
         <v>45</v>
       </c>
       <c r="E56" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F56" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="12"/>
       <c r="D57" t="s">
+        <v>335</v>
+      </c>
+      <c r="E57" t="s">
+        <v>268</v>
+      </c>
+      <c r="F57" t="s">
         <v>337</v>
-      </c>
-      <c r="E57" t="s">
-        <v>270</v>
-      </c>
-      <c r="F57" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3099,19 +3099,19 @@
         <v>140</v>
       </c>
       <c r="F58" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="12"/>
       <c r="D59" t="s">
+        <v>336</v>
+      </c>
+      <c r="E59" t="s">
+        <v>140</v>
+      </c>
+      <c r="F59" t="s">
         <v>338</v>
-      </c>
-      <c r="E59" t="s">
-        <v>140</v>
-      </c>
-      <c r="F59" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3123,10 +3123,10 @@
         <v>47</v>
       </c>
       <c r="E60" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F60" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3138,7 +3138,7 @@
         <v>50</v>
       </c>
       <c r="E61" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F61" t="s">
         <v>150</v>
@@ -3153,250 +3153,250 @@
         <v>52</v>
       </c>
       <c r="E62" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F62" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="12"/>
       <c r="D63" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F63" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="12"/>
       <c r="D64" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E64" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F64" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="12"/>
       <c r="D65" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E65" t="s">
         <v>140</v>
       </c>
       <c r="F65" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="12"/>
       <c r="D66" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E66" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F66" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="12"/>
       <c r="D67" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E67" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F67" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="12"/>
       <c r="D68" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E68" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F68" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="12"/>
       <c r="D69" t="s">
+        <v>343</v>
+      </c>
+      <c r="E69" t="s">
+        <v>268</v>
+      </c>
+      <c r="F69" t="s">
         <v>345</v>
-      </c>
-      <c r="E69" t="s">
-        <v>270</v>
-      </c>
-      <c r="F69" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="12"/>
       <c r="D70" t="s">
+        <v>344</v>
+      </c>
+      <c r="E70" t="s">
+        <v>268</v>
+      </c>
+      <c r="F70" t="s">
         <v>346</v>
-      </c>
-      <c r="E70" t="s">
-        <v>270</v>
-      </c>
-      <c r="F70" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="12"/>
       <c r="D71" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E71" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F71" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="12"/>
       <c r="D72" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E72" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F72" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="12"/>
       <c r="D73" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E73" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F73" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="12"/>
       <c r="D74" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E74" t="s">
         <v>140</v>
       </c>
       <c r="F74" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="12"/>
       <c r="D75" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E75" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F75" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="12"/>
       <c r="D76" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E76" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F76" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="12"/>
       <c r="D77" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E77" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F77" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="12"/>
       <c r="D78" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E78" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F78" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="12"/>
       <c r="D79" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E79" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F79" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="12"/>
       <c r="D80" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E80" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F80" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="12"/>
       <c r="D81" t="s">
+        <v>391</v>
+      </c>
+      <c r="E81" t="s">
+        <v>268</v>
+      </c>
+      <c r="F81" t="s">
         <v>393</v>
-      </c>
-      <c r="E81" t="s">
-        <v>270</v>
-      </c>
-      <c r="F81" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="12"/>
       <c r="D82" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E82" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F82" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3407,7 +3407,7 @@
     </row>
     <row r="85" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="12" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B85" t="s">
         <v>94</v>
@@ -3419,7 +3419,7 @@
         <v>140</v>
       </c>
       <c r="F85" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3434,7 +3434,7 @@
         <v>140</v>
       </c>
       <c r="F86" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3449,7 +3449,7 @@
         <v>140</v>
       </c>
       <c r="F87" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3464,187 +3464,187 @@
         <v>140</v>
       </c>
       <c r="F88" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="12"/>
       <c r="B89" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D89" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E89" t="s">
         <v>140</v>
       </c>
       <c r="F89" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="12"/>
       <c r="B90" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D90" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E90" t="s">
         <v>140</v>
       </c>
       <c r="F90" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="12"/>
       <c r="B91" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D91" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E91" t="s">
         <v>140</v>
       </c>
       <c r="F91" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="12"/>
       <c r="B92" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D92" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E92" t="s">
         <v>140</v>
       </c>
       <c r="F92" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="12"/>
       <c r="B93" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D93" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E93" t="s">
         <v>140</v>
       </c>
       <c r="F93" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="12"/>
       <c r="B94" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D94" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E94" t="s">
         <v>140</v>
       </c>
       <c r="F94" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="12"/>
       <c r="B95" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D95" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E95" t="s">
         <v>140</v>
       </c>
       <c r="F95" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="12"/>
       <c r="B96" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D96" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E96" t="s">
         <v>140</v>
       </c>
       <c r="F96" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="12"/>
       <c r="B97" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D97" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E97" t="s">
         <v>140</v>
       </c>
       <c r="F97" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="12"/>
       <c r="B98" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D98" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E98" t="s">
         <v>140</v>
       </c>
       <c r="F98" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="12"/>
       <c r="B99" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D99" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E99" t="s">
         <v>140</v>
       </c>
       <c r="F99" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="12"/>
       <c r="B100" t="s">
+        <v>294</v>
+      </c>
+      <c r="D100" t="s">
+        <v>322</v>
+      </c>
+      <c r="E100" t="s">
+        <v>140</v>
+      </c>
+      <c r="F100" t="s">
         <v>296</v>
-      </c>
-      <c r="D100" t="s">
-        <v>324</v>
-      </c>
-      <c r="E100" t="s">
-        <v>140</v>
-      </c>
-      <c r="F100" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3655,7 +3655,7 @@
     </row>
     <row r="103" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="12" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B103" t="s">
         <v>67</v>
@@ -3667,7 +3667,7 @@
         <v>140</v>
       </c>
       <c r="F103" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3682,7 +3682,7 @@
         <v>140</v>
       </c>
       <c r="F104" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3694,10 +3694,10 @@
         <v>86</v>
       </c>
       <c r="E105" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F105" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3709,10 +3709,10 @@
         <v>87</v>
       </c>
       <c r="E106" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F106" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3724,7 +3724,7 @@
         <v>88</v>
       </c>
       <c r="E107" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F107" t="s">
         <v>152</v>
@@ -3733,217 +3733,217 @@
     <row r="108" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="12"/>
       <c r="D108" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E108" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F108" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="12"/>
       <c r="D109" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E109" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F109" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="12"/>
       <c r="D110" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E110" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F110" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="12"/>
       <c r="D111" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E111" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F111" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="12"/>
       <c r="D112" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E112" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F112" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="12"/>
       <c r="D113" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E113" t="s">
         <v>140</v>
       </c>
       <c r="F113" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="12"/>
       <c r="D114" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E114" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F114" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="12"/>
       <c r="D115" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E115" t="s">
         <v>140</v>
       </c>
       <c r="F115" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="12"/>
       <c r="D116" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E116" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F116" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="12"/>
       <c r="D117" t="s">
+        <v>374</v>
+      </c>
+      <c r="E117" t="s">
+        <v>268</v>
+      </c>
+      <c r="F117" t="s">
         <v>376</v>
-      </c>
-      <c r="E117" t="s">
-        <v>270</v>
-      </c>
-      <c r="F117" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="12"/>
       <c r="D118" t="s">
+        <v>375</v>
+      </c>
+      <c r="E118" t="s">
+        <v>268</v>
+      </c>
+      <c r="F118" t="s">
         <v>377</v>
-      </c>
-      <c r="E118" t="s">
-        <v>270</v>
-      </c>
-      <c r="F118" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="12"/>
       <c r="D119" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E119" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F119" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="12"/>
       <c r="D120" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E120" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F120" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="12"/>
       <c r="D121" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E121" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F121" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="12"/>
       <c r="D122" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E122" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F122" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="12"/>
       <c r="D123" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E123" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F123" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="12"/>
       <c r="D124" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E124" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F124" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="12"/>
       <c r="D125" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E125" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F125" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3954,280 +3954,280 @@
     </row>
     <row r="128" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="12" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D128" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="E128" t="s">
         <v>140</v>
       </c>
       <c r="F128" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="12"/>
       <c r="D129" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E129" t="s">
         <v>140</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="12"/>
       <c r="D130" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="E130" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F130" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="12"/>
       <c r="D131" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="E131" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F131" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="12"/>
       <c r="D132" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="E132" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F132" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="12"/>
       <c r="D133" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="E133" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F133" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" s="12"/>
       <c r="D134" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="E134" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F134" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="12"/>
       <c r="D135" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="E135" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F135" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="12"/>
       <c r="D136" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="E136" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F136" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="12"/>
       <c r="D137" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="E137" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F137" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="12"/>
       <c r="D138" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="E138" t="s">
         <v>140</v>
       </c>
       <c r="F138" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="12"/>
       <c r="D139" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="E139" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F139" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="12"/>
       <c r="D140" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E140" t="s">
         <v>140</v>
       </c>
       <c r="F140" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="12"/>
       <c r="D141" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E141" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F141" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="12"/>
       <c r="D142" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="E142" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F142" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="12"/>
       <c r="D143" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="E143" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F143" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="12"/>
       <c r="D144" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E144" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F144" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="12"/>
       <c r="D145" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="E145" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F145" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="12"/>
       <c r="D146" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E146" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F146" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="12"/>
       <c r="D147" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E147" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F147" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="12"/>
       <c r="D148" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E148" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F148" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="12"/>
       <c r="D149" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="E149" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F149" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="12"/>
       <c r="D150" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E150" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F150" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -4238,7 +4238,7 @@
     </row>
     <row r="153" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="12" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D153" t="s">
         <v>89</v>
@@ -4247,7 +4247,7 @@
         <v>140</v>
       </c>
       <c r="F153" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="154" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4259,7 +4259,7 @@
         <v>140</v>
       </c>
       <c r="F154" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="155" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4268,10 +4268,10 @@
         <v>91</v>
       </c>
       <c r="E155" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F155" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="156" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4280,10 +4280,10 @@
         <v>92</v>
       </c>
       <c r="E156" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F156" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4292,7 +4292,7 @@
         <v>93</v>
       </c>
       <c r="E157" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F157" t="s">
         <v>151</v>
@@ -4301,217 +4301,217 @@
     <row r="158" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="12"/>
       <c r="D158" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E158" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F158" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="12"/>
       <c r="D159" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E159" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F159" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="12"/>
       <c r="D160" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E160" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F160" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="12"/>
       <c r="D161" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E161" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F161" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="12"/>
       <c r="D162" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E162" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F162" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="12"/>
       <c r="D163" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E163" t="s">
         <v>140</v>
       </c>
       <c r="F163" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="12"/>
       <c r="D164" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E164" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F164" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="12"/>
       <c r="D165" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E165" t="s">
         <v>140</v>
       </c>
       <c r="F165" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="166" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="12"/>
       <c r="D166" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E166" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F166" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="12"/>
       <c r="D167" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E167" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F167" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="12"/>
       <c r="D168" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E168" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F168" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="169" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="12"/>
       <c r="D169" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E169" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F169" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="170" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="12"/>
       <c r="D170" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E170" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F170" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="12"/>
       <c r="D171" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E171" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F171" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="12"/>
       <c r="D172" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E172" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F172" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="12"/>
       <c r="D173" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E173" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F173" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="12"/>
       <c r="D174" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E174" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F174" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="12"/>
       <c r="D175" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E175" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F175" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="176" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4519,7 +4519,7 @@
     </row>
     <row r="178" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="12" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B178" t="s">
         <v>98</v>
@@ -4531,7 +4531,7 @@
         <v>140</v>
       </c>
       <c r="F178" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4543,7 +4543,7 @@
         <v>101</v>
       </c>
       <c r="E179" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F179" t="s">
         <v>153</v>
@@ -4573,22 +4573,22 @@
         <v>105</v>
       </c>
       <c r="E181" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F181" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="182" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="12"/>
       <c r="D182" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E182" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F182" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="183" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4600,10 +4600,10 @@
         <v>107</v>
       </c>
       <c r="E183" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F183" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="184" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4621,174 +4621,174 @@
     <row r="185" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="12"/>
       <c r="D185" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E185" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F185" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="12"/>
       <c r="D186" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E186" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F186" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="12"/>
       <c r="D187" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E187" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F187" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="188" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="12"/>
       <c r="D188" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="E188" t="s">
         <v>140</v>
       </c>
       <c r="F188" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="189" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="12"/>
       <c r="D189" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E189" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F189" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="190" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="12"/>
       <c r="D190" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E190" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F190" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="12"/>
       <c r="D191" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E191" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F191" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="192" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="12"/>
       <c r="D192" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E192" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F192" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="193" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="12"/>
       <c r="D193" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E193" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F193" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="194" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="12"/>
       <c r="D194" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E194" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F194" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="195" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="12"/>
       <c r="D195" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E195" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F195" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="196" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="12"/>
       <c r="D196" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="E196" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F196" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="197" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="12"/>
       <c r="D197" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E197" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F197" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="200" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="12" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B200" t="s">
         <v>109</v>
       </c>
       <c r="D200" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E200" t="s">
         <v>140</v>
       </c>
       <c r="F200" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="201" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4797,13 +4797,13 @@
         <v>110</v>
       </c>
       <c r="D201" t="s">
+        <v>226</v>
+      </c>
+      <c r="E201" t="s">
+        <v>269</v>
+      </c>
+      <c r="F201" t="s">
         <v>228</v>
-      </c>
-      <c r="E201" t="s">
-        <v>271</v>
-      </c>
-      <c r="F201" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="202" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4812,67 +4812,67 @@
         <v>111</v>
       </c>
       <c r="D202" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E202" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F202" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="203" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="12"/>
       <c r="D203" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="E203" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F203" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="204" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="12"/>
       <c r="D204" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E204" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F204" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="205" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="12"/>
       <c r="D205" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="E205" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F205" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="206" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="12"/>
       <c r="D206" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="E206" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F206" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="207" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="12"/>
       <c r="D207" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="E207" t="s">
         <v>140</v>
@@ -4881,138 +4881,138 @@
     <row r="208" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="12"/>
       <c r="D208" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E208" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F208" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="209" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="12"/>
       <c r="D209" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E209" t="s">
         <v>140</v>
       </c>
       <c r="F209" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="210" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="12"/>
       <c r="D210" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E210" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F210" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="211" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="12"/>
       <c r="D211" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E211" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F211" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="212" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="12"/>
       <c r="D212" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="E212" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F212" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="213" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="12"/>
       <c r="D213" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E213" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F213" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="214" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="12"/>
       <c r="D214" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E214" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F214" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="215" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="12"/>
       <c r="D215" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E215" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F215" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="216" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="12"/>
       <c r="D216" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="E216" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F216" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="217" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="12"/>
       <c r="D217" t="s">
+        <v>472</v>
+      </c>
+      <c r="E217" t="s">
+        <v>268</v>
+      </c>
+      <c r="F217" t="s">
         <v>474</v>
-      </c>
-      <c r="E217" t="s">
-        <v>270</v>
-      </c>
-      <c r="F217" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="218" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="12"/>
       <c r="D218" t="s">
+        <v>473</v>
+      </c>
+      <c r="E218" t="s">
+        <v>268</v>
+      </c>
+      <c r="F218" t="s">
         <v>475</v>
-      </c>
-      <c r="E218" t="s">
-        <v>270</v>
-      </c>
-      <c r="F218" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="221" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="12" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B221" t="s">
         <v>48</v>
@@ -5021,7 +5021,7 @@
         <v>156</v>
       </c>
       <c r="E221" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F221" t="s">
         <v>159</v>
@@ -5033,7 +5033,7 @@
         <v>157</v>
       </c>
       <c r="E222" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F222" t="s">
         <v>158</v>
@@ -5048,7 +5048,7 @@
         <v>142</v>
       </c>
       <c r="F223" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="224" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5066,25 +5066,25 @@
     <row r="225" spans="1:6" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="12"/>
       <c r="D225" s="9" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E225" s="9" t="s">
         <v>142</v>
       </c>
       <c r="F225" s="9" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="226" spans="1:6" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="12"/>
       <c r="D226" s="9" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E226" s="9" t="s">
         <v>142</v>
       </c>
       <c r="F226" s="9" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="227" spans="1:6" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5095,7 +5095,7 @@
     </row>
     <row r="230" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="12" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B230" t="s">
         <v>24</v>
@@ -5107,7 +5107,7 @@
         <v>140</v>
       </c>
       <c r="F230" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="231" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5119,10 +5119,10 @@
         <v>54</v>
       </c>
       <c r="E231" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F231" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="232" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5137,7 +5137,7 @@
         <v>140</v>
       </c>
       <c r="F232" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="233" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5152,19 +5152,19 @@
         <v>140</v>
       </c>
       <c r="F233" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="234" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="12"/>
       <c r="D234" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E234" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F234" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="235" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5179,7 +5179,7 @@
         <v>140</v>
       </c>
       <c r="F235" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="236" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5194,7 +5194,7 @@
         <v>140</v>
       </c>
       <c r="F236" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="237" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5209,7 +5209,7 @@
         <v>140</v>
       </c>
       <c r="F237" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="238" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5221,46 +5221,46 @@
         <v>66</v>
       </c>
       <c r="E238" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F238" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="239" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="12"/>
       <c r="D239" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E239" t="s">
         <v>140</v>
       </c>
       <c r="F239" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="240" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="12"/>
       <c r="D240" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E240" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F240" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="241" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="12"/>
       <c r="D241" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E241" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F241" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="244" spans="1:6" ht="21" x14ac:dyDescent="0.35">
@@ -5277,7 +5277,7 @@
         <v>142</v>
       </c>
       <c r="F244" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="247" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5285,16 +5285,16 @@
         <v>119</v>
       </c>
       <c r="B247" t="s">
+        <v>519</v>
+      </c>
+      <c r="D247" t="s">
+        <v>520</v>
+      </c>
+      <c r="E247" t="s">
+        <v>506</v>
+      </c>
+      <c r="F247" t="s">
         <v>521</v>
-      </c>
-      <c r="D247" t="s">
-        <v>522</v>
-      </c>
-      <c r="E247" t="s">
-        <v>508</v>
-      </c>
-      <c r="F247" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="248" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5306,10 +5306,10 @@
         <v>134</v>
       </c>
       <c r="E248" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F248" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
     </row>
     <row r="249" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5321,10 +5321,10 @@
         <v>163</v>
       </c>
       <c r="E249" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F249" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
     </row>
     <row r="250" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5333,16 +5333,16 @@
         <v>130</v>
       </c>
       <c r="C250" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D250" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E250" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F250" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="251" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5354,10 +5354,10 @@
         <v>133</v>
       </c>
       <c r="E251" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F251" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="252" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5369,10 +5369,10 @@
         <v>164</v>
       </c>
       <c r="E252" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F252" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="253" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5381,13 +5381,13 @@
         <v>139</v>
       </c>
       <c r="D253" t="s">
+        <v>211</v>
+      </c>
+      <c r="E253" t="s">
+        <v>506</v>
+      </c>
+      <c r="F253" t="s">
         <v>213</v>
-      </c>
-      <c r="E253" t="s">
-        <v>508</v>
-      </c>
-      <c r="F253" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="254" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5399,10 +5399,10 @@
         <v>129</v>
       </c>
       <c r="E254" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F254" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
     </row>
     <row r="255" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5414,7 +5414,7 @@
         <v>138</v>
       </c>
       <c r="E255" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F255" t="s">
         <v>165</v>
@@ -5429,7 +5429,7 @@
         <v>135</v>
       </c>
       <c r="E256" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F256" t="s">
         <v>166</v>
@@ -5444,7 +5444,7 @@
         <v>136</v>
       </c>
       <c r="E257" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F257" t="s">
         <v>167</v>
@@ -5459,7 +5459,7 @@
         <v>137</v>
       </c>
       <c r="E258" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F258" t="s">
         <v>168</v>
@@ -5471,13 +5471,13 @@
         <v>0</v>
       </c>
       <c r="D259" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E259" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F259" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="260" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5486,10 +5486,10 @@
         <v>0</v>
       </c>
       <c r="D260" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E260" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F260" t="s">
         <v>169</v>
@@ -5498,16 +5498,16 @@
     <row r="261" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A261" s="12"/>
       <c r="B261" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D261" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E261" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F261" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="262" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5519,7 +5519,7 @@
         <v>0</v>
       </c>
       <c r="F262" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="263" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5528,13 +5528,13 @@
         <v>124</v>
       </c>
       <c r="D263" t="s">
+        <v>207</v>
+      </c>
+      <c r="E263" t="s">
+        <v>506</v>
+      </c>
+      <c r="F263" t="s">
         <v>209</v>
-      </c>
-      <c r="E263" t="s">
-        <v>508</v>
-      </c>
-      <c r="F263" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="264" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5543,25 +5543,25 @@
         <v>125</v>
       </c>
       <c r="D264" t="s">
+        <v>208</v>
+      </c>
+      <c r="E264" t="s">
+        <v>506</v>
+      </c>
+      <c r="F264" t="s">
         <v>210</v>
-      </c>
-      <c r="E264" t="s">
-        <v>508</v>
-      </c>
-      <c r="F264" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="265" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A265" s="12"/>
       <c r="D265" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="E265" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F265" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
     </row>
     <row r="266" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5572,28 +5572,28 @@
     </row>
     <row r="268" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" s="13" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D268" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E268" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F268" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="269" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" s="13"/>
       <c r="D269" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="E269" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F269" t="s">
-        <v>628</v>
+        <v>638</v>
       </c>
     </row>
     <row r="270" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5602,13 +5602,13 @@
         <v>181</v>
       </c>
       <c r="D270" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E270" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F270" t="s">
-        <v>629</v>
+        <v>639</v>
       </c>
     </row>
     <row r="271" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5617,13 +5617,13 @@
         <v>182</v>
       </c>
       <c r="D271" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E271" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F271" t="s">
-        <v>630</v>
+        <v>636</v>
       </c>
     </row>
     <row r="272" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5632,85 +5632,85 @@
         <v>183</v>
       </c>
       <c r="D272" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E272" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F272" t="s">
-        <v>631</v>
+        <v>637</v>
       </c>
     </row>
     <row r="273" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A273" s="13"/>
       <c r="D273" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E273" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F273" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
     </row>
     <row r="274" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" s="13"/>
       <c r="D274" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E274" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F274" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
     </row>
     <row r="275" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A275" s="13"/>
       <c r="D275" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E275" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F275" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="276" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A276" s="13"/>
       <c r="D276" t="s">
-        <v>184</v>
+        <v>634</v>
       </c>
       <c r="E276" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F276" t="s">
-        <v>191</v>
+        <v>635</v>
       </c>
     </row>
     <row r="277" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A277" s="13"/>
       <c r="D277" t="s">
+        <v>189</v>
+      </c>
+      <c r="E277" t="s">
+        <v>506</v>
+      </c>
+      <c r="F277" t="s">
         <v>190</v>
-      </c>
-      <c r="E277" t="s">
-        <v>508</v>
-      </c>
-      <c r="F277" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="278" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A278" s="13"/>
       <c r="D278" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E278" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F278" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
     </row>
     <row r="281" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5772,7 +5772,7 @@
         <v>0</v>
       </c>
       <c r="F285" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="286" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5819,13 +5819,13 @@
         <v>0</v>
       </c>
       <c r="D290" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E290" t="s">
         <v>142</v>
       </c>
       <c r="F290" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="291" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5849,13 +5849,13 @@
         <v>0</v>
       </c>
       <c r="D292" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="E292" t="s">
         <v>142</v>
       </c>
       <c r="F292" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="293" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5864,13 +5864,13 @@
         <v>0</v>
       </c>
       <c r="D293" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="E293" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F293" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="294" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5882,7 +5882,7 @@
         <v>144</v>
       </c>
       <c r="E294" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F294" t="s">
         <v>177</v>
@@ -5897,7 +5897,7 @@
         <v>145</v>
       </c>
       <c r="E295" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F295" t="s">
         <v>178</v>
@@ -5912,7 +5912,7 @@
         <v>146</v>
       </c>
       <c r="E296" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F296" t="s">
         <v>179</v>
@@ -5927,7 +5927,7 @@
         <v>147</v>
       </c>
       <c r="E297" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F297" t="s">
         <v>180</v>
@@ -5941,106 +5941,106 @@
     </row>
     <row r="300" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A300" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D300" t="s">
+        <v>192</v>
+      </c>
+      <c r="F300" t="s">
         <v>193</v>
-      </c>
-      <c r="D300" t="s">
-        <v>194</v>
-      </c>
-      <c r="F300" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="301" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A301" s="12"/>
       <c r="D301" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F301" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="302" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A302" s="12"/>
       <c r="D302" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F302" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="303" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A303" s="12"/>
       <c r="D303" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F303" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="304" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A304" s="12"/>
       <c r="D304" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F304" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="305" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A305" s="12"/>
       <c r="B305" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D305" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F305" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="306" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A306" s="12"/>
       <c r="B306" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D306" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F306" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="307" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A307" s="12"/>
       <c r="B307" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D307" t="s">
+        <v>219</v>
+      </c>
+      <c r="F307" t="s">
         <v>221</v>
-      </c>
-      <c r="F307" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="308" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A308" s="12"/>
       <c r="B308" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D308" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F308" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="309" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A309" s="12"/>
       <c r="D309" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F309" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="310" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -6048,22 +6048,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A268:A278"/>
     <mergeCell ref="A44:A82"/>
     <mergeCell ref="A18:A41"/>
     <mergeCell ref="A3:A15"/>
     <mergeCell ref="A103:A125"/>
+    <mergeCell ref="A200:A218"/>
+    <mergeCell ref="A178:A197"/>
+    <mergeCell ref="A128:A150"/>
+    <mergeCell ref="A153:A175"/>
+    <mergeCell ref="A85:A100"/>
     <mergeCell ref="A300:A309"/>
     <mergeCell ref="A288:A297"/>
     <mergeCell ref="A281:A285"/>
     <mergeCell ref="A221:A226"/>
     <mergeCell ref="A230:A241"/>
     <mergeCell ref="A247:A265"/>
-    <mergeCell ref="A200:A218"/>
-    <mergeCell ref="A178:A197"/>
-    <mergeCell ref="A128:A150"/>
-    <mergeCell ref="A153:A175"/>
-    <mergeCell ref="A85:A100"/>
+    <mergeCell ref="A268:A278"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GearSwap - v0.800 STRIKES BACK
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variables.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="642">
   <si>
     <t>N/A</t>
   </si>
@@ -1959,6 +1959,12 @@
   </si>
   <si>
     <t>Passes the resources line for the spell with a few modifications. Occurs when the outgoing action packet is cued. verify_equip(), force_send(), and cast_delay() are implemented in this phase. cancel_spell() is also implemented in this phase.</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Library that deals with lists.</t>
   </si>
 </sst>
 </file>
@@ -2352,22 +2358,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F310"/>
+  <dimension ref="A1:F311"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F262" workbookViewId="0">
-      <selection activeCell="F270" sqref="F270"/>
+    <sheetView tabSelected="1" topLeftCell="A283" workbookViewId="0">
+      <selection activeCell="D289" sqref="D289"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" customWidth="1"/>
-    <col min="4" max="4" width="40.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="202.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="202.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.95" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="25.9" x14ac:dyDescent="0.5">
       <c r="B1" s="6" t="s">
         <v>503</v>
       </c>
@@ -2382,7 +2388,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
@@ -2399,7 +2405,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" t="s">
         <v>2</v>
@@ -2414,7 +2420,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" t="s">
         <v>4</v>
@@ -2429,7 +2435,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" t="s">
         <v>6</v>
@@ -2444,7 +2450,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" t="s">
         <v>8</v>
@@ -2459,7 +2465,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" t="s">
         <v>10</v>
@@ -2474,7 +2480,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" t="s">
         <v>12</v>
@@ -2489,7 +2495,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" t="s">
         <v>14</v>
@@ -2504,7 +2510,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" t="s">
         <v>16</v>
@@ -2519,7 +2525,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" t="s">
         <v>18</v>
@@ -2534,7 +2540,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="D13" t="s">
         <v>250</v>
@@ -2546,7 +2552,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="D14" t="s">
         <v>251</v>
@@ -2558,7 +2564,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="D15" t="s">
         <v>252</v>
@@ -2570,13 +2576,13 @@
         <v>254</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>618</v>
       </c>
@@ -2593,7 +2599,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" t="s">
         <v>74</v>
@@ -2608,7 +2614,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" t="s">
         <v>76</v>
@@ -2623,7 +2629,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" t="s">
         <v>78</v>
@@ -2638,7 +2644,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" t="s">
         <v>80</v>
@@ -2653,7 +2659,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" t="s">
         <v>82</v>
@@ -2668,7 +2674,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="D24" t="s">
         <v>601</v>
@@ -2680,7 +2686,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="D25" t="s">
         <v>584</v>
@@ -2692,7 +2698,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="D26" t="s">
         <v>585</v>
@@ -2704,7 +2710,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="D27" t="s">
         <v>586</v>
@@ -2716,7 +2722,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="D28" t="s">
         <v>587</v>
@@ -2728,7 +2734,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="D29" t="s">
         <v>588</v>
@@ -2740,7 +2746,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="D30" t="s">
         <v>589</v>
@@ -2752,7 +2758,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="D31" t="s">
         <v>590</v>
@@ -2764,7 +2770,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="D32" t="s">
         <v>591</v>
@@ -2776,7 +2782,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="D33" t="s">
         <v>592</v>
@@ -2788,7 +2794,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="D34" t="s">
         <v>593</v>
@@ -2800,7 +2806,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="D35" t="s">
         <v>594</v>
@@ -2812,7 +2818,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="D36" t="s">
         <v>595</v>
@@ -2824,7 +2830,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
       <c r="D37" t="s">
         <v>596</v>
@@ -2836,7 +2842,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
       <c r="D38" t="s">
         <v>597</v>
@@ -2848,7 +2854,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="D39" t="s">
         <v>598</v>
@@ -2860,7 +2866,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="D40" t="s">
         <v>599</v>
@@ -2872,7 +2878,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="D41" t="s">
         <v>600</v>
@@ -2884,7 +2890,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>350</v>
       </c>
@@ -2901,7 +2907,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" t="s">
         <v>22</v>
@@ -2916,7 +2922,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" t="s">
         <v>26</v>
@@ -2931,7 +2937,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" t="s">
         <v>28</v>
@@ -2946,7 +2952,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" t="s">
         <v>30</v>
@@ -2961,7 +2967,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12"/>
       <c r="B49" t="s">
         <v>32</v>
@@ -2976,7 +2982,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>
       <c r="B50" t="s">
         <v>33</v>
@@ -2991,7 +2997,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
       <c r="B51" t="s">
         <v>36</v>
@@ -3006,7 +3012,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
       <c r="B52" t="s">
         <v>38</v>
@@ -3021,7 +3027,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12"/>
       <c r="D53" t="s">
         <v>331</v>
@@ -3033,7 +3039,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
       <c r="B54" t="s">
         <v>40</v>
@@ -3048,7 +3054,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
       <c r="D55" t="s">
         <v>333</v>
@@ -3060,7 +3066,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
       <c r="B56" t="s">
         <v>41</v>
@@ -3075,7 +3081,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
       <c r="D57" t="s">
         <v>335</v>
@@ -3087,7 +3093,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12"/>
       <c r="B58" t="s">
         <v>42</v>
@@ -3102,7 +3108,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
       <c r="D59" t="s">
         <v>336</v>
@@ -3114,7 +3120,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12"/>
       <c r="B60" t="s">
         <v>43</v>
@@ -3129,7 +3135,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12"/>
       <c r="B61" t="s">
         <v>49</v>
@@ -3144,7 +3150,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12"/>
       <c r="B62" t="s">
         <v>51</v>
@@ -3159,7 +3165,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="D63" t="s">
         <v>323</v>
@@ -3171,7 +3177,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="D64" t="s">
         <v>325</v>
@@ -3183,7 +3189,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="D65" t="s">
         <v>327</v>
@@ -3195,7 +3201,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="D66" t="s">
         <v>329</v>
@@ -3207,7 +3213,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="D67" t="s">
         <v>330</v>
@@ -3219,7 +3225,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="D68" t="s">
         <v>341</v>
@@ -3231,7 +3237,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="D69" t="s">
         <v>343</v>
@@ -3243,7 +3249,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="D70" t="s">
         <v>344</v>
@@ -3255,7 +3261,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="D71" t="s">
         <v>347</v>
@@ -3267,7 +3273,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="D72" t="s">
         <v>384</v>
@@ -3279,7 +3285,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12"/>
       <c r="D73" t="s">
         <v>385</v>
@@ -3291,7 +3297,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12"/>
       <c r="D74" t="s">
         <v>386</v>
@@ -3303,7 +3309,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12"/>
       <c r="D75" t="s">
         <v>431</v>
@@ -3315,7 +3321,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12"/>
       <c r="D76" t="s">
         <v>522</v>
@@ -3327,7 +3333,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12"/>
       <c r="D77" t="s">
         <v>387</v>
@@ -3339,7 +3345,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12"/>
       <c r="D78" t="s">
         <v>388</v>
@@ -3351,7 +3357,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12"/>
       <c r="D79" t="s">
         <v>389</v>
@@ -3363,7 +3369,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12"/>
       <c r="D80" t="s">
         <v>390</v>
@@ -3375,7 +3381,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12"/>
       <c r="D81" t="s">
         <v>391</v>
@@ -3387,7 +3393,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12"/>
       <c r="D82" t="s">
         <v>392</v>
@@ -3399,13 +3405,13 @@
         <v>381</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
     </row>
-    <row r="84" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="7"/>
     </row>
-    <row r="85" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
         <v>349</v>
       </c>
@@ -3422,7 +3428,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12"/>
       <c r="B86" t="s">
         <v>95</v>
@@ -3437,7 +3443,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12"/>
       <c r="B87" t="s">
         <v>96</v>
@@ -3452,7 +3458,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12"/>
       <c r="B88" t="s">
         <v>97</v>
@@ -3467,7 +3473,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12"/>
       <c r="B89" t="s">
         <v>283</v>
@@ -3482,7 +3488,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12"/>
       <c r="B90" t="s">
         <v>284</v>
@@ -3497,7 +3503,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
       <c r="B91" t="s">
         <v>285</v>
@@ -3512,7 +3518,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
       <c r="B92" t="s">
         <v>286</v>
@@ -3527,7 +3533,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12"/>
       <c r="B93" t="s">
         <v>287</v>
@@ -3542,7 +3548,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12"/>
       <c r="B94" t="s">
         <v>288</v>
@@ -3557,7 +3563,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12"/>
       <c r="B95" t="s">
         <v>289</v>
@@ -3572,7 +3578,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12"/>
       <c r="B96" t="s">
         <v>290</v>
@@ -3587,7 +3593,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
       <c r="B97" t="s">
         <v>291</v>
@@ -3602,7 +3608,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
       <c r="B98" t="s">
         <v>292</v>
@@ -3617,7 +3623,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
       <c r="B99" t="s">
         <v>293</v>
@@ -3632,7 +3638,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12"/>
       <c r="B100" t="s">
         <v>294</v>
@@ -3647,13 +3653,13 @@
         <v>296</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3"/>
     </row>
-    <row r="102" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
     </row>
-    <row r="103" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="s">
         <v>354</v>
       </c>
@@ -3670,7 +3676,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12"/>
       <c r="B104" t="s">
         <v>68</v>
@@ -3685,7 +3691,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12"/>
       <c r="B105" t="s">
         <v>69</v>
@@ -3700,7 +3706,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12"/>
       <c r="B106" t="s">
         <v>70</v>
@@ -3715,7 +3721,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="12"/>
       <c r="B107" t="s">
         <v>71</v>
@@ -3730,7 +3736,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="12"/>
       <c r="D108" t="s">
         <v>358</v>
@@ -3742,7 +3748,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="12"/>
       <c r="D109" t="s">
         <v>365</v>
@@ -3754,7 +3760,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="12"/>
       <c r="D110" t="s">
         <v>366</v>
@@ -3766,7 +3772,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="12"/>
       <c r="D111" t="s">
         <v>357</v>
@@ -3778,7 +3784,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="12"/>
       <c r="D112" t="s">
         <v>359</v>
@@ -3790,7 +3796,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="12"/>
       <c r="D113" t="s">
         <v>360</v>
@@ -3802,7 +3808,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="12"/>
       <c r="D114" t="s">
         <v>430</v>
@@ -3814,7 +3820,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="12"/>
       <c r="D115" t="s">
         <v>583</v>
@@ -3826,7 +3832,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="12"/>
       <c r="D116" t="s">
         <v>524</v>
@@ -3838,7 +3844,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12"/>
       <c r="D117" t="s">
         <v>374</v>
@@ -3850,7 +3856,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="12"/>
       <c r="D118" t="s">
         <v>375</v>
@@ -3862,7 +3868,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="12"/>
       <c r="D119" t="s">
         <v>362</v>
@@ -3874,7 +3880,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="12"/>
       <c r="D120" t="s">
         <v>363</v>
@@ -3886,7 +3892,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="12"/>
       <c r="D121" t="s">
         <v>364</v>
@@ -3898,7 +3904,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="12"/>
       <c r="D122" t="s">
         <v>356</v>
@@ -3910,7 +3916,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="12"/>
       <c r="D123" t="s">
         <v>361</v>
@@ -3922,7 +3928,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="12"/>
       <c r="D124" t="s">
         <v>372</v>
@@ -3934,7 +3940,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="12"/>
       <c r="D125" t="s">
         <v>382</v>
@@ -3946,13 +3952,13 @@
         <v>383</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="10"/>
     </row>
-    <row r="127" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
     </row>
-    <row r="128" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="12" t="s">
         <v>539</v>
       </c>
@@ -3966,7 +3972,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="12"/>
       <c r="D129" t="s">
         <v>560</v>
@@ -3978,7 +3984,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="12"/>
       <c r="D130" t="s">
         <v>561</v>
@@ -3990,7 +3996,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="12"/>
       <c r="D131" t="s">
         <v>562</v>
@@ -4002,7 +4008,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="12"/>
       <c r="D132" t="s">
         <v>563</v>
@@ -4014,7 +4020,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="12"/>
       <c r="D133" t="s">
         <v>564</v>
@@ -4026,7 +4032,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="12"/>
       <c r="D134" t="s">
         <v>565</v>
@@ -4038,7 +4044,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="12"/>
       <c r="D135" t="s">
         <v>566</v>
@@ -4050,7 +4056,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="12"/>
       <c r="D136" t="s">
         <v>567</v>
@@ -4062,7 +4068,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="12"/>
       <c r="D137" t="s">
         <v>568</v>
@@ -4074,7 +4080,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="12"/>
       <c r="D138" t="s">
         <v>569</v>
@@ -4086,7 +4092,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="12"/>
       <c r="D139" t="s">
         <v>570</v>
@@ -4098,7 +4104,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="12"/>
       <c r="D140" t="s">
         <v>571</v>
@@ -4110,7 +4116,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="12"/>
       <c r="D141" t="s">
         <v>572</v>
@@ -4122,7 +4128,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="12"/>
       <c r="D142" t="s">
         <v>573</v>
@@ -4134,7 +4140,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="12"/>
       <c r="D143" t="s">
         <v>574</v>
@@ -4146,7 +4152,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="12"/>
       <c r="D144" t="s">
         <v>575</v>
@@ -4158,7 +4164,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="12"/>
       <c r="D145" t="s">
         <v>576</v>
@@ -4170,7 +4176,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="12"/>
       <c r="D146" t="s">
         <v>577</v>
@@ -4182,7 +4188,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="12"/>
       <c r="D147" t="s">
         <v>578</v>
@@ -4194,7 +4200,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="12"/>
       <c r="D148" t="s">
         <v>579</v>
@@ -4206,7 +4212,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="12"/>
       <c r="D149" t="s">
         <v>580</v>
@@ -4218,7 +4224,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="12"/>
       <c r="D150" t="s">
         <v>581</v>
@@ -4230,13 +4236,13 @@
         <v>417</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="11"/>
     </row>
-    <row r="152" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
     </row>
-    <row r="153" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="12" t="s">
         <v>355</v>
       </c>
@@ -4250,7 +4256,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="12"/>
       <c r="D154" t="s">
         <v>90</v>
@@ -4262,7 +4268,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="12"/>
       <c r="D155" t="s">
         <v>91</v>
@@ -4274,7 +4280,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="12"/>
       <c r="D156" t="s">
         <v>92</v>
@@ -4286,7 +4292,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="12"/>
       <c r="D157" t="s">
         <v>93</v>
@@ -4298,7 +4304,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="12"/>
       <c r="D158" t="s">
         <v>398</v>
@@ -4310,7 +4316,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="12"/>
       <c r="D159" t="s">
         <v>403</v>
@@ -4322,7 +4328,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="12"/>
       <c r="D160" t="s">
         <v>404</v>
@@ -4334,7 +4340,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="12"/>
       <c r="D161" t="s">
         <v>405</v>
@@ -4346,7 +4352,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="12"/>
       <c r="D162" t="s">
         <v>406</v>
@@ -4358,7 +4364,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="12"/>
       <c r="D163" t="s">
         <v>407</v>
@@ -4370,7 +4376,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="12"/>
       <c r="D164" t="s">
         <v>429</v>
@@ -4382,7 +4388,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="12"/>
       <c r="D165" t="s">
         <v>534</v>
@@ -4394,7 +4400,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="12"/>
       <c r="D166" t="s">
         <v>525</v>
@@ -4406,7 +4412,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="12"/>
       <c r="D167" t="s">
         <v>408</v>
@@ -4418,7 +4424,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="12"/>
       <c r="D168" t="s">
         <v>409</v>
@@ -4430,7 +4436,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="12"/>
       <c r="D169" t="s">
         <v>410</v>
@@ -4442,7 +4448,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="12"/>
       <c r="D170" t="s">
         <v>411</v>
@@ -4454,7 +4460,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="12"/>
       <c r="D171" t="s">
         <v>412</v>
@@ -4466,7 +4472,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="12"/>
       <c r="D172" t="s">
         <v>413</v>
@@ -4478,7 +4484,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="12"/>
       <c r="D173" t="s">
         <v>414</v>
@@ -4490,7 +4496,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="12"/>
       <c r="D174" t="s">
         <v>415</v>
@@ -4502,7 +4508,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="12"/>
       <c r="D175" t="s">
         <v>416</v>
@@ -4514,10 +4520,10 @@
         <v>417</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="3"/>
     </row>
-    <row r="178" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="12" t="s">
         <v>351</v>
       </c>
@@ -4534,7 +4540,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="12"/>
       <c r="B179" t="s">
         <v>100</v>
@@ -4549,7 +4555,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="12"/>
       <c r="B180" t="s">
         <v>102</v>
@@ -4564,7 +4570,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12"/>
       <c r="B181" t="s">
         <v>104</v>
@@ -4579,7 +4585,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="12"/>
       <c r="D182" t="s">
         <v>434</v>
@@ -4591,7 +4597,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="12"/>
       <c r="B183" t="s">
         <v>108</v>
@@ -4606,7 +4612,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="12"/>
       <c r="B184" t="s">
         <v>106</v>
@@ -4618,7 +4624,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="12"/>
       <c r="D185" t="s">
         <v>437</v>
@@ -4630,7 +4636,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="12"/>
       <c r="D186" t="s">
         <v>438</v>
@@ -4642,7 +4648,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="12"/>
       <c r="D187" t="s">
         <v>439</v>
@@ -4654,7 +4660,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="12"/>
       <c r="D188" t="s">
         <v>528</v>
@@ -4666,7 +4672,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="189" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="12"/>
       <c r="D189" t="s">
         <v>526</v>
@@ -4678,7 +4684,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="190" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="12"/>
       <c r="D190" t="s">
         <v>440</v>
@@ -4690,7 +4696,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="191" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="12"/>
       <c r="D191" t="s">
         <v>441</v>
@@ -4702,7 +4708,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="192" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="12"/>
       <c r="D192" t="s">
         <v>442</v>
@@ -4714,7 +4720,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="12"/>
       <c r="D193" t="s">
         <v>443</v>
@@ -4726,7 +4732,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="194" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="12"/>
       <c r="D194" t="s">
         <v>444</v>
@@ -4738,7 +4744,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="195" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="12"/>
       <c r="D195" t="s">
         <v>445</v>
@@ -4750,7 +4756,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="196" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="12"/>
       <c r="D196" t="s">
         <v>446</v>
@@ -4762,7 +4768,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="12"/>
       <c r="D197" t="s">
         <v>447</v>
@@ -4774,7 +4780,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="200" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="12" t="s">
         <v>352</v>
       </c>
@@ -4791,7 +4797,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="201" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="12"/>
       <c r="B201" t="s">
         <v>110</v>
@@ -4806,7 +4812,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="202" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="12"/>
       <c r="B202" t="s">
         <v>111</v>
@@ -4821,7 +4827,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="203" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="12"/>
       <c r="D203" t="s">
         <v>460</v>
@@ -4833,7 +4839,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="204" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="12"/>
       <c r="D204" t="s">
         <v>461</v>
@@ -4845,7 +4851,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="205" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="12"/>
       <c r="D205" t="s">
         <v>462</v>
@@ -4857,7 +4863,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="206" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="12"/>
       <c r="D206" t="s">
         <v>463</v>
@@ -4869,7 +4875,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="207" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="12"/>
       <c r="D207" t="s">
         <v>465</v>
@@ -4878,7 +4884,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="12"/>
       <c r="D208" t="s">
         <v>464</v>
@@ -4890,7 +4896,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="209" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="12"/>
       <c r="D209" t="s">
         <v>533</v>
@@ -4902,7 +4908,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="210" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="12"/>
       <c r="D210" t="s">
         <v>527</v>
@@ -4914,7 +4920,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="12"/>
       <c r="D211" t="s">
         <v>466</v>
@@ -4926,7 +4932,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="212" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="12"/>
       <c r="D212" t="s">
         <v>467</v>
@@ -4938,7 +4944,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="213" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="12"/>
       <c r="D213" t="s">
         <v>468</v>
@@ -4950,7 +4956,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="214" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="12"/>
       <c r="D214" t="s">
         <v>469</v>
@@ -4962,7 +4968,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="12"/>
       <c r="D215" t="s">
         <v>470</v>
@@ -4974,7 +4980,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="216" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="12"/>
       <c r="D216" t="s">
         <v>471</v>
@@ -4986,7 +4992,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="217" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="12"/>
       <c r="D217" t="s">
         <v>472</v>
@@ -4998,7 +5004,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="218" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="12"/>
       <c r="D218" t="s">
         <v>473</v>
@@ -5010,7 +5016,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="221" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="12" t="s">
         <v>496</v>
       </c>
@@ -5027,7 +5033,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="222" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="12"/>
       <c r="D222" t="s">
         <v>157</v>
@@ -5039,7 +5045,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="223" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="12"/>
       <c r="D223" t="s">
         <v>160</v>
@@ -5051,7 +5057,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="12"/>
       <c r="D224" t="s">
         <v>161</v>
@@ -5063,7 +5069,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="225" spans="1:6" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="12"/>
       <c r="D225" s="9" t="s">
         <v>495</v>
@@ -5075,7 +5081,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="226" spans="1:6" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="12"/>
       <c r="D226" s="9" t="s">
         <v>497</v>
@@ -5087,13 +5093,13 @@
         <v>509</v>
       </c>
     </row>
-    <row r="227" spans="1:6" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="3"/>
     </row>
-    <row r="228" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:6" s="9" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A228" s="2"/>
     </row>
-    <row r="230" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="12" t="s">
         <v>353</v>
       </c>
@@ -5110,7 +5116,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="12"/>
       <c r="B231" t="s">
         <v>53</v>
@@ -5125,7 +5131,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="12"/>
       <c r="B232" t="s">
         <v>55</v>
@@ -5140,7 +5146,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="233" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="12"/>
       <c r="B233" t="s">
         <v>58</v>
@@ -5155,7 +5161,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="234" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="12"/>
       <c r="D234" t="s">
         <v>498</v>
@@ -5167,7 +5173,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="235" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="12"/>
       <c r="B235" t="s">
         <v>59</v>
@@ -5182,7 +5188,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="236" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="12"/>
       <c r="B236" t="s">
         <v>61</v>
@@ -5197,7 +5203,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="237" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="12"/>
       <c r="B237" t="s">
         <v>63</v>
@@ -5212,7 +5218,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="238" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="12"/>
       <c r="B238" t="s">
         <v>64</v>
@@ -5227,7 +5233,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="239" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="12"/>
       <c r="D239" t="s">
         <v>499</v>
@@ -5239,7 +5245,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="12"/>
       <c r="D240" t="s">
         <v>500</v>
@@ -5251,7 +5257,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="241" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="12"/>
       <c r="D241" t="s">
         <v>501</v>
@@ -5280,7 +5286,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="247" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="12" t="s">
         <v>119</v>
       </c>
@@ -5297,7 +5303,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="248" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="12"/>
       <c r="B248" t="s">
         <v>122</v>
@@ -5312,7 +5318,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="249" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="12"/>
       <c r="B249" t="s">
         <v>123</v>
@@ -5327,7 +5333,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="250" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="12"/>
       <c r="B250" t="s">
         <v>130</v>
@@ -5345,7 +5351,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="251" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="12"/>
       <c r="B251" t="s">
         <v>131</v>
@@ -5360,7 +5366,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="252" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="12"/>
       <c r="B252" t="s">
         <v>117</v>
@@ -5375,7 +5381,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="253" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="12"/>
       <c r="B253" t="s">
         <v>139</v>
@@ -5390,7 +5396,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="254" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="12"/>
       <c r="B254" t="s">
         <v>0</v>
@@ -5405,7 +5411,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="255" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="12"/>
       <c r="B255" t="s">
         <v>0</v>
@@ -5420,7 +5426,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="256" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="12"/>
       <c r="B256" t="s">
         <v>0</v>
@@ -5435,7 +5441,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="257" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="12"/>
       <c r="B257" t="s">
         <v>0</v>
@@ -5450,7 +5456,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="258" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="12"/>
       <c r="B258" t="s">
         <v>0</v>
@@ -5465,7 +5471,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="259" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="12"/>
       <c r="B259" t="s">
         <v>0</v>
@@ -5480,7 +5486,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="260" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="12"/>
       <c r="B260" t="s">
         <v>0</v>
@@ -5495,7 +5501,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="261" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="12"/>
       <c r="B261" t="s">
         <v>205</v>
@@ -5510,7 +5516,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="262" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="12"/>
       <c r="B262" t="s">
         <v>121</v>
@@ -5522,7 +5528,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="263" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="12"/>
       <c r="B263" t="s">
         <v>124</v>
@@ -5537,7 +5543,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="264" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="12"/>
       <c r="B264" t="s">
         <v>125</v>
@@ -5552,7 +5558,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="265" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="12"/>
       <c r="D265" t="s">
         <v>619</v>
@@ -5567,10 +5573,10 @@
     <row r="266" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A266" s="3"/>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A267" s="2"/>
     </row>
-    <row r="268" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="13" t="s">
         <v>624</v>
       </c>
@@ -5584,7 +5590,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="269" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="13"/>
       <c r="D269" t="s">
         <v>625</v>
@@ -5596,7 +5602,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="270" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="13"/>
       <c r="B270" t="s">
         <v>181</v>
@@ -5611,7 +5617,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="271" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="13"/>
       <c r="B271" t="s">
         <v>182</v>
@@ -5626,7 +5632,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="272" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="13"/>
       <c r="B272" t="s">
         <v>183</v>
@@ -5641,7 +5647,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="273" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" s="13"/>
       <c r="D273" t="s">
         <v>185</v>
@@ -5653,7 +5659,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="274" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="13"/>
       <c r="D274" t="s">
         <v>184</v>
@@ -5665,7 +5671,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="275" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A275" s="13"/>
       <c r="D275" t="s">
         <v>517</v>
@@ -5677,7 +5683,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="276" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="13"/>
       <c r="D276" t="s">
         <v>634</v>
@@ -5689,7 +5695,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="277" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A277" s="13"/>
       <c r="D277" t="s">
         <v>189</v>
@@ -5701,7 +5707,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="278" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A278" s="13"/>
       <c r="D278" t="s">
         <v>202</v>
@@ -5713,7 +5719,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="281" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="12" t="s">
         <v>127</v>
       </c>
@@ -5727,7 +5733,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="282" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" s="12"/>
       <c r="B282" t="s">
         <v>116</v>
@@ -5739,7 +5745,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="283" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="12"/>
       <c r="B283" t="s">
         <v>118</v>
@@ -5751,7 +5757,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="284" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="12"/>
       <c r="B284" t="s">
         <v>128</v>
@@ -5763,7 +5769,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="285" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A285" s="12"/>
       <c r="B285" t="s">
         <v>121</v>
@@ -5775,13 +5781,13 @@
         <v>235</v>
       </c>
     </row>
-    <row r="286" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A286" s="3"/>
     </row>
-    <row r="287" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A287" s="3"/>
     </row>
-    <row r="288" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A288" s="13" t="s">
         <v>143</v>
       </c>
@@ -5798,7 +5804,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="289" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289" s="13"/>
       <c r="B289" t="s">
         <v>0</v>
@@ -5813,7 +5819,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="290" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290" s="13"/>
       <c r="B290" t="s">
         <v>0</v>
@@ -5828,7 +5834,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="291" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="13"/>
       <c r="B291" t="s">
         <v>0</v>
@@ -5843,211 +5849,233 @@
         <v>176</v>
       </c>
     </row>
-    <row r="292" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A292" s="13"/>
       <c r="B292" t="s">
         <v>0</v>
       </c>
       <c r="D292" t="s">
-        <v>512</v>
+        <v>640</v>
       </c>
       <c r="E292" t="s">
         <v>142</v>
       </c>
       <c r="F292" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="293" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A293" s="13"/>
       <c r="B293" t="s">
         <v>0</v>
       </c>
       <c r="D293" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="E293" t="s">
-        <v>506</v>
+        <v>142</v>
       </c>
       <c r="F293" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="294" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="13"/>
       <c r="B294" t="s">
         <v>0</v>
       </c>
       <c r="D294" t="s">
-        <v>144</v>
+        <v>514</v>
       </c>
       <c r="E294" t="s">
         <v>506</v>
       </c>
       <c r="F294" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="295" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A295" s="13"/>
       <c r="B295" t="s">
         <v>0</v>
       </c>
       <c r="D295" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E295" t="s">
         <v>506</v>
       </c>
       <c r="F295" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="296" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A296" s="13"/>
       <c r="B296" t="s">
         <v>0</v>
       </c>
       <c r="D296" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E296" t="s">
         <v>506</v>
       </c>
       <c r="F296" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="297" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A297" s="13"/>
       <c r="B297" t="s">
         <v>0</v>
       </c>
       <c r="D297" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E297" t="s">
         <v>506</v>
       </c>
       <c r="F297" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A298" s="13"/>
+      <c r="B298" t="s">
+        <v>0</v>
+      </c>
+      <c r="D298" t="s">
+        <v>147</v>
+      </c>
+      <c r="E298" t="s">
+        <v>506</v>
+      </c>
+      <c r="F298" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="298" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A298" s="8"/>
-    </row>
-    <row r="299" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" s="8"/>
     </row>
-    <row r="300" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A300" s="12" t="s">
+    <row r="300" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="8"/>
+    </row>
+    <row r="301" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A301" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="D300" t="s">
+      <c r="D301" t="s">
         <v>192</v>
       </c>
-      <c r="F300" t="s">
+      <c r="F301" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="301" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A301" s="12"/>
-      <c r="D301" t="s">
-        <v>194</v>
-      </c>
-      <c r="F301" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="302" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="12"/>
       <c r="D302" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F302" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="303" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="12"/>
       <c r="D303" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F303" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="304" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="12"/>
       <c r="D304" t="s">
+        <v>197</v>
+      </c>
+      <c r="F304" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A305" s="12"/>
+      <c r="D305" t="s">
         <v>200</v>
       </c>
-      <c r="F304" t="s">
+      <c r="F305" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="305" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A305" s="12"/>
-      <c r="B305" t="s">
-        <v>231</v>
-      </c>
-      <c r="D305" t="s">
-        <v>216</v>
-      </c>
-      <c r="F305" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="306" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A306" s="12"/>
       <c r="B306" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D306" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F306" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="307" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A307" s="12"/>
       <c r="B307" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D307" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F307" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="308" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A308" s="12"/>
       <c r="B308" t="s">
+        <v>233</v>
+      </c>
+      <c r="D308" t="s">
+        <v>219</v>
+      </c>
+      <c r="F308" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A309" s="12"/>
+      <c r="B309" t="s">
         <v>232</v>
       </c>
-      <c r="D308" t="s">
+      <c r="D309" t="s">
         <v>229</v>
       </c>
-      <c r="F308" t="s">
+      <c r="F309" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="309" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A309" s="12"/>
-      <c r="D309" t="s">
+    <row r="310" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A310" s="12"/>
+      <c r="D310" t="s">
         <v>510</v>
       </c>
-      <c r="F309" t="s">
+      <c r="F310" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="310" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A310" s="3"/>
+    <row r="311" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A311" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A301:A310"/>
+    <mergeCell ref="A281:A285"/>
+    <mergeCell ref="A221:A226"/>
+    <mergeCell ref="A230:A241"/>
+    <mergeCell ref="A247:A265"/>
+    <mergeCell ref="A268:A278"/>
+    <mergeCell ref="A288:A298"/>
     <mergeCell ref="A44:A82"/>
     <mergeCell ref="A18:A41"/>
     <mergeCell ref="A3:A15"/>
@@ -6057,13 +6085,6 @@
     <mergeCell ref="A128:A150"/>
     <mergeCell ref="A153:A175"/>
     <mergeCell ref="A85:A100"/>
-    <mergeCell ref="A300:A309"/>
-    <mergeCell ref="A288:A297"/>
-    <mergeCell ref="A281:A285"/>
-    <mergeCell ref="A221:A226"/>
-    <mergeCell ref="A230:A241"/>
-    <mergeCell ref="A247:A265"/>
-    <mergeCell ref="A268:A278"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6076,7 +6097,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6088,7 +6109,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
GS - Documentation Updates
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variables.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="639">
   <si>
     <t>N/A</t>
   </si>
@@ -1524,9 +1524,6 @@
     <t>function</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>Library that deals with sets.</t>
   </si>
   <si>
@@ -1920,9 +1917,6 @@
     <t>Passes the resources line for the spell with a few modifications. Occurs when the outgoing action packet is cued. verify_equip(), force_send(), and cast_delay() are implemented in this phase. cancel_spell() is also implemented in this phase.</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>Library that deals with lists.</t>
   </si>
   <si>
@@ -1930,6 +1924,15 @@
   </si>
   <si>
     <t>Prints directly to console.</t>
+  </si>
+  <si>
+    <t>S or set</t>
+  </si>
+  <si>
+    <t>T or table</t>
+  </si>
+  <si>
+    <t>L or list</t>
   </si>
 </sst>
 </file>
@@ -2325,20 +2328,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="C257" sqref="C257"/>
+    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
+      <selection activeCell="D291" sqref="D291"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" customWidth="1"/>
-    <col min="4" max="4" width="40.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="202.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="202.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.95" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="25.9" x14ac:dyDescent="0.5">
       <c r="B1" s="6" t="s">
         <v>498</v>
       </c>
@@ -2353,7 +2356,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
@@ -2370,7 +2373,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" t="s">
         <v>2</v>
@@ -2385,7 +2388,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" t="s">
         <v>4</v>
@@ -2400,7 +2403,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" t="s">
         <v>6</v>
@@ -2415,7 +2418,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" t="s">
         <v>8</v>
@@ -2430,7 +2433,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" t="s">
         <v>10</v>
@@ -2445,7 +2448,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" t="s">
         <v>12</v>
@@ -2460,7 +2463,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" t="s">
         <v>14</v>
@@ -2475,7 +2478,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" t="s">
         <v>16</v>
@@ -2490,7 +2493,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" t="s">
         <v>18</v>
@@ -2505,7 +2508,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="D13" t="s">
         <v>245</v>
@@ -2517,7 +2520,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="D14" t="s">
         <v>246</v>
@@ -2529,7 +2532,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="D15" t="s">
         <v>247</v>
@@ -2541,15 +2544,15 @@
         <v>249</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B18" t="s">
         <v>72</v>
@@ -2564,7 +2567,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" t="s">
         <v>74</v>
@@ -2579,7 +2582,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" t="s">
         <v>76</v>
@@ -2594,7 +2597,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" t="s">
         <v>78</v>
@@ -2609,7 +2612,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" t="s">
         <v>80</v>
@@ -2624,7 +2627,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" t="s">
         <v>82</v>
@@ -2639,58 +2642,58 @@
         <v>276</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="D24" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E24" t="s">
         <v>264</v>
       </c>
       <c r="F24" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="D25" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E25" t="s">
         <v>263</v>
       </c>
       <c r="F25" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="D26" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E26" t="s">
         <v>263</v>
       </c>
       <c r="F26" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="D27" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E27" t="s">
         <v>263</v>
       </c>
       <c r="F27" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="D28" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E28" t="s">
         <v>263</v>
@@ -2699,163 +2702,163 @@
         <v>362</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="D29" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E29" t="s">
         <v>138</v>
       </c>
       <c r="F29" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="D30" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E30" t="s">
         <v>263</v>
       </c>
       <c r="F30" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="D31" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E31" t="s">
         <v>138</v>
       </c>
       <c r="F31" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="D32" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E32" t="s">
         <v>263</v>
       </c>
       <c r="F32" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="D33" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E33" t="s">
         <v>263</v>
       </c>
       <c r="F33" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="D34" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E34" t="s">
         <v>263</v>
       </c>
       <c r="F34" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="D35" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E35" t="s">
         <v>263</v>
       </c>
       <c r="F35" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="D36" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E36" t="s">
         <v>263</v>
       </c>
       <c r="F36" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
       <c r="D37" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E37" t="s">
         <v>263</v>
       </c>
       <c r="F37" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
       <c r="D38" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E38" t="s">
         <v>263</v>
       </c>
       <c r="F38" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="D39" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E39" t="s">
         <v>263</v>
       </c>
       <c r="F39" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="D40" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E40" t="s">
         <v>263</v>
       </c>
       <c r="F40" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="D41" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E41" t="s">
         <v>263</v>
       </c>
       <c r="F41" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>345</v>
       </c>
@@ -2872,7 +2875,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" t="s">
         <v>22</v>
@@ -2887,7 +2890,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" t="s">
         <v>26</v>
@@ -2902,7 +2905,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" t="s">
         <v>28</v>
@@ -2917,7 +2920,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" t="s">
         <v>30</v>
@@ -2932,7 +2935,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12"/>
       <c r="B49" t="s">
         <v>32</v>
@@ -2947,7 +2950,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>
       <c r="B50" t="s">
         <v>33</v>
@@ -2962,7 +2965,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
       <c r="B51" t="s">
         <v>36</v>
@@ -2977,7 +2980,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
       <c r="B52" t="s">
         <v>38</v>
@@ -2992,7 +2995,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12"/>
       <c r="D53" t="s">
         <v>326</v>
@@ -3004,7 +3007,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
       <c r="B54" t="s">
         <v>40</v>
@@ -3019,7 +3022,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
       <c r="D55" t="s">
         <v>328</v>
@@ -3031,7 +3034,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
       <c r="B56" t="s">
         <v>41</v>
@@ -3046,7 +3049,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
       <c r="D57" t="s">
         <v>330</v>
@@ -3058,7 +3061,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12"/>
       <c r="B58" t="s">
         <v>42</v>
@@ -3073,7 +3076,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
       <c r="D59" t="s">
         <v>331</v>
@@ -3085,7 +3088,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12"/>
       <c r="B60" t="s">
         <v>43</v>
@@ -3100,7 +3103,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12"/>
       <c r="B61" t="s">
         <v>49</v>
@@ -3115,7 +3118,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12"/>
       <c r="B62" t="s">
         <v>51</v>
@@ -3130,7 +3133,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="D63" t="s">
         <v>318</v>
@@ -3142,7 +3145,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="D64" t="s">
         <v>320</v>
@@ -3154,7 +3157,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="D65" t="s">
         <v>322</v>
@@ -3166,7 +3169,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="D66" t="s">
         <v>324</v>
@@ -3178,7 +3181,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="D67" t="s">
         <v>325</v>
@@ -3190,7 +3193,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="D68" t="s">
         <v>336</v>
@@ -3202,7 +3205,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="D69" t="s">
         <v>338</v>
@@ -3214,7 +3217,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="D70" t="s">
         <v>339</v>
@@ -3226,7 +3229,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="D71" t="s">
         <v>342</v>
@@ -3238,7 +3241,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="D72" t="s">
         <v>379</v>
@@ -3250,7 +3253,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12"/>
       <c r="D73" t="s">
         <v>380</v>
@@ -3262,7 +3265,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12"/>
       <c r="D74" t="s">
         <v>381</v>
@@ -3274,7 +3277,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12"/>
       <c r="D75" t="s">
         <v>426</v>
@@ -3286,19 +3289,19 @@
         <v>396</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12"/>
       <c r="D76" t="s">
+        <v>516</v>
+      </c>
+      <c r="E76" t="s">
+        <v>263</v>
+      </c>
+      <c r="F76" t="s">
         <v>517</v>
       </c>
-      <c r="E76" t="s">
-        <v>263</v>
-      </c>
-      <c r="F76" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12"/>
       <c r="D77" t="s">
         <v>382</v>
@@ -3310,7 +3313,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12"/>
       <c r="D78" t="s">
         <v>383</v>
@@ -3322,7 +3325,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12"/>
       <c r="D79" t="s">
         <v>384</v>
@@ -3334,7 +3337,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12"/>
       <c r="D80" t="s">
         <v>385</v>
@@ -3346,7 +3349,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12"/>
       <c r="D81" t="s">
         <v>386</v>
@@ -3358,7 +3361,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12"/>
       <c r="D82" t="s">
         <v>387</v>
@@ -3370,13 +3373,13 @@
         <v>376</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
     </row>
-    <row r="84" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="7"/>
     </row>
-    <row r="85" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
         <v>344</v>
       </c>
@@ -3393,7 +3396,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12"/>
       <c r="B86" t="s">
         <v>95</v>
@@ -3408,7 +3411,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12"/>
       <c r="B87" t="s">
         <v>96</v>
@@ -3423,7 +3426,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12"/>
       <c r="B88" t="s">
         <v>97</v>
@@ -3438,7 +3441,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12"/>
       <c r="B89" t="s">
         <v>278</v>
@@ -3453,7 +3456,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12"/>
       <c r="B90" t="s">
         <v>279</v>
@@ -3468,7 +3471,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
       <c r="B91" t="s">
         <v>280</v>
@@ -3483,7 +3486,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
       <c r="B92" t="s">
         <v>281</v>
@@ -3498,7 +3501,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12"/>
       <c r="B93" t="s">
         <v>282</v>
@@ -3513,7 +3516,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12"/>
       <c r="B94" t="s">
         <v>283</v>
@@ -3528,7 +3531,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12"/>
       <c r="B95" t="s">
         <v>284</v>
@@ -3543,7 +3546,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12"/>
       <c r="B96" t="s">
         <v>285</v>
@@ -3558,7 +3561,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
       <c r="B97" t="s">
         <v>286</v>
@@ -3573,7 +3576,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
       <c r="B98" t="s">
         <v>287</v>
@@ -3588,7 +3591,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
       <c r="B99" t="s">
         <v>288</v>
@@ -3603,7 +3606,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12"/>
       <c r="B100" t="s">
         <v>289</v>
@@ -3618,13 +3621,13 @@
         <v>291</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3"/>
     </row>
-    <row r="102" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
     </row>
-    <row r="103" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="s">
         <v>349</v>
       </c>
@@ -3641,7 +3644,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12"/>
       <c r="B104" t="s">
         <v>68</v>
@@ -3656,7 +3659,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12"/>
       <c r="B105" t="s">
         <v>69</v>
@@ -3671,7 +3674,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12"/>
       <c r="B106" t="s">
         <v>70</v>
@@ -3686,7 +3689,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="12"/>
       <c r="B107" t="s">
         <v>71</v>
@@ -3701,7 +3704,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="12"/>
       <c r="D108" t="s">
         <v>353</v>
@@ -3713,7 +3716,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="12"/>
       <c r="D109" t="s">
         <v>360</v>
@@ -3725,7 +3728,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="12"/>
       <c r="D110" t="s">
         <v>361</v>
@@ -3737,7 +3740,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="12"/>
       <c r="D111" t="s">
         <v>352</v>
@@ -3749,7 +3752,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="12"/>
       <c r="D112" t="s">
         <v>354</v>
@@ -3761,7 +3764,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="12"/>
       <c r="D113" t="s">
         <v>355</v>
@@ -3773,7 +3776,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="12"/>
       <c r="D114" t="s">
         <v>425</v>
@@ -3785,31 +3788,31 @@
         <v>363</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="12"/>
       <c r="D115" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E115" t="s">
         <v>138</v>
       </c>
       <c r="F115" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="12"/>
       <c r="D116" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E116" t="s">
         <v>263</v>
       </c>
       <c r="F116" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12"/>
       <c r="D117" t="s">
         <v>369</v>
@@ -3821,7 +3824,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="12"/>
       <c r="D118" t="s">
         <v>370</v>
@@ -3833,7 +3836,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="12"/>
       <c r="D119" t="s">
         <v>357</v>
@@ -3845,7 +3848,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="12"/>
       <c r="D120" t="s">
         <v>358</v>
@@ -3857,7 +3860,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="12"/>
       <c r="D121" t="s">
         <v>359</v>
@@ -3869,7 +3872,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="12"/>
       <c r="D122" t="s">
         <v>351</v>
@@ -3881,7 +3884,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="12"/>
       <c r="D123" t="s">
         <v>356</v>
@@ -3893,7 +3896,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="12"/>
       <c r="D124" t="s">
         <v>367</v>
@@ -3905,7 +3908,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="12"/>
       <c r="D125" t="s">
         <v>377</v>
@@ -3917,30 +3920,30 @@
         <v>378</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="10"/>
     </row>
-    <row r="127" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
     </row>
-    <row r="128" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="12" t="s">
+        <v>533</v>
+      </c>
+      <c r="D128" t="s">
+        <v>553</v>
+      </c>
+      <c r="E128" t="s">
+        <v>138</v>
+      </c>
+      <c r="F128" t="s">
         <v>534</v>
       </c>
-      <c r="D128" t="s">
-        <v>554</v>
-      </c>
-      <c r="E128" t="s">
-        <v>138</v>
-      </c>
-      <c r="F128" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="12"/>
       <c r="D129" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E129" t="s">
         <v>138</v>
@@ -3949,94 +3952,94 @@
         <v>261</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="12"/>
       <c r="D130" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E130" t="s">
         <v>263</v>
       </c>
       <c r="F130" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="12"/>
       <c r="D131" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E131" t="s">
         <v>263</v>
       </c>
       <c r="F131" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="12"/>
       <c r="D132" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E132" t="s">
         <v>264</v>
       </c>
       <c r="F132" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="12"/>
       <c r="D133" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E133" t="s">
         <v>264</v>
       </c>
       <c r="F133" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="12"/>
       <c r="D134" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E134" t="s">
         <v>263</v>
       </c>
       <c r="F134" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="12"/>
       <c r="D135" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E135" t="s">
         <v>263</v>
       </c>
       <c r="F135" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="12"/>
       <c r="D136" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E136" t="s">
         <v>263</v>
       </c>
       <c r="F136" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="12"/>
       <c r="D137" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E137" t="s">
         <v>263</v>
@@ -4045,154 +4048,154 @@
         <v>362</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="12"/>
       <c r="D138" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E138" t="s">
         <v>138</v>
       </c>
       <c r="F138" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="12"/>
       <c r="D139" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E139" t="s">
         <v>263</v>
       </c>
       <c r="F139" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="12"/>
       <c r="D140" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E140" t="s">
         <v>138</v>
       </c>
       <c r="F140" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="12"/>
       <c r="D141" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E141" t="s">
         <v>263</v>
       </c>
       <c r="F141" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="12"/>
       <c r="D142" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E142" t="s">
         <v>263</v>
       </c>
       <c r="F142" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="12"/>
       <c r="D143" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E143" t="s">
         <v>263</v>
       </c>
       <c r="F143" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="12"/>
       <c r="D144" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E144" t="s">
         <v>263</v>
       </c>
       <c r="F144" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="12"/>
       <c r="D145" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E145" t="s">
         <v>263</v>
       </c>
       <c r="F145" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="12"/>
       <c r="D146" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E146" t="s">
         <v>263</v>
       </c>
       <c r="F146" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="12"/>
       <c r="D147" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E147" t="s">
         <v>263</v>
       </c>
       <c r="F147" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="12"/>
       <c r="D148" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E148" t="s">
         <v>263</v>
       </c>
       <c r="F148" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="12"/>
       <c r="D149" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E149" t="s">
         <v>263</v>
       </c>
       <c r="F149" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="12"/>
       <c r="D150" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E150" t="s">
         <v>263</v>
@@ -4201,13 +4204,13 @@
         <v>412</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="11"/>
     </row>
-    <row r="152" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
     </row>
-    <row r="153" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="12" t="s">
         <v>350</v>
       </c>
@@ -4221,7 +4224,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="12"/>
       <c r="D154" t="s">
         <v>90</v>
@@ -4233,7 +4236,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="12"/>
       <c r="D155" t="s">
         <v>91</v>
@@ -4245,7 +4248,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="12"/>
       <c r="D156" t="s">
         <v>92</v>
@@ -4257,7 +4260,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="12"/>
       <c r="D157" t="s">
         <v>93</v>
@@ -4269,7 +4272,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="12"/>
       <c r="D158" t="s">
         <v>393</v>
@@ -4281,7 +4284,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="12"/>
       <c r="D159" t="s">
         <v>398</v>
@@ -4293,7 +4296,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="12"/>
       <c r="D160" t="s">
         <v>399</v>
@@ -4305,7 +4308,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="12"/>
       <c r="D161" t="s">
         <v>400</v>
@@ -4314,10 +4317,10 @@
         <v>263</v>
       </c>
       <c r="F161" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="12"/>
       <c r="D162" t="s">
         <v>401</v>
@@ -4329,7 +4332,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="12"/>
       <c r="D163" t="s">
         <v>402</v>
@@ -4338,10 +4341,10 @@
         <v>138</v>
       </c>
       <c r="F163" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="12"/>
       <c r="D164" t="s">
         <v>424</v>
@@ -4350,34 +4353,34 @@
         <v>263</v>
       </c>
       <c r="F164" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="12"/>
       <c r="D165" t="s">
+        <v>528</v>
+      </c>
+      <c r="E165" t="s">
+        <v>138</v>
+      </c>
+      <c r="F165" t="s">
         <v>529</v>
       </c>
-      <c r="E165" t="s">
-        <v>138</v>
-      </c>
-      <c r="F165" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="166" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="12"/>
       <c r="D166" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E166" t="s">
         <v>263</v>
       </c>
       <c r="F166" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="12"/>
       <c r="D167" t="s">
         <v>403</v>
@@ -4389,7 +4392,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="12"/>
       <c r="D168" t="s">
         <v>404</v>
@@ -4401,7 +4404,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="12"/>
       <c r="D169" t="s">
         <v>405</v>
@@ -4413,7 +4416,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="12"/>
       <c r="D170" t="s">
         <v>406</v>
@@ -4425,7 +4428,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="12"/>
       <c r="D171" t="s">
         <v>407</v>
@@ -4437,7 +4440,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="12"/>
       <c r="D172" t="s">
         <v>408</v>
@@ -4449,7 +4452,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="12"/>
       <c r="D173" t="s">
         <v>409</v>
@@ -4461,7 +4464,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="12"/>
       <c r="D174" t="s">
         <v>410</v>
@@ -4473,7 +4476,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="12"/>
       <c r="D175" t="s">
         <v>411</v>
@@ -4485,10 +4488,10 @@
         <v>412</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="3"/>
     </row>
-    <row r="178" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="12" t="s">
         <v>346</v>
       </c>
@@ -4505,7 +4508,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="12"/>
       <c r="B179" t="s">
         <v>100</v>
@@ -4520,7 +4523,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="12"/>
       <c r="B180" t="s">
         <v>102</v>
@@ -4535,7 +4538,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12"/>
       <c r="B181" t="s">
         <v>104</v>
@@ -4550,7 +4553,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="12"/>
       <c r="D182" t="s">
         <v>429</v>
@@ -4562,7 +4565,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="12"/>
       <c r="B183" t="s">
         <v>108</v>
@@ -4577,7 +4580,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="12"/>
       <c r="B184" t="s">
         <v>106</v>
@@ -4589,7 +4592,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="12"/>
       <c r="D185" t="s">
         <v>432</v>
@@ -4601,7 +4604,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="12"/>
       <c r="D186" t="s">
         <v>433</v>
@@ -4613,7 +4616,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="12"/>
       <c r="D187" t="s">
         <v>434</v>
@@ -4625,31 +4628,31 @@
         <v>451</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="12"/>
       <c r="D188" t="s">
+        <v>522</v>
+      </c>
+      <c r="E188" t="s">
+        <v>138</v>
+      </c>
+      <c r="F188" t="s">
         <v>523</v>
       </c>
-      <c r="E188" t="s">
-        <v>138</v>
-      </c>
-      <c r="F188" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="189" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="12"/>
       <c r="D189" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E189" t="s">
         <v>263</v>
       </c>
       <c r="F189" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="12"/>
       <c r="D190" t="s">
         <v>435</v>
@@ -4661,7 +4664,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="191" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="12"/>
       <c r="D191" t="s">
         <v>436</v>
@@ -4673,7 +4676,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="192" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="12"/>
       <c r="D192" t="s">
         <v>437</v>
@@ -4685,7 +4688,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="12"/>
       <c r="D193" t="s">
         <v>438</v>
@@ -4697,7 +4700,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="194" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="12"/>
       <c r="D194" t="s">
         <v>439</v>
@@ -4709,7 +4712,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="195" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="12"/>
       <c r="D195" t="s">
         <v>440</v>
@@ -4721,7 +4724,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="196" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="12"/>
       <c r="D196" t="s">
         <v>441</v>
@@ -4733,7 +4736,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="12"/>
       <c r="D197" t="s">
         <v>442</v>
@@ -4745,7 +4748,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="200" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="12" t="s">
         <v>347</v>
       </c>
@@ -4762,7 +4765,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="201" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="12"/>
       <c r="B201" t="s">
         <v>110</v>
@@ -4777,7 +4780,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="202" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="12"/>
       <c r="B202" t="s">
         <v>111</v>
@@ -4792,7 +4795,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="203" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="12"/>
       <c r="D203" t="s">
         <v>455</v>
@@ -4804,7 +4807,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="204" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="12"/>
       <c r="D204" t="s">
         <v>456</v>
@@ -4816,7 +4819,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="205" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="12"/>
       <c r="D205" t="s">
         <v>457</v>
@@ -4828,7 +4831,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="206" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="12"/>
       <c r="D206" t="s">
         <v>458</v>
@@ -4840,7 +4843,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="207" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="12"/>
       <c r="D207" t="s">
         <v>460</v>
@@ -4849,7 +4852,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="12"/>
       <c r="D208" t="s">
         <v>459</v>
@@ -4861,31 +4864,31 @@
         <v>477</v>
       </c>
     </row>
-    <row r="209" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="12"/>
       <c r="D209" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E209" t="s">
         <v>138</v>
       </c>
       <c r="F209" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="210" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="12"/>
       <c r="D210" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E210" t="s">
         <v>263</v>
       </c>
       <c r="F210" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="211" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="12"/>
       <c r="D211" t="s">
         <v>461</v>
@@ -4897,7 +4900,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="212" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="12"/>
       <c r="D212" t="s">
         <v>462</v>
@@ -4909,7 +4912,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="213" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="12"/>
       <c r="D213" t="s">
         <v>463</v>
@@ -4921,7 +4924,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="214" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="12"/>
       <c r="D214" t="s">
         <v>464</v>
@@ -4933,7 +4936,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="12"/>
       <c r="D215" t="s">
         <v>465</v>
@@ -4945,7 +4948,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="216" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="12"/>
       <c r="D216" t="s">
         <v>466</v>
@@ -4957,7 +4960,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="217" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="12"/>
       <c r="D217" t="s">
         <v>467</v>
@@ -4969,7 +4972,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="218" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="12"/>
       <c r="D218" t="s">
         <v>468</v>
@@ -4981,7 +4984,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="221" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="12" t="s">
         <v>491</v>
       </c>
@@ -4998,7 +5001,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="222" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="12"/>
       <c r="D222" t="s">
         <v>155</v>
@@ -5010,7 +5013,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="223" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="12"/>
       <c r="D223" t="s">
         <v>158</v>
@@ -5022,7 +5025,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="12"/>
       <c r="D224" t="s">
         <v>159</v>
@@ -5034,7 +5037,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="225" spans="1:6" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="12"/>
       <c r="D225" s="9" t="s">
         <v>490</v>
@@ -5043,10 +5046,10 @@
         <v>140</v>
       </c>
       <c r="F225" s="9" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="12"/>
       <c r="D226" s="9" t="s">
         <v>492</v>
@@ -5055,16 +5058,16 @@
         <v>140</v>
       </c>
       <c r="F226" s="9" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="3"/>
     </row>
-    <row r="228" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:6" s="9" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A228" s="2"/>
     </row>
-    <row r="230" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="12" t="s">
         <v>348</v>
       </c>
@@ -5081,7 +5084,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="12"/>
       <c r="B231" t="s">
         <v>53</v>
@@ -5096,7 +5099,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="12"/>
       <c r="B232" t="s">
         <v>55</v>
@@ -5111,7 +5114,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="233" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="12"/>
       <c r="B233" t="s">
         <v>58</v>
@@ -5126,7 +5129,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="234" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="12"/>
       <c r="D234" t="s">
         <v>493</v>
@@ -5138,7 +5141,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="235" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="12"/>
       <c r="B235" t="s">
         <v>59</v>
@@ -5153,7 +5156,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="236" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="12"/>
       <c r="B236" t="s">
         <v>61</v>
@@ -5168,7 +5171,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="237" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="12"/>
       <c r="B237" t="s">
         <v>63</v>
@@ -5183,7 +5186,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="238" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="12"/>
       <c r="B238" t="s">
         <v>64</v>
@@ -5198,7 +5201,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="239" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="12"/>
       <c r="D239" t="s">
         <v>494</v>
@@ -5210,7 +5213,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="240" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="12"/>
       <c r="D240" t="s">
         <v>495</v>
@@ -5222,7 +5225,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="241" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="12"/>
       <c r="D241" t="s">
         <v>496</v>
@@ -5251,7 +5254,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="247" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="12" t="s">
         <v>119</v>
       </c>
@@ -5259,31 +5262,31 @@
         <v>201</v>
       </c>
       <c r="D247" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E247" t="s">
         <v>501</v>
       </c>
       <c r="F247" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="12"/>
       <c r="B248" t="s">
+        <v>513</v>
+      </c>
+      <c r="D248" t="s">
         <v>514</v>
-      </c>
-      <c r="D248" t="s">
-        <v>515</v>
       </c>
       <c r="E248" t="s">
         <v>501</v>
       </c>
       <c r="F248" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="12"/>
       <c r="B249" t="s">
         <v>122</v>
@@ -5295,10 +5298,10 @@
         <v>501</v>
       </c>
       <c r="F249" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="250" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="12"/>
       <c r="B250" t="s">
         <v>121</v>
@@ -5310,7 +5313,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="251" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="12"/>
       <c r="B251" t="s">
         <v>123</v>
@@ -5322,10 +5325,10 @@
         <v>501</v>
       </c>
       <c r="F251" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="12"/>
       <c r="B252" t="s">
         <v>117</v>
@@ -5337,22 +5340,22 @@
         <v>501</v>
       </c>
       <c r="F252" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="253" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="12"/>
       <c r="D253" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E253" t="s">
         <v>501</v>
       </c>
       <c r="F253" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="254" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="12"/>
       <c r="B254" t="s">
         <v>124</v>
@@ -5367,7 +5370,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="255" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="12"/>
       <c r="B255" t="s">
         <v>125</v>
@@ -5382,7 +5385,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="256" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="12"/>
       <c r="B256" t="s">
         <v>129</v>
@@ -5397,10 +5400,10 @@
         <v>501</v>
       </c>
       <c r="F256" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="257" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="12"/>
       <c r="B257" t="s">
         <v>130</v>
@@ -5412,10 +5415,10 @@
         <v>501</v>
       </c>
       <c r="F257" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="258" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="12"/>
       <c r="B258" t="s">
         <v>137</v>
@@ -5430,7 +5433,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="259" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="12"/>
       <c r="B259" t="s">
         <v>0</v>
@@ -5445,7 +5448,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="260" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="12"/>
       <c r="B260" t="s">
         <v>0</v>
@@ -5460,7 +5463,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="261" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="12"/>
       <c r="B261" t="s">
         <v>0</v>
@@ -5475,7 +5478,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="262" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="12"/>
       <c r="B262" t="s">
         <v>0</v>
@@ -5487,33 +5490,33 @@
         <v>501</v>
       </c>
       <c r="F262" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="12"/>
       <c r="B263" t="s">
         <v>0</v>
       </c>
       <c r="D263" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E263" t="s">
         <v>501</v>
       </c>
       <c r="F263" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="264" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" s="3"/>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A265" s="2"/>
     </row>
-    <row r="266" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="13" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D266" t="s">
         <v>199</v>
@@ -5525,19 +5528,19 @@
         <v>200</v>
       </c>
     </row>
-    <row r="267" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="13"/>
       <c r="D267" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E267" t="s">
         <v>501</v>
       </c>
       <c r="F267" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="268" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="13"/>
       <c r="B268" t="s">
         <v>177</v>
@@ -5549,10 +5552,10 @@
         <v>501</v>
       </c>
       <c r="F268" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="269" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="13"/>
       <c r="B269" t="s">
         <v>178</v>
@@ -5564,10 +5567,10 @@
         <v>501</v>
       </c>
       <c r="F269" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="270" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="13"/>
       <c r="B270" t="s">
         <v>179</v>
@@ -5579,10 +5582,10 @@
         <v>501</v>
       </c>
       <c r="F270" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="271" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="13"/>
       <c r="D271" t="s">
         <v>181</v>
@@ -5591,10 +5594,10 @@
         <v>501</v>
       </c>
       <c r="F271" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="272" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="13"/>
       <c r="D272" t="s">
         <v>180</v>
@@ -5603,34 +5606,34 @@
         <v>501</v>
       </c>
       <c r="F272" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="273" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" s="13"/>
       <c r="D273" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E273" t="s">
         <v>501</v>
       </c>
       <c r="F273" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="274" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="13"/>
       <c r="D274" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E274" t="s">
         <v>501</v>
       </c>
       <c r="F274" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="275" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A275" s="13"/>
       <c r="D275" t="s">
         <v>185</v>
@@ -5642,7 +5645,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="276" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="13"/>
       <c r="D276" t="s">
         <v>198</v>
@@ -5651,10 +5654,10 @@
         <v>501</v>
       </c>
       <c r="F276" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="279" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A279" s="12" t="s">
         <v>127</v>
       </c>
@@ -5668,7 +5671,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="280" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A280" s="12"/>
       <c r="B280" t="s">
         <v>116</v>
@@ -5680,7 +5683,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="281" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="12"/>
       <c r="B281" t="s">
         <v>118</v>
@@ -5692,7 +5695,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="282" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" s="12"/>
       <c r="B282" t="s">
         <v>128</v>
@@ -5704,7 +5707,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="283" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="12"/>
       <c r="B283" t="s">
         <v>121</v>
@@ -5716,13 +5719,13 @@
         <v>230</v>
       </c>
     </row>
-    <row r="284" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="3"/>
     </row>
-    <row r="285" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A285" s="3"/>
     </row>
-    <row r="286" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A286" s="13" t="s">
         <v>141</v>
       </c>
@@ -5739,7 +5742,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="287" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A287" s="13"/>
       <c r="B287" t="s">
         <v>0</v>
@@ -5754,28 +5757,28 @@
         <v>171</v>
       </c>
     </row>
-    <row r="288" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A288" s="13"/>
       <c r="B288" t="s">
         <v>0</v>
       </c>
       <c r="D288" t="s">
-        <v>502</v>
+        <v>636</v>
       </c>
       <c r="E288" t="s">
         <v>140</v>
       </c>
       <c r="F288" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="289" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289" s="13"/>
       <c r="B289" t="s">
         <v>0</v>
       </c>
       <c r="D289" t="s">
-        <v>140</v>
+        <v>637</v>
       </c>
       <c r="E289" t="s">
         <v>140</v>
@@ -5784,52 +5787,52 @@
         <v>172</v>
       </c>
     </row>
-    <row r="290" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290" s="13"/>
       <c r="B290" t="s">
         <v>0</v>
       </c>
       <c r="D290" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="E290" t="s">
         <v>140</v>
       </c>
       <c r="F290" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="291" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="13"/>
       <c r="B291" t="s">
         <v>0</v>
       </c>
       <c r="D291" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E291" t="s">
         <v>140</v>
       </c>
       <c r="F291" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="292" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A292" s="13"/>
       <c r="B292" t="s">
         <v>0</v>
       </c>
       <c r="D292" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E292" t="s">
         <v>501</v>
       </c>
       <c r="F292" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="293" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A293" s="13"/>
       <c r="B293" t="s">
         <v>0</v>
@@ -5844,7 +5847,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="294" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="13"/>
       <c r="B294" t="s">
         <v>0</v>
@@ -5859,7 +5862,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="295" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A295" s="13"/>
       <c r="B295" t="s">
         <v>0</v>
@@ -5874,7 +5877,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="296" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A296" s="13"/>
       <c r="B296" t="s">
         <v>0</v>
@@ -5889,13 +5892,13 @@
         <v>176</v>
       </c>
     </row>
-    <row r="297" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A297" s="8"/>
     </row>
-    <row r="298" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A298" s="8"/>
     </row>
-    <row r="299" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" s="12" t="s">
         <v>187</v>
       </c>
@@ -5906,7 +5909,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="300" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A300" s="12"/>
       <c r="D300" t="s">
         <v>190</v>
@@ -5915,7 +5918,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="301" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A301" s="12"/>
       <c r="D301" t="s">
         <v>192</v>
@@ -5924,7 +5927,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="302" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="12"/>
       <c r="D302" t="s">
         <v>193</v>
@@ -5933,7 +5936,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="303" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="12"/>
       <c r="D303" t="s">
         <v>196</v>
@@ -5942,7 +5945,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="304" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="12"/>
       <c r="B304" t="s">
         <v>226</v>
@@ -5954,7 +5957,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="305" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A305" s="12"/>
       <c r="B305" t="s">
         <v>229</v>
@@ -5966,7 +5969,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="306" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A306" s="12"/>
       <c r="B306" t="s">
         <v>228</v>
@@ -5978,7 +5981,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="307" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A307" s="12"/>
       <c r="B307" t="s">
         <v>227</v>
@@ -5990,20 +5993,27 @@
         <v>225</v>
       </c>
     </row>
-    <row r="308" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A308" s="12"/>
       <c r="D308" t="s">
+        <v>504</v>
+      </c>
+      <c r="F308" t="s">
         <v>505</v>
       </c>
-      <c r="F308" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="309" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="309" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A309" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A299:A308"/>
+    <mergeCell ref="A279:A283"/>
+    <mergeCell ref="A221:A226"/>
+    <mergeCell ref="A230:A241"/>
+    <mergeCell ref="A266:A276"/>
+    <mergeCell ref="A286:A296"/>
+    <mergeCell ref="A247:A263"/>
     <mergeCell ref="A44:A82"/>
     <mergeCell ref="A18:A41"/>
     <mergeCell ref="A3:A15"/>
@@ -6013,13 +6023,6 @@
     <mergeCell ref="A128:A150"/>
     <mergeCell ref="A153:A175"/>
     <mergeCell ref="A85:A100"/>
-    <mergeCell ref="A299:A308"/>
-    <mergeCell ref="A279:A283"/>
-    <mergeCell ref="A221:A226"/>
-    <mergeCell ref="A230:A241"/>
-    <mergeCell ref="A266:A276"/>
-    <mergeCell ref="A286:A296"/>
-    <mergeCell ref="A247:A263"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6032,7 +6035,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6044,7 +6047,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
GearSwap v0.811 - Bug Squashing
Now featuring a lowered memory footprint, accurate player.equipment, a
filter that stops you from sending action packets for JAs you don't
have, and refactoring in flow.lua.
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variables.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1896,9 +1896,6 @@
     <t>Delays the current spell by however many seconds you choose. Valid only in precast.</t>
   </si>
   <si>
-    <t>Returns true or false based on whether or not you are in the middle of an action. True between precast and aftercast. Will not be accurate if packets are dropped.</t>
-  </si>
-  <si>
     <t>buff_change(name,gain)</t>
   </si>
   <si>
@@ -1933,6 +1930,9 @@
   </si>
   <si>
     <t>L or list</t>
+  </si>
+  <si>
+    <t>Returns true or false based on whether or not you are in the middle of an action. True between precast and aftercast. If it is true, also returns the resources line of the spell being cast.</t>
   </si>
 </sst>
 </file>
@@ -2328,20 +2328,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
-      <selection activeCell="D291" sqref="D291"/>
+    <sheetView tabSelected="1" topLeftCell="F238" workbookViewId="0">
+      <selection activeCell="F254" sqref="F254"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="202.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="4" max="4" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="202.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="25.95" x14ac:dyDescent="0.5">
       <c r="B1" s="6" t="s">
         <v>498</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" t="s">
         <v>2</v>
@@ -2388,7 +2388,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" t="s">
         <v>4</v>
@@ -2403,7 +2403,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
       <c r="B6" t="s">
         <v>6</v>
@@ -2418,7 +2418,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" t="s">
         <v>8</v>
@@ -2433,7 +2433,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="B8" t="s">
         <v>10</v>
@@ -2448,7 +2448,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" t="s">
         <v>12</v>
@@ -2463,7 +2463,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="B10" t="s">
         <v>14</v>
@@ -2478,7 +2478,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12"/>
       <c r="B11" t="s">
         <v>16</v>
@@ -2493,7 +2493,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
       <c r="B12" t="s">
         <v>18</v>
@@ -2508,7 +2508,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="D13" t="s">
         <v>245</v>
@@ -2520,7 +2520,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="D14" t="s">
         <v>246</v>
@@ -2532,7 +2532,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="D15" t="s">
         <v>247</v>
@@ -2544,13 +2544,13 @@
         <v>249</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>612</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" t="s">
         <v>74</v>
@@ -2582,7 +2582,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
       <c r="B20" t="s">
         <v>76</v>
@@ -2597,7 +2597,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
       <c r="B21" t="s">
         <v>78</v>
@@ -2612,7 +2612,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
       <c r="B22" t="s">
         <v>80</v>
@@ -2627,7 +2627,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" t="s">
         <v>82</v>
@@ -2642,7 +2642,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12"/>
       <c r="D24" t="s">
         <v>595</v>
@@ -2654,7 +2654,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12"/>
       <c r="D25" t="s">
         <v>578</v>
@@ -2666,7 +2666,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12"/>
       <c r="D26" t="s">
         <v>579</v>
@@ -2678,7 +2678,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12"/>
       <c r="D27" t="s">
         <v>580</v>
@@ -2690,7 +2690,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
       <c r="D28" t="s">
         <v>581</v>
@@ -2702,7 +2702,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="12"/>
       <c r="D29" t="s">
         <v>582</v>
@@ -2714,7 +2714,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12"/>
       <c r="D30" t="s">
         <v>583</v>
@@ -2726,7 +2726,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="12"/>
       <c r="D31" t="s">
         <v>584</v>
@@ -2738,7 +2738,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12"/>
       <c r="D32" t="s">
         <v>585</v>
@@ -2750,7 +2750,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="12"/>
       <c r="D33" t="s">
         <v>586</v>
@@ -2762,7 +2762,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="12"/>
       <c r="D34" t="s">
         <v>587</v>
@@ -2774,7 +2774,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12"/>
       <c r="D35" t="s">
         <v>588</v>
@@ -2786,7 +2786,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="12"/>
       <c r="D36" t="s">
         <v>589</v>
@@ -2798,7 +2798,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12"/>
       <c r="D37" t="s">
         <v>590</v>
@@ -2810,7 +2810,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="12"/>
       <c r="D38" t="s">
         <v>591</v>
@@ -2822,7 +2822,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="12"/>
       <c r="D39" t="s">
         <v>592</v>
@@ -2834,7 +2834,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="12"/>
       <c r="D40" t="s">
         <v>593</v>
@@ -2846,7 +2846,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="12"/>
       <c r="D41" t="s">
         <v>594</v>
@@ -2858,7 +2858,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>345</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="12"/>
       <c r="B45" t="s">
         <v>22</v>
@@ -2890,7 +2890,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="12"/>
       <c r="B46" t="s">
         <v>26</v>
@@ -2905,7 +2905,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="12"/>
       <c r="B47" t="s">
         <v>28</v>
@@ -2920,7 +2920,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="12"/>
       <c r="B48" t="s">
         <v>30</v>
@@ -2935,7 +2935,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="12"/>
       <c r="B49" t="s">
         <v>32</v>
@@ -2950,7 +2950,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="12"/>
       <c r="B50" t="s">
         <v>33</v>
@@ -2965,7 +2965,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="12"/>
       <c r="B51" t="s">
         <v>36</v>
@@ -2980,7 +2980,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="12"/>
       <c r="B52" t="s">
         <v>38</v>
@@ -2995,7 +2995,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="12"/>
       <c r="D53" t="s">
         <v>326</v>
@@ -3007,7 +3007,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="12"/>
       <c r="B54" t="s">
         <v>40</v>
@@ -3022,7 +3022,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="12"/>
       <c r="D55" t="s">
         <v>328</v>
@@ -3034,7 +3034,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="12"/>
       <c r="B56" t="s">
         <v>41</v>
@@ -3049,7 +3049,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="12"/>
       <c r="D57" t="s">
         <v>330</v>
@@ -3061,7 +3061,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="12"/>
       <c r="B58" t="s">
         <v>42</v>
@@ -3076,7 +3076,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="12"/>
       <c r="D59" t="s">
         <v>331</v>
@@ -3088,7 +3088,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="12"/>
       <c r="B60" t="s">
         <v>43</v>
@@ -3103,7 +3103,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="12"/>
       <c r="B61" t="s">
         <v>49</v>
@@ -3118,7 +3118,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="12"/>
       <c r="B62" t="s">
         <v>51</v>
@@ -3133,7 +3133,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="12"/>
       <c r="D63" t="s">
         <v>318</v>
@@ -3145,7 +3145,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="12"/>
       <c r="D64" t="s">
         <v>320</v>
@@ -3157,7 +3157,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="12"/>
       <c r="D65" t="s">
         <v>322</v>
@@ -3169,7 +3169,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="12"/>
       <c r="D66" t="s">
         <v>324</v>
@@ -3181,7 +3181,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="12"/>
       <c r="D67" t="s">
         <v>325</v>
@@ -3193,7 +3193,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="12"/>
       <c r="D68" t="s">
         <v>336</v>
@@ -3205,7 +3205,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="12"/>
       <c r="D69" t="s">
         <v>338</v>
@@ -3217,7 +3217,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="12"/>
       <c r="D70" t="s">
         <v>339</v>
@@ -3229,7 +3229,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="12"/>
       <c r="D71" t="s">
         <v>342</v>
@@ -3241,7 +3241,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="12"/>
       <c r="D72" t="s">
         <v>379</v>
@@ -3253,7 +3253,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="12"/>
       <c r="D73" t="s">
         <v>380</v>
@@ -3265,7 +3265,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="12"/>
       <c r="D74" t="s">
         <v>381</v>
@@ -3277,7 +3277,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="12"/>
       <c r="D75" t="s">
         <v>426</v>
@@ -3289,7 +3289,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="12"/>
       <c r="D76" t="s">
         <v>516</v>
@@ -3301,7 +3301,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="12"/>
       <c r="D77" t="s">
         <v>382</v>
@@ -3313,7 +3313,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="12"/>
       <c r="D78" t="s">
         <v>383</v>
@@ -3325,7 +3325,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="12"/>
       <c r="D79" t="s">
         <v>384</v>
@@ -3337,7 +3337,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="12"/>
       <c r="D80" t="s">
         <v>385</v>
@@ -3349,7 +3349,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="12"/>
       <c r="D81" t="s">
         <v>386</v>
@@ -3361,7 +3361,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="12"/>
       <c r="D82" t="s">
         <v>387</v>
@@ -3373,13 +3373,13 @@
         <v>376</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
     </row>
-    <row r="84" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="7"/>
     </row>
-    <row r="85" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="12" t="s">
         <v>344</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="12"/>
       <c r="B86" t="s">
         <v>95</v>
@@ -3411,7 +3411,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="12"/>
       <c r="B87" t="s">
         <v>96</v>
@@ -3426,7 +3426,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="12"/>
       <c r="B88" t="s">
         <v>97</v>
@@ -3441,7 +3441,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="12"/>
       <c r="B89" t="s">
         <v>278</v>
@@ -3456,7 +3456,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="12"/>
       <c r="B90" t="s">
         <v>279</v>
@@ -3471,7 +3471,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="12"/>
       <c r="B91" t="s">
         <v>280</v>
@@ -3486,7 +3486,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="12"/>
       <c r="B92" t="s">
         <v>281</v>
@@ -3501,7 +3501,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="12"/>
       <c r="B93" t="s">
         <v>282</v>
@@ -3516,7 +3516,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="12"/>
       <c r="B94" t="s">
         <v>283</v>
@@ -3531,7 +3531,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="12"/>
       <c r="B95" t="s">
         <v>284</v>
@@ -3546,7 +3546,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="12"/>
       <c r="B96" t="s">
         <v>285</v>
@@ -3561,7 +3561,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="12"/>
       <c r="B97" t="s">
         <v>286</v>
@@ -3576,7 +3576,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="12"/>
       <c r="B98" t="s">
         <v>287</v>
@@ -3591,7 +3591,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="12"/>
       <c r="B99" t="s">
         <v>288</v>
@@ -3606,7 +3606,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="12"/>
       <c r="B100" t="s">
         <v>289</v>
@@ -3621,13 +3621,13 @@
         <v>291</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3"/>
     </row>
-    <row r="102" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
     </row>
-    <row r="103" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="12" t="s">
         <v>349</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="12"/>
       <c r="B104" t="s">
         <v>68</v>
@@ -3659,7 +3659,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="12"/>
       <c r="B105" t="s">
         <v>69</v>
@@ -3674,7 +3674,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="12"/>
       <c r="B106" t="s">
         <v>70</v>
@@ -3689,7 +3689,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="12"/>
       <c r="B107" t="s">
         <v>71</v>
@@ -3704,7 +3704,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="12"/>
       <c r="D108" t="s">
         <v>353</v>
@@ -3716,7 +3716,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="12"/>
       <c r="D109" t="s">
         <v>360</v>
@@ -3728,7 +3728,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="12"/>
       <c r="D110" t="s">
         <v>361</v>
@@ -3740,7 +3740,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="12"/>
       <c r="D111" t="s">
         <v>352</v>
@@ -3752,7 +3752,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="12"/>
       <c r="D112" t="s">
         <v>354</v>
@@ -3764,7 +3764,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="12"/>
       <c r="D113" t="s">
         <v>355</v>
@@ -3776,7 +3776,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="12"/>
       <c r="D114" t="s">
         <v>425</v>
@@ -3788,7 +3788,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="12"/>
       <c r="D115" t="s">
         <v>577</v>
@@ -3800,7 +3800,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="12"/>
       <c r="D116" t="s">
         <v>518</v>
@@ -3812,7 +3812,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="12"/>
       <c r="D117" t="s">
         <v>369</v>
@@ -3824,7 +3824,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="12"/>
       <c r="D118" t="s">
         <v>370</v>
@@ -3836,7 +3836,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="12"/>
       <c r="D119" t="s">
         <v>357</v>
@@ -3848,7 +3848,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="12"/>
       <c r="D120" t="s">
         <v>358</v>
@@ -3860,7 +3860,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="12"/>
       <c r="D121" t="s">
         <v>359</v>
@@ -3872,7 +3872,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="12"/>
       <c r="D122" t="s">
         <v>351</v>
@@ -3884,7 +3884,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="12"/>
       <c r="D123" t="s">
         <v>356</v>
@@ -3896,7 +3896,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="12"/>
       <c r="D124" t="s">
         <v>367</v>
@@ -3908,7 +3908,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="12"/>
       <c r="D125" t="s">
         <v>377</v>
@@ -3920,13 +3920,13 @@
         <v>378</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="10"/>
     </row>
-    <row r="127" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
     </row>
-    <row r="128" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="12" t="s">
         <v>533</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="12"/>
       <c r="D129" t="s">
         <v>554</v>
@@ -3952,7 +3952,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="12"/>
       <c r="D130" t="s">
         <v>555</v>
@@ -3964,7 +3964,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="12"/>
       <c r="D131" t="s">
         <v>556</v>
@@ -3976,7 +3976,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="12"/>
       <c r="D132" t="s">
         <v>557</v>
@@ -3988,7 +3988,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="12"/>
       <c r="D133" t="s">
         <v>558</v>
@@ -4000,7 +4000,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" s="12"/>
       <c r="D134" t="s">
         <v>559</v>
@@ -4012,7 +4012,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="12"/>
       <c r="D135" t="s">
         <v>560</v>
@@ -4024,7 +4024,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="12"/>
       <c r="D136" t="s">
         <v>561</v>
@@ -4036,7 +4036,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="12"/>
       <c r="D137" t="s">
         <v>562</v>
@@ -4048,7 +4048,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="12"/>
       <c r="D138" t="s">
         <v>563</v>
@@ -4060,7 +4060,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="12"/>
       <c r="D139" t="s">
         <v>564</v>
@@ -4072,7 +4072,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="12"/>
       <c r="D140" t="s">
         <v>565</v>
@@ -4084,7 +4084,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="12"/>
       <c r="D141" t="s">
         <v>566</v>
@@ -4096,7 +4096,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="12"/>
       <c r="D142" t="s">
         <v>567</v>
@@ -4108,7 +4108,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="12"/>
       <c r="D143" t="s">
         <v>568</v>
@@ -4120,7 +4120,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="12"/>
       <c r="D144" t="s">
         <v>569</v>
@@ -4132,7 +4132,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="12"/>
       <c r="D145" t="s">
         <v>570</v>
@@ -4144,7 +4144,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="12"/>
       <c r="D146" t="s">
         <v>571</v>
@@ -4156,7 +4156,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="12"/>
       <c r="D147" t="s">
         <v>572</v>
@@ -4168,7 +4168,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="12"/>
       <c r="D148" t="s">
         <v>573</v>
@@ -4180,7 +4180,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="12"/>
       <c r="D149" t="s">
         <v>574</v>
@@ -4192,7 +4192,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="12"/>
       <c r="D150" t="s">
         <v>575</v>
@@ -4204,13 +4204,13 @@
         <v>412</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="11"/>
     </row>
-    <row r="152" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
     </row>
-    <row r="153" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="12" t="s">
         <v>350</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="12"/>
       <c r="D154" t="s">
         <v>90</v>
@@ -4236,7 +4236,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="12"/>
       <c r="D155" t="s">
         <v>91</v>
@@ -4248,7 +4248,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="12"/>
       <c r="D156" t="s">
         <v>92</v>
@@ -4260,7 +4260,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="12"/>
       <c r="D157" t="s">
         <v>93</v>
@@ -4272,7 +4272,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="12"/>
       <c r="D158" t="s">
         <v>393</v>
@@ -4284,7 +4284,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="12"/>
       <c r="D159" t="s">
         <v>398</v>
@@ -4296,7 +4296,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="12"/>
       <c r="D160" t="s">
         <v>399</v>
@@ -4308,7 +4308,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="12"/>
       <c r="D161" t="s">
         <v>400</v>
@@ -4320,7 +4320,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="12"/>
       <c r="D162" t="s">
         <v>401</v>
@@ -4332,7 +4332,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="12"/>
       <c r="D163" t="s">
         <v>402</v>
@@ -4344,7 +4344,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="12"/>
       <c r="D164" t="s">
         <v>424</v>
@@ -4356,7 +4356,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="12"/>
       <c r="D165" t="s">
         <v>528</v>
@@ -4368,7 +4368,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="12"/>
       <c r="D166" t="s">
         <v>519</v>
@@ -4380,7 +4380,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="12"/>
       <c r="D167" t="s">
         <v>403</v>
@@ -4392,7 +4392,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="12"/>
       <c r="D168" t="s">
         <v>404</v>
@@ -4404,7 +4404,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="12"/>
       <c r="D169" t="s">
         <v>405</v>
@@ -4416,7 +4416,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="12"/>
       <c r="D170" t="s">
         <v>406</v>
@@ -4428,7 +4428,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="12"/>
       <c r="D171" t="s">
         <v>407</v>
@@ -4440,7 +4440,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="12"/>
       <c r="D172" t="s">
         <v>408</v>
@@ -4452,7 +4452,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="12"/>
       <c r="D173" t="s">
         <v>409</v>
@@ -4464,7 +4464,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="12"/>
       <c r="D174" t="s">
         <v>410</v>
@@ -4476,7 +4476,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="12"/>
       <c r="D175" t="s">
         <v>411</v>
@@ -4488,10 +4488,10 @@
         <v>412</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="3"/>
     </row>
-    <row r="178" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="12" t="s">
         <v>346</v>
       </c>
@@ -4508,7 +4508,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="12"/>
       <c r="B179" t="s">
         <v>100</v>
@@ -4523,7 +4523,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="12"/>
       <c r="B180" t="s">
         <v>102</v>
@@ -4538,7 +4538,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="12"/>
       <c r="B181" t="s">
         <v>104</v>
@@ -4553,7 +4553,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="12"/>
       <c r="D182" t="s">
         <v>429</v>
@@ -4565,7 +4565,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="12"/>
       <c r="B183" t="s">
         <v>108</v>
@@ -4580,7 +4580,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="12"/>
       <c r="B184" t="s">
         <v>106</v>
@@ -4592,7 +4592,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="12"/>
       <c r="D185" t="s">
         <v>432</v>
@@ -4604,7 +4604,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="12"/>
       <c r="D186" t="s">
         <v>433</v>
@@ -4616,7 +4616,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="12"/>
       <c r="D187" t="s">
         <v>434</v>
@@ -4628,7 +4628,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="12"/>
       <c r="D188" t="s">
         <v>522</v>
@@ -4640,7 +4640,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="189" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="12"/>
       <c r="D189" t="s">
         <v>520</v>
@@ -4652,7 +4652,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="190" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="12"/>
       <c r="D190" t="s">
         <v>435</v>
@@ -4664,7 +4664,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="191" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="12"/>
       <c r="D191" t="s">
         <v>436</v>
@@ -4676,7 +4676,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="192" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="12"/>
       <c r="D192" t="s">
         <v>437</v>
@@ -4688,7 +4688,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="12"/>
       <c r="D193" t="s">
         <v>438</v>
@@ -4700,7 +4700,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="194" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="12"/>
       <c r="D194" t="s">
         <v>439</v>
@@ -4712,7 +4712,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="195" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="12"/>
       <c r="D195" t="s">
         <v>440</v>
@@ -4724,7 +4724,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="196" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="12"/>
       <c r="D196" t="s">
         <v>441</v>
@@ -4736,7 +4736,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="12"/>
       <c r="D197" t="s">
         <v>442</v>
@@ -4748,7 +4748,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="200" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="12" t="s">
         <v>347</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="201" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="12"/>
       <c r="B201" t="s">
         <v>110</v>
@@ -4780,7 +4780,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="202" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="12"/>
       <c r="B202" t="s">
         <v>111</v>
@@ -4795,7 +4795,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="203" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="12"/>
       <c r="D203" t="s">
         <v>455</v>
@@ -4807,7 +4807,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="204" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="12"/>
       <c r="D204" t="s">
         <v>456</v>
@@ -4819,7 +4819,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="205" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="12"/>
       <c r="D205" t="s">
         <v>457</v>
@@ -4831,7 +4831,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="206" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="12"/>
       <c r="D206" t="s">
         <v>458</v>
@@ -4843,7 +4843,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="207" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="12"/>
       <c r="D207" t="s">
         <v>460</v>
@@ -4852,7 +4852,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="12"/>
       <c r="D208" t="s">
         <v>459</v>
@@ -4864,7 +4864,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="209" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="12"/>
       <c r="D209" t="s">
         <v>527</v>
@@ -4876,7 +4876,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="210" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="12"/>
       <c r="D210" t="s">
         <v>521</v>
@@ -4888,7 +4888,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="12"/>
       <c r="D211" t="s">
         <v>461</v>
@@ -4900,7 +4900,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="212" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="12"/>
       <c r="D212" t="s">
         <v>462</v>
@@ -4912,7 +4912,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="213" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="12"/>
       <c r="D213" t="s">
         <v>463</v>
@@ -4924,7 +4924,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="214" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="12"/>
       <c r="D214" t="s">
         <v>464</v>
@@ -4936,7 +4936,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="12"/>
       <c r="D215" t="s">
         <v>465</v>
@@ -4948,7 +4948,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="216" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="12"/>
       <c r="D216" t="s">
         <v>466</v>
@@ -4960,7 +4960,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="217" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="12"/>
       <c r="D217" t="s">
         <v>467</v>
@@ -4972,7 +4972,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="218" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="12"/>
       <c r="D218" t="s">
         <v>468</v>
@@ -4984,7 +4984,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="221" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="12" t="s">
         <v>491</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="222" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="12"/>
       <c r="D222" t="s">
         <v>155</v>
@@ -5013,7 +5013,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="223" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="12"/>
       <c r="D223" t="s">
         <v>158</v>
@@ -5025,7 +5025,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="12"/>
       <c r="D224" t="s">
         <v>159</v>
@@ -5037,7 +5037,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="225" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="12"/>
       <c r="D225" s="9" t="s">
         <v>490</v>
@@ -5049,7 +5049,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="226" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="12"/>
       <c r="D226" s="9" t="s">
         <v>492</v>
@@ -5061,13 +5061,13 @@
         <v>503</v>
       </c>
     </row>
-    <row r="227" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:6" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="3"/>
     </row>
-    <row r="228" spans="1:6" s="9" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A228" s="2"/>
     </row>
-    <row r="230" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="12" t="s">
         <v>348</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="12"/>
       <c r="B231" t="s">
         <v>53</v>
@@ -5099,7 +5099,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="12"/>
       <c r="B232" t="s">
         <v>55</v>
@@ -5114,7 +5114,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="233" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="12"/>
       <c r="B233" t="s">
         <v>58</v>
@@ -5129,7 +5129,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="234" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="12"/>
       <c r="D234" t="s">
         <v>493</v>
@@ -5141,7 +5141,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="235" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="12"/>
       <c r="B235" t="s">
         <v>59</v>
@@ -5156,7 +5156,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="236" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="12"/>
       <c r="B236" t="s">
         <v>61</v>
@@ -5171,7 +5171,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="237" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="12"/>
       <c r="B237" t="s">
         <v>63</v>
@@ -5186,7 +5186,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="238" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="12"/>
       <c r="B238" t="s">
         <v>64</v>
@@ -5201,7 +5201,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="239" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="12"/>
       <c r="D239" t="s">
         <v>494</v>
@@ -5213,7 +5213,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="240" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="12"/>
       <c r="D240" t="s">
         <v>495</v>
@@ -5225,7 +5225,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="241" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="12"/>
       <c r="D241" t="s">
         <v>496</v>
@@ -5254,7 +5254,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="247" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="12" t="s">
         <v>119</v>
       </c>
@@ -5271,7 +5271,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="248" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="12"/>
       <c r="B248" t="s">
         <v>513</v>
@@ -5286,7 +5286,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="249" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="12"/>
       <c r="B249" t="s">
         <v>122</v>
@@ -5301,7 +5301,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="250" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="12"/>
       <c r="B250" t="s">
         <v>121</v>
@@ -5313,7 +5313,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="251" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="12"/>
       <c r="B251" t="s">
         <v>123</v>
@@ -5328,7 +5328,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="252" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="12"/>
       <c r="B252" t="s">
         <v>117</v>
@@ -5343,7 +5343,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="253" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="12"/>
       <c r="D253" t="s">
         <v>613</v>
@@ -5352,10 +5352,10 @@
         <v>501</v>
       </c>
       <c r="F253" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="254" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="12"/>
       <c r="B254" t="s">
         <v>124</v>
@@ -5370,7 +5370,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="255" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="12"/>
       <c r="B255" t="s">
         <v>125</v>
@@ -5385,7 +5385,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="256" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="12"/>
       <c r="B256" t="s">
         <v>129</v>
@@ -5403,7 +5403,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="257" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" s="12"/>
       <c r="B257" t="s">
         <v>130</v>
@@ -5418,7 +5418,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="258" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="12"/>
       <c r="B258" t="s">
         <v>137</v>
@@ -5433,7 +5433,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="259" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" s="12"/>
       <c r="B259" t="s">
         <v>0</v>
@@ -5448,7 +5448,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="260" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="12"/>
       <c r="B260" t="s">
         <v>0</v>
@@ -5463,7 +5463,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="261" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A261" s="12"/>
       <c r="B261" t="s">
         <v>0</v>
@@ -5478,7 +5478,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="262" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A262" s="12"/>
       <c r="B262" t="s">
         <v>0</v>
@@ -5493,28 +5493,28 @@
         <v>510</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A263" s="12"/>
       <c r="B263" t="s">
         <v>0</v>
       </c>
       <c r="D263" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E263" t="s">
         <v>501</v>
       </c>
       <c r="F263" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="264" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" s="3"/>
     </row>
-    <row r="265" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A265" s="2"/>
     </row>
-    <row r="266" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A266" s="13" t="s">
         <v>618</v>
       </c>
@@ -5528,7 +5528,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="267" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A267" s="13"/>
       <c r="D267" t="s">
         <v>619</v>
@@ -5537,10 +5537,10 @@
         <v>501</v>
       </c>
       <c r="F267" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="268" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" s="13"/>
       <c r="B268" t="s">
         <v>177</v>
@@ -5552,10 +5552,10 @@
         <v>501</v>
       </c>
       <c r="F268" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="269" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" s="13"/>
       <c r="B269" t="s">
         <v>178</v>
@@ -5567,10 +5567,10 @@
         <v>501</v>
       </c>
       <c r="F269" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="270" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A270" s="13"/>
       <c r="B270" t="s">
         <v>179</v>
@@ -5582,10 +5582,10 @@
         <v>501</v>
       </c>
       <c r="F270" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="271" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A271" s="13"/>
       <c r="D271" t="s">
         <v>181</v>
@@ -5597,7 +5597,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="272" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A272" s="13"/>
       <c r="D272" t="s">
         <v>180</v>
@@ -5609,7 +5609,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="273" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A273" s="13"/>
       <c r="D273" t="s">
         <v>511</v>
@@ -5621,19 +5621,19 @@
         <v>512</v>
       </c>
     </row>
-    <row r="274" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" s="13"/>
       <c r="D274" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E274" t="s">
         <v>501</v>
       </c>
       <c r="F274" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="275" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A275" s="13"/>
       <c r="D275" t="s">
         <v>185</v>
@@ -5645,7 +5645,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="276" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A276" s="13"/>
       <c r="D276" t="s">
         <v>198</v>
@@ -5657,7 +5657,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="279" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A279" s="12" t="s">
         <v>127</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="280" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A280" s="12"/>
       <c r="B280" t="s">
         <v>116</v>
@@ -5683,7 +5683,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="281" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A281" s="12"/>
       <c r="B281" t="s">
         <v>118</v>
@@ -5695,7 +5695,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="282" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A282" s="12"/>
       <c r="B282" t="s">
         <v>128</v>
@@ -5707,7 +5707,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="283" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A283" s="12"/>
       <c r="B283" t="s">
         <v>121</v>
@@ -5719,13 +5719,13 @@
         <v>230</v>
       </c>
     </row>
-    <row r="284" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="3"/>
     </row>
-    <row r="285" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A285" s="3"/>
     </row>
-    <row r="286" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A286" s="13" t="s">
         <v>141</v>
       </c>
@@ -5742,7 +5742,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="287" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A287" s="13"/>
       <c r="B287" t="s">
         <v>0</v>
@@ -5757,13 +5757,13 @@
         <v>171</v>
       </c>
     </row>
-    <row r="288" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A288" s="13"/>
       <c r="B288" t="s">
         <v>0</v>
       </c>
       <c r="D288" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="E288" t="s">
         <v>140</v>
@@ -5772,13 +5772,13 @@
         <v>502</v>
       </c>
     </row>
-    <row r="289" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A289" s="13"/>
       <c r="B289" t="s">
         <v>0</v>
       </c>
       <c r="D289" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E289" t="s">
         <v>140</v>
@@ -5787,22 +5787,22 @@
         <v>172</v>
       </c>
     </row>
-    <row r="290" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A290" s="13"/>
       <c r="B290" t="s">
         <v>0</v>
       </c>
       <c r="D290" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E290" t="s">
         <v>140</v>
       </c>
       <c r="F290" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="291" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A291" s="13"/>
       <c r="B291" t="s">
         <v>0</v>
@@ -5817,7 +5817,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="292" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A292" s="13"/>
       <c r="B292" t="s">
         <v>0</v>
@@ -5832,7 +5832,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="293" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A293" s="13"/>
       <c r="B293" t="s">
         <v>0</v>
@@ -5847,7 +5847,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="294" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A294" s="13"/>
       <c r="B294" t="s">
         <v>0</v>
@@ -5862,7 +5862,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="295" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A295" s="13"/>
       <c r="B295" t="s">
         <v>0</v>
@@ -5877,7 +5877,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="296" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A296" s="13"/>
       <c r="B296" t="s">
         <v>0</v>
@@ -5892,13 +5892,13 @@
         <v>176</v>
       </c>
     </row>
-    <row r="297" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A297" s="8"/>
     </row>
-    <row r="298" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A298" s="8"/>
     </row>
-    <row r="299" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A299" s="12" t="s">
         <v>187</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="300" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A300" s="12"/>
       <c r="D300" t="s">
         <v>190</v>
@@ -5918,7 +5918,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="301" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A301" s="12"/>
       <c r="D301" t="s">
         <v>192</v>
@@ -5927,7 +5927,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="302" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A302" s="12"/>
       <c r="D302" t="s">
         <v>193</v>
@@ -5936,7 +5936,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="303" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A303" s="12"/>
       <c r="D303" t="s">
         <v>196</v>
@@ -5945,7 +5945,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="304" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A304" s="12"/>
       <c r="B304" t="s">
         <v>226</v>
@@ -5957,7 +5957,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="305" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A305" s="12"/>
       <c r="B305" t="s">
         <v>229</v>
@@ -5969,7 +5969,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="306" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A306" s="12"/>
       <c r="B306" t="s">
         <v>228</v>
@@ -5981,7 +5981,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="307" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A307" s="12"/>
       <c r="B307" t="s">
         <v>227</v>
@@ -5993,7 +5993,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="308" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A308" s="12"/>
       <c r="D308" t="s">
         <v>504</v>
@@ -6002,18 +6002,11 @@
         <v>505</v>
       </c>
     </row>
-    <row r="309" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A309" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A299:A308"/>
-    <mergeCell ref="A279:A283"/>
-    <mergeCell ref="A221:A226"/>
-    <mergeCell ref="A230:A241"/>
-    <mergeCell ref="A266:A276"/>
-    <mergeCell ref="A286:A296"/>
-    <mergeCell ref="A247:A263"/>
     <mergeCell ref="A44:A82"/>
     <mergeCell ref="A18:A41"/>
     <mergeCell ref="A3:A15"/>
@@ -6023,6 +6016,13 @@
     <mergeCell ref="A128:A150"/>
     <mergeCell ref="A153:A175"/>
     <mergeCell ref="A85:A100"/>
+    <mergeCell ref="A299:A308"/>
+    <mergeCell ref="A279:A283"/>
+    <mergeCell ref="A221:A226"/>
+    <mergeCell ref="A230:A241"/>
+    <mergeCell ref="A266:A276"/>
+    <mergeCell ref="A286:A296"/>
+    <mergeCell ref="A247:A263"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6035,7 +6035,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6047,7 +6047,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
GearSwap v0.812 - More bugfixing
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variables.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="643">
   <si>
     <t>N/A</t>
   </si>
@@ -1933,6 +1933,18 @@
   </si>
   <si>
     <t>Returns true or false based on whether or not you are in the middle of an action. True between precast and aftercast. If it is true, also returns the resources line of the spell being cast.</t>
+  </si>
+  <si>
+    <t>Current weather's name. Respects scholar spells/buffs.</t>
+  </si>
+  <si>
+    <t>Current weather's element. Respects scholar spells/buffs.</t>
+  </si>
+  <si>
+    <t>world.real_weather</t>
+  </si>
+  <si>
+    <t>world.real_weather_element</t>
   </si>
 </sst>
 </file>
@@ -2326,22 +2338,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F309"/>
+  <dimension ref="A1:F311"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F238" workbookViewId="0">
-      <selection activeCell="F254" sqref="F254"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="E239" sqref="E239"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" customWidth="1"/>
-    <col min="4" max="4" width="40.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="202.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="202.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.95" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="25.9" x14ac:dyDescent="0.5">
       <c r="B1" s="6" t="s">
         <v>498</v>
       </c>
@@ -2356,7 +2368,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
@@ -2373,7 +2385,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" t="s">
         <v>2</v>
@@ -2388,7 +2400,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" t="s">
         <v>4</v>
@@ -2403,7 +2415,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" t="s">
         <v>6</v>
@@ -2418,7 +2430,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" t="s">
         <v>8</v>
@@ -2433,7 +2445,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" t="s">
         <v>10</v>
@@ -2448,7 +2460,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" t="s">
         <v>12</v>
@@ -2463,7 +2475,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" t="s">
         <v>14</v>
@@ -2478,7 +2490,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" t="s">
         <v>16</v>
@@ -2493,7 +2505,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" t="s">
         <v>18</v>
@@ -2508,7 +2520,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="D13" t="s">
         <v>245</v>
@@ -2520,7 +2532,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="D14" t="s">
         <v>246</v>
@@ -2532,7 +2544,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="D15" t="s">
         <v>247</v>
@@ -2544,13 +2556,13 @@
         <v>249</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>612</v>
       </c>
@@ -2567,7 +2579,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" t="s">
         <v>74</v>
@@ -2582,7 +2594,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" t="s">
         <v>76</v>
@@ -2597,7 +2609,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" t="s">
         <v>78</v>
@@ -2612,7 +2624,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" t="s">
         <v>80</v>
@@ -2627,7 +2639,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" t="s">
         <v>82</v>
@@ -2642,7 +2654,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="D24" t="s">
         <v>595</v>
@@ -2654,7 +2666,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="D25" t="s">
         <v>578</v>
@@ -2666,7 +2678,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="D26" t="s">
         <v>579</v>
@@ -2678,7 +2690,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="D27" t="s">
         <v>580</v>
@@ -2690,7 +2702,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="D28" t="s">
         <v>581</v>
@@ -2702,7 +2714,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="D29" t="s">
         <v>582</v>
@@ -2714,7 +2726,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="D30" t="s">
         <v>583</v>
@@ -2726,7 +2738,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="D31" t="s">
         <v>584</v>
@@ -2738,7 +2750,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="D32" t="s">
         <v>585</v>
@@ -2750,7 +2762,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="D33" t="s">
         <v>586</v>
@@ -2762,7 +2774,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="D34" t="s">
         <v>587</v>
@@ -2774,7 +2786,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="D35" t="s">
         <v>588</v>
@@ -2786,7 +2798,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="D36" t="s">
         <v>589</v>
@@ -2798,7 +2810,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
       <c r="D37" t="s">
         <v>590</v>
@@ -2810,7 +2822,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
       <c r="D38" t="s">
         <v>591</v>
@@ -2822,7 +2834,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="D39" t="s">
         <v>592</v>
@@ -2834,7 +2846,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="D40" t="s">
         <v>593</v>
@@ -2846,7 +2858,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="D41" t="s">
         <v>594</v>
@@ -2858,7 +2870,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>345</v>
       </c>
@@ -2875,7 +2887,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" t="s">
         <v>22</v>
@@ -2890,7 +2902,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" t="s">
         <v>26</v>
@@ -2905,7 +2917,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" t="s">
         <v>28</v>
@@ -2920,7 +2932,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" t="s">
         <v>30</v>
@@ -2935,7 +2947,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12"/>
       <c r="B49" t="s">
         <v>32</v>
@@ -2950,7 +2962,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>
       <c r="B50" t="s">
         <v>33</v>
@@ -2965,7 +2977,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
       <c r="B51" t="s">
         <v>36</v>
@@ -2980,7 +2992,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
       <c r="B52" t="s">
         <v>38</v>
@@ -2995,7 +3007,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12"/>
       <c r="D53" t="s">
         <v>326</v>
@@ -3007,7 +3019,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
       <c r="B54" t="s">
         <v>40</v>
@@ -3022,7 +3034,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
       <c r="D55" t="s">
         <v>328</v>
@@ -3034,7 +3046,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
       <c r="B56" t="s">
         <v>41</v>
@@ -3049,7 +3061,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
       <c r="D57" t="s">
         <v>330</v>
@@ -3061,7 +3073,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12"/>
       <c r="B58" t="s">
         <v>42</v>
@@ -3076,7 +3088,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
       <c r="D59" t="s">
         <v>331</v>
@@ -3088,7 +3100,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12"/>
       <c r="B60" t="s">
         <v>43</v>
@@ -3103,7 +3115,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12"/>
       <c r="B61" t="s">
         <v>49</v>
@@ -3118,7 +3130,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12"/>
       <c r="B62" t="s">
         <v>51</v>
@@ -3133,7 +3145,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="D63" t="s">
         <v>318</v>
@@ -3145,7 +3157,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="D64" t="s">
         <v>320</v>
@@ -3157,7 +3169,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="D65" t="s">
         <v>322</v>
@@ -3169,7 +3181,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="D66" t="s">
         <v>324</v>
@@ -3181,7 +3193,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="D67" t="s">
         <v>325</v>
@@ -3193,7 +3205,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="D68" t="s">
         <v>336</v>
@@ -3205,7 +3217,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="D69" t="s">
         <v>338</v>
@@ -3217,7 +3229,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="D70" t="s">
         <v>339</v>
@@ -3229,7 +3241,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="D71" t="s">
         <v>342</v>
@@ -3241,7 +3253,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="D72" t="s">
         <v>379</v>
@@ -3253,7 +3265,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12"/>
       <c r="D73" t="s">
         <v>380</v>
@@ -3265,7 +3277,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12"/>
       <c r="D74" t="s">
         <v>381</v>
@@ -3277,7 +3289,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12"/>
       <c r="D75" t="s">
         <v>426</v>
@@ -3289,7 +3301,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12"/>
       <c r="D76" t="s">
         <v>516</v>
@@ -3301,7 +3313,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12"/>
       <c r="D77" t="s">
         <v>382</v>
@@ -3313,7 +3325,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12"/>
       <c r="D78" t="s">
         <v>383</v>
@@ -3325,7 +3337,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12"/>
       <c r="D79" t="s">
         <v>384</v>
@@ -3337,7 +3349,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12"/>
       <c r="D80" t="s">
         <v>385</v>
@@ -3349,7 +3361,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12"/>
       <c r="D81" t="s">
         <v>386</v>
@@ -3361,7 +3373,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12"/>
       <c r="D82" t="s">
         <v>387</v>
@@ -3373,13 +3385,13 @@
         <v>376</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
     </row>
-    <row r="84" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="7"/>
     </row>
-    <row r="85" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
         <v>344</v>
       </c>
@@ -3396,7 +3408,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12"/>
       <c r="B86" t="s">
         <v>95</v>
@@ -3411,7 +3423,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12"/>
       <c r="B87" t="s">
         <v>96</v>
@@ -3426,7 +3438,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12"/>
       <c r="B88" t="s">
         <v>97</v>
@@ -3441,7 +3453,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12"/>
       <c r="B89" t="s">
         <v>278</v>
@@ -3456,7 +3468,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12"/>
       <c r="B90" t="s">
         <v>279</v>
@@ -3471,7 +3483,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
       <c r="B91" t="s">
         <v>280</v>
@@ -3486,7 +3498,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
       <c r="B92" t="s">
         <v>281</v>
@@ -3501,7 +3513,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12"/>
       <c r="B93" t="s">
         <v>282</v>
@@ -3516,7 +3528,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12"/>
       <c r="B94" t="s">
         <v>283</v>
@@ -3531,7 +3543,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12"/>
       <c r="B95" t="s">
         <v>284</v>
@@ -3546,7 +3558,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12"/>
       <c r="B96" t="s">
         <v>285</v>
@@ -3561,7 +3573,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
       <c r="B97" t="s">
         <v>286</v>
@@ -3576,7 +3588,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
       <c r="B98" t="s">
         <v>287</v>
@@ -3591,7 +3603,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
       <c r="B99" t="s">
         <v>288</v>
@@ -3606,7 +3618,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12"/>
       <c r="B100" t="s">
         <v>289</v>
@@ -3621,13 +3633,13 @@
         <v>291</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3"/>
     </row>
-    <row r="102" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
     </row>
-    <row r="103" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="s">
         <v>349</v>
       </c>
@@ -3644,7 +3656,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12"/>
       <c r="B104" t="s">
         <v>68</v>
@@ -3659,7 +3671,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12"/>
       <c r="B105" t="s">
         <v>69</v>
@@ -3674,7 +3686,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12"/>
       <c r="B106" t="s">
         <v>70</v>
@@ -3689,7 +3701,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="12"/>
       <c r="B107" t="s">
         <v>71</v>
@@ -3704,7 +3716,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="12"/>
       <c r="D108" t="s">
         <v>353</v>
@@ -3716,7 +3728,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="12"/>
       <c r="D109" t="s">
         <v>360</v>
@@ -3728,7 +3740,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="12"/>
       <c r="D110" t="s">
         <v>361</v>
@@ -3740,7 +3752,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="12"/>
       <c r="D111" t="s">
         <v>352</v>
@@ -3752,7 +3764,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="12"/>
       <c r="D112" t="s">
         <v>354</v>
@@ -3764,7 +3776,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="12"/>
       <c r="D113" t="s">
         <v>355</v>
@@ -3776,7 +3788,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="12"/>
       <c r="D114" t="s">
         <v>425</v>
@@ -3788,7 +3800,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="12"/>
       <c r="D115" t="s">
         <v>577</v>
@@ -3800,7 +3812,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="12"/>
       <c r="D116" t="s">
         <v>518</v>
@@ -3812,7 +3824,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12"/>
       <c r="D117" t="s">
         <v>369</v>
@@ -3824,7 +3836,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="12"/>
       <c r="D118" t="s">
         <v>370</v>
@@ -3836,7 +3848,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="12"/>
       <c r="D119" t="s">
         <v>357</v>
@@ -3848,7 +3860,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="12"/>
       <c r="D120" t="s">
         <v>358</v>
@@ -3860,7 +3872,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="12"/>
       <c r="D121" t="s">
         <v>359</v>
@@ -3872,7 +3884,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="12"/>
       <c r="D122" t="s">
         <v>351</v>
@@ -3884,7 +3896,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="12"/>
       <c r="D123" t="s">
         <v>356</v>
@@ -3896,7 +3908,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="12"/>
       <c r="D124" t="s">
         <v>367</v>
@@ -3908,7 +3920,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="12"/>
       <c r="D125" t="s">
         <v>377</v>
@@ -3920,13 +3932,13 @@
         <v>378</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="10"/>
     </row>
-    <row r="127" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
     </row>
-    <row r="128" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="12" t="s">
         <v>533</v>
       </c>
@@ -3940,7 +3952,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="12"/>
       <c r="D129" t="s">
         <v>554</v>
@@ -3952,7 +3964,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="12"/>
       <c r="D130" t="s">
         <v>555</v>
@@ -3964,7 +3976,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="12"/>
       <c r="D131" t="s">
         <v>556</v>
@@ -3976,7 +3988,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="12"/>
       <c r="D132" t="s">
         <v>557</v>
@@ -3988,7 +4000,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="12"/>
       <c r="D133" t="s">
         <v>558</v>
@@ -4000,7 +4012,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="12"/>
       <c r="D134" t="s">
         <v>559</v>
@@ -4012,7 +4024,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="12"/>
       <c r="D135" t="s">
         <v>560</v>
@@ -4024,7 +4036,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="12"/>
       <c r="D136" t="s">
         <v>561</v>
@@ -4036,7 +4048,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="12"/>
       <c r="D137" t="s">
         <v>562</v>
@@ -4048,7 +4060,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="12"/>
       <c r="D138" t="s">
         <v>563</v>
@@ -4060,7 +4072,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="12"/>
       <c r="D139" t="s">
         <v>564</v>
@@ -4072,7 +4084,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="12"/>
       <c r="D140" t="s">
         <v>565</v>
@@ -4084,7 +4096,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="12"/>
       <c r="D141" t="s">
         <v>566</v>
@@ -4096,7 +4108,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="12"/>
       <c r="D142" t="s">
         <v>567</v>
@@ -4108,7 +4120,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="12"/>
       <c r="D143" t="s">
         <v>568</v>
@@ -4120,7 +4132,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="12"/>
       <c r="D144" t="s">
         <v>569</v>
@@ -4132,7 +4144,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="12"/>
       <c r="D145" t="s">
         <v>570</v>
@@ -4144,7 +4156,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="12"/>
       <c r="D146" t="s">
         <v>571</v>
@@ -4156,7 +4168,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="12"/>
       <c r="D147" t="s">
         <v>572</v>
@@ -4168,7 +4180,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="12"/>
       <c r="D148" t="s">
         <v>573</v>
@@ -4180,7 +4192,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="12"/>
       <c r="D149" t="s">
         <v>574</v>
@@ -4192,7 +4204,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="12"/>
       <c r="D150" t="s">
         <v>575</v>
@@ -4204,13 +4216,13 @@
         <v>412</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="11"/>
     </row>
-    <row r="152" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
     </row>
-    <row r="153" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="12" t="s">
         <v>350</v>
       </c>
@@ -4224,7 +4236,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="12"/>
       <c r="D154" t="s">
         <v>90</v>
@@ -4236,7 +4248,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="12"/>
       <c r="D155" t="s">
         <v>91</v>
@@ -4248,7 +4260,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="12"/>
       <c r="D156" t="s">
         <v>92</v>
@@ -4260,7 +4272,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="12"/>
       <c r="D157" t="s">
         <v>93</v>
@@ -4272,7 +4284,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="12"/>
       <c r="D158" t="s">
         <v>393</v>
@@ -4284,7 +4296,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="12"/>
       <c r="D159" t="s">
         <v>398</v>
@@ -4296,7 +4308,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="12"/>
       <c r="D160" t="s">
         <v>399</v>
@@ -4308,7 +4320,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="12"/>
       <c r="D161" t="s">
         <v>400</v>
@@ -4320,7 +4332,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="12"/>
       <c r="D162" t="s">
         <v>401</v>
@@ -4332,7 +4344,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="12"/>
       <c r="D163" t="s">
         <v>402</v>
@@ -4344,7 +4356,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="12"/>
       <c r="D164" t="s">
         <v>424</v>
@@ -4356,7 +4368,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="12"/>
       <c r="D165" t="s">
         <v>528</v>
@@ -4368,7 +4380,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="12"/>
       <c r="D166" t="s">
         <v>519</v>
@@ -4380,7 +4392,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="12"/>
       <c r="D167" t="s">
         <v>403</v>
@@ -4392,7 +4404,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="12"/>
       <c r="D168" t="s">
         <v>404</v>
@@ -4404,7 +4416,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="12"/>
       <c r="D169" t="s">
         <v>405</v>
@@ -4416,7 +4428,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="12"/>
       <c r="D170" t="s">
         <v>406</v>
@@ -4428,7 +4440,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="12"/>
       <c r="D171" t="s">
         <v>407</v>
@@ -4440,7 +4452,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="12"/>
       <c r="D172" t="s">
         <v>408</v>
@@ -4452,7 +4464,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="12"/>
       <c r="D173" t="s">
         <v>409</v>
@@ -4464,7 +4476,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="12"/>
       <c r="D174" t="s">
         <v>410</v>
@@ -4476,7 +4488,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="12"/>
       <c r="D175" t="s">
         <v>411</v>
@@ -4488,10 +4500,10 @@
         <v>412</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="3"/>
     </row>
-    <row r="178" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="12" t="s">
         <v>346</v>
       </c>
@@ -4508,7 +4520,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="12"/>
       <c r="B179" t="s">
         <v>100</v>
@@ -4523,7 +4535,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="12"/>
       <c r="B180" t="s">
         <v>102</v>
@@ -4538,7 +4550,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12"/>
       <c r="B181" t="s">
         <v>104</v>
@@ -4553,7 +4565,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="12"/>
       <c r="D182" t="s">
         <v>429</v>
@@ -4565,7 +4577,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="12"/>
       <c r="B183" t="s">
         <v>108</v>
@@ -4580,7 +4592,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="12"/>
       <c r="B184" t="s">
         <v>106</v>
@@ -4592,7 +4604,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="12"/>
       <c r="D185" t="s">
         <v>432</v>
@@ -4604,7 +4616,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="12"/>
       <c r="D186" t="s">
         <v>433</v>
@@ -4616,7 +4628,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="12"/>
       <c r="D187" t="s">
         <v>434</v>
@@ -4628,7 +4640,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="12"/>
       <c r="D188" t="s">
         <v>522</v>
@@ -4640,7 +4652,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="189" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="12"/>
       <c r="D189" t="s">
         <v>520</v>
@@ -4652,7 +4664,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="190" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="12"/>
       <c r="D190" t="s">
         <v>435</v>
@@ -4664,7 +4676,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="191" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="12"/>
       <c r="D191" t="s">
         <v>436</v>
@@ -4676,7 +4688,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="192" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="12"/>
       <c r="D192" t="s">
         <v>437</v>
@@ -4688,7 +4700,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="12"/>
       <c r="D193" t="s">
         <v>438</v>
@@ -4700,7 +4712,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="194" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="12"/>
       <c r="D194" t="s">
         <v>439</v>
@@ -4712,7 +4724,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="195" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="12"/>
       <c r="D195" t="s">
         <v>440</v>
@@ -4724,7 +4736,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="196" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="12"/>
       <c r="D196" t="s">
         <v>441</v>
@@ -4736,7 +4748,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="12"/>
       <c r="D197" t="s">
         <v>442</v>
@@ -4748,7 +4760,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="200" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="12" t="s">
         <v>347</v>
       </c>
@@ -4765,7 +4777,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="201" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="12"/>
       <c r="B201" t="s">
         <v>110</v>
@@ -4780,7 +4792,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="202" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="12"/>
       <c r="B202" t="s">
         <v>111</v>
@@ -4795,7 +4807,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="203" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="12"/>
       <c r="D203" t="s">
         <v>455</v>
@@ -4807,7 +4819,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="204" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="12"/>
       <c r="D204" t="s">
         <v>456</v>
@@ -4819,7 +4831,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="205" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="12"/>
       <c r="D205" t="s">
         <v>457</v>
@@ -4831,7 +4843,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="206" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="12"/>
       <c r="D206" t="s">
         <v>458</v>
@@ -4843,7 +4855,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="207" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="12"/>
       <c r="D207" t="s">
         <v>460</v>
@@ -4852,7 +4864,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="12"/>
       <c r="D208" t="s">
         <v>459</v>
@@ -4864,7 +4876,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="209" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="12"/>
       <c r="D209" t="s">
         <v>527</v>
@@ -4876,7 +4888,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="210" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="12"/>
       <c r="D210" t="s">
         <v>521</v>
@@ -4888,7 +4900,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="12"/>
       <c r="D211" t="s">
         <v>461</v>
@@ -4900,7 +4912,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="212" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="12"/>
       <c r="D212" t="s">
         <v>462</v>
@@ -4912,7 +4924,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="213" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="12"/>
       <c r="D213" t="s">
         <v>463</v>
@@ -4924,7 +4936,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="214" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="12"/>
       <c r="D214" t="s">
         <v>464</v>
@@ -4936,7 +4948,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="12"/>
       <c r="D215" t="s">
         <v>465</v>
@@ -4948,7 +4960,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="216" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="12"/>
       <c r="D216" t="s">
         <v>466</v>
@@ -4960,7 +4972,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="217" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="12"/>
       <c r="D217" t="s">
         <v>467</v>
@@ -4972,7 +4984,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="218" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="12"/>
       <c r="D218" t="s">
         <v>468</v>
@@ -4984,7 +4996,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="221" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="12" t="s">
         <v>491</v>
       </c>
@@ -5001,7 +5013,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="222" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="12"/>
       <c r="D222" t="s">
         <v>155</v>
@@ -5013,7 +5025,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="223" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="12"/>
       <c r="D223" t="s">
         <v>158</v>
@@ -5025,7 +5037,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="12"/>
       <c r="D224" t="s">
         <v>159</v>
@@ -5037,7 +5049,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="225" spans="1:6" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="12"/>
       <c r="D225" s="9" t="s">
         <v>490</v>
@@ -5049,7 +5061,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="226" spans="1:6" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="12"/>
       <c r="D226" s="9" t="s">
         <v>492</v>
@@ -5061,14 +5073,14 @@
         <v>503</v>
       </c>
     </row>
-    <row r="227" spans="1:6" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="3"/>
     </row>
-    <row r="228" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:6" s="9" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A228" s="2"/>
     </row>
-    <row r="230" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A230" s="12" t="s">
+    <row r="230" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="3" t="s">
         <v>348</v>
       </c>
       <c r="B230" t="s">
@@ -5084,8 +5096,8 @@
         <v>489</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A231" s="12"/>
+    <row r="231" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="3"/>
       <c r="B231" t="s">
         <v>53</v>
       </c>
@@ -5099,8 +5111,8 @@
         <v>497</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A232" s="12"/>
+    <row r="232" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="3"/>
       <c r="B232" t="s">
         <v>55</v>
       </c>
@@ -5114,8 +5126,8 @@
         <v>488</v>
       </c>
     </row>
-    <row r="233" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A233" s="12"/>
+    <row r="233" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="3"/>
       <c r="B233" t="s">
         <v>58</v>
       </c>
@@ -5129,8 +5141,8 @@
         <v>487</v>
       </c>
     </row>
-    <row r="234" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="12"/>
+    <row r="234" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="3"/>
       <c r="D234" t="s">
         <v>493</v>
       </c>
@@ -5141,8 +5153,8 @@
         <v>231</v>
       </c>
     </row>
-    <row r="235" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A235" s="12"/>
+    <row r="235" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="3"/>
       <c r="B235" t="s">
         <v>59</v>
       </c>
@@ -5153,11 +5165,11 @@
         <v>138</v>
       </c>
       <c r="F235" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A236" s="12"/>
+        <v>639</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="3"/>
       <c r="B236" t="s">
         <v>61</v>
       </c>
@@ -5168,845 +5180,875 @@
         <v>138</v>
       </c>
       <c r="F236" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="3"/>
+      <c r="D237" t="s">
+        <v>641</v>
+      </c>
+      <c r="E237" t="s">
+        <v>138</v>
+      </c>
+      <c r="F237" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="3"/>
+      <c r="D238" t="s">
+        <v>642</v>
+      </c>
+      <c r="E238" t="s">
+        <v>138</v>
+      </c>
+      <c r="F238" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="237" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A237" s="12"/>
-      <c r="B237" t="s">
+    <row r="239" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="3"/>
+      <c r="B239" t="s">
         <v>63</v>
       </c>
-      <c r="D237" t="s">
+      <c r="D239" t="s">
         <v>65</v>
       </c>
-      <c r="E237" t="s">
-        <v>138</v>
-      </c>
-      <c r="F237" t="s">
+      <c r="E239" t="s">
+        <v>138</v>
+      </c>
+      <c r="F239" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="238" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A238" s="12"/>
-      <c r="B238" t="s">
+    <row r="240" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="3"/>
+      <c r="B240" t="s">
         <v>64</v>
       </c>
-      <c r="D238" t="s">
+      <c r="D240" t="s">
         <v>66</v>
       </c>
-      <c r="E238" t="s">
-        <v>263</v>
-      </c>
-      <c r="F238" t="s">
+      <c r="E240" t="s">
+        <v>263</v>
+      </c>
+      <c r="F240" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="239" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A239" s="12"/>
-      <c r="D239" t="s">
+    <row r="241" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="3"/>
+      <c r="D241" t="s">
         <v>494</v>
       </c>
-      <c r="E239" t="s">
-        <v>138</v>
-      </c>
-      <c r="F239" t="s">
+      <c r="E241" t="s">
+        <v>138</v>
+      </c>
+      <c r="F241" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="240" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A240" s="12"/>
-      <c r="D240" t="s">
+    <row r="242" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="3"/>
+      <c r="D242" t="s">
         <v>495</v>
       </c>
-      <c r="E240" t="s">
-        <v>263</v>
-      </c>
-      <c r="F240" t="s">
+      <c r="E242" t="s">
+        <v>263</v>
+      </c>
+      <c r="F242" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="241" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A241" s="12"/>
-      <c r="D241" t="s">
+    <row r="243" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="3"/>
+      <c r="D243" t="s">
         <v>496</v>
       </c>
-      <c r="E241" t="s">
+      <c r="E243" t="s">
         <v>264</v>
       </c>
-      <c r="F241" t="s">
+      <c r="F243" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="244" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A244" s="4" t="s">
+    <row r="246" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A246" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B244" t="s">
+      <c r="B246" t="s">
         <v>120</v>
       </c>
-      <c r="D244" t="s">
+      <c r="D246" t="s">
         <v>120</v>
       </c>
-      <c r="E244" t="s">
+      <c r="E246" t="s">
         <v>140</v>
       </c>
-      <c r="F244" t="s">
+      <c r="F246" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="247" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A247" s="12" t="s">
+    <row r="249" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A249" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B247" t="s">
+      <c r="B249" t="s">
         <v>201</v>
       </c>
-      <c r="D247" t="s">
+      <c r="D249" t="s">
         <v>614</v>
-      </c>
-      <c r="E247" t="s">
-        <v>501</v>
-      </c>
-      <c r="F247" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A248" s="12"/>
-      <c r="B248" t="s">
-        <v>513</v>
-      </c>
-      <c r="D248" t="s">
-        <v>514</v>
-      </c>
-      <c r="E248" t="s">
-        <v>501</v>
-      </c>
-      <c r="F248" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A249" s="12"/>
-      <c r="B249" t="s">
-        <v>122</v>
-      </c>
-      <c r="D249" t="s">
-        <v>133</v>
       </c>
       <c r="E249" t="s">
         <v>501</v>
       </c>
       <c r="F249" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="250" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="12"/>
       <c r="B250" t="s">
-        <v>121</v>
+        <v>513</v>
       </c>
       <c r="D250" t="s">
-        <v>0</v>
+        <v>514</v>
+      </c>
+      <c r="E250" t="s">
+        <v>501</v>
       </c>
       <c r="F250" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="12"/>
       <c r="B251" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D251" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="E251" t="s">
         <v>501</v>
       </c>
       <c r="F251" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="12"/>
       <c r="B252" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D252" t="s">
-        <v>162</v>
-      </c>
-      <c r="E252" t="s">
-        <v>501</v>
+        <v>0</v>
       </c>
       <c r="F252" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="253" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="12"/>
+      <c r="B253" t="s">
+        <v>123</v>
+      </c>
       <c r="D253" t="s">
-        <v>613</v>
+        <v>161</v>
       </c>
       <c r="E253" t="s">
         <v>501</v>
       </c>
       <c r="F253" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="254" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="12"/>
       <c r="B254" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D254" t="s">
-        <v>203</v>
+        <v>162</v>
       </c>
       <c r="E254" t="s">
         <v>501</v>
       </c>
       <c r="F254" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="255" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="12"/>
-      <c r="B255" t="s">
-        <v>125</v>
-      </c>
       <c r="D255" t="s">
-        <v>204</v>
+        <v>613</v>
       </c>
       <c r="E255" t="s">
         <v>501</v>
       </c>
       <c r="F255" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="256" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="12"/>
       <c r="B256" t="s">
-        <v>129</v>
-      </c>
-      <c r="C256" s="5" t="s">
-        <v>212</v>
+        <v>124</v>
       </c>
       <c r="D256" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="E256" t="s">
         <v>501</v>
       </c>
       <c r="F256" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="257" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="12"/>
       <c r="B257" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D257" t="s">
-        <v>132</v>
+        <v>204</v>
       </c>
       <c r="E257" t="s">
         <v>501</v>
       </c>
       <c r="F257" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="258" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="12"/>
       <c r="B258" t="s">
-        <v>137</v>
+        <v>129</v>
+      </c>
+      <c r="C258" s="5" t="s">
+        <v>212</v>
       </c>
       <c r="D258" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="E258" t="s">
         <v>501</v>
       </c>
       <c r="F258" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="259" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="12"/>
       <c r="B259" t="s">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="D259" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E259" t="s">
         <v>501</v>
       </c>
       <c r="F259" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="260" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="12"/>
       <c r="B260" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
       <c r="D260" t="s">
-        <v>134</v>
+        <v>207</v>
       </c>
       <c r="E260" t="s">
         <v>501</v>
       </c>
       <c r="F260" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="261" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="12"/>
       <c r="B261" t="s">
         <v>0</v>
       </c>
       <c r="D261" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E261" t="s">
         <v>501</v>
       </c>
       <c r="F261" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="262" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="12"/>
       <c r="B262" t="s">
         <v>0</v>
       </c>
       <c r="D262" t="s">
-        <v>209</v>
+        <v>134</v>
       </c>
       <c r="E262" t="s">
         <v>501</v>
       </c>
       <c r="F262" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="12"/>
       <c r="B263" t="s">
         <v>0</v>
       </c>
       <c r="D263" t="s">
-        <v>633</v>
+        <v>135</v>
       </c>
       <c r="E263" t="s">
         <v>501</v>
       </c>
       <c r="F263" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A264" s="12"/>
+      <c r="B264" t="s">
+        <v>0</v>
+      </c>
+      <c r="D264" t="s">
+        <v>209</v>
+      </c>
+      <c r="E264" t="s">
+        <v>501</v>
+      </c>
+      <c r="F264" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265" s="12"/>
+      <c r="B265" t="s">
+        <v>0</v>
+      </c>
+      <c r="D265" t="s">
+        <v>633</v>
+      </c>
+      <c r="E265" t="s">
+        <v>501</v>
+      </c>
+      <c r="F265" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="264" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A264" s="3"/>
-    </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A265" s="2"/>
-    </row>
-    <row r="266" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A266" s="13" t="s">
+    <row r="266" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A266" s="3"/>
+    </row>
+    <row r="267" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A267" s="2"/>
+    </row>
+    <row r="268" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A268" s="13" t="s">
         <v>618</v>
       </c>
-      <c r="D266" t="s">
+      <c r="D268" t="s">
         <v>199</v>
-      </c>
-      <c r="E266" t="s">
-        <v>501</v>
-      </c>
-      <c r="F266" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="267" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A267" s="13"/>
-      <c r="D267" t="s">
-        <v>619</v>
-      </c>
-      <c r="E267" t="s">
-        <v>501</v>
-      </c>
-      <c r="F267" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="268" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A268" s="13"/>
-      <c r="B268" t="s">
-        <v>177</v>
-      </c>
-      <c r="D268" t="s">
-        <v>184</v>
       </c>
       <c r="E268" t="s">
         <v>501</v>
       </c>
       <c r="F268" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="269" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="13"/>
-      <c r="B269" t="s">
-        <v>178</v>
-      </c>
       <c r="D269" t="s">
-        <v>183</v>
+        <v>619</v>
       </c>
       <c r="E269" t="s">
         <v>501</v>
       </c>
       <c r="F269" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="270" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="13"/>
       <c r="B270" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D270" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E270" t="s">
         <v>501</v>
       </c>
       <c r="F270" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="271" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="13"/>
+      <c r="B271" t="s">
+        <v>178</v>
+      </c>
       <c r="D271" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E271" t="s">
         <v>501</v>
       </c>
       <c r="F271" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="272" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="13"/>
+      <c r="B272" t="s">
+        <v>179</v>
+      </c>
       <c r="D272" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E272" t="s">
         <v>501</v>
       </c>
       <c r="F272" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="273" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" s="13"/>
       <c r="D273" t="s">
-        <v>511</v>
+        <v>181</v>
       </c>
       <c r="E273" t="s">
         <v>501</v>
       </c>
       <c r="F273" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="274" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="13"/>
       <c r="D274" t="s">
-        <v>626</v>
+        <v>180</v>
       </c>
       <c r="E274" t="s">
         <v>501</v>
       </c>
       <c r="F274" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="275" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A275" s="13"/>
       <c r="D275" t="s">
-        <v>185</v>
+        <v>511</v>
       </c>
       <c r="E275" t="s">
         <v>501</v>
       </c>
       <c r="F275" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="276" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="13"/>
       <c r="D276" t="s">
-        <v>198</v>
+        <v>626</v>
       </c>
       <c r="E276" t="s">
         <v>501</v>
       </c>
       <c r="F276" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A277" s="13"/>
+      <c r="D277" t="s">
+        <v>185</v>
+      </c>
+      <c r="E277" t="s">
+        <v>501</v>
+      </c>
+      <c r="F277" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A278" s="13"/>
+      <c r="D278" t="s">
+        <v>198</v>
+      </c>
+      <c r="E278" t="s">
+        <v>501</v>
+      </c>
+      <c r="F278" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="279" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A279" s="12" t="s">
+    <row r="281" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A281" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="B279" t="s">
+      <c r="B281" t="s">
         <v>126</v>
-      </c>
-      <c r="D279" t="s">
-        <v>0</v>
-      </c>
-      <c r="F279" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="280" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A280" s="12"/>
-      <c r="B280" t="s">
-        <v>116</v>
-      </c>
-      <c r="D280" t="s">
-        <v>0</v>
-      </c>
-      <c r="F280" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="281" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A281" s="12"/>
-      <c r="B281" t="s">
-        <v>118</v>
       </c>
       <c r="D281" t="s">
         <v>0</v>
       </c>
       <c r="F281" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="282" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" s="12"/>
       <c r="B282" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="D282" t="s">
         <v>0</v>
       </c>
       <c r="F282" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="283" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="12"/>
       <c r="B283" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D283" t="s">
         <v>0</v>
       </c>
       <c r="F283" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A284" s="12"/>
+      <c r="B284" t="s">
+        <v>128</v>
+      </c>
+      <c r="D284" t="s">
+        <v>0</v>
+      </c>
+      <c r="F284" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A285" s="12"/>
+      <c r="B285" t="s">
+        <v>121</v>
+      </c>
+      <c r="D285" t="s">
+        <v>0</v>
+      </c>
+      <c r="F285" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="284" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A284" s="3"/>
-    </row>
-    <row r="285" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A285" s="3"/>
-    </row>
-    <row r="286" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A286" s="13" t="s">
+    <row r="286" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A286" s="3"/>
+    </row>
+    <row r="287" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A287" s="3"/>
+    </row>
+    <row r="288" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A288" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="B286" t="s">
-        <v>0</v>
-      </c>
-      <c r="D286" t="s">
-        <v>138</v>
-      </c>
-      <c r="E286" t="s">
-        <v>140</v>
-      </c>
-      <c r="F286" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="287" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A287" s="13"/>
-      <c r="B287" t="s">
-        <v>0</v>
-      </c>
-      <c r="D287" t="s">
-        <v>139</v>
-      </c>
-      <c r="E287" t="s">
-        <v>140</v>
-      </c>
-      <c r="F287" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="288" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A288" s="13"/>
       <c r="B288" t="s">
         <v>0</v>
       </c>
       <c r="D288" t="s">
-        <v>635</v>
+        <v>138</v>
       </c>
       <c r="E288" t="s">
         <v>140</v>
       </c>
       <c r="F288" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="289" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289" s="13"/>
       <c r="B289" t="s">
         <v>0</v>
       </c>
       <c r="D289" t="s">
-        <v>636</v>
+        <v>139</v>
       </c>
       <c r="E289" t="s">
         <v>140</v>
       </c>
       <c r="F289" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="290" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290" s="13"/>
       <c r="B290" t="s">
         <v>0</v>
       </c>
       <c r="D290" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="E290" t="s">
         <v>140</v>
       </c>
       <c r="F290" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="291" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="13"/>
       <c r="B291" t="s">
         <v>0</v>
       </c>
       <c r="D291" t="s">
-        <v>506</v>
+        <v>636</v>
       </c>
       <c r="E291" t="s">
         <v>140</v>
       </c>
       <c r="F291" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="292" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A292" s="13"/>
       <c r="B292" t="s">
         <v>0</v>
       </c>
       <c r="D292" t="s">
-        <v>508</v>
+        <v>637</v>
       </c>
       <c r="E292" t="s">
-        <v>501</v>
+        <v>140</v>
       </c>
       <c r="F292" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="293" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A293" s="13"/>
       <c r="B293" t="s">
         <v>0</v>
       </c>
       <c r="D293" t="s">
-        <v>142</v>
+        <v>506</v>
       </c>
       <c r="E293" t="s">
-        <v>501</v>
+        <v>140</v>
       </c>
       <c r="F293" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="294" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="13"/>
       <c r="B294" t="s">
         <v>0</v>
       </c>
       <c r="D294" t="s">
-        <v>143</v>
+        <v>508</v>
       </c>
       <c r="E294" t="s">
         <v>501</v>
       </c>
       <c r="F294" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="295" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A295" s="13"/>
       <c r="B295" t="s">
         <v>0</v>
       </c>
       <c r="D295" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E295" t="s">
         <v>501</v>
       </c>
       <c r="F295" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="296" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A296" s="13"/>
       <c r="B296" t="s">
         <v>0</v>
       </c>
       <c r="D296" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E296" t="s">
         <v>501</v>
       </c>
       <c r="F296" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A297" s="13"/>
+      <c r="B297" t="s">
+        <v>0</v>
+      </c>
+      <c r="D297" t="s">
+        <v>144</v>
+      </c>
+      <c r="E297" t="s">
+        <v>501</v>
+      </c>
+      <c r="F297" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A298" s="13"/>
+      <c r="B298" t="s">
+        <v>0</v>
+      </c>
+      <c r="D298" t="s">
+        <v>145</v>
+      </c>
+      <c r="E298" t="s">
+        <v>501</v>
+      </c>
+      <c r="F298" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="297" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A297" s="8"/>
-    </row>
-    <row r="298" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A298" s="8"/>
-    </row>
-    <row r="299" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A299" s="12" t="s">
+    <row r="299" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A299" s="8"/>
+    </row>
+    <row r="300" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="8"/>
+    </row>
+    <row r="301" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A301" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="D299" t="s">
+      <c r="D301" t="s">
         <v>188</v>
       </c>
-      <c r="F299" t="s">
+      <c r="F301" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="300" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A300" s="12"/>
-      <c r="D300" t="s">
-        <v>190</v>
-      </c>
-      <c r="F300" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="301" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A301" s="12"/>
-      <c r="D301" t="s">
-        <v>192</v>
-      </c>
-      <c r="F301" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="302" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="12"/>
       <c r="D302" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F302" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="303" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="12"/>
       <c r="D303" t="s">
+        <v>192</v>
+      </c>
+      <c r="F303" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A304" s="12"/>
+      <c r="D304" t="s">
+        <v>193</v>
+      </c>
+      <c r="F304" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A305" s="12"/>
+      <c r="D305" t="s">
         <v>196</v>
       </c>
-      <c r="F303" t="s">
+      <c r="F305" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="304" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A304" s="12"/>
-      <c r="B304" t="s">
-        <v>226</v>
-      </c>
-      <c r="D304" t="s">
-        <v>211</v>
-      </c>
-      <c r="F304" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="305" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A305" s="12"/>
-      <c r="B305" t="s">
-        <v>229</v>
-      </c>
-      <c r="D305" t="s">
-        <v>215</v>
-      </c>
-      <c r="F305" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="306" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A306" s="12"/>
       <c r="B306" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D306" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F306" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="307" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A307" s="12"/>
       <c r="B307" t="s">
+        <v>229</v>
+      </c>
+      <c r="D307" t="s">
+        <v>215</v>
+      </c>
+      <c r="F307" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A308" s="12"/>
+      <c r="B308" t="s">
+        <v>228</v>
+      </c>
+      <c r="D308" t="s">
+        <v>214</v>
+      </c>
+      <c r="F308" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A309" s="12"/>
+      <c r="B309" t="s">
         <v>227</v>
       </c>
-      <c r="D307" t="s">
+      <c r="D309" t="s">
         <v>224</v>
       </c>
-      <c r="F307" t="s">
+      <c r="F309" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="308" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A308" s="12"/>
-      <c r="D308" t="s">
+    <row r="310" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A310" s="12"/>
+      <c r="D310" t="s">
         <v>504</v>
       </c>
-      <c r="F308" t="s">
+      <c r="F310" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="309" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A309" s="3"/>
+    <row r="311" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A311" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="15">
+    <mergeCell ref="A301:A310"/>
+    <mergeCell ref="A281:A285"/>
+    <mergeCell ref="A221:A226"/>
+    <mergeCell ref="A268:A278"/>
+    <mergeCell ref="A288:A298"/>
+    <mergeCell ref="A249:A265"/>
     <mergeCell ref="A44:A82"/>
     <mergeCell ref="A18:A41"/>
     <mergeCell ref="A3:A15"/>
@@ -6016,13 +6058,6 @@
     <mergeCell ref="A128:A150"/>
     <mergeCell ref="A153:A175"/>
     <mergeCell ref="A85:A100"/>
-    <mergeCell ref="A299:A308"/>
-    <mergeCell ref="A279:A283"/>
-    <mergeCell ref="A221:A226"/>
-    <mergeCell ref="A230:A241"/>
-    <mergeCell ref="A266:A276"/>
-    <mergeCell ref="A286:A296"/>
-    <mergeCell ref="A247:A263"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6035,7 +6070,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6047,7 +6082,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
GearSwap - Monipulator fixes
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variables.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="641">
   <si>
     <t>N/A</t>
   </si>
@@ -1935,16 +1935,10 @@
     <t>Returns true or false based on whether or not you are in the middle of an action. True between precast and aftercast. If it is true, also returns the resources line of the spell being cast.</t>
   </si>
   <si>
-    <t>Current weather's name. Respects scholar spells/buffs.</t>
-  </si>
-  <si>
-    <t>Current weather's element. Respects scholar spells/buffs.</t>
-  </si>
-  <si>
-    <t>world.real_weather</t>
-  </si>
-  <si>
-    <t>world.real_weather_element</t>
+    <t>player.mob_name</t>
+  </si>
+  <si>
+    <t>User's name from the monster array. This will be different from player.name when you are a monipulator.</t>
   </si>
 </sst>
 </file>
@@ -2338,10 +2332,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F311"/>
+  <dimension ref="A1:F310"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
-      <selection activeCell="E239" sqref="E239"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2889,2182 +2883,2182 @@
     </row>
     <row r="45" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
-      <c r="B45" t="s">
-        <v>22</v>
-      </c>
       <c r="D45" t="s">
-        <v>23</v>
+        <v>639</v>
       </c>
       <c r="E45" t="s">
         <v>138</v>
       </c>
       <c r="F45" t="s">
-        <v>266</v>
+        <v>640</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D46" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E46" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F46" t="s">
-        <v>251</v>
+        <v>266</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D47" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E47" t="s">
         <v>263</v>
       </c>
       <c r="F47" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D48" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E48" t="s">
         <v>263</v>
       </c>
       <c r="F48" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12"/>
       <c r="B49" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D49" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E49" t="s">
         <v>263</v>
       </c>
       <c r="F49" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>
       <c r="B50" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E50" t="s">
         <v>263</v>
       </c>
       <c r="F50" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
       <c r="B51" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D51" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E51" t="s">
         <v>263</v>
       </c>
       <c r="F51" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
       <c r="B52" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D52" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E52" t="s">
         <v>263</v>
       </c>
       <c r="F52" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12"/>
+      <c r="B53" t="s">
+        <v>38</v>
+      </c>
       <c r="D53" t="s">
-        <v>326</v>
+        <v>39</v>
       </c>
       <c r="E53" t="s">
         <v>263</v>
       </c>
       <c r="F53" t="s">
-        <v>327</v>
+        <v>267</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
-      <c r="B54" t="s">
-        <v>40</v>
-      </c>
       <c r="D54" t="s">
-        <v>44</v>
+        <v>326</v>
       </c>
       <c r="E54" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F54" t="s">
-        <v>257</v>
+        <v>327</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
+      <c r="B55" t="s">
+        <v>40</v>
+      </c>
       <c r="D55" t="s">
-        <v>328</v>
+        <v>44</v>
       </c>
       <c r="E55" t="s">
         <v>138</v>
       </c>
       <c r="F55" t="s">
-        <v>329</v>
+        <v>257</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
-      <c r="B56" t="s">
-        <v>41</v>
-      </c>
       <c r="D56" t="s">
-        <v>45</v>
+        <v>328</v>
       </c>
       <c r="E56" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F56" t="s">
-        <v>268</v>
+        <v>329</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
+      <c r="B57" t="s">
+        <v>41</v>
+      </c>
       <c r="D57" t="s">
-        <v>330</v>
+        <v>45</v>
       </c>
       <c r="E57" t="s">
         <v>263</v>
       </c>
       <c r="F57" t="s">
-        <v>332</v>
+        <v>268</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12"/>
-      <c r="B58" t="s">
-        <v>42</v>
-      </c>
       <c r="D58" t="s">
-        <v>46</v>
+        <v>330</v>
       </c>
       <c r="E58" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F58" t="s">
-        <v>258</v>
+        <v>332</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
+      <c r="B59" t="s">
+        <v>42</v>
+      </c>
       <c r="D59" t="s">
-        <v>331</v>
+        <v>46</v>
       </c>
       <c r="E59" t="s">
         <v>138</v>
       </c>
       <c r="F59" t="s">
-        <v>333</v>
+        <v>258</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12"/>
-      <c r="B60" t="s">
-        <v>43</v>
-      </c>
       <c r="D60" t="s">
-        <v>47</v>
+        <v>331</v>
       </c>
       <c r="E60" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F60" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12"/>
       <c r="B61" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D61" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E61" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F61" t="s">
-        <v>148</v>
+        <v>269</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12"/>
       <c r="B62" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D62" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E62" t="s">
         <v>264</v>
       </c>
       <c r="F62" t="s">
-        <v>259</v>
+        <v>148</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
+      <c r="B63" t="s">
+        <v>51</v>
+      </c>
       <c r="D63" t="s">
-        <v>318</v>
+        <v>52</v>
       </c>
       <c r="E63" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F63" t="s">
-        <v>319</v>
+        <v>259</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="D64" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E64" t="s">
         <v>263</v>
       </c>
       <c r="F64" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="D65" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E65" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F65" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="D66" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E66" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F66" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="D67" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E67" t="s">
         <v>263</v>
       </c>
       <c r="F67" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="D68" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="E68" t="s">
         <v>263</v>
       </c>
       <c r="F68" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="D69" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E69" t="s">
         <v>263</v>
       </c>
       <c r="F69" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="D70" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E70" t="s">
         <v>263</v>
       </c>
       <c r="F70" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="D71" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E71" t="s">
         <v>263</v>
       </c>
       <c r="F71" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="D72" t="s">
-        <v>379</v>
+        <v>342</v>
       </c>
       <c r="E72" t="s">
         <v>263</v>
       </c>
       <c r="F72" t="s">
-        <v>397</v>
+        <v>343</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12"/>
       <c r="D73" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E73" t="s">
         <v>263</v>
       </c>
       <c r="F73" t="s">
-        <v>362</v>
+        <v>397</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12"/>
       <c r="D74" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E74" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F74" t="s">
-        <v>427</v>
+        <v>362</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12"/>
       <c r="D75" t="s">
-        <v>426</v>
+        <v>381</v>
       </c>
       <c r="E75" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F75" t="s">
-        <v>396</v>
+        <v>427</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12"/>
       <c r="D76" t="s">
-        <v>516</v>
+        <v>426</v>
       </c>
       <c r="E76" t="s">
         <v>263</v>
       </c>
       <c r="F76" t="s">
-        <v>517</v>
+        <v>396</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12"/>
       <c r="D77" t="s">
-        <v>382</v>
+        <v>516</v>
       </c>
       <c r="E77" t="s">
         <v>263</v>
       </c>
       <c r="F77" t="s">
-        <v>395</v>
+        <v>517</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12"/>
       <c r="D78" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E78" t="s">
         <v>263</v>
       </c>
       <c r="F78" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12"/>
       <c r="D79" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E79" t="s">
         <v>263</v>
       </c>
       <c r="F79" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12"/>
       <c r="D80" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E80" t="s">
         <v>263</v>
       </c>
       <c r="F80" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12"/>
       <c r="D81" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E81" t="s">
         <v>263</v>
       </c>
       <c r="F81" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12"/>
       <c r="D82" t="s">
+        <v>386</v>
+      </c>
+      <c r="E82" t="s">
+        <v>263</v>
+      </c>
+      <c r="F82" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="12"/>
+      <c r="D83" t="s">
         <v>387</v>
       </c>
-      <c r="E82" t="s">
-        <v>263</v>
-      </c>
-      <c r="F82" t="s">
+      <c r="E83" t="s">
+        <v>263</v>
+      </c>
+      <c r="F83" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="7"/>
-    </row>
-    <row r="84" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="7"/>
     </row>
-    <row r="85" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="12" t="s">
+    <row r="85" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="7"/>
+    </row>
+    <row r="86" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>94</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D86" t="s">
         <v>112</v>
       </c>
-      <c r="E85" t="s">
-        <v>138</v>
-      </c>
-      <c r="F85" t="s">
+      <c r="E86" t="s">
+        <v>138</v>
+      </c>
+      <c r="F86" t="s">
         <v>290</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="12"/>
-      <c r="B86" t="s">
-        <v>95</v>
-      </c>
-      <c r="D86" t="s">
-        <v>113</v>
-      </c>
-      <c r="E86" t="s">
-        <v>138</v>
-      </c>
-      <c r="F86" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12"/>
       <c r="B87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D87" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E87" t="s">
         <v>138</v>
       </c>
       <c r="F87" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12"/>
       <c r="B88" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D88" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E88" t="s">
         <v>138</v>
       </c>
       <c r="F88" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12"/>
       <c r="B89" t="s">
-        <v>278</v>
+        <v>97</v>
       </c>
       <c r="D89" t="s">
-        <v>306</v>
+        <v>115</v>
       </c>
       <c r="E89" t="s">
         <v>138</v>
       </c>
       <c r="F89" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12"/>
       <c r="B90" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D90" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E90" t="s">
         <v>138</v>
       </c>
       <c r="F90" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
       <c r="B91" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D91" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E91" t="s">
         <v>138</v>
       </c>
       <c r="F91" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
       <c r="B92" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D92" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E92" t="s">
         <v>138</v>
       </c>
       <c r="F92" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12"/>
       <c r="B93" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D93" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E93" t="s">
         <v>138</v>
       </c>
       <c r="F93" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12"/>
       <c r="B94" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D94" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E94" t="s">
         <v>138</v>
       </c>
       <c r="F94" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12"/>
       <c r="B95" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D95" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E95" t="s">
         <v>138</v>
       </c>
       <c r="F95" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12"/>
       <c r="B96" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D96" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E96" t="s">
         <v>138</v>
       </c>
       <c r="F96" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
       <c r="B97" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D97" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E97" t="s">
         <v>138</v>
       </c>
       <c r="F97" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
       <c r="B98" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D98" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E98" t="s">
         <v>138</v>
       </c>
       <c r="F98" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
       <c r="B99" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D99" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E99" t="s">
         <v>138</v>
       </c>
       <c r="F99" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12"/>
       <c r="B100" t="s">
+        <v>288</v>
+      </c>
+      <c r="D100" t="s">
+        <v>316</v>
+      </c>
+      <c r="E100" t="s">
+        <v>138</v>
+      </c>
+      <c r="F100" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="12"/>
+      <c r="B101" t="s">
         <v>289</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D101" t="s">
         <v>317</v>
       </c>
-      <c r="E100" t="s">
-        <v>138</v>
-      </c>
-      <c r="F100" t="s">
+      <c r="E101" t="s">
+        <v>138</v>
+      </c>
+      <c r="F101" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="3"/>
-    </row>
-    <row r="102" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3"/>
     </row>
     <row r="103" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="12" t="s">
+      <c r="A103" s="3"/>
+    </row>
+    <row r="104" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B104" t="s">
         <v>67</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D104" t="s">
         <v>84</v>
       </c>
-      <c r="E103" t="s">
-        <v>138</v>
-      </c>
-      <c r="F103" t="s">
+      <c r="E104" t="s">
+        <v>138</v>
+      </c>
+      <c r="F104" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="12"/>
-      <c r="B104" t="s">
-        <v>68</v>
-      </c>
-      <c r="D104" t="s">
-        <v>85</v>
-      </c>
-      <c r="E104" t="s">
-        <v>138</v>
-      </c>
-      <c r="F104" s="5" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12"/>
       <c r="B105" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D105" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E105" t="s">
-        <v>263</v>
-      </c>
-      <c r="F105" t="s">
-        <v>270</v>
+        <v>138</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12"/>
       <c r="B106" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D106" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E106" t="s">
         <v>263</v>
       </c>
       <c r="F106" t="s">
-        <v>244</v>
+        <v>270</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="12"/>
       <c r="B107" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D107" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E107" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F107" t="s">
-        <v>150</v>
+        <v>244</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="12"/>
+      <c r="B108" t="s">
+        <v>71</v>
+      </c>
       <c r="D108" t="s">
-        <v>353</v>
+        <v>88</v>
       </c>
       <c r="E108" t="s">
         <v>264</v>
       </c>
       <c r="F108" t="s">
-        <v>366</v>
+        <v>150</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="12"/>
       <c r="D109" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="E109" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F109" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="12"/>
       <c r="D110" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E110" t="s">
         <v>263</v>
       </c>
       <c r="F110" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="12"/>
       <c r="D111" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="E111" t="s">
         <v>263</v>
       </c>
       <c r="F111" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="12"/>
       <c r="D112" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E112" t="s">
         <v>263</v>
       </c>
       <c r="F112" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="12"/>
       <c r="D113" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E113" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F113" t="s">
-        <v>428</v>
+        <v>362</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="12"/>
       <c r="D114" t="s">
-        <v>425</v>
+        <v>355</v>
       </c>
       <c r="E114" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F114" t="s">
-        <v>363</v>
+        <v>428</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="12"/>
       <c r="D115" t="s">
-        <v>577</v>
+        <v>425</v>
       </c>
       <c r="E115" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F115" t="s">
-        <v>576</v>
+        <v>363</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="12"/>
       <c r="D116" t="s">
-        <v>518</v>
+        <v>577</v>
       </c>
       <c r="E116" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F116" t="s">
-        <v>517</v>
+        <v>576</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12"/>
       <c r="D117" t="s">
-        <v>369</v>
+        <v>518</v>
       </c>
       <c r="E117" t="s">
         <v>263</v>
       </c>
       <c r="F117" t="s">
-        <v>371</v>
+        <v>517</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="12"/>
       <c r="D118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E118" t="s">
         <v>263</v>
       </c>
       <c r="F118" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="12"/>
       <c r="D119" t="s">
-        <v>357</v>
+        <v>370</v>
       </c>
       <c r="E119" t="s">
         <v>263</v>
       </c>
       <c r="F119" t="s">
-        <v>389</v>
+        <v>372</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="12"/>
       <c r="D120" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E120" t="s">
         <v>263</v>
       </c>
       <c r="F120" t="s">
-        <v>373</v>
+        <v>389</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="12"/>
       <c r="D121" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E121" t="s">
         <v>263</v>
       </c>
       <c r="F121" t="s">
-        <v>392</v>
+        <v>373</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="12"/>
       <c r="D122" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
       <c r="E122" t="s">
         <v>263</v>
       </c>
       <c r="F122" t="s">
-        <v>376</v>
+        <v>392</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="12"/>
       <c r="D123" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="E123" t="s">
         <v>263</v>
       </c>
       <c r="F123" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="12"/>
       <c r="D124" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
       <c r="E124" t="s">
         <v>263</v>
       </c>
       <c r="F124" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="12"/>
       <c r="D125" t="s">
+        <v>367</v>
+      </c>
+      <c r="E125" t="s">
+        <v>263</v>
+      </c>
+      <c r="F125" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="12"/>
+      <c r="D126" t="s">
         <v>377</v>
       </c>
-      <c r="E125" t="s">
-        <v>263</v>
-      </c>
-      <c r="F125" t="s">
+      <c r="E126" t="s">
+        <v>263</v>
+      </c>
+      <c r="F126" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="10"/>
-    </row>
     <row r="127" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="3"/>
-    </row>
-    <row r="128" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="12" t="s">
+      <c r="A127" s="10"/>
+    </row>
+    <row r="128" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="3"/>
+    </row>
+    <row r="129" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="12" t="s">
         <v>533</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D129" t="s">
         <v>553</v>
       </c>
-      <c r="E128" t="s">
-        <v>138</v>
-      </c>
-      <c r="F128" t="s">
+      <c r="E129" t="s">
+        <v>138</v>
+      </c>
+      <c r="F129" t="s">
         <v>534</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="12"/>
-      <c r="D129" t="s">
-        <v>554</v>
-      </c>
-      <c r="E129" t="s">
-        <v>138</v>
-      </c>
-      <c r="F129" s="5" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="12"/>
       <c r="D130" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E130" t="s">
-        <v>263</v>
-      </c>
-      <c r="F130" t="s">
-        <v>535</v>
+        <v>138</v>
+      </c>
+      <c r="F130" s="5" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="12"/>
       <c r="D131" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E131" t="s">
         <v>263</v>
       </c>
       <c r="F131" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="12"/>
       <c r="D132" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E132" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F132" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="12"/>
       <c r="D133" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E133" t="s">
         <v>264</v>
       </c>
       <c r="F133" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="12"/>
       <c r="D134" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E134" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F134" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="12"/>
       <c r="D135" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E135" t="s">
         <v>263</v>
       </c>
       <c r="F135" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="12"/>
       <c r="D136" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E136" t="s">
         <v>263</v>
       </c>
       <c r="F136" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="12"/>
       <c r="D137" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E137" t="s">
         <v>263</v>
       </c>
       <c r="F137" t="s">
-        <v>362</v>
+        <v>541</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="12"/>
       <c r="D138" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E138" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F138" t="s">
-        <v>542</v>
+        <v>362</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="12"/>
       <c r="D139" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E139" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F139" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="12"/>
       <c r="D140" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E140" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F140" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="12"/>
       <c r="D141" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E141" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F141" t="s">
-        <v>517</v>
+        <v>544</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="12"/>
       <c r="D142" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E142" t="s">
         <v>263</v>
       </c>
       <c r="F142" t="s">
-        <v>545</v>
+        <v>517</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="12"/>
       <c r="D143" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E143" t="s">
         <v>263</v>
       </c>
       <c r="F143" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="12"/>
       <c r="D144" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E144" t="s">
         <v>263</v>
       </c>
       <c r="F144" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="12"/>
       <c r="D145" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E145" t="s">
         <v>263</v>
       </c>
       <c r="F145" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="12"/>
       <c r="D146" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E146" t="s">
         <v>263</v>
       </c>
       <c r="F146" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="12"/>
       <c r="D147" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E147" t="s">
         <v>263</v>
       </c>
       <c r="F147" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="12"/>
       <c r="D148" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E148" t="s">
         <v>263</v>
       </c>
       <c r="F148" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="12"/>
       <c r="D149" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E149" t="s">
         <v>263</v>
       </c>
       <c r="F149" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="12"/>
       <c r="D150" t="s">
+        <v>574</v>
+      </c>
+      <c r="E150" t="s">
+        <v>263</v>
+      </c>
+      <c r="F150" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" s="12"/>
+      <c r="D151" t="s">
         <v>575</v>
       </c>
-      <c r="E150" t="s">
-        <v>263</v>
-      </c>
-      <c r="F150" t="s">
+      <c r="E151" t="s">
+        <v>263</v>
+      </c>
+      <c r="F151" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A151" s="11"/>
-    </row>
-    <row r="152" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="3"/>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" s="11"/>
     </row>
     <row r="153" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="12" t="s">
+      <c r="A153" s="3"/>
+    </row>
+    <row r="154" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="12" t="s">
         <v>350</v>
       </c>
-      <c r="D153" t="s">
+      <c r="D154" t="s">
         <v>89</v>
       </c>
-      <c r="E153" t="s">
-        <v>138</v>
-      </c>
-      <c r="F153" t="s">
+      <c r="E154" t="s">
+        <v>138</v>
+      </c>
+      <c r="F154" t="s">
         <v>277</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="12"/>
-      <c r="D154" t="s">
-        <v>90</v>
-      </c>
-      <c r="E154" t="s">
-        <v>138</v>
-      </c>
-      <c r="F154" s="5" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="155" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="12"/>
       <c r="D155" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E155" t="s">
-        <v>263</v>
-      </c>
-      <c r="F155" t="s">
-        <v>274</v>
+        <v>138</v>
+      </c>
+      <c r="F155" s="5" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="156" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="12"/>
       <c r="D156" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E156" t="s">
         <v>263</v>
       </c>
       <c r="F156" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="12"/>
       <c r="D157" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E157" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F157" t="s">
-        <v>149</v>
+        <v>271</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="12"/>
       <c r="D158" t="s">
-        <v>393</v>
+        <v>93</v>
       </c>
       <c r="E158" t="s">
         <v>264</v>
       </c>
       <c r="F158" t="s">
-        <v>423</v>
+        <v>149</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="12"/>
       <c r="D159" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="E159" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F159" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="12"/>
       <c r="D160" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E160" t="s">
         <v>263</v>
       </c>
       <c r="F160" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="12"/>
       <c r="D161" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E161" t="s">
         <v>263</v>
       </c>
       <c r="F161" t="s">
-        <v>532</v>
+        <v>422</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="12"/>
       <c r="D162" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E162" t="s">
         <v>263</v>
       </c>
       <c r="F162" t="s">
-        <v>362</v>
+        <v>532</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="12"/>
       <c r="D163" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E163" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F163" t="s">
-        <v>530</v>
+        <v>362</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="12"/>
       <c r="D164" t="s">
-        <v>424</v>
+        <v>402</v>
       </c>
       <c r="E164" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F164" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="12"/>
       <c r="D165" t="s">
-        <v>528</v>
+        <v>424</v>
       </c>
       <c r="E165" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F165" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="166" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="12"/>
       <c r="D166" t="s">
-        <v>519</v>
+        <v>528</v>
       </c>
       <c r="E166" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F166" t="s">
-        <v>517</v>
+        <v>529</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="12"/>
       <c r="D167" t="s">
-        <v>403</v>
+        <v>519</v>
       </c>
       <c r="E167" t="s">
         <v>263</v>
       </c>
       <c r="F167" t="s">
-        <v>420</v>
+        <v>517</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="12"/>
       <c r="D168" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E168" t="s">
         <v>263</v>
       </c>
       <c r="F168" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="169" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="12"/>
       <c r="D169" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E169" t="s">
         <v>263</v>
       </c>
       <c r="F169" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="170" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="12"/>
       <c r="D170" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E170" t="s">
         <v>263</v>
       </c>
       <c r="F170" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="12"/>
       <c r="D171" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E171" t="s">
         <v>263</v>
       </c>
       <c r="F171" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="12"/>
       <c r="D172" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E172" t="s">
         <v>263</v>
       </c>
       <c r="F172" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="12"/>
       <c r="D173" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E173" t="s">
         <v>263</v>
       </c>
       <c r="F173" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="12"/>
       <c r="D174" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E174" t="s">
         <v>263</v>
       </c>
       <c r="F174" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="12"/>
       <c r="D175" t="s">
+        <v>410</v>
+      </c>
+      <c r="E175" t="s">
+        <v>263</v>
+      </c>
+      <c r="F175" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="12"/>
+      <c r="D176" t="s">
         <v>411</v>
       </c>
-      <c r="E175" t="s">
-        <v>263</v>
-      </c>
-      <c r="F175" t="s">
+      <c r="E176" t="s">
+        <v>263</v>
+      </c>
+      <c r="F176" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="3"/>
-    </row>
-    <row r="178" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="12" t="s">
+    <row r="177" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="3"/>
+    </row>
+    <row r="179" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B179" t="s">
         <v>98</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D179" t="s">
         <v>99</v>
       </c>
-      <c r="E178" t="s">
-        <v>138</v>
-      </c>
-      <c r="F178" t="s">
+      <c r="E179" t="s">
+        <v>138</v>
+      </c>
+      <c r="F179" t="s">
         <v>454</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="12"/>
-      <c r="B179" t="s">
-        <v>100</v>
-      </c>
-      <c r="D179" t="s">
-        <v>101</v>
-      </c>
-      <c r="E179" t="s">
-        <v>264</v>
-      </c>
-      <c r="F179" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="180" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="12"/>
       <c r="B180" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D180" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E180" t="s">
-        <v>138</v>
+        <v>264</v>
       </c>
       <c r="F180" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="181" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12"/>
       <c r="B181" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D181" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E181" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F181" t="s">
-        <v>430</v>
+        <v>153</v>
       </c>
     </row>
     <row r="182" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="12"/>
+      <c r="B182" t="s">
+        <v>104</v>
+      </c>
       <c r="D182" t="s">
-        <v>429</v>
+        <v>105</v>
       </c>
       <c r="E182" t="s">
         <v>263</v>
       </c>
       <c r="F182" t="s">
-        <v>453</v>
+        <v>430</v>
       </c>
     </row>
     <row r="183" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="12"/>
-      <c r="B183" t="s">
-        <v>108</v>
-      </c>
       <c r="D183" t="s">
-        <v>107</v>
+        <v>429</v>
       </c>
       <c r="E183" t="s">
         <v>263</v>
       </c>
       <c r="F183" t="s">
-        <v>431</v>
+        <v>453</v>
       </c>
     </row>
     <row r="184" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="12"/>
       <c r="B184" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D184" t="s">
-        <v>0</v>
+        <v>107</v>
+      </c>
+      <c r="E184" t="s">
+        <v>263</v>
       </c>
       <c r="F184" t="s">
-        <v>152</v>
+        <v>431</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="12"/>
+      <c r="B185" t="s">
+        <v>106</v>
+      </c>
       <c r="D185" t="s">
-        <v>432</v>
-      </c>
-      <c r="E185" t="s">
-        <v>263</v>
+        <v>0</v>
       </c>
       <c r="F185" t="s">
-        <v>452</v>
+        <v>152</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="12"/>
       <c r="D186" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E186" t="s">
         <v>263</v>
       </c>
       <c r="F186" t="s">
-        <v>362</v>
+        <v>452</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="12"/>
       <c r="D187" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E187" t="s">
         <v>263</v>
       </c>
       <c r="F187" t="s">
-        <v>451</v>
+        <v>362</v>
       </c>
     </row>
     <row r="188" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="12"/>
       <c r="D188" t="s">
-        <v>522</v>
+        <v>434</v>
       </c>
       <c r="E188" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F188" t="s">
-        <v>523</v>
+        <v>451</v>
       </c>
     </row>
     <row r="189" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="12"/>
       <c r="D189" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="E189" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F189" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="190" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="12"/>
       <c r="D190" t="s">
-        <v>435</v>
+        <v>520</v>
       </c>
       <c r="E190" t="s">
         <v>263</v>
       </c>
       <c r="F190" t="s">
-        <v>450</v>
+        <v>524</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="12"/>
       <c r="D191" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E191" t="s">
         <v>263</v>
       </c>
       <c r="F191" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="192" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="12"/>
       <c r="D192" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E192" t="s">
         <v>263</v>
       </c>
       <c r="F192" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="193" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="12"/>
       <c r="D193" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E193" t="s">
         <v>263</v>
       </c>
       <c r="F193" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="194" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="12"/>
       <c r="D194" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E194" t="s">
         <v>263</v>
       </c>
       <c r="F194" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="195" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="12"/>
       <c r="D195" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E195" t="s">
         <v>263</v>
       </c>
       <c r="F195" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="196" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="12"/>
       <c r="D196" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E196" t="s">
         <v>263</v>
       </c>
       <c r="F196" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="197" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="12"/>
       <c r="D197" t="s">
+        <v>441</v>
+      </c>
+      <c r="E197" t="s">
+        <v>263</v>
+      </c>
+      <c r="F197" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="12"/>
+      <c r="D198" t="s">
         <v>442</v>
       </c>
-      <c r="E197" t="s">
-        <v>263</v>
-      </c>
-      <c r="F197" t="s">
+      <c r="E198" t="s">
+        <v>263</v>
+      </c>
+      <c r="F198" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="200" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="12" t="s">
+    <row r="201" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="12" t="s">
         <v>347</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B201" t="s">
         <v>109</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D201" t="s">
         <v>220</v>
       </c>
-      <c r="E200" t="s">
-        <v>138</v>
-      </c>
-      <c r="F200" t="s">
+      <c r="E201" t="s">
+        <v>138</v>
+      </c>
+      <c r="F201" t="s">
         <v>481</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="12"/>
-      <c r="B201" t="s">
-        <v>110</v>
-      </c>
-      <c r="D201" t="s">
-        <v>221</v>
-      </c>
-      <c r="E201" t="s">
-        <v>264</v>
-      </c>
-      <c r="F201" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="202" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="12"/>
       <c r="B202" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D202" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E202" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F202" t="s">
-        <v>482</v>
+        <v>223</v>
       </c>
     </row>
     <row r="203" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="12"/>
+      <c r="B203" t="s">
+        <v>111</v>
+      </c>
       <c r="D203" t="s">
-        <v>455</v>
+        <v>222</v>
       </c>
       <c r="E203" t="s">
         <v>263</v>
       </c>
       <c r="F203" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
     <row r="204" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="12"/>
       <c r="D204" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E204" t="s">
         <v>263</v>
       </c>
       <c r="F204" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="205" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="12"/>
       <c r="D205" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E205" t="s">
         <v>263</v>
       </c>
       <c r="F205" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="206" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="12"/>
       <c r="D206" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E206" t="s">
         <v>263</v>
       </c>
       <c r="F206" t="s">
-        <v>362</v>
+        <v>478</v>
       </c>
     </row>
     <row r="207" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="12"/>
       <c r="D207" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E207" t="s">
-        <v>138</v>
+        <v>263</v>
+      </c>
+      <c r="F207" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="208" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="12"/>
       <c r="D208" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="E208" t="s">
-        <v>263</v>
-      </c>
-      <c r="F208" t="s">
-        <v>477</v>
+        <v>138</v>
       </c>
     </row>
     <row r="209" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="12"/>
       <c r="D209" t="s">
-        <v>527</v>
+        <v>459</v>
       </c>
       <c r="E209" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F209" t="s">
-        <v>525</v>
+        <v>477</v>
       </c>
     </row>
     <row r="210" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="12"/>
       <c r="D210" t="s">
-        <v>521</v>
+        <v>527</v>
       </c>
       <c r="E210" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F210" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="211" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="12"/>
       <c r="D211" t="s">
-        <v>461</v>
+        <v>521</v>
       </c>
       <c r="E211" t="s">
         <v>263</v>
       </c>
       <c r="F211" t="s">
-        <v>476</v>
+        <v>526</v>
       </c>
     </row>
     <row r="212" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="12"/>
       <c r="D212" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E212" t="s">
         <v>263</v>
       </c>
       <c r="F212" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="213" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="12"/>
       <c r="D213" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E213" t="s">
         <v>263</v>
       </c>
       <c r="F213" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="214" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="12"/>
       <c r="D214" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E214" t="s">
         <v>263</v>
       </c>
       <c r="F214" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="215" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="12"/>
       <c r="D215" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E215" t="s">
         <v>263</v>
       </c>
       <c r="F215" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="216" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="12"/>
       <c r="D216" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E216" t="s">
         <v>263</v>
       </c>
       <c r="F216" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="217" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="12"/>
       <c r="D217" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E217" t="s">
         <v>263</v>
       </c>
       <c r="F217" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="218" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="12"/>
       <c r="D218" t="s">
+        <v>467</v>
+      </c>
+      <c r="E218" t="s">
+        <v>263</v>
+      </c>
+      <c r="F218" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A219" s="12"/>
+      <c r="D219" t="s">
         <v>468</v>
       </c>
-      <c r="E218" t="s">
-        <v>263</v>
-      </c>
-      <c r="F218" t="s">
+      <c r="E219" t="s">
+        <v>263</v>
+      </c>
+      <c r="F219" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="221" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A221" s="12" t="s">
+    <row r="222" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A222" s="12" t="s">
         <v>491</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B222" t="s">
         <v>48</v>
       </c>
-      <c r="D221" t="s">
+      <c r="D222" t="s">
         <v>154</v>
       </c>
-      <c r="E221" t="s">
-        <v>263</v>
-      </c>
-      <c r="F221" t="s">
+      <c r="E222" t="s">
+        <v>263</v>
+      </c>
+      <c r="F222" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="12"/>
-      <c r="D222" t="s">
-        <v>155</v>
-      </c>
-      <c r="E222" t="s">
-        <v>263</v>
-      </c>
-      <c r="F222" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="223" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="12"/>
       <c r="D223" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E223" t="s">
-        <v>140</v>
+        <v>263</v>
       </c>
       <c r="F223" t="s">
-        <v>500</v>
+        <v>156</v>
       </c>
     </row>
     <row r="224" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="12"/>
       <c r="D224" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E224" t="s">
         <v>140</v>
       </c>
       <c r="F224" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="12"/>
+      <c r="D225" t="s">
+        <v>159</v>
+      </c>
+      <c r="E225" t="s">
+        <v>140</v>
+      </c>
+      <c r="F225" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="12"/>
-      <c r="D225" s="9" t="s">
-        <v>490</v>
-      </c>
-      <c r="E225" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="F225" s="9" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="226" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="12"/>
       <c r="D226" s="9" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E226" s="9" t="s">
         <v>140</v>
@@ -5073,400 +5067,403 @@
         <v>503</v>
       </c>
     </row>
-    <row r="227" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A227" s="3"/>
-    </row>
-    <row r="228" spans="1:6" s="9" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A228" s="2"/>
-    </row>
-    <row r="230" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="3" t="s">
+    <row r="227" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="12"/>
+      <c r="D227" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="E227" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F227" s="9" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="3"/>
+    </row>
+    <row r="229" spans="1:6" s="9" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A229" s="2"/>
+    </row>
+    <row r="231" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="12" t="s">
         <v>348</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B231" t="s">
         <v>24</v>
       </c>
-      <c r="D230" t="s">
+      <c r="D231" t="s">
         <v>25</v>
       </c>
-      <c r="E230" t="s">
-        <v>138</v>
-      </c>
-      <c r="F230" t="s">
+      <c r="E231" t="s">
+        <v>138</v>
+      </c>
+      <c r="F231" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="3"/>
-      <c r="B231" t="s">
+    <row r="232" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="12"/>
+      <c r="B232" t="s">
         <v>53</v>
       </c>
-      <c r="D231" t="s">
+      <c r="D232" t="s">
         <v>54</v>
       </c>
-      <c r="E231" t="s">
-        <v>263</v>
-      </c>
-      <c r="F231" t="s">
+      <c r="E232" t="s">
+        <v>263</v>
+      </c>
+      <c r="F232" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="3"/>
-      <c r="B232" t="s">
+    <row r="233" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="12"/>
+      <c r="B233" t="s">
         <v>55</v>
       </c>
-      <c r="D232" t="s">
+      <c r="D233" t="s">
         <v>56</v>
       </c>
-      <c r="E232" t="s">
-        <v>138</v>
-      </c>
-      <c r="F232" t="s">
+      <c r="E233" t="s">
+        <v>138</v>
+      </c>
+      <c r="F233" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="233" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="3"/>
-      <c r="B233" t="s">
+    <row r="234" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="12"/>
+      <c r="B234" t="s">
         <v>58</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D234" t="s">
         <v>57</v>
       </c>
-      <c r="E233" t="s">
-        <v>138</v>
-      </c>
-      <c r="F233" t="s">
+      <c r="E234" t="s">
+        <v>138</v>
+      </c>
+      <c r="F234" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="234" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="3"/>
-      <c r="D234" t="s">
+    <row r="235" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="12"/>
+      <c r="D235" t="s">
         <v>493</v>
       </c>
-      <c r="E234" t="s">
-        <v>263</v>
-      </c>
-      <c r="F234" t="s">
+      <c r="E235" t="s">
+        <v>263</v>
+      </c>
+      <c r="F235" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="235" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="3"/>
-      <c r="B235" t="s">
+    <row r="236" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="12"/>
+      <c r="B236" t="s">
         <v>59</v>
       </c>
-      <c r="D235" t="s">
+      <c r="D236" t="s">
         <v>60</v>
       </c>
-      <c r="E235" t="s">
-        <v>138</v>
-      </c>
-      <c r="F235" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="3"/>
-      <c r="B236" t="s">
+      <c r="E236" t="s">
+        <v>138</v>
+      </c>
+      <c r="F236" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="12"/>
+      <c r="B237" t="s">
         <v>61</v>
       </c>
-      <c r="D236" t="s">
+      <c r="D237" t="s">
         <v>62</v>
       </c>
-      <c r="E236" t="s">
-        <v>138</v>
-      </c>
-      <c r="F236" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="237" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="3"/>
-      <c r="D237" t="s">
-        <v>641</v>
-      </c>
       <c r="E237" t="s">
         <v>138</v>
       </c>
       <c r="F237" t="s">
-        <v>486</v>
+        <v>232</v>
       </c>
     </row>
     <row r="238" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="3"/>
+      <c r="A238" s="12"/>
+      <c r="B238" t="s">
+        <v>63</v>
+      </c>
       <c r="D238" t="s">
-        <v>642</v>
+        <v>65</v>
       </c>
       <c r="E238" t="s">
         <v>138</v>
       </c>
       <c r="F238" t="s">
-        <v>232</v>
+        <v>485</v>
       </c>
     </row>
     <row r="239" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="3"/>
+      <c r="A239" s="12"/>
       <c r="B239" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D239" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E239" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F239" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="240" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="3"/>
-      <c r="B240" t="s">
-        <v>64</v>
-      </c>
+      <c r="A240" s="12"/>
       <c r="D240" t="s">
-        <v>66</v>
+        <v>494</v>
       </c>
       <c r="E240" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F240" t="s">
-        <v>484</v>
+        <v>233</v>
       </c>
     </row>
     <row r="241" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="3"/>
+      <c r="A241" s="12"/>
       <c r="D241" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="E241" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F241" t="s">
-        <v>233</v>
+        <v>483</v>
       </c>
     </row>
     <row r="242" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="3"/>
+      <c r="A242" s="12"/>
       <c r="D242" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E242" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F242" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="243" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A243" s="3"/>
-      <c r="D243" t="s">
-        <v>496</v>
-      </c>
-      <c r="E243" t="s">
-        <v>264</v>
-      </c>
-      <c r="F243" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="246" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A246" s="4" t="s">
+    <row r="245" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A245" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B246" t="s">
+      <c r="B245" t="s">
         <v>120</v>
       </c>
-      <c r="D246" t="s">
+      <c r="D245" t="s">
         <v>120</v>
       </c>
-      <c r="E246" t="s">
+      <c r="E245" t="s">
         <v>140</v>
       </c>
-      <c r="F246" t="s">
+      <c r="F245" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="249" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A249" s="12" t="s">
+    <row r="248" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="12" t="s">
         <v>119</v>
       </c>
+      <c r="B248" t="s">
+        <v>201</v>
+      </c>
+      <c r="D248" t="s">
+        <v>614</v>
+      </c>
+      <c r="E248" t="s">
+        <v>501</v>
+      </c>
+      <c r="F248" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A249" s="12"/>
       <c r="B249" t="s">
-        <v>201</v>
+        <v>513</v>
       </c>
       <c r="D249" t="s">
-        <v>614</v>
+        <v>514</v>
       </c>
       <c r="E249" t="s">
         <v>501</v>
       </c>
       <c r="F249" t="s">
-        <v>615</v>
+        <v>515</v>
       </c>
     </row>
     <row r="250" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="12"/>
       <c r="B250" t="s">
-        <v>513</v>
+        <v>122</v>
       </c>
       <c r="D250" t="s">
-        <v>514</v>
+        <v>133</v>
       </c>
       <c r="E250" t="s">
         <v>501</v>
       </c>
       <c r="F250" t="s">
-        <v>515</v>
+        <v>624</v>
       </c>
     </row>
     <row r="251" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="12"/>
       <c r="B251" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D251" t="s">
-        <v>133</v>
-      </c>
-      <c r="E251" t="s">
-        <v>501</v>
+        <v>0</v>
       </c>
       <c r="F251" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="12"/>
       <c r="B252" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D252" t="s">
-        <v>0</v>
+        <v>161</v>
+      </c>
+      <c r="E252" t="s">
+        <v>501</v>
       </c>
       <c r="F252" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="253" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="12"/>
       <c r="B253" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D253" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E253" t="s">
         <v>501</v>
       </c>
       <c r="F253" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
     </row>
     <row r="254" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="12"/>
-      <c r="B254" t="s">
-        <v>117</v>
-      </c>
       <c r="D254" t="s">
-        <v>162</v>
+        <v>613</v>
       </c>
       <c r="E254" t="s">
         <v>501</v>
       </c>
       <c r="F254" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="255" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="12"/>
+      <c r="B255" t="s">
+        <v>124</v>
+      </c>
       <c r="D255" t="s">
-        <v>613</v>
+        <v>203</v>
       </c>
       <c r="E255" t="s">
         <v>501</v>
       </c>
       <c r="F255" t="s">
-        <v>638</v>
+        <v>205</v>
       </c>
     </row>
     <row r="256" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="12"/>
       <c r="B256" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D256" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E256" t="s">
         <v>501</v>
       </c>
       <c r="F256" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="257" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="12"/>
       <c r="B257" t="s">
-        <v>125</v>
+        <v>129</v>
+      </c>
+      <c r="C257" s="5" t="s">
+        <v>212</v>
       </c>
       <c r="D257" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="E257" t="s">
         <v>501</v>
       </c>
       <c r="F257" t="s">
-        <v>206</v>
+        <v>616</v>
       </c>
     </row>
     <row r="258" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="12"/>
       <c r="B258" t="s">
-        <v>129</v>
-      </c>
-      <c r="C258" s="5" t="s">
-        <v>212</v>
+        <v>130</v>
       </c>
       <c r="D258" t="s">
-        <v>213</v>
+        <v>132</v>
       </c>
       <c r="E258" t="s">
         <v>501</v>
       </c>
       <c r="F258" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="259" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="12"/>
       <c r="B259" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="D259" t="s">
-        <v>132</v>
+        <v>207</v>
       </c>
       <c r="E259" t="s">
         <v>501</v>
       </c>
       <c r="F259" t="s">
-        <v>617</v>
+        <v>208</v>
       </c>
     </row>
     <row r="260" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="12"/>
       <c r="B260" t="s">
-        <v>137</v>
+        <v>0</v>
       </c>
       <c r="D260" t="s">
-        <v>207</v>
+        <v>136</v>
       </c>
       <c r="E260" t="s">
         <v>501</v>
       </c>
       <c r="F260" t="s">
-        <v>208</v>
+        <v>163</v>
       </c>
     </row>
     <row r="261" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5475,13 +5472,13 @@
         <v>0</v>
       </c>
       <c r="D261" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E261" t="s">
         <v>501</v>
       </c>
       <c r="F261" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="262" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5490,13 +5487,13 @@
         <v>0</v>
       </c>
       <c r="D262" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E262" t="s">
         <v>501</v>
       </c>
       <c r="F262" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="263" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5505,292 +5502,292 @@
         <v>0</v>
       </c>
       <c r="D263" t="s">
-        <v>135</v>
+        <v>209</v>
       </c>
       <c r="E263" t="s">
         <v>501</v>
       </c>
       <c r="F263" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="264" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="12"/>
       <c r="B264" t="s">
         <v>0</v>
       </c>
       <c r="D264" t="s">
-        <v>209</v>
+        <v>633</v>
       </c>
       <c r="E264" t="s">
         <v>501</v>
       </c>
       <c r="F264" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A265" s="12"/>
-      <c r="B265" t="s">
-        <v>0</v>
-      </c>
-      <c r="D265" t="s">
-        <v>633</v>
-      </c>
-      <c r="E265" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A265" s="3"/>
+    </row>
+    <row r="266" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A266" s="2"/>
+    </row>
+    <row r="267" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A267" s="13" t="s">
+        <v>618</v>
+      </c>
+      <c r="D267" t="s">
+        <v>199</v>
+      </c>
+      <c r="E267" t="s">
         <v>501</v>
       </c>
-      <c r="F265" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="266" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A266" s="3"/>
-    </row>
-    <row r="267" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A267" s="2"/>
-    </row>
-    <row r="268" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A268" s="13" t="s">
-        <v>618</v>
-      </c>
+      <c r="F267" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A268" s="13"/>
       <c r="D268" t="s">
-        <v>199</v>
+        <v>619</v>
       </c>
       <c r="E268" t="s">
         <v>501</v>
       </c>
       <c r="F268" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="269" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="13"/>
+      <c r="B269" t="s">
+        <v>177</v>
+      </c>
       <c r="D269" t="s">
-        <v>619</v>
+        <v>184</v>
       </c>
       <c r="E269" t="s">
         <v>501</v>
       </c>
       <c r="F269" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="270" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="13"/>
       <c r="B270" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D270" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E270" t="s">
         <v>501</v>
       </c>
       <c r="F270" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
     </row>
     <row r="271" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="13"/>
       <c r="B271" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D271" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E271" t="s">
         <v>501</v>
       </c>
       <c r="F271" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="272" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="13"/>
-      <c r="B272" t="s">
-        <v>179</v>
-      </c>
       <c r="D272" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E272" t="s">
         <v>501</v>
       </c>
       <c r="F272" t="s">
-        <v>629</v>
+        <v>620</v>
       </c>
     </row>
     <row r="273" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" s="13"/>
       <c r="D273" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E273" t="s">
         <v>501</v>
       </c>
       <c r="F273" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="274" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="13"/>
       <c r="D274" t="s">
-        <v>180</v>
+        <v>511</v>
       </c>
       <c r="E274" t="s">
         <v>501</v>
       </c>
       <c r="F274" t="s">
-        <v>621</v>
+        <v>512</v>
       </c>
     </row>
     <row r="275" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A275" s="13"/>
       <c r="D275" t="s">
-        <v>511</v>
+        <v>626</v>
       </c>
       <c r="E275" t="s">
         <v>501</v>
       </c>
       <c r="F275" t="s">
-        <v>512</v>
+        <v>627</v>
       </c>
     </row>
     <row r="276" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="13"/>
       <c r="D276" t="s">
-        <v>626</v>
+        <v>185</v>
       </c>
       <c r="E276" t="s">
         <v>501</v>
       </c>
       <c r="F276" t="s">
-        <v>627</v>
+        <v>186</v>
       </c>
     </row>
     <row r="277" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A277" s="13"/>
       <c r="D277" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="E277" t="s">
         <v>501</v>
       </c>
       <c r="F277" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="278" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A278" s="13"/>
-      <c r="D278" t="s">
-        <v>198</v>
-      </c>
-      <c r="E278" t="s">
-        <v>501</v>
-      </c>
-      <c r="F278" t="s">
         <v>622</v>
       </c>
     </row>
+    <row r="280" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A280" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B280" t="s">
+        <v>126</v>
+      </c>
+      <c r="D280" t="s">
+        <v>0</v>
+      </c>
+      <c r="F280" t="s">
+        <v>166</v>
+      </c>
+    </row>
     <row r="281" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A281" s="12" t="s">
-        <v>127</v>
-      </c>
+      <c r="A281" s="12"/>
       <c r="B281" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D281" t="s">
         <v>0</v>
       </c>
       <c r="F281" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="282" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" s="12"/>
       <c r="B282" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D282" t="s">
         <v>0</v>
       </c>
       <c r="F282" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="283" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="12"/>
       <c r="B283" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D283" t="s">
         <v>0</v>
       </c>
       <c r="F283" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="284" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="12"/>
       <c r="B284" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D284" t="s">
         <v>0</v>
       </c>
       <c r="F284" t="s">
-        <v>169</v>
+        <v>230</v>
       </c>
     </row>
     <row r="285" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A285" s="12"/>
-      <c r="B285" t="s">
-        <v>121</v>
-      </c>
-      <c r="D285" t="s">
-        <v>0</v>
-      </c>
-      <c r="F285" t="s">
-        <v>230</v>
-      </c>
+      <c r="A285" s="3"/>
     </row>
     <row r="286" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A286" s="3"/>
     </row>
     <row r="287" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A287" s="3"/>
-    </row>
-    <row r="288" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A288" s="13" t="s">
+      <c r="A287" s="13" t="s">
         <v>141</v>
       </c>
+      <c r="B287" t="s">
+        <v>0</v>
+      </c>
+      <c r="D287" t="s">
+        <v>138</v>
+      </c>
+      <c r="E287" t="s">
+        <v>140</v>
+      </c>
+      <c r="F287" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A288" s="13"/>
       <c r="B288" t="s">
         <v>0</v>
       </c>
       <c r="D288" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E288" t="s">
         <v>140</v>
       </c>
       <c r="F288" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="289" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289" s="13"/>
       <c r="B289" t="s">
         <v>0</v>
       </c>
       <c r="D289" t="s">
-        <v>139</v>
+        <v>635</v>
       </c>
       <c r="E289" t="s">
         <v>140</v>
       </c>
       <c r="F289" t="s">
-        <v>171</v>
+        <v>502</v>
       </c>
     </row>
     <row r="290" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5799,13 +5796,13 @@
         <v>0</v>
       </c>
       <c r="D290" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="E290" t="s">
         <v>140</v>
       </c>
       <c r="F290" t="s">
-        <v>502</v>
+        <v>172</v>
       </c>
     </row>
     <row r="291" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5814,13 +5811,13 @@
         <v>0</v>
       </c>
       <c r="D291" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="E291" t="s">
         <v>140</v>
       </c>
       <c r="F291" t="s">
-        <v>172</v>
+        <v>632</v>
       </c>
     </row>
     <row r="292" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5829,13 +5826,13 @@
         <v>0</v>
       </c>
       <c r="D292" t="s">
-        <v>637</v>
+        <v>506</v>
       </c>
       <c r="E292" t="s">
         <v>140</v>
       </c>
       <c r="F292" t="s">
-        <v>632</v>
+        <v>507</v>
       </c>
     </row>
     <row r="293" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5844,13 +5841,13 @@
         <v>0</v>
       </c>
       <c r="D293" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="E293" t="s">
-        <v>140</v>
+        <v>501</v>
       </c>
       <c r="F293" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="294" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5859,13 +5856,13 @@
         <v>0</v>
       </c>
       <c r="D294" t="s">
-        <v>508</v>
+        <v>142</v>
       </c>
       <c r="E294" t="s">
         <v>501</v>
       </c>
       <c r="F294" t="s">
-        <v>509</v>
+        <v>173</v>
       </c>
     </row>
     <row r="295" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5874,13 +5871,13 @@
         <v>0</v>
       </c>
       <c r="D295" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E295" t="s">
         <v>501</v>
       </c>
       <c r="F295" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="296" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5889,13 +5886,13 @@
         <v>0</v>
       </c>
       <c r="D296" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E296" t="s">
         <v>501</v>
       </c>
       <c r="F296" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="297" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5904,160 +5901,146 @@
         <v>0</v>
       </c>
       <c r="D297" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E297" t="s">
         <v>501</v>
       </c>
       <c r="F297" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="298" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A298" s="13"/>
-      <c r="B298" t="s">
-        <v>0</v>
-      </c>
-      <c r="D298" t="s">
-        <v>145</v>
-      </c>
-      <c r="E298" t="s">
-        <v>501</v>
-      </c>
-      <c r="F298" t="s">
-        <v>176</v>
-      </c>
+      <c r="A298" s="8"/>
     </row>
     <row r="299" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" s="8"/>
     </row>
-    <row r="300" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A300" s="8"/>
+    <row r="300" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D300" t="s">
+        <v>188</v>
+      </c>
+      <c r="F300" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="301" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A301" s="12" t="s">
-        <v>187</v>
-      </c>
+      <c r="A301" s="12"/>
       <c r="D301" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="F301" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="302" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="12"/>
       <c r="D302" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F302" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="303" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="12"/>
       <c r="D303" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F303" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="304" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="12"/>
       <c r="D304" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="F304" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="305" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A305" s="12"/>
+      <c r="B305" t="s">
+        <v>226</v>
+      </c>
       <c r="D305" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="F305" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
     </row>
     <row r="306" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A306" s="12"/>
       <c r="B306" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D306" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="F306" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="307" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A307" s="12"/>
       <c r="B307" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D307" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F307" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="308" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A308" s="12"/>
       <c r="B308" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D308" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="F308" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="309" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A309" s="12"/>
-      <c r="B309" t="s">
-        <v>227</v>
-      </c>
       <c r="D309" t="s">
-        <v>224</v>
+        <v>504</v>
       </c>
       <c r="F309" t="s">
-        <v>225</v>
+        <v>505</v>
       </c>
     </row>
     <row r="310" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A310" s="12"/>
-      <c r="D310" t="s">
-        <v>504</v>
-      </c>
-      <c r="F310" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="311" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A311" s="3"/>
+      <c r="A310" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A301:A310"/>
-    <mergeCell ref="A281:A285"/>
-    <mergeCell ref="A221:A226"/>
-    <mergeCell ref="A268:A278"/>
-    <mergeCell ref="A288:A298"/>
-    <mergeCell ref="A249:A265"/>
-    <mergeCell ref="A44:A82"/>
+  <mergeCells count="16">
+    <mergeCell ref="A300:A309"/>
+    <mergeCell ref="A280:A284"/>
+    <mergeCell ref="A222:A227"/>
+    <mergeCell ref="A231:A242"/>
+    <mergeCell ref="A267:A277"/>
+    <mergeCell ref="A287:A297"/>
+    <mergeCell ref="A248:A264"/>
     <mergeCell ref="A18:A41"/>
     <mergeCell ref="A3:A15"/>
-    <mergeCell ref="A103:A125"/>
-    <mergeCell ref="A200:A218"/>
-    <mergeCell ref="A178:A197"/>
-    <mergeCell ref="A128:A150"/>
-    <mergeCell ref="A153:A175"/>
-    <mergeCell ref="A85:A100"/>
+    <mergeCell ref="A104:A126"/>
+    <mergeCell ref="A201:A219"/>
+    <mergeCell ref="A179:A198"/>
+    <mergeCell ref="A129:A151"/>
+    <mergeCell ref="A154:A176"/>
+    <mergeCell ref="A86:A101"/>
+    <mergeCell ref="A44:A83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GearSwap v0.815 - Initial commit
Automaton Information
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variables.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="690">
   <si>
     <t>N/A</t>
   </si>
@@ -1377,9 +1377,6 @@
     <t>User's pet's model size.</t>
   </si>
   <si>
-    <t>MPP of the user's pet if it is available.</t>
-  </si>
-  <si>
     <t>Name of the user's pet.</t>
   </si>
   <si>
@@ -1939,6 +1936,156 @@
   </si>
   <si>
     <t>User's name from the monster array. This will be different from player.name when you are a monipulator.</t>
+  </si>
+  <si>
+    <t>These values are not valid in get_sets()</t>
+  </si>
+  <si>
+    <t>PUP special values:</t>
+  </si>
+  <si>
+    <t>pet.ranged</t>
+  </si>
+  <si>
+    <t>pet.max_ranged</t>
+  </si>
+  <si>
+    <t>pet.melee</t>
+  </si>
+  <si>
+    <t>pet.max_melee</t>
+  </si>
+  <si>
+    <t>pet.magic</t>
+  </si>
+  <si>
+    <t>pet.max_magic</t>
+  </si>
+  <si>
+    <t>pet.str</t>
+  </si>
+  <si>
+    <t>pet.dex</t>
+  </si>
+  <si>
+    <t>pet.vit</t>
+  </si>
+  <si>
+    <t>pet.agi</t>
+  </si>
+  <si>
+    <t>pet.int</t>
+  </si>
+  <si>
+    <t>pet.mnd</t>
+  </si>
+  <si>
+    <t>pet.chr</t>
+  </si>
+  <si>
+    <t>pet.str_add</t>
+  </si>
+  <si>
+    <t>pet.dex_add</t>
+  </si>
+  <si>
+    <t>pet.agi_add</t>
+  </si>
+  <si>
+    <t>pet.vit_add</t>
+  </si>
+  <si>
+    <t>pet.int_add</t>
+  </si>
+  <si>
+    <t>pet.mnd_add</t>
+  </si>
+  <si>
+    <t>pet.chr_add</t>
+  </si>
+  <si>
+    <t>pet.hp</t>
+  </si>
+  <si>
+    <t>pet.mp</t>
+  </si>
+  <si>
+    <t>pet.head</t>
+  </si>
+  <si>
+    <t>pet.frame</t>
+  </si>
+  <si>
+    <t>pet.attachments</t>
+  </si>
+  <si>
+    <t>pet.available_attachments</t>
+  </si>
+  <si>
+    <t>pet.available_heads</t>
+  </si>
+  <si>
+    <t>pet.available_frames</t>
+  </si>
+  <si>
+    <t>Table keyed to the currently equipped attachments. Pet.attachments.strobe would be true if you have stobe equipped.</t>
+  </si>
+  <si>
+    <t>Table keyed to the currently available attachments (owned). Pet.available_attachments.strobe would be true if own strobe.</t>
+  </si>
+  <si>
+    <t>Table keyed to the currently available frames (owned).</t>
+  </si>
+  <si>
+    <t>Table keyed to the currently available heads (owned).</t>
+  </si>
+  <si>
+    <t>Currently equipped head.</t>
+  </si>
+  <si>
+    <t>Currently equipped frame.</t>
+  </si>
+  <si>
+    <t>Base automaton CHR.</t>
+  </si>
+  <si>
+    <t>Base automaton MND.</t>
+  </si>
+  <si>
+    <t>MND added to automaton's base.</t>
+  </si>
+  <si>
+    <t>CHR added to automaton's base.</t>
+  </si>
+  <si>
+    <t>INT added to automaton's base.</t>
+  </si>
+  <si>
+    <t>AGI added to automaton's base.</t>
+  </si>
+  <si>
+    <t>DEX added to automaton's base.</t>
+  </si>
+  <si>
+    <t>STR added to automaton's base.</t>
+  </si>
+  <si>
+    <t>VIT added to automaton's base.</t>
+  </si>
+  <si>
+    <t>Base automaton INT.</t>
+  </si>
+  <si>
+    <t>Base automaton VIT.</t>
+  </si>
+  <si>
+    <t>Base automaton AGI.</t>
+  </si>
+  <si>
+    <t>Base automaton DEX.</t>
+  </si>
+  <si>
+    <t>Base automaton STR.</t>
   </si>
 </sst>
 </file>
@@ -2332,10 +2479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F310"/>
+  <dimension ref="A1:F339"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:A83"/>
+    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
+      <selection activeCell="D228" sqref="D228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,11 +2496,11 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25.9" x14ac:dyDescent="0.5">
       <c r="B1" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>262</v>
@@ -2558,7 +2705,7 @@
     </row>
     <row r="18" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B18" t="s">
         <v>72</v>
@@ -2651,55 +2798,55 @@
     <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="D24" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E24" t="s">
         <v>264</v>
       </c>
       <c r="F24" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="D25" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E25" t="s">
         <v>263</v>
       </c>
       <c r="F25" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="D26" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E26" t="s">
         <v>263</v>
       </c>
       <c r="F26" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="D27" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E27" t="s">
         <v>263</v>
       </c>
       <c r="F27" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="D28" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E28" t="s">
         <v>263</v>
@@ -2711,157 +2858,157 @@
     <row r="29" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="D29" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E29" t="s">
         <v>138</v>
       </c>
       <c r="F29" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="D30" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E30" t="s">
         <v>263</v>
       </c>
       <c r="F30" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="D31" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E31" t="s">
         <v>138</v>
       </c>
       <c r="F31" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="D32" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E32" t="s">
         <v>263</v>
       </c>
       <c r="F32" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="D33" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E33" t="s">
         <v>263</v>
       </c>
       <c r="F33" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="D34" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E34" t="s">
         <v>263</v>
       </c>
       <c r="F34" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="D35" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E35" t="s">
         <v>263</v>
       </c>
       <c r="F35" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="D36" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E36" t="s">
         <v>263</v>
       </c>
       <c r="F36" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
       <c r="D37" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E37" t="s">
         <v>263</v>
       </c>
       <c r="F37" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
       <c r="D38" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E38" t="s">
         <v>263</v>
       </c>
       <c r="F38" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="D39" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E39" t="s">
         <v>263</v>
       </c>
       <c r="F39" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="D40" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E40" t="s">
         <v>263</v>
       </c>
       <c r="F40" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="D41" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E41" t="s">
         <v>263</v>
       </c>
       <c r="F41" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2884,13 +3031,13 @@
     <row r="45" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="D45" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E45" t="s">
         <v>138</v>
       </c>
       <c r="F45" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3310,13 +3457,13 @@
     <row r="77" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12"/>
       <c r="D77" t="s">
+        <v>515</v>
+      </c>
+      <c r="E77" t="s">
+        <v>263</v>
+      </c>
+      <c r="F77" t="s">
         <v>516</v>
-      </c>
-      <c r="E77" t="s">
-        <v>263</v>
-      </c>
-      <c r="F77" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3639,7 +3786,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
     </row>
     <row r="103" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3809,25 +3956,25 @@
     <row r="116" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="12"/>
       <c r="D116" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E116" t="s">
         <v>138</v>
       </c>
       <c r="F116" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12"/>
       <c r="D117" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E117" t="s">
         <v>263</v>
       </c>
       <c r="F117" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3946,22 +4093,22 @@
     </row>
     <row r="129" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="12" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D129" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E129" t="s">
         <v>138</v>
       </c>
       <c r="F129" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="12"/>
       <c r="D130" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E130" t="s">
         <v>138</v>
@@ -3973,91 +4120,91 @@
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="12"/>
       <c r="D131" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E131" t="s">
         <v>263</v>
       </c>
       <c r="F131" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="12"/>
       <c r="D132" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E132" t="s">
         <v>263</v>
       </c>
       <c r="F132" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="12"/>
       <c r="D133" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E133" t="s">
         <v>264</v>
       </c>
       <c r="F133" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="12"/>
       <c r="D134" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E134" t="s">
         <v>264</v>
       </c>
       <c r="F134" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="12"/>
       <c r="D135" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E135" t="s">
         <v>263</v>
       </c>
       <c r="F135" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="12"/>
       <c r="D136" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E136" t="s">
         <v>263</v>
       </c>
       <c r="F136" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="12"/>
       <c r="D137" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E137" t="s">
         <v>263</v>
       </c>
       <c r="F137" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="12"/>
       <c r="D138" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E138" t="s">
         <v>263</v>
@@ -4069,151 +4216,151 @@
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="12"/>
       <c r="D139" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E139" t="s">
         <v>138</v>
       </c>
       <c r="F139" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="12"/>
       <c r="D140" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E140" t="s">
         <v>263</v>
       </c>
       <c r="F140" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="12"/>
       <c r="D141" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E141" t="s">
         <v>138</v>
       </c>
       <c r="F141" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="12"/>
       <c r="D142" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E142" t="s">
         <v>263</v>
       </c>
       <c r="F142" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="12"/>
       <c r="D143" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E143" t="s">
         <v>263</v>
       </c>
       <c r="F143" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="12"/>
       <c r="D144" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E144" t="s">
         <v>263</v>
       </c>
       <c r="F144" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="12"/>
       <c r="D145" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E145" t="s">
         <v>263</v>
       </c>
       <c r="F145" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="12"/>
       <c r="D146" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E146" t="s">
         <v>263</v>
       </c>
       <c r="F146" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="12"/>
       <c r="D147" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E147" t="s">
         <v>263</v>
       </c>
       <c r="F147" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="12"/>
       <c r="D148" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E148" t="s">
         <v>263</v>
       </c>
       <c r="F148" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="12"/>
       <c r="D149" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E149" t="s">
         <v>263</v>
       </c>
       <c r="F149" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="12"/>
       <c r="D150" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E150" t="s">
         <v>263</v>
       </c>
       <c r="F150" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="12"/>
       <c r="D151" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E151" t="s">
         <v>263</v>
@@ -4335,7 +4482,7 @@
         <v>263</v>
       </c>
       <c r="F162" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4359,7 +4506,7 @@
         <v>138</v>
       </c>
       <c r="F164" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4371,31 +4518,31 @@
         <v>263</v>
       </c>
       <c r="F165" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="166" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="12"/>
       <c r="D166" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E166" t="s">
         <v>138</v>
       </c>
       <c r="F166" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="12"/>
       <c r="D167" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E167" t="s">
         <v>263</v>
       </c>
       <c r="F167" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4523,7 +4670,7 @@
         <v>138</v>
       </c>
       <c r="F179" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="180" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4573,86 +4720,86 @@
     </row>
     <row r="183" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="12"/>
+      <c r="B183" t="s">
+        <v>108</v>
+      </c>
       <c r="D183" t="s">
-        <v>429</v>
+        <v>107</v>
       </c>
       <c r="E183" t="s">
         <v>263</v>
       </c>
       <c r="F183" t="s">
-        <v>453</v>
+        <v>431</v>
       </c>
     </row>
     <row r="184" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="12"/>
       <c r="B184" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D184" t="s">
-        <v>107</v>
-      </c>
-      <c r="E184" t="s">
-        <v>263</v>
+        <v>0</v>
       </c>
       <c r="F184" t="s">
-        <v>431</v>
+        <v>152</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="12"/>
-      <c r="B185" t="s">
-        <v>106</v>
-      </c>
       <c r="D185" t="s">
-        <v>0</v>
+        <v>432</v>
+      </c>
+      <c r="E185" t="s">
+        <v>263</v>
       </c>
       <c r="F185" t="s">
-        <v>152</v>
+        <v>452</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="12"/>
       <c r="D186" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="E186" t="s">
         <v>263</v>
       </c>
       <c r="F186" t="s">
-        <v>452</v>
+        <v>362</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="12"/>
       <c r="D187" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="E187" t="s">
         <v>263</v>
       </c>
       <c r="F187" t="s">
-        <v>362</v>
+        <v>451</v>
       </c>
     </row>
     <row r="188" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="12"/>
       <c r="D188" t="s">
-        <v>434</v>
+        <v>521</v>
       </c>
       <c r="E188" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F188" t="s">
-        <v>451</v>
+        <v>522</v>
       </c>
     </row>
     <row r="189" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="12"/>
       <c r="D189" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="E189" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F189" t="s">
         <v>523</v>
@@ -4661,1386 +4808,1704 @@
     <row r="190" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="12"/>
       <c r="D190" t="s">
-        <v>520</v>
+        <v>435</v>
       </c>
       <c r="E190" t="s">
         <v>263</v>
       </c>
       <c r="F190" t="s">
-        <v>524</v>
+        <v>450</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="12"/>
       <c r="D191" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="E191" t="s">
         <v>263</v>
       </c>
       <c r="F191" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="192" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="12"/>
       <c r="D192" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="E192" t="s">
         <v>263</v>
       </c>
       <c r="F192" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="193" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="12"/>
       <c r="D193" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="E193" t="s">
         <v>263</v>
       </c>
       <c r="F193" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="194" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="12"/>
       <c r="D194" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E194" t="s">
         <v>263</v>
       </c>
       <c r="F194" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="195" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="12"/>
       <c r="D195" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E195" t="s">
         <v>263</v>
       </c>
       <c r="F195" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="196" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="12"/>
       <c r="D196" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E196" t="s">
         <v>263</v>
       </c>
       <c r="F196" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="197" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="12"/>
       <c r="D197" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E197" t="s">
         <v>263</v>
       </c>
       <c r="F197" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="12"/>
       <c r="D198" t="s">
-        <v>442</v>
-      </c>
-      <c r="E198" t="s">
-        <v>263</v>
+        <v>641</v>
       </c>
       <c r="F198" t="s">
-        <v>443</v>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="12"/>
+      <c r="D199" t="s">
+        <v>662</v>
+      </c>
+      <c r="E199" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="12"/>
+      <c r="D200" t="s">
+        <v>663</v>
+      </c>
+      <c r="E200" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="201" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="B201" t="s">
-        <v>109</v>
-      </c>
+      <c r="A201" s="12"/>
       <c r="D201" t="s">
-        <v>220</v>
+        <v>429</v>
       </c>
       <c r="E201" t="s">
-        <v>138</v>
-      </c>
-      <c r="F201" t="s">
-        <v>481</v>
+        <v>263</v>
       </c>
     </row>
     <row r="202" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="12"/>
-      <c r="B202" t="s">
-        <v>110</v>
-      </c>
       <c r="D202" t="s">
-        <v>221</v>
+        <v>644</v>
       </c>
       <c r="E202" t="s">
-        <v>264</v>
-      </c>
-      <c r="F202" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="12"/>
-      <c r="B203" t="s">
-        <v>111</v>
-      </c>
       <c r="D203" t="s">
-        <v>222</v>
+        <v>645</v>
       </c>
       <c r="E203" t="s">
         <v>263</v>
       </c>
-      <c r="F203" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="12"/>
       <c r="D204" t="s">
-        <v>455</v>
+        <v>642</v>
       </c>
       <c r="E204" t="s">
         <v>263</v>
       </c>
-      <c r="F204" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="12"/>
       <c r="D205" t="s">
-        <v>456</v>
+        <v>643</v>
       </c>
       <c r="E205" t="s">
         <v>263</v>
       </c>
-      <c r="F205" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="12"/>
       <c r="D206" t="s">
-        <v>457</v>
+        <v>646</v>
       </c>
       <c r="E206" t="s">
         <v>263</v>
       </c>
-      <c r="F206" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="207" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="12"/>
       <c r="D207" t="s">
-        <v>458</v>
+        <v>647</v>
       </c>
       <c r="E207" t="s">
         <v>263</v>
       </c>
-      <c r="F207" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="208" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="12"/>
       <c r="D208" t="s">
-        <v>460</v>
+        <v>648</v>
       </c>
       <c r="E208" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="209" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+      <c r="F208" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="12"/>
       <c r="D209" t="s">
-        <v>459</v>
+        <v>655</v>
       </c>
       <c r="E209" t="s">
         <v>263</v>
       </c>
       <c r="F209" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="210" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="12"/>
       <c r="D210" t="s">
-        <v>527</v>
+        <v>649</v>
       </c>
       <c r="E210" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F210" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="211" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="12"/>
       <c r="D211" t="s">
-        <v>521</v>
+        <v>656</v>
       </c>
       <c r="E211" t="s">
         <v>263</v>
       </c>
       <c r="F211" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="212" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="12"/>
       <c r="D212" t="s">
-        <v>461</v>
+        <v>650</v>
       </c>
       <c r="E212" t="s">
         <v>263</v>
       </c>
       <c r="F212" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="12"/>
       <c r="D213" t="s">
-        <v>462</v>
+        <v>658</v>
       </c>
       <c r="E213" t="s">
         <v>263</v>
       </c>
       <c r="F213" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="214" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="12"/>
       <c r="D214" t="s">
-        <v>463</v>
+        <v>651</v>
       </c>
       <c r="E214" t="s">
         <v>263</v>
       </c>
       <c r="F214" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="215" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="12"/>
       <c r="D215" t="s">
-        <v>464</v>
+        <v>657</v>
       </c>
       <c r="E215" t="s">
         <v>263</v>
       </c>
       <c r="F215" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="216" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="12"/>
       <c r="D216" t="s">
-        <v>465</v>
+        <v>652</v>
       </c>
       <c r="E216" t="s">
         <v>263</v>
       </c>
       <c r="F216" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="12"/>
       <c r="D217" t="s">
-        <v>466</v>
+        <v>659</v>
       </c>
       <c r="E217" t="s">
         <v>263</v>
       </c>
       <c r="F217" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="12"/>
       <c r="D218" t="s">
-        <v>467</v>
+        <v>653</v>
       </c>
       <c r="E218" t="s">
         <v>263</v>
       </c>
       <c r="F218" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="12"/>
       <c r="D219" t="s">
-        <v>468</v>
+        <v>660</v>
       </c>
       <c r="E219" t="s">
         <v>263</v>
       </c>
       <c r="F219" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="12" t="s">
-        <v>491</v>
-      </c>
-      <c r="B222" t="s">
-        <v>48</v>
-      </c>
+        <v>678</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" s="12"/>
+      <c r="D220" t="s">
+        <v>654</v>
+      </c>
+      <c r="E220" t="s">
+        <v>263</v>
+      </c>
+      <c r="F220" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" s="12"/>
+      <c r="D221" t="s">
+        <v>661</v>
+      </c>
+      <c r="E221" t="s">
+        <v>263</v>
+      </c>
+      <c r="F221" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" s="12"/>
       <c r="D222" t="s">
-        <v>154</v>
+        <v>664</v>
       </c>
       <c r="E222" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F222" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="12"/>
       <c r="D223" t="s">
-        <v>155</v>
+        <v>665</v>
       </c>
       <c r="E223" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F223" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="12"/>
       <c r="D224" t="s">
-        <v>158</v>
+        <v>666</v>
       </c>
       <c r="E224" t="s">
         <v>140</v>
       </c>
       <c r="F224" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="12"/>
       <c r="D225" t="s">
-        <v>159</v>
+        <v>667</v>
       </c>
       <c r="E225" t="s">
         <v>140</v>
       </c>
       <c r="F225" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="12"/>
-      <c r="D226" s="9" t="s">
-        <v>490</v>
-      </c>
-      <c r="E226" s="9" t="s">
+      <c r="D226" t="s">
+        <v>668</v>
+      </c>
+      <c r="E226" t="s">
         <v>140</v>
       </c>
-      <c r="F226" s="9" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F226" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="12"/>
-      <c r="D227" s="9" t="s">
-        <v>492</v>
-      </c>
-      <c r="E227" s="9" t="s">
+      <c r="D227" t="s">
+        <v>669</v>
+      </c>
+      <c r="E227" t="s">
         <v>140</v>
       </c>
-      <c r="F227" s="9" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A228" s="3"/>
-    </row>
-    <row r="229" spans="1:6" s="9" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A229" s="2"/>
+      <c r="F227" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="B230" t="s">
+        <v>109</v>
+      </c>
+      <c r="D230" t="s">
+        <v>220</v>
+      </c>
+      <c r="E230" t="s">
+        <v>138</v>
+      </c>
+      <c r="F230" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="231" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="12" t="s">
-        <v>348</v>
-      </c>
+      <c r="A231" s="12"/>
       <c r="B231" t="s">
-        <v>24</v>
+        <v>110</v>
       </c>
       <c r="D231" t="s">
-        <v>25</v>
+        <v>221</v>
       </c>
       <c r="E231" t="s">
-        <v>138</v>
+        <v>264</v>
       </c>
       <c r="F231" t="s">
-        <v>489</v>
+        <v>223</v>
       </c>
     </row>
     <row r="232" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="12"/>
       <c r="B232" t="s">
-        <v>53</v>
+        <v>111</v>
       </c>
       <c r="D232" t="s">
-        <v>54</v>
+        <v>222</v>
       </c>
       <c r="E232" t="s">
         <v>263</v>
       </c>
       <c r="F232" t="s">
-        <v>497</v>
+        <v>481</v>
       </c>
     </row>
     <row r="233" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="12"/>
-      <c r="B233" t="s">
-        <v>55</v>
-      </c>
       <c r="D233" t="s">
-        <v>56</v>
+        <v>454</v>
       </c>
       <c r="E233" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F233" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
     </row>
     <row r="234" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="12"/>
-      <c r="B234" t="s">
-        <v>58</v>
-      </c>
       <c r="D234" t="s">
-        <v>57</v>
+        <v>455</v>
       </c>
       <c r="E234" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F234" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
     </row>
     <row r="235" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="12"/>
       <c r="D235" t="s">
-        <v>493</v>
+        <v>456</v>
       </c>
       <c r="E235" t="s">
         <v>263</v>
       </c>
       <c r="F235" t="s">
-        <v>231</v>
+        <v>477</v>
       </c>
     </row>
     <row r="236" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="12"/>
-      <c r="B236" t="s">
-        <v>59</v>
-      </c>
       <c r="D236" t="s">
-        <v>60</v>
+        <v>457</v>
       </c>
       <c r="E236" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F236" t="s">
-        <v>486</v>
+        <v>362</v>
       </c>
     </row>
     <row r="237" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="12"/>
-      <c r="B237" t="s">
-        <v>61</v>
-      </c>
       <c r="D237" t="s">
-        <v>62</v>
+        <v>459</v>
       </c>
       <c r="E237" t="s">
         <v>138</v>
       </c>
-      <c r="F237" t="s">
-        <v>232</v>
-      </c>
     </row>
     <row r="238" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="12"/>
-      <c r="B238" t="s">
-        <v>63</v>
-      </c>
       <c r="D238" t="s">
-        <v>65</v>
+        <v>458</v>
       </c>
       <c r="E238" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F238" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
     </row>
     <row r="239" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="12"/>
-      <c r="B239" t="s">
-        <v>64</v>
-      </c>
       <c r="D239" t="s">
-        <v>66</v>
+        <v>526</v>
       </c>
       <c r="E239" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="F239" t="s">
-        <v>484</v>
+        <v>524</v>
       </c>
     </row>
     <row r="240" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="12"/>
       <c r="D240" t="s">
-        <v>494</v>
+        <v>520</v>
       </c>
       <c r="E240" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="F240" t="s">
-        <v>233</v>
+        <v>525</v>
       </c>
     </row>
     <row r="241" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="12"/>
       <c r="D241" t="s">
-        <v>495</v>
+        <v>460</v>
       </c>
       <c r="E241" t="s">
         <v>263</v>
       </c>
       <c r="F241" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
     </row>
     <row r="242" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="12"/>
       <c r="D242" t="s">
-        <v>496</v>
+        <v>461</v>
       </c>
       <c r="E242" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F242" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="245" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A245" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B245" t="s">
-        <v>120</v>
-      </c>
+        <v>474</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="12"/>
+      <c r="D243" t="s">
+        <v>462</v>
+      </c>
+      <c r="E243" t="s">
+        <v>263</v>
+      </c>
+      <c r="F243" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="12"/>
+      <c r="D244" t="s">
+        <v>463</v>
+      </c>
+      <c r="E244" t="s">
+        <v>263</v>
+      </c>
+      <c r="F244" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="12"/>
       <c r="D245" t="s">
-        <v>120</v>
+        <v>464</v>
       </c>
       <c r="E245" t="s">
-        <v>140</v>
+        <v>263</v>
       </c>
       <c r="F245" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A248" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B248" t="s">
-        <v>201</v>
-      </c>
+        <v>471</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="12"/>
+      <c r="D246" t="s">
+        <v>465</v>
+      </c>
+      <c r="E246" t="s">
+        <v>263</v>
+      </c>
+      <c r="F246" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="12"/>
+      <c r="D247" t="s">
+        <v>466</v>
+      </c>
+      <c r="E247" t="s">
+        <v>263</v>
+      </c>
+      <c r="F247" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="12"/>
       <c r="D248" t="s">
-        <v>614</v>
+        <v>467</v>
       </c>
       <c r="E248" t="s">
-        <v>501</v>
+        <v>263</v>
       </c>
       <c r="F248" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A249" s="12"/>
-      <c r="B249" t="s">
-        <v>513</v>
-      </c>
-      <c r="D249" t="s">
-        <v>514</v>
-      </c>
-      <c r="E249" t="s">
-        <v>501</v>
-      </c>
-      <c r="F249" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="250" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A250" s="12"/>
-      <c r="B250" t="s">
-        <v>122</v>
-      </c>
-      <c r="D250" t="s">
-        <v>133</v>
-      </c>
-      <c r="E250" t="s">
-        <v>501</v>
-      </c>
-      <c r="F250" t="s">
-        <v>624</v>
+        <v>469</v>
       </c>
     </row>
     <row r="251" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A251" s="12"/>
+      <c r="A251" s="12" t="s">
+        <v>490</v>
+      </c>
       <c r="B251" t="s">
-        <v>121</v>
+        <v>48</v>
       </c>
       <c r="D251" t="s">
-        <v>0</v>
+        <v>154</v>
+      </c>
+      <c r="E251" t="s">
+        <v>263</v>
       </c>
       <c r="F251" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="12"/>
-      <c r="B252" t="s">
-        <v>123</v>
-      </c>
       <c r="D252" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E252" t="s">
-        <v>501</v>
+        <v>263</v>
       </c>
       <c r="F252" t="s">
-        <v>623</v>
+        <v>156</v>
       </c>
     </row>
     <row r="253" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="12"/>
-      <c r="B253" t="s">
-        <v>117</v>
-      </c>
       <c r="D253" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E253" t="s">
-        <v>501</v>
+        <v>140</v>
       </c>
       <c r="F253" t="s">
-        <v>625</v>
+        <v>499</v>
       </c>
     </row>
     <row r="254" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="12"/>
       <c r="D254" t="s">
-        <v>613</v>
+        <v>159</v>
       </c>
       <c r="E254" t="s">
-        <v>501</v>
+        <v>140</v>
       </c>
       <c r="F254" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="255" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="12"/>
-      <c r="B255" t="s">
-        <v>124</v>
-      </c>
-      <c r="D255" t="s">
-        <v>203</v>
-      </c>
-      <c r="E255" t="s">
-        <v>501</v>
-      </c>
-      <c r="F255" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="256" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D255" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="E255" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F255" s="9" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="12"/>
-      <c r="B256" t="s">
-        <v>125</v>
-      </c>
-      <c r="D256" t="s">
-        <v>204</v>
-      </c>
-      <c r="E256" t="s">
-        <v>501</v>
-      </c>
-      <c r="F256" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="257" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A257" s="12"/>
-      <c r="B257" t="s">
-        <v>129</v>
-      </c>
-      <c r="C257" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="D257" t="s">
-        <v>213</v>
-      </c>
-      <c r="E257" t="s">
-        <v>501</v>
-      </c>
-      <c r="F257" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="258" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A258" s="12"/>
-      <c r="B258" t="s">
-        <v>130</v>
-      </c>
-      <c r="D258" t="s">
-        <v>132</v>
-      </c>
-      <c r="E258" t="s">
-        <v>501</v>
-      </c>
-      <c r="F258" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="259" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A259" s="12"/>
-      <c r="B259" t="s">
-        <v>137</v>
-      </c>
-      <c r="D259" t="s">
-        <v>207</v>
-      </c>
-      <c r="E259" t="s">
-        <v>501</v>
-      </c>
-      <c r="F259" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="260" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A260" s="12"/>
+      <c r="D256" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="E256" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F256" s="9" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="3"/>
+    </row>
+    <row r="258" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A258" s="2"/>
+    </row>
+    <row r="260" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="12" t="s">
+        <v>348</v>
+      </c>
       <c r="B260" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D260" t="s">
-        <v>136</v>
+        <v>25</v>
       </c>
       <c r="E260" t="s">
-        <v>501</v>
+        <v>138</v>
       </c>
       <c r="F260" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="261" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="12"/>
       <c r="B261" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="D261" t="s">
-        <v>134</v>
+        <v>54</v>
       </c>
       <c r="E261" t="s">
-        <v>501</v>
+        <v>263</v>
       </c>
       <c r="F261" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="262" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="12"/>
       <c r="B262" t="s">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="D262" t="s">
-        <v>135</v>
+        <v>56</v>
       </c>
       <c r="E262" t="s">
-        <v>501</v>
+        <v>138</v>
       </c>
       <c r="F262" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="263" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="12"/>
       <c r="B263" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="D263" t="s">
-        <v>209</v>
+        <v>57</v>
       </c>
       <c r="E263" t="s">
-        <v>501</v>
+        <v>138</v>
       </c>
       <c r="F263" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="12"/>
-      <c r="B264" t="s">
-        <v>0</v>
-      </c>
       <c r="D264" t="s">
-        <v>633</v>
+        <v>492</v>
       </c>
       <c r="E264" t="s">
-        <v>501</v>
+        <v>263</v>
       </c>
       <c r="F264" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="265" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A265" s="3"/>
-    </row>
-    <row r="266" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A266" s="2"/>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="12"/>
+      <c r="B265" t="s">
+        <v>59</v>
+      </c>
+      <c r="D265" t="s">
+        <v>60</v>
+      </c>
+      <c r="E265" t="s">
+        <v>138</v>
+      </c>
+      <c r="F265" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A266" s="12"/>
+      <c r="B266" t="s">
+        <v>61</v>
+      </c>
+      <c r="D266" t="s">
+        <v>62</v>
+      </c>
+      <c r="E266" t="s">
+        <v>138</v>
+      </c>
+      <c r="F266" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="267" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A267" s="13" t="s">
-        <v>618</v>
+      <c r="A267" s="12"/>
+      <c r="B267" t="s">
+        <v>63</v>
       </c>
       <c r="D267" t="s">
-        <v>199</v>
+        <v>65</v>
       </c>
       <c r="E267" t="s">
-        <v>501</v>
+        <v>138</v>
       </c>
       <c r="F267" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="268" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A268" s="13"/>
+        <v>484</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A268" s="12"/>
+      <c r="B268" t="s">
+        <v>64</v>
+      </c>
       <c r="D268" t="s">
-        <v>619</v>
+        <v>66</v>
       </c>
       <c r="E268" t="s">
-        <v>501</v>
+        <v>263</v>
       </c>
       <c r="F268" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="269" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A269" s="13"/>
-      <c r="B269" t="s">
-        <v>177</v>
-      </c>
+        <v>483</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A269" s="12"/>
       <c r="D269" t="s">
-        <v>184</v>
+        <v>493</v>
       </c>
       <c r="E269" t="s">
-        <v>501</v>
+        <v>138</v>
       </c>
       <c r="F269" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="270" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A270" s="13"/>
-      <c r="B270" t="s">
-        <v>178</v>
-      </c>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A270" s="12"/>
       <c r="D270" t="s">
-        <v>183</v>
+        <v>494</v>
       </c>
       <c r="E270" t="s">
-        <v>501</v>
+        <v>263</v>
       </c>
       <c r="F270" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="271" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A271" s="13"/>
-      <c r="B271" t="s">
-        <v>179</v>
-      </c>
+        <v>482</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A271" s="12"/>
       <c r="D271" t="s">
-        <v>182</v>
+        <v>495</v>
       </c>
       <c r="E271" t="s">
-        <v>501</v>
+        <v>264</v>
       </c>
       <c r="F271" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="272" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A272" s="13"/>
-      <c r="D272" t="s">
-        <v>181</v>
-      </c>
-      <c r="E272" t="s">
-        <v>501</v>
-      </c>
-      <c r="F272" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="273" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A273" s="13"/>
-      <c r="D273" t="s">
-        <v>180</v>
-      </c>
-      <c r="E273" t="s">
-        <v>501</v>
-      </c>
-      <c r="F273" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="274" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A274" s="13"/>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A274" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B274" t="s">
+        <v>120</v>
+      </c>
       <c r="D274" t="s">
-        <v>511</v>
+        <v>120</v>
       </c>
       <c r="E274" t="s">
-        <v>501</v>
+        <v>140</v>
       </c>
       <c r="F274" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A277" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B277" t="s">
+        <v>201</v>
+      </c>
+      <c r="D277" t="s">
+        <v>613</v>
+      </c>
+      <c r="E277" t="s">
+        <v>500</v>
+      </c>
+      <c r="F277" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A278" s="12"/>
+      <c r="B278" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="275" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A275" s="13"/>
-      <c r="D275" t="s">
-        <v>626</v>
-      </c>
-      <c r="E275" t="s">
-        <v>501</v>
-      </c>
-      <c r="F275" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="276" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A276" s="13"/>
-      <c r="D276" t="s">
-        <v>185</v>
-      </c>
-      <c r="E276" t="s">
-        <v>501</v>
-      </c>
-      <c r="F276" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="277" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A277" s="13"/>
-      <c r="D277" t="s">
-        <v>198</v>
-      </c>
-      <c r="E277" t="s">
-        <v>501</v>
-      </c>
-      <c r="F277" t="s">
-        <v>622</v>
+      <c r="D278" t="s">
+        <v>513</v>
+      </c>
+      <c r="E278" t="s">
+        <v>500</v>
+      </c>
+      <c r="F278" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A279" s="12"/>
+      <c r="B279" t="s">
+        <v>122</v>
+      </c>
+      <c r="D279" t="s">
+        <v>133</v>
+      </c>
+      <c r="E279" t="s">
+        <v>500</v>
+      </c>
+      <c r="F279" t="s">
+        <v>623</v>
       </c>
     </row>
     <row r="280" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A280" s="12" t="s">
-        <v>127</v>
-      </c>
+      <c r="A280" s="12"/>
       <c r="B280" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D280" t="s">
         <v>0</v>
       </c>
       <c r="F280" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="281" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="12"/>
       <c r="B281" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="D281" t="s">
-        <v>0</v>
+        <v>161</v>
+      </c>
+      <c r="E281" t="s">
+        <v>500</v>
       </c>
       <c r="F281" t="s">
-        <v>167</v>
+        <v>622</v>
       </c>
     </row>
     <row r="282" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" s="12"/>
       <c r="B282" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D282" t="s">
-        <v>0</v>
+        <v>162</v>
+      </c>
+      <c r="E282" t="s">
+        <v>500</v>
       </c>
       <c r="F282" t="s">
-        <v>168</v>
+        <v>624</v>
       </c>
     </row>
     <row r="283" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="12"/>
-      <c r="B283" t="s">
-        <v>128</v>
-      </c>
       <c r="D283" t="s">
-        <v>0</v>
+        <v>612</v>
+      </c>
+      <c r="E283" t="s">
+        <v>500</v>
       </c>
       <c r="F283" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="284" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="12"/>
       <c r="B284" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D284" t="s">
-        <v>0</v>
+        <v>203</v>
+      </c>
+      <c r="E284" t="s">
+        <v>500</v>
       </c>
       <c r="F284" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="285" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A285" s="3"/>
-    </row>
-    <row r="286" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A286" s="3"/>
-    </row>
-    <row r="287" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A287" s="13" t="s">
-        <v>141</v>
-      </c>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A285" s="12"/>
+      <c r="B285" t="s">
+        <v>125</v>
+      </c>
+      <c r="D285" t="s">
+        <v>204</v>
+      </c>
+      <c r="E285" t="s">
+        <v>500</v>
+      </c>
+      <c r="F285" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A286" s="12"/>
+      <c r="B286" t="s">
+        <v>129</v>
+      </c>
+      <c r="C286" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D286" t="s">
+        <v>213</v>
+      </c>
+      <c r="E286" t="s">
+        <v>500</v>
+      </c>
+      <c r="F286" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A287" s="12"/>
       <c r="B287" t="s">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="D287" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E287" t="s">
-        <v>140</v>
+        <v>500</v>
       </c>
       <c r="F287" t="s">
-        <v>170</v>
+        <v>616</v>
       </c>
     </row>
     <row r="288" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A288" s="13"/>
+      <c r="A288" s="12"/>
       <c r="B288" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
       <c r="D288" t="s">
-        <v>139</v>
+        <v>207</v>
       </c>
       <c r="E288" t="s">
-        <v>140</v>
+        <v>500</v>
       </c>
       <c r="F288" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="289" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A289" s="13"/>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A289" s="12"/>
       <c r="B289" t="s">
         <v>0</v>
       </c>
       <c r="D289" t="s">
-        <v>635</v>
+        <v>136</v>
       </c>
       <c r="E289" t="s">
-        <v>140</v>
+        <v>500</v>
       </c>
       <c r="F289" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="290" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A290" s="13"/>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A290" s="12"/>
       <c r="B290" t="s">
         <v>0</v>
       </c>
       <c r="D290" t="s">
-        <v>636</v>
+        <v>134</v>
       </c>
       <c r="E290" t="s">
-        <v>140</v>
+        <v>500</v>
       </c>
       <c r="F290" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="291" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A291" s="13"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A291" s="12"/>
       <c r="B291" t="s">
         <v>0</v>
       </c>
       <c r="D291" t="s">
-        <v>637</v>
+        <v>135</v>
       </c>
       <c r="E291" t="s">
-        <v>140</v>
+        <v>500</v>
       </c>
       <c r="F291" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="292" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A292" s="13"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A292" s="12"/>
       <c r="B292" t="s">
         <v>0</v>
       </c>
       <c r="D292" t="s">
-        <v>506</v>
+        <v>209</v>
       </c>
       <c r="E292" t="s">
-        <v>140</v>
+        <v>500</v>
       </c>
       <c r="F292" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="293" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A293" s="13"/>
+        <v>509</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A293" s="12"/>
       <c r="B293" t="s">
         <v>0</v>
       </c>
       <c r="D293" t="s">
-        <v>508</v>
+        <v>632</v>
       </c>
       <c r="E293" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F293" t="s">
-        <v>509</v>
+        <v>633</v>
       </c>
     </row>
     <row r="294" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A294" s="13"/>
-      <c r="B294" t="s">
-        <v>0</v>
-      </c>
-      <c r="D294" t="s">
-        <v>142</v>
-      </c>
-      <c r="E294" t="s">
-        <v>501</v>
-      </c>
-      <c r="F294" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="295" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A295" s="13"/>
-      <c r="B295" t="s">
-        <v>0</v>
-      </c>
-      <c r="D295" t="s">
-        <v>143</v>
-      </c>
-      <c r="E295" t="s">
-        <v>501</v>
-      </c>
-      <c r="F295" t="s">
-        <v>174</v>
-      </c>
+      <c r="A294" s="3"/>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A295" s="2"/>
     </row>
     <row r="296" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A296" s="13"/>
-      <c r="B296" t="s">
-        <v>0</v>
+      <c r="A296" s="13" t="s">
+        <v>617</v>
       </c>
       <c r="D296" t="s">
-        <v>144</v>
+        <v>199</v>
       </c>
       <c r="E296" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F296" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
     </row>
     <row r="297" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A297" s="13"/>
-      <c r="B297" t="s">
+      <c r="D297" t="s">
+        <v>618</v>
+      </c>
+      <c r="E297" t="s">
+        <v>500</v>
+      </c>
+      <c r="F297" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A298" s="13"/>
+      <c r="B298" t="s">
+        <v>177</v>
+      </c>
+      <c r="D298" t="s">
+        <v>184</v>
+      </c>
+      <c r="E298" t="s">
+        <v>500</v>
+      </c>
+      <c r="F298" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A299" s="13"/>
+      <c r="B299" t="s">
+        <v>178</v>
+      </c>
+      <c r="D299" t="s">
+        <v>183</v>
+      </c>
+      <c r="E299" t="s">
+        <v>500</v>
+      </c>
+      <c r="F299" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="13"/>
+      <c r="B300" t="s">
+        <v>179</v>
+      </c>
+      <c r="D300" t="s">
+        <v>182</v>
+      </c>
+      <c r="E300" t="s">
+        <v>500</v>
+      </c>
+      <c r="F300" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A301" s="13"/>
+      <c r="D301" t="s">
+        <v>181</v>
+      </c>
+      <c r="E301" t="s">
+        <v>500</v>
+      </c>
+      <c r="F301" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A302" s="13"/>
+      <c r="D302" t="s">
+        <v>180</v>
+      </c>
+      <c r="E302" t="s">
+        <v>500</v>
+      </c>
+      <c r="F302" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A303" s="13"/>
+      <c r="D303" t="s">
+        <v>510</v>
+      </c>
+      <c r="E303" t="s">
+        <v>500</v>
+      </c>
+      <c r="F303" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A304" s="13"/>
+      <c r="D304" t="s">
+        <v>625</v>
+      </c>
+      <c r="E304" t="s">
+        <v>500</v>
+      </c>
+      <c r="F304" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A305" s="13"/>
+      <c r="D305" t="s">
+        <v>185</v>
+      </c>
+      <c r="E305" t="s">
+        <v>500</v>
+      </c>
+      <c r="F305" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A306" s="13"/>
+      <c r="D306" t="s">
+        <v>198</v>
+      </c>
+      <c r="E306" t="s">
+        <v>500</v>
+      </c>
+      <c r="F306" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A309" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B309" t="s">
+        <v>126</v>
+      </c>
+      <c r="D309" t="s">
         <v>0</v>
       </c>
-      <c r="D297" t="s">
+      <c r="F309" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A310" s="12"/>
+      <c r="B310" t="s">
+        <v>116</v>
+      </c>
+      <c r="D310" t="s">
+        <v>0</v>
+      </c>
+      <c r="F310" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A311" s="12"/>
+      <c r="B311" t="s">
+        <v>118</v>
+      </c>
+      <c r="D311" t="s">
+        <v>0</v>
+      </c>
+      <c r="F311" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A312" s="12"/>
+      <c r="B312" t="s">
+        <v>128</v>
+      </c>
+      <c r="D312" t="s">
+        <v>0</v>
+      </c>
+      <c r="F312" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A313" s="12"/>
+      <c r="B313" t="s">
+        <v>121</v>
+      </c>
+      <c r="D313" t="s">
+        <v>0</v>
+      </c>
+      <c r="F313" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A314" s="3"/>
+    </row>
+    <row r="315" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A315" s="3"/>
+    </row>
+    <row r="316" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A316" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B316" t="s">
+        <v>0</v>
+      </c>
+      <c r="D316" t="s">
+        <v>138</v>
+      </c>
+      <c r="E316" t="s">
+        <v>140</v>
+      </c>
+      <c r="F316" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A317" s="13"/>
+      <c r="B317" t="s">
+        <v>0</v>
+      </c>
+      <c r="D317" t="s">
+        <v>139</v>
+      </c>
+      <c r="E317" t="s">
+        <v>140</v>
+      </c>
+      <c r="F317" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A318" s="13"/>
+      <c r="B318" t="s">
+        <v>0</v>
+      </c>
+      <c r="D318" t="s">
+        <v>634</v>
+      </c>
+      <c r="E318" t="s">
+        <v>140</v>
+      </c>
+      <c r="F318" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A319" s="13"/>
+      <c r="B319" t="s">
+        <v>0</v>
+      </c>
+      <c r="D319" t="s">
+        <v>635</v>
+      </c>
+      <c r="E319" t="s">
+        <v>140</v>
+      </c>
+      <c r="F319" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A320" s="13"/>
+      <c r="B320" t="s">
+        <v>0</v>
+      </c>
+      <c r="D320" t="s">
+        <v>636</v>
+      </c>
+      <c r="E320" t="s">
+        <v>140</v>
+      </c>
+      <c r="F320" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A321" s="13"/>
+      <c r="B321" t="s">
+        <v>0</v>
+      </c>
+      <c r="D321" t="s">
+        <v>505</v>
+      </c>
+      <c r="E321" t="s">
+        <v>140</v>
+      </c>
+      <c r="F321" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A322" s="13"/>
+      <c r="B322" t="s">
+        <v>0</v>
+      </c>
+      <c r="D322" t="s">
+        <v>507</v>
+      </c>
+      <c r="E322" t="s">
+        <v>500</v>
+      </c>
+      <c r="F322" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="323" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A323" s="13"/>
+      <c r="B323" t="s">
+        <v>0</v>
+      </c>
+      <c r="D323" t="s">
+        <v>142</v>
+      </c>
+      <c r="E323" t="s">
+        <v>500</v>
+      </c>
+      <c r="F323" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A324" s="13"/>
+      <c r="B324" t="s">
+        <v>0</v>
+      </c>
+      <c r="D324" t="s">
+        <v>143</v>
+      </c>
+      <c r="E324" t="s">
+        <v>500</v>
+      </c>
+      <c r="F324" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A325" s="13"/>
+      <c r="B325" t="s">
+        <v>0</v>
+      </c>
+      <c r="D325" t="s">
+        <v>144</v>
+      </c>
+      <c r="E325" t="s">
+        <v>500</v>
+      </c>
+      <c r="F325" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A326" s="13"/>
+      <c r="B326" t="s">
+        <v>0</v>
+      </c>
+      <c r="D326" t="s">
         <v>145</v>
       </c>
-      <c r="E297" t="s">
-        <v>501</v>
-      </c>
-      <c r="F297" t="s">
+      <c r="E326" t="s">
+        <v>500</v>
+      </c>
+      <c r="F326" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="298" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A298" s="8"/>
-    </row>
-    <row r="299" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A299" s="8"/>
-    </row>
-    <row r="300" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A300" s="12" t="s">
+    <row r="327" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A327" s="8"/>
+    </row>
+    <row r="328" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A328" s="8"/>
+    </row>
+    <row r="329" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A329" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="D300" t="s">
+      <c r="D329" t="s">
         <v>188</v>
       </c>
-      <c r="F300" t="s">
+      <c r="F329" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="301" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A301" s="12"/>
-      <c r="D301" t="s">
+    <row r="330" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A330" s="12"/>
+      <c r="D330" t="s">
         <v>190</v>
       </c>
-      <c r="F301" t="s">
+      <c r="F330" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="302" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A302" s="12"/>
-      <c r="D302" t="s">
+    <row r="331" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A331" s="12"/>
+      <c r="D331" t="s">
         <v>192</v>
       </c>
-      <c r="F302" t="s">
+      <c r="F331" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="303" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A303" s="12"/>
-      <c r="D303" t="s">
+    <row r="332" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A332" s="12"/>
+      <c r="D332" t="s">
         <v>193</v>
       </c>
-      <c r="F303" t="s">
+      <c r="F332" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="304" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A304" s="12"/>
-      <c r="D304" t="s">
+    <row r="333" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A333" s="12"/>
+      <c r="D333" t="s">
         <v>196</v>
       </c>
-      <c r="F304" t="s">
+      <c r="F333" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="305" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A305" s="12"/>
-      <c r="B305" t="s">
+    <row r="334" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A334" s="12"/>
+      <c r="B334" t="s">
         <v>226</v>
       </c>
-      <c r="D305" t="s">
+      <c r="D334" t="s">
         <v>211</v>
       </c>
-      <c r="F305" t="s">
+      <c r="F334" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="306" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A306" s="12"/>
-      <c r="B306" t="s">
+    <row r="335" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A335" s="12"/>
+      <c r="B335" t="s">
         <v>229</v>
       </c>
-      <c r="D306" t="s">
+      <c r="D335" t="s">
         <v>215</v>
       </c>
-      <c r="F306" t="s">
+      <c r="F335" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="307" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A307" s="12"/>
-      <c r="B307" t="s">
+    <row r="336" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A336" s="12"/>
+      <c r="B336" t="s">
         <v>228</v>
       </c>
-      <c r="D307" t="s">
+      <c r="D336" t="s">
         <v>214</v>
       </c>
-      <c r="F307" t="s">
+      <c r="F336" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="308" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A308" s="12"/>
-      <c r="B308" t="s">
+    <row r="337" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A337" s="12"/>
+      <c r="B337" t="s">
         <v>227</v>
       </c>
-      <c r="D308" t="s">
+      <c r="D337" t="s">
         <v>224</v>
       </c>
-      <c r="F308" t="s">
+      <c r="F337" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="309" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A309" s="12"/>
-      <c r="D309" t="s">
+    <row r="338" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A338" s="12"/>
+      <c r="D338" t="s">
+        <v>503</v>
+      </c>
+      <c r="F338" t="s">
         <v>504</v>
       </c>
-      <c r="F309" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="310" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A310" s="3"/>
+    </row>
+    <row r="339" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A339" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A300:A309"/>
-    <mergeCell ref="A280:A284"/>
-    <mergeCell ref="A222:A227"/>
-    <mergeCell ref="A231:A242"/>
-    <mergeCell ref="A267:A277"/>
-    <mergeCell ref="A287:A297"/>
-    <mergeCell ref="A248:A264"/>
     <mergeCell ref="A18:A41"/>
     <mergeCell ref="A3:A15"/>
     <mergeCell ref="A104:A126"/>
-    <mergeCell ref="A201:A219"/>
-    <mergeCell ref="A179:A198"/>
+    <mergeCell ref="A230:A248"/>
     <mergeCell ref="A129:A151"/>
     <mergeCell ref="A154:A176"/>
     <mergeCell ref="A86:A101"/>
     <mergeCell ref="A44:A83"/>
+    <mergeCell ref="A179:A227"/>
+    <mergeCell ref="A329:A338"/>
+    <mergeCell ref="A309:A313"/>
+    <mergeCell ref="A251:A256"/>
+    <mergeCell ref="A260:A271"/>
+    <mergeCell ref="A296:A306"/>
+    <mergeCell ref="A316:A326"/>
+    <mergeCell ref="A277:A293"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add ability to filter items searched for in validate function. Update docs to match.
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variables.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725" iterate="1"/>
 </workbook>
 </file>
 
@@ -1527,12 +1527,6 @@
     <t>Contains all of the information above (position, distance, etc.) if the given party member has loaded since you zoned. Information may not be accurate if they are further than 50 yalms. This table is similar to the above information for targets.</t>
   </si>
   <si>
-    <t>//gs validate</t>
-  </si>
-  <si>
-    <t>This command checks to see whether the equipment in "sets" also exists in your inventory.</t>
-  </si>
-  <si>
     <t>os</t>
   </si>
   <si>
@@ -2101,13 +2095,19 @@
   </si>
   <si>
     <t>Table keyed to the full english names of equipment pieces. Value is the number of items with that name in inventory.</t>
+  </si>
+  <si>
+    <t>//gs validate &lt;filter&gt;</t>
+  </si>
+  <si>
+    <t>This command checks to see whether the equipment in "sets" also exists in your inventory. &lt;filter&gt; is an optional list of words that restricts the output to only those items that contain text from one of the filter's words.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2282,7 +2282,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2317,7 +2316,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2493,14 +2491,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101:A144"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
@@ -2509,7 +2507,7 @@
     <col min="6" max="6" width="202.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="26.25">
       <c r="B1" s="6" t="s">
         <v>497</v>
       </c>
@@ -2524,9 +2522,9 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="14.45" customHeight="1">
       <c r="A3" s="13" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D3" t="s">
         <v>199</v>
@@ -2538,19 +2536,19 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="14.45" customHeight="1">
       <c r="A4" s="13"/>
       <c r="D4" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E4" t="s">
         <v>500</v>
       </c>
       <c r="F4" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1">
       <c r="A5" s="13"/>
       <c r="B5" t="s">
         <v>177</v>
@@ -2562,10 +2560,10 @@
         <v>500</v>
       </c>
       <c r="F5" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="13"/>
       <c r="B6" t="s">
         <v>178</v>
@@ -2577,10 +2575,10 @@
         <v>500</v>
       </c>
       <c r="F6" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="13"/>
       <c r="B7" t="s">
         <v>179</v>
@@ -2592,10 +2590,10 @@
         <v>500</v>
       </c>
       <c r="F7" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="13"/>
       <c r="D8" t="s">
         <v>181</v>
@@ -2604,10 +2602,10 @@
         <v>500</v>
       </c>
       <c r="F8" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="13"/>
       <c r="D9" t="s">
         <v>180</v>
@@ -2616,34 +2614,34 @@
         <v>500</v>
       </c>
       <c r="F9" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="13"/>
       <c r="D10" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E10" t="s">
         <v>500</v>
       </c>
       <c r="F10" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="13"/>
       <c r="D11" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="E11" t="s">
         <v>500</v>
       </c>
       <c r="F11" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="13"/>
       <c r="D12" t="s">
         <v>185</v>
@@ -2655,7 +2653,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="13"/>
       <c r="D13" t="s">
         <v>198</v>
@@ -2664,10 +2662,10 @@
         <v>500</v>
       </c>
       <c r="F13" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="12" t="s">
         <v>119</v>
       </c>
@@ -2675,31 +2673,31 @@
         <v>201</v>
       </c>
       <c r="D16" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="E16" t="s">
         <v>500</v>
       </c>
       <c r="F16" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="14.45" customHeight="1">
       <c r="A17" s="12"/>
       <c r="B17" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D17" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E17" t="s">
         <v>500</v>
       </c>
       <c r="F17" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="14.45" customHeight="1">
       <c r="A18" s="12"/>
       <c r="B18" t="s">
         <v>122</v>
@@ -2711,10 +2709,10 @@
         <v>500</v>
       </c>
       <c r="F18" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="14.45" customHeight="1">
       <c r="A19" s="12"/>
       <c r="B19" t="s">
         <v>121</v>
@@ -2726,7 +2724,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="12"/>
       <c r="B20" t="s">
         <v>123</v>
@@ -2738,10 +2736,10 @@
         <v>500</v>
       </c>
       <c r="F20" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="14.45" customHeight="1">
       <c r="A21" s="12"/>
       <c r="B21" t="s">
         <v>117</v>
@@ -2753,22 +2751,22 @@
         <v>500</v>
       </c>
       <c r="F21" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="14.45" customHeight="1">
       <c r="A22" s="12"/>
       <c r="D22" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="E22" t="s">
         <v>500</v>
       </c>
       <c r="F22" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" customHeight="1">
       <c r="A23" s="12"/>
       <c r="B23" t="s">
         <v>124</v>
@@ -2783,7 +2781,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" customHeight="1">
       <c r="A24" s="12"/>
       <c r="B24" t="s">
         <v>125</v>
@@ -2798,7 +2796,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15" customHeight="1">
       <c r="A25" s="12"/>
       <c r="B25" t="s">
         <v>129</v>
@@ -2813,10 +2811,10 @@
         <v>500</v>
       </c>
       <c r="F25" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15" customHeight="1">
       <c r="A26" s="12"/>
       <c r="B26" t="s">
         <v>130</v>
@@ -2828,10 +2826,10 @@
         <v>500</v>
       </c>
       <c r="F26" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15" customHeight="1">
       <c r="A27" s="12"/>
       <c r="B27" t="s">
         <v>137</v>
@@ -2846,7 +2844,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15" customHeight="1">
       <c r="A28" s="12"/>
       <c r="B28" t="s">
         <v>0</v>
@@ -2861,7 +2859,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15" customHeight="1">
       <c r="A29" s="12"/>
       <c r="B29" t="s">
         <v>0</v>
@@ -2876,7 +2874,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" customHeight="1">
       <c r="A30" s="12"/>
       <c r="B30" t="s">
         <v>0</v>
@@ -2891,7 +2889,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" customHeight="1">
       <c r="A31" s="12"/>
       <c r="B31" t="s">
         <v>0</v>
@@ -2903,31 +2901,31 @@
         <v>500</v>
       </c>
       <c r="F31" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="12"/>
       <c r="B32" t="s">
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="E32" t="s">
         <v>500</v>
       </c>
       <c r="F32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="14.45" customHeight="1">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="14.45" customHeight="1">
       <c r="A35" s="13" t="s">
         <v>141</v>
       </c>
@@ -2944,7 +2942,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15" customHeight="1">
       <c r="A36" s="13"/>
       <c r="B36" t="s">
         <v>0</v>
@@ -2959,13 +2957,13 @@
         <v>171</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="14.45" customHeight="1">
       <c r="A37" s="13"/>
       <c r="B37" t="s">
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E37" t="s">
         <v>140</v>
@@ -2974,13 +2972,13 @@
         <v>501</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="14.45" customHeight="1">
       <c r="A38" s="13"/>
       <c r="B38" t="s">
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E38" t="s">
         <v>140</v>
@@ -2989,52 +2987,52 @@
         <v>172</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="14.45" customHeight="1">
       <c r="A39" s="13"/>
       <c r="B39" t="s">
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E39" t="s">
         <v>140</v>
       </c>
       <c r="F39" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="14.45" customHeight="1">
       <c r="A40" s="13"/>
       <c r="B40" t="s">
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E40" t="s">
         <v>140</v>
       </c>
       <c r="F40" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="14.45" customHeight="1">
       <c r="A41" s="13"/>
       <c r="B41" t="s">
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E41" t="s">
         <v>500</v>
       </c>
       <c r="F41" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="14.45" customHeight="1">
       <c r="A42" s="13"/>
       <c r="B42" t="s">
         <v>0</v>
@@ -3049,7 +3047,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="14.45" customHeight="1">
       <c r="A43" s="13"/>
       <c r="B43" t="s">
         <v>0</v>
@@ -3064,7 +3062,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="14.45" customHeight="1">
       <c r="A44" s="13"/>
       <c r="B44" t="s">
         <v>0</v>
@@ -3079,7 +3077,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="14.45" customHeight="1">
       <c r="A45" s="13"/>
       <c r="B45" t="s">
         <v>0</v>
@@ -3094,13 +3092,13 @@
         <v>176</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="14.45" customHeight="1">
       <c r="A46" s="8"/>
     </row>
-    <row r="47" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="14.45" customHeight="1">
       <c r="A47" s="8"/>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="15" customHeight="1">
       <c r="A48" s="12" t="s">
         <v>187</v>
       </c>
@@ -3111,7 +3109,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="15" customHeight="1">
       <c r="A49" s="12"/>
       <c r="D49" t="s">
         <v>190</v>
@@ -3120,7 +3118,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="15" customHeight="1">
       <c r="A50" s="12"/>
       <c r="D50" t="s">
         <v>192</v>
@@ -3129,7 +3127,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="15" customHeight="1">
       <c r="A51" s="12"/>
       <c r="D51" t="s">
         <v>193</v>
@@ -3138,7 +3136,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="15" customHeight="1">
       <c r="A52" s="12"/>
       <c r="D52" t="s">
         <v>196</v>
@@ -3147,7 +3145,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="15" customHeight="1">
       <c r="A53" s="12"/>
       <c r="B53" t="s">
         <v>226</v>
@@ -3159,7 +3157,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="15" customHeight="1">
       <c r="A54" s="12"/>
       <c r="B54" t="s">
         <v>229</v>
@@ -3171,7 +3169,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="15" customHeight="1">
       <c r="A55" s="12"/>
       <c r="B55" t="s">
         <v>228</v>
@@ -3183,7 +3181,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="15" customHeight="1">
       <c r="A56" s="12"/>
       <c r="B56" t="s">
         <v>227</v>
@@ -3195,19 +3193,19 @@
         <v>225</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="14.45" customHeight="1">
       <c r="A57" s="12"/>
       <c r="D57" t="s">
-        <v>503</v>
+        <v>693</v>
       </c>
       <c r="F57" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="14.45" customHeight="1">
       <c r="A58" s="3"/>
     </row>
-    <row r="60" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="14.45" customHeight="1">
       <c r="A60" s="12" t="s">
         <v>1</v>
       </c>
@@ -3224,7 +3222,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="14.45" customHeight="1">
       <c r="A61" s="12"/>
       <c r="B61" t="s">
         <v>2</v>
@@ -3239,7 +3237,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="14.45" customHeight="1">
       <c r="A62" s="12"/>
       <c r="B62" t="s">
         <v>4</v>
@@ -3254,7 +3252,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="14.45" customHeight="1">
       <c r="A63" s="12"/>
       <c r="B63" t="s">
         <v>6</v>
@@ -3269,7 +3267,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="14.45" customHeight="1">
       <c r="A64" s="12"/>
       <c r="B64" t="s">
         <v>8</v>
@@ -3284,7 +3282,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="14.45" customHeight="1">
       <c r="A65" s="12"/>
       <c r="B65" t="s">
         <v>10</v>
@@ -3299,7 +3297,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="14.45" customHeight="1">
       <c r="A66" s="12"/>
       <c r="B66" t="s">
         <v>12</v>
@@ -3314,7 +3312,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="14.45" customHeight="1">
       <c r="A67" s="12"/>
       <c r="B67" t="s">
         <v>14</v>
@@ -3329,7 +3327,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="14.45" customHeight="1">
       <c r="A68" s="12"/>
       <c r="B68" t="s">
         <v>16</v>
@@ -3344,7 +3342,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="14.45" customHeight="1">
       <c r="A69" s="12"/>
       <c r="B69" t="s">
         <v>18</v>
@@ -3359,7 +3357,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="14.45" customHeight="1">
       <c r="A70" s="12"/>
       <c r="D70" t="s">
         <v>245</v>
@@ -3371,7 +3369,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="14.45" customHeight="1">
       <c r="A71" s="12"/>
       <c r="D71" t="s">
         <v>246</v>
@@ -3383,7 +3381,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="14.45" customHeight="1">
       <c r="A72" s="12"/>
       <c r="D72" t="s">
         <v>247</v>
@@ -3395,15 +3393,15 @@
         <v>249</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="14.45" customHeight="1">
       <c r="A73" s="3"/>
     </row>
-    <row r="74" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="14.45" customHeight="1">
       <c r="A74" s="3"/>
     </row>
-    <row r="75" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="14.45" customHeight="1">
       <c r="A75" s="12" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B75" t="s">
         <v>72</v>
@@ -3418,7 +3416,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="14.45" customHeight="1">
       <c r="A76" s="12"/>
       <c r="B76" t="s">
         <v>74</v>
@@ -3433,7 +3431,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="14.45" customHeight="1">
       <c r="A77" s="12"/>
       <c r="B77" t="s">
         <v>76</v>
@@ -3448,7 +3446,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="15" customHeight="1">
       <c r="A78" s="12"/>
       <c r="B78" t="s">
         <v>78</v>
@@ -3463,7 +3461,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="15" customHeight="1">
       <c r="A79" s="12"/>
       <c r="B79" t="s">
         <v>80</v>
@@ -3478,7 +3476,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="15" customHeight="1">
       <c r="A80" s="12"/>
       <c r="B80" t="s">
         <v>82</v>
@@ -3493,58 +3491,58 @@
         <v>276</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="14.25" customHeight="1">
       <c r="A81" s="12"/>
       <c r="D81" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E81" t="s">
         <v>264</v>
       </c>
       <c r="F81" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="14.45" customHeight="1">
       <c r="A82" s="12"/>
       <c r="D82" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E82" t="s">
         <v>263</v>
       </c>
       <c r="F82" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="14.45" customHeight="1">
       <c r="A83" s="12"/>
       <c r="D83" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="E83" t="s">
         <v>263</v>
       </c>
       <c r="F83" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="14.45" customHeight="1">
       <c r="A84" s="12"/>
       <c r="D84" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E84" t="s">
         <v>263</v>
       </c>
       <c r="F84" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="14.45" customHeight="1">
       <c r="A85" s="12"/>
       <c r="D85" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E85" t="s">
         <v>263</v>
@@ -3553,163 +3551,163 @@
         <v>362</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="14.45" customHeight="1">
       <c r="A86" s="12"/>
       <c r="D86" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E86" t="s">
         <v>138</v>
       </c>
       <c r="F86" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="14.45" customHeight="1">
       <c r="A87" s="12"/>
       <c r="D87" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="E87" t="s">
         <v>263</v>
       </c>
       <c r="F87" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="14.45" customHeight="1">
       <c r="A88" s="12"/>
       <c r="D88" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E88" t="s">
         <v>138</v>
       </c>
       <c r="F88" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="14.45" customHeight="1">
       <c r="A89" s="12"/>
       <c r="D89" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="E89" t="s">
         <v>263</v>
       </c>
       <c r="F89" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="14.45" customHeight="1">
       <c r="A90" s="12"/>
       <c r="D90" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E90" t="s">
         <v>263</v>
       </c>
       <c r="F90" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="14.45" customHeight="1">
       <c r="A91" s="12"/>
       <c r="D91" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E91" t="s">
         <v>263</v>
       </c>
       <c r="F91" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="14.45" customHeight="1">
       <c r="A92" s="12"/>
       <c r="D92" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E92" t="s">
         <v>263</v>
       </c>
       <c r="F92" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="14.45" customHeight="1">
       <c r="A93" s="12"/>
       <c r="D93" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="E93" t="s">
         <v>263</v>
       </c>
       <c r="F93" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="14.45" customHeight="1">
       <c r="A94" s="12"/>
       <c r="D94" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="E94" t="s">
         <v>263</v>
       </c>
       <c r="F94" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="14.45" customHeight="1">
       <c r="A95" s="12"/>
       <c r="D95" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E95" t="s">
         <v>263</v>
       </c>
       <c r="F95" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="14.45" customHeight="1">
       <c r="A96" s="12"/>
       <c r="D96" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E96" t="s">
         <v>263</v>
       </c>
       <c r="F96" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="14.45" customHeight="1">
       <c r="A97" s="12"/>
       <c r="D97" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E97" t="s">
         <v>263</v>
       </c>
       <c r="F97" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="14.45" customHeight="1">
       <c r="A98" s="12"/>
       <c r="D98" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E98" t="s">
         <v>263</v>
       </c>
       <c r="F98" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="14.45" customHeight="1">
       <c r="A101" s="12" t="s">
         <v>345</v>
       </c>
@@ -3726,19 +3724,19 @@
         <v>265</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="14.45" customHeight="1">
       <c r="A102" s="12"/>
       <c r="D102" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="E102" t="s">
         <v>138</v>
       </c>
       <c r="F102" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="14.45" customHeight="1">
       <c r="A103" s="12"/>
       <c r="B103" t="s">
         <v>22</v>
@@ -3753,7 +3751,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="14.45" customHeight="1">
       <c r="A104" s="12"/>
       <c r="B104" t="s">
         <v>26</v>
@@ -3768,7 +3766,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="14.45" customHeight="1">
       <c r="A105" s="12"/>
       <c r="B105" t="s">
         <v>28</v>
@@ -3783,7 +3781,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="14.45" customHeight="1">
       <c r="A106" s="12"/>
       <c r="B106" t="s">
         <v>30</v>
@@ -3798,7 +3796,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="14.45" customHeight="1">
       <c r="A107" s="12"/>
       <c r="B107" t="s">
         <v>32</v>
@@ -3813,7 +3811,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="14.45" customHeight="1">
       <c r="A108" s="12"/>
       <c r="B108" t="s">
         <v>33</v>
@@ -3828,7 +3826,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="14.45" customHeight="1">
       <c r="A109" s="12"/>
       <c r="B109" t="s">
         <v>36</v>
@@ -3843,7 +3841,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="14.45" customHeight="1">
       <c r="A110" s="12"/>
       <c r="B110" t="s">
         <v>38</v>
@@ -3858,7 +3856,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="14.45" customHeight="1">
       <c r="A111" s="12"/>
       <c r="D111" t="s">
         <v>326</v>
@@ -3870,7 +3868,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="14.45" customHeight="1">
       <c r="A112" s="12"/>
       <c r="B112" t="s">
         <v>40</v>
@@ -3885,7 +3883,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="14.45" customHeight="1">
       <c r="A113" s="12"/>
       <c r="D113" t="s">
         <v>328</v>
@@ -3897,7 +3895,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="14.45" customHeight="1">
       <c r="A114" s="12"/>
       <c r="B114" t="s">
         <v>41</v>
@@ -3912,7 +3910,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="14.45" customHeight="1">
       <c r="A115" s="12"/>
       <c r="D115" t="s">
         <v>330</v>
@@ -3924,7 +3922,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="14.45" customHeight="1">
       <c r="A116" s="12"/>
       <c r="B116" t="s">
         <v>42</v>
@@ -3939,7 +3937,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="14.45" customHeight="1">
       <c r="A117" s="12"/>
       <c r="D117" t="s">
         <v>331</v>
@@ -3951,7 +3949,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="14.45" customHeight="1">
       <c r="A118" s="12"/>
       <c r="B118" t="s">
         <v>43</v>
@@ -3966,7 +3964,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="14.45" customHeight="1">
       <c r="A119" s="12"/>
       <c r="B119" t="s">
         <v>49</v>
@@ -3981,7 +3979,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="14.45" customHeight="1">
       <c r="A120" s="12"/>
       <c r="B120" t="s">
         <v>51</v>
@@ -3996,7 +3994,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" ht="14.45" customHeight="1">
       <c r="A121" s="12"/>
       <c r="D121" t="s">
         <v>318</v>
@@ -4008,7 +4006,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" ht="14.45" customHeight="1">
       <c r="A122" s="12"/>
       <c r="D122" t="s">
         <v>320</v>
@@ -4020,7 +4018,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" ht="14.45" customHeight="1">
       <c r="A123" s="12"/>
       <c r="D123" t="s">
         <v>322</v>
@@ -4032,7 +4030,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" ht="14.45" customHeight="1">
       <c r="A124" s="12"/>
       <c r="D124" t="s">
         <v>324</v>
@@ -4044,7 +4042,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" ht="14.45" customHeight="1">
       <c r="A125" s="12"/>
       <c r="D125" t="s">
         <v>325</v>
@@ -4056,7 +4054,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="14.45" customHeight="1">
       <c r="A126" s="12"/>
       <c r="D126" t="s">
         <v>336</v>
@@ -4068,7 +4066,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="14.45" customHeight="1">
       <c r="A127" s="12"/>
       <c r="D127" t="s">
         <v>338</v>
@@ -4080,7 +4078,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" ht="14.45" customHeight="1">
       <c r="A128" s="12"/>
       <c r="D128" t="s">
         <v>339</v>
@@ -4092,7 +4090,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="14.45" customHeight="1">
       <c r="A129" s="12"/>
       <c r="D129" t="s">
         <v>342</v>
@@ -4104,7 +4102,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" ht="14.45" customHeight="1">
       <c r="A130" s="12"/>
       <c r="D130" t="s">
         <v>379</v>
@@ -4116,7 +4114,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" ht="14.45" customHeight="1">
       <c r="A131" s="12"/>
       <c r="D131" t="s">
         <v>380</v>
@@ -4128,7 +4126,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" ht="14.45" customHeight="1">
       <c r="A132" s="12"/>
       <c r="D132" t="s">
         <v>381</v>
@@ -4140,7 +4138,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" ht="14.45" customHeight="1">
       <c r="A133" s="12"/>
       <c r="D133" t="s">
         <v>426</v>
@@ -4152,19 +4150,19 @@
         <v>396</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" ht="14.45" customHeight="1">
       <c r="A134" s="12"/>
       <c r="D134" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E134" t="s">
         <v>263</v>
       </c>
       <c r="F134" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" ht="14.45" customHeight="1">
       <c r="A135" s="12"/>
       <c r="D135" t="s">
         <v>382</v>
@@ -4176,7 +4174,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" ht="14.45" customHeight="1">
       <c r="A136" s="12"/>
       <c r="D136" t="s">
         <v>383</v>
@@ -4188,7 +4186,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" ht="14.45" customHeight="1">
       <c r="A137" s="12"/>
       <c r="D137" t="s">
         <v>384</v>
@@ -4200,7 +4198,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" ht="14.45" customHeight="1">
       <c r="A138" s="12"/>
       <c r="D138" t="s">
         <v>385</v>
@@ -4212,7 +4210,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" ht="14.45" customHeight="1">
       <c r="A139" s="12"/>
       <c r="D139" t="s">
         <v>386</v>
@@ -4224,7 +4222,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" ht="14.45" customHeight="1">
       <c r="A140" s="12"/>
       <c r="D140" t="s">
         <v>387</v>
@@ -4236,61 +4234,61 @@
         <v>376</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" ht="14.45" customHeight="1">
       <c r="A141" s="12"/>
       <c r="D141" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="E141" t="s">
         <v>140</v>
       </c>
       <c r="F141" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" ht="14.45" customHeight="1">
       <c r="A142" s="12"/>
       <c r="D142" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E142" t="s">
         <v>140</v>
       </c>
       <c r="F142" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" ht="14.45" customHeight="1">
       <c r="A143" s="12"/>
       <c r="D143" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="E143" t="s">
         <v>140</v>
       </c>
       <c r="F143" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" ht="14.45" customHeight="1">
       <c r="A144" s="12"/>
       <c r="D144" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="E144" t="s">
         <v>140</v>
       </c>
       <c r="F144" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" ht="14.45" customHeight="1">
       <c r="A145" s="7"/>
     </row>
-    <row r="146" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" ht="14.45" customHeight="1">
       <c r="A146" s="7"/>
     </row>
-    <row r="147" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" ht="14.45" customHeight="1">
       <c r="A147" s="12" t="s">
         <v>344</v>
       </c>
@@ -4307,7 +4305,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" ht="14.45" customHeight="1">
       <c r="A148" s="12"/>
       <c r="B148" t="s">
         <v>95</v>
@@ -4322,7 +4320,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" ht="14.45" customHeight="1">
       <c r="A149" s="12"/>
       <c r="B149" t="s">
         <v>96</v>
@@ -4337,7 +4335,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" ht="14.45" customHeight="1">
       <c r="A150" s="12"/>
       <c r="B150" t="s">
         <v>97</v>
@@ -4352,7 +4350,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" ht="14.45" customHeight="1">
       <c r="A151" s="12"/>
       <c r="B151" t="s">
         <v>278</v>
@@ -4367,7 +4365,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" ht="14.45" customHeight="1">
       <c r="A152" s="12"/>
       <c r="B152" t="s">
         <v>279</v>
@@ -4382,7 +4380,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" ht="14.45" customHeight="1">
       <c r="A153" s="12"/>
       <c r="B153" t="s">
         <v>280</v>
@@ -4397,7 +4395,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" ht="14.45" customHeight="1">
       <c r="A154" s="12"/>
       <c r="B154" t="s">
         <v>281</v>
@@ -4412,7 +4410,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" ht="14.45" customHeight="1">
       <c r="A155" s="12"/>
       <c r="B155" t="s">
         <v>282</v>
@@ -4427,7 +4425,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" ht="14.45" customHeight="1">
       <c r="A156" s="12"/>
       <c r="B156" t="s">
         <v>283</v>
@@ -4442,7 +4440,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" ht="14.45" customHeight="1">
       <c r="A157" s="12"/>
       <c r="B157" t="s">
         <v>284</v>
@@ -4457,7 +4455,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" ht="14.45" customHeight="1">
       <c r="A158" s="12"/>
       <c r="B158" t="s">
         <v>285</v>
@@ -4472,7 +4470,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" ht="14.45" customHeight="1">
       <c r="A159" s="12"/>
       <c r="B159" t="s">
         <v>286</v>
@@ -4487,7 +4485,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="14.45" customHeight="1">
       <c r="A160" s="12"/>
       <c r="B160" t="s">
         <v>287</v>
@@ -4502,7 +4500,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" ht="14.45" customHeight="1">
       <c r="A161" s="12"/>
       <c r="B161" t="s">
         <v>288</v>
@@ -4517,7 +4515,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" ht="14.45" customHeight="1">
       <c r="A162" s="12"/>
       <c r="B162" t="s">
         <v>289</v>
@@ -4532,13 +4530,13 @@
         <v>291</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="14.45" customHeight="1">
       <c r="A163" s="3"/>
     </row>
-    <row r="164" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" ht="14.45" customHeight="1">
       <c r="A164" s="3"/>
     </row>
-    <row r="165" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" ht="14.45" customHeight="1">
       <c r="A165" s="12" t="s">
         <v>349</v>
       </c>
@@ -4555,7 +4553,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" ht="14.45" customHeight="1">
       <c r="A166" s="12"/>
       <c r="B166" t="s">
         <v>68</v>
@@ -4570,7 +4568,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" ht="14.45" customHeight="1">
       <c r="A167" s="12"/>
       <c r="B167" t="s">
         <v>69</v>
@@ -4585,7 +4583,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" ht="14.45" customHeight="1">
       <c r="A168" s="12"/>
       <c r="B168" t="s">
         <v>70</v>
@@ -4600,7 +4598,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" ht="14.45" customHeight="1">
       <c r="A169" s="12"/>
       <c r="B169" t="s">
         <v>71</v>
@@ -4615,7 +4613,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" ht="14.45" customHeight="1">
       <c r="A170" s="12"/>
       <c r="D170" t="s">
         <v>353</v>
@@ -4627,7 +4625,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" ht="14.45" customHeight="1">
       <c r="A171" s="12"/>
       <c r="D171" t="s">
         <v>360</v>
@@ -4639,7 +4637,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" ht="14.45" customHeight="1">
       <c r="A172" s="12"/>
       <c r="D172" t="s">
         <v>361</v>
@@ -4651,7 +4649,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" ht="14.45" customHeight="1">
       <c r="A173" s="12"/>
       <c r="D173" t="s">
         <v>352</v>
@@ -4663,7 +4661,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" ht="14.45" customHeight="1">
       <c r="A174" s="12"/>
       <c r="D174" t="s">
         <v>354</v>
@@ -4675,7 +4673,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" ht="14.45" customHeight="1">
       <c r="A175" s="12"/>
       <c r="D175" t="s">
         <v>355</v>
@@ -4687,7 +4685,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="14.45" customHeight="1">
       <c r="A176" s="12"/>
       <c r="D176" t="s">
         <v>425</v>
@@ -4699,31 +4697,31 @@
         <v>363</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" ht="14.45" customHeight="1">
       <c r="A177" s="12"/>
       <c r="D177" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="E177" t="s">
         <v>138</v>
       </c>
       <c r="F177" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" ht="14.45" customHeight="1">
       <c r="A178" s="12"/>
       <c r="D178" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E178" t="s">
         <v>263</v>
       </c>
       <c r="F178" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" ht="14.45" customHeight="1">
       <c r="A179" s="12"/>
       <c r="D179" t="s">
         <v>369</v>
@@ -4735,7 +4733,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" ht="14.45" customHeight="1">
       <c r="A180" s="12"/>
       <c r="D180" t="s">
         <v>370</v>
@@ -4747,7 +4745,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" ht="14.45" customHeight="1">
       <c r="A181" s="12"/>
       <c r="D181" t="s">
         <v>357</v>
@@ -4759,7 +4757,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" ht="14.45" customHeight="1">
       <c r="A182" s="12"/>
       <c r="D182" t="s">
         <v>358</v>
@@ -4771,7 +4769,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" ht="14.45" customHeight="1">
       <c r="A183" s="12"/>
       <c r="D183" t="s">
         <v>359</v>
@@ -4783,7 +4781,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" ht="14.45" customHeight="1">
       <c r="A184" s="12"/>
       <c r="D184" t="s">
         <v>351</v>
@@ -4795,7 +4793,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" ht="14.45" customHeight="1">
       <c r="A185" s="12"/>
       <c r="D185" t="s">
         <v>356</v>
@@ -4807,7 +4805,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" ht="14.45" customHeight="1">
       <c r="A186" s="12"/>
       <c r="D186" t="s">
         <v>367</v>
@@ -4819,7 +4817,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" ht="14.45" customHeight="1">
       <c r="A187" s="12"/>
       <c r="D187" t="s">
         <v>377</v>
@@ -4831,30 +4829,30 @@
         <v>378</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" ht="14.45" customHeight="1">
       <c r="A188" s="10"/>
     </row>
-    <row r="189" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" ht="14.45" customHeight="1">
       <c r="A189" s="3"/>
     </row>
-    <row r="190" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" ht="21" customHeight="1">
       <c r="A190" s="12" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D190" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E190" t="s">
         <v>138</v>
       </c>
       <c r="F190" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6">
       <c r="A191" s="12"/>
       <c r="D191" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="E191" t="s">
         <v>138</v>
@@ -4863,94 +4861,94 @@
         <v>261</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6">
       <c r="A192" s="12"/>
       <c r="D192" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E192" t="s">
         <v>263</v>
       </c>
       <c r="F192" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6">
       <c r="A193" s="12"/>
       <c r="D193" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="E193" t="s">
         <v>263</v>
       </c>
       <c r="F193" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6">
       <c r="A194" s="12"/>
       <c r="D194" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="E194" t="s">
         <v>264</v>
       </c>
       <c r="F194" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6">
       <c r="A195" s="12"/>
       <c r="D195" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E195" t="s">
         <v>264</v>
       </c>
       <c r="F195" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6">
       <c r="A196" s="12"/>
       <c r="D196" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="E196" t="s">
         <v>263</v>
       </c>
       <c r="F196" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6">
       <c r="A197" s="12"/>
       <c r="D197" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E197" t="s">
         <v>263</v>
       </c>
       <c r="F197" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6">
       <c r="A198" s="12"/>
       <c r="D198" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E198" t="s">
         <v>263</v>
       </c>
       <c r="F198" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6">
       <c r="A199" s="12"/>
       <c r="D199" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="E199" t="s">
         <v>263</v>
@@ -4959,154 +4957,154 @@
         <v>362</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6">
       <c r="A200" s="12"/>
       <c r="D200" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E200" t="s">
         <v>138</v>
       </c>
       <c r="F200" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6">
       <c r="A201" s="12"/>
       <c r="D201" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="E201" t="s">
         <v>263</v>
       </c>
       <c r="F201" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6">
       <c r="A202" s="12"/>
       <c r="D202" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="E202" t="s">
         <v>138</v>
       </c>
       <c r="F202" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6">
       <c r="A203" s="12"/>
       <c r="D203" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="E203" t="s">
         <v>263</v>
       </c>
       <c r="F203" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6">
       <c r="A204" s="12"/>
       <c r="D204" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="E204" t="s">
         <v>263</v>
       </c>
       <c r="F204" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6">
       <c r="A205" s="12"/>
       <c r="D205" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="E205" t="s">
         <v>263</v>
       </c>
       <c r="F205" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6">
       <c r="A206" s="12"/>
       <c r="D206" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="E206" t="s">
         <v>263</v>
       </c>
       <c r="F206" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6">
       <c r="A207" s="12"/>
       <c r="D207" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="E207" t="s">
         <v>263</v>
       </c>
       <c r="F207" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6">
       <c r="A208" s="12"/>
       <c r="D208" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="E208" t="s">
         <v>263</v>
       </c>
       <c r="F208" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6">
       <c r="A209" s="12"/>
       <c r="D209" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="E209" t="s">
         <v>263</v>
       </c>
       <c r="F209" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6">
       <c r="A210" s="12"/>
       <c r="D210" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="E210" t="s">
         <v>263</v>
       </c>
       <c r="F210" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6">
       <c r="A211" s="12"/>
       <c r="D211" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E211" t="s">
         <v>263</v>
       </c>
       <c r="F211" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6">
       <c r="A212" s="12"/>
       <c r="D212" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E212" t="s">
         <v>263</v>
@@ -5115,13 +5113,13 @@
         <v>412</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6">
       <c r="A213" s="11"/>
     </row>
-    <row r="214" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" ht="14.45" customHeight="1">
       <c r="A214" s="3"/>
     </row>
-    <row r="215" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" ht="14.45" customHeight="1">
       <c r="A215" s="12" t="s">
         <v>350</v>
       </c>
@@ -5135,7 +5133,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="216" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" ht="14.45" customHeight="1">
       <c r="A216" s="12"/>
       <c r="D216" t="s">
         <v>90</v>
@@ -5147,7 +5145,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="217" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" ht="14.45" customHeight="1">
       <c r="A217" s="12"/>
       <c r="D217" t="s">
         <v>91</v>
@@ -5159,7 +5157,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="218" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" ht="14.45" customHeight="1">
       <c r="A218" s="12"/>
       <c r="D218" t="s">
         <v>92</v>
@@ -5171,7 +5169,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="219" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" ht="14.45" customHeight="1">
       <c r="A219" s="12"/>
       <c r="D219" t="s">
         <v>93</v>
@@ -5183,7 +5181,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="220" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" ht="14.45" customHeight="1">
       <c r="A220" s="12"/>
       <c r="D220" t="s">
         <v>393</v>
@@ -5195,7 +5193,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="221" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" ht="14.45" customHeight="1">
       <c r="A221" s="12"/>
       <c r="D221" t="s">
         <v>398</v>
@@ -5207,7 +5205,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="222" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" ht="14.45" customHeight="1">
       <c r="A222" s="12"/>
       <c r="D222" t="s">
         <v>399</v>
@@ -5219,7 +5217,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="223" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" ht="14.45" customHeight="1">
       <c r="A223" s="12"/>
       <c r="D223" t="s">
         <v>400</v>
@@ -5228,10 +5226,10 @@
         <v>263</v>
       </c>
       <c r="F223" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" ht="14.45" customHeight="1">
       <c r="A224" s="12"/>
       <c r="D224" t="s">
         <v>401</v>
@@ -5243,7 +5241,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="225" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" ht="14.45" customHeight="1">
       <c r="A225" s="12"/>
       <c r="D225" t="s">
         <v>402</v>
@@ -5252,10 +5250,10 @@
         <v>138</v>
       </c>
       <c r="F225" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" ht="14.45" customHeight="1">
       <c r="A226" s="12"/>
       <c r="D226" t="s">
         <v>424</v>
@@ -5264,34 +5262,34 @@
         <v>263</v>
       </c>
       <c r="F226" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" ht="14.45" customHeight="1">
       <c r="A227" s="12"/>
       <c r="D227" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E227" t="s">
         <v>138</v>
       </c>
       <c r="F227" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" ht="14.45" customHeight="1">
       <c r="A228" s="12"/>
       <c r="D228" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="E228" t="s">
         <v>263</v>
       </c>
       <c r="F228" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" ht="14.45" customHeight="1">
       <c r="A229" s="12"/>
       <c r="D229" t="s">
         <v>403</v>
@@ -5303,7 +5301,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="230" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" ht="14.45" customHeight="1">
       <c r="A230" s="12"/>
       <c r="D230" t="s">
         <v>404</v>
@@ -5315,7 +5313,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" ht="14.45" customHeight="1">
       <c r="A231" s="12"/>
       <c r="D231" t="s">
         <v>405</v>
@@ -5327,7 +5325,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" ht="14.45" customHeight="1">
       <c r="A232" s="12"/>
       <c r="D232" t="s">
         <v>406</v>
@@ -5339,7 +5337,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="233" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" ht="14.45" customHeight="1">
       <c r="A233" s="12"/>
       <c r="D233" t="s">
         <v>407</v>
@@ -5351,7 +5349,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="234" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" ht="14.45" customHeight="1">
       <c r="A234" s="12"/>
       <c r="D234" t="s">
         <v>408</v>
@@ -5363,7 +5361,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="235" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" ht="14.45" customHeight="1">
       <c r="A235" s="12"/>
       <c r="D235" t="s">
         <v>409</v>
@@ -5375,7 +5373,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="236" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" ht="14.45" customHeight="1">
       <c r="A236" s="12"/>
       <c r="D236" t="s">
         <v>410</v>
@@ -5387,7 +5385,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="237" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" ht="14.45" customHeight="1">
       <c r="A237" s="12"/>
       <c r="D237" t="s">
         <v>411</v>
@@ -5399,10 +5397,10 @@
         <v>412</v>
       </c>
     </row>
-    <row r="238" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" ht="14.45" customHeight="1">
       <c r="A238" s="3"/>
     </row>
-    <row r="240" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" ht="14.45" customHeight="1">
       <c r="A240" s="12" t="s">
         <v>346</v>
       </c>
@@ -5419,7 +5417,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="241" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" ht="14.45" customHeight="1">
       <c r="A241" s="12"/>
       <c r="B241" t="s">
         <v>100</v>
@@ -5434,7 +5432,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="242" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" ht="14.45" customHeight="1">
       <c r="A242" s="12"/>
       <c r="B242" t="s">
         <v>102</v>
@@ -5449,7 +5447,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="243" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" ht="14.45" customHeight="1">
       <c r="A243" s="12"/>
       <c r="B243" t="s">
         <v>104</v>
@@ -5464,7 +5462,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="244" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" ht="14.45" customHeight="1">
       <c r="A244" s="12"/>
       <c r="B244" t="s">
         <v>108</v>
@@ -5479,7 +5477,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="245" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" ht="14.45" customHeight="1">
       <c r="A245" s="12"/>
       <c r="B245" t="s">
         <v>106</v>
@@ -5491,7 +5489,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="246" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" ht="14.45" customHeight="1">
       <c r="A246" s="12"/>
       <c r="D246" t="s">
         <v>432</v>
@@ -5503,7 +5501,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="247" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" ht="14.45" customHeight="1">
       <c r="A247" s="12"/>
       <c r="D247" t="s">
         <v>433</v>
@@ -5515,7 +5513,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="248" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" ht="14.45" customHeight="1">
       <c r="A248" s="12"/>
       <c r="D248" t="s">
         <v>434</v>
@@ -5527,31 +5525,31 @@
         <v>451</v>
       </c>
     </row>
-    <row r="249" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" ht="14.45" customHeight="1">
       <c r="A249" s="12"/>
       <c r="D249" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E249" t="s">
         <v>138</v>
       </c>
       <c r="F249" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="250" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" ht="14.45" customHeight="1">
       <c r="A250" s="12"/>
       <c r="D250" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E250" t="s">
         <v>263</v>
       </c>
       <c r="F250" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" ht="14.45" customHeight="1">
       <c r="A251" s="12"/>
       <c r="D251" t="s">
         <v>435</v>
@@ -5563,7 +5561,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="252" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" ht="14.45" customHeight="1">
       <c r="A252" s="12"/>
       <c r="D252" t="s">
         <v>436</v>
@@ -5575,7 +5573,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="253" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" ht="14.45" customHeight="1">
       <c r="A253" s="12"/>
       <c r="D253" t="s">
         <v>437</v>
@@ -5587,7 +5585,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="254" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" ht="14.45" customHeight="1">
       <c r="A254" s="12"/>
       <c r="D254" t="s">
         <v>438</v>
@@ -5599,7 +5597,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="255" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" ht="14.45" customHeight="1">
       <c r="A255" s="12"/>
       <c r="D255" t="s">
         <v>439</v>
@@ -5611,7 +5609,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="256" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" ht="14.45" customHeight="1">
       <c r="A256" s="12"/>
       <c r="D256" t="s">
         <v>440</v>
@@ -5623,7 +5621,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="257" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" ht="14.45" customHeight="1">
       <c r="A257" s="12"/>
       <c r="D257" t="s">
         <v>441</v>
@@ -5635,7 +5633,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="258" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6" ht="14.45" customHeight="1">
       <c r="A258" s="12"/>
       <c r="D258" t="s">
         <v>442</v>
@@ -5647,34 +5645,34 @@
         <v>443</v>
       </c>
     </row>
-    <row r="259" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" ht="14.45" customHeight="1">
       <c r="A259" s="12"/>
       <c r="D259" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="F259" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="260" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" ht="14.45" customHeight="1">
       <c r="A260" s="12"/>
       <c r="D260" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="E260" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="261" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" ht="14.45" customHeight="1">
       <c r="A261" s="12"/>
       <c r="D261" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="E261" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="262" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" ht="14.45" customHeight="1">
       <c r="A262" s="12"/>
       <c r="D262" t="s">
         <v>429</v>
@@ -5683,301 +5681,301 @@
         <v>263</v>
       </c>
     </row>
-    <row r="263" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6" ht="14.45" customHeight="1">
       <c r="A263" s="12"/>
       <c r="D263" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="E263" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6">
       <c r="A264" s="12"/>
       <c r="D264" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="E264" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6">
       <c r="A265" s="12"/>
       <c r="D265" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="E265" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6">
       <c r="A266" s="12"/>
       <c r="D266" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="E266" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6">
       <c r="A267" s="12"/>
       <c r="D267" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="E267" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6">
       <c r="A268" s="12"/>
       <c r="D268" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="E268" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6">
       <c r="A269" s="12"/>
       <c r="D269" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="E269" t="s">
         <v>263</v>
       </c>
       <c r="F269" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6">
       <c r="A270" s="12"/>
       <c r="D270" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="E270" t="s">
         <v>263</v>
       </c>
       <c r="F270" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6">
       <c r="A271" s="12"/>
       <c r="D271" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="E271" t="s">
         <v>263</v>
       </c>
       <c r="F271" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6">
       <c r="A272" s="12"/>
       <c r="D272" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="E272" t="s">
         <v>263</v>
       </c>
       <c r="F272" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6">
       <c r="A273" s="12"/>
       <c r="D273" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="E273" t="s">
         <v>263</v>
       </c>
       <c r="F273" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6">
       <c r="A274" s="12"/>
       <c r="D274" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="E274" t="s">
         <v>263</v>
       </c>
       <c r="F274" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6">
       <c r="A275" s="12"/>
       <c r="D275" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="E275" t="s">
         <v>263</v>
       </c>
       <c r="F275" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6">
       <c r="A276" s="12"/>
       <c r="D276" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="E276" t="s">
         <v>263</v>
       </c>
       <c r="F276" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6">
       <c r="A277" s="12"/>
       <c r="D277" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="E277" t="s">
         <v>263</v>
       </c>
       <c r="F277" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6">
       <c r="A278" s="12"/>
       <c r="D278" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="E278" t="s">
         <v>263</v>
       </c>
       <c r="F278" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6">
       <c r="A279" s="12"/>
       <c r="D279" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="E279" t="s">
         <v>263</v>
       </c>
       <c r="F279" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6">
       <c r="A280" s="12"/>
       <c r="D280" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="E280" t="s">
         <v>263</v>
       </c>
       <c r="F280" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6">
       <c r="A281" s="12"/>
       <c r="D281" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="E281" t="s">
         <v>263</v>
       </c>
       <c r="F281" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6">
       <c r="A282" s="12"/>
       <c r="D282" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="E282" t="s">
         <v>263</v>
       </c>
       <c r="F282" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6">
       <c r="A283" s="12"/>
       <c r="D283" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="E283" t="s">
         <v>138</v>
       </c>
       <c r="F283" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6">
       <c r="A284" s="12"/>
       <c r="D284" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="E284" t="s">
         <v>138</v>
       </c>
       <c r="F284" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6">
       <c r="A285" s="12"/>
       <c r="D285" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="E285" t="s">
         <v>140</v>
       </c>
       <c r="F285" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6">
       <c r="A286" s="12"/>
       <c r="D286" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="E286" t="s">
         <v>140</v>
       </c>
       <c r="F286" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6">
       <c r="A287" s="12"/>
       <c r="D287" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="E287" t="s">
         <v>140</v>
       </c>
       <c r="F287" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6">
       <c r="A288" s="12"/>
       <c r="D288" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="E288" t="s">
         <v>140</v>
       </c>
       <c r="F288" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="291" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" ht="14.45" customHeight="1">
       <c r="A291" s="12" t="s">
         <v>347</v>
       </c>
@@ -5994,7 +5992,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="292" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" ht="14.45" customHeight="1">
       <c r="A292" s="12"/>
       <c r="B292" t="s">
         <v>110</v>
@@ -6009,7 +6007,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="293" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" ht="14.45" customHeight="1">
       <c r="A293" s="12"/>
       <c r="B293" t="s">
         <v>111</v>
@@ -6024,7 +6022,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="294" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" ht="14.45" customHeight="1">
       <c r="A294" s="12"/>
       <c r="D294" t="s">
         <v>454</v>
@@ -6036,7 +6034,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="295" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" ht="14.45" customHeight="1">
       <c r="A295" s="12"/>
       <c r="D295" t="s">
         <v>455</v>
@@ -6048,7 +6046,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="296" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" ht="14.45" customHeight="1">
       <c r="A296" s="12"/>
       <c r="D296" t="s">
         <v>456</v>
@@ -6060,7 +6058,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="297" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" ht="14.45" customHeight="1">
       <c r="A297" s="12"/>
       <c r="D297" t="s">
         <v>457</v>
@@ -6072,7 +6070,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="298" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" ht="14.45" customHeight="1">
       <c r="A298" s="12"/>
       <c r="D298" t="s">
         <v>459</v>
@@ -6081,7 +6079,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="299" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" ht="14.45" customHeight="1">
       <c r="A299" s="12"/>
       <c r="D299" t="s">
         <v>458</v>
@@ -6093,31 +6091,31 @@
         <v>476</v>
       </c>
     </row>
-    <row r="300" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" ht="14.45" customHeight="1">
       <c r="A300" s="12"/>
       <c r="D300" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E300" t="s">
         <v>138</v>
       </c>
       <c r="F300" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="301" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" ht="14.45" customHeight="1">
       <c r="A301" s="12"/>
       <c r="D301" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E301" t="s">
         <v>263</v>
       </c>
       <c r="F301" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="302" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" ht="14.45" customHeight="1">
       <c r="A302" s="12"/>
       <c r="D302" t="s">
         <v>460</v>
@@ -6129,7 +6127,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="303" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6" ht="14.45" customHeight="1">
       <c r="A303" s="12"/>
       <c r="D303" t="s">
         <v>461</v>
@@ -6141,7 +6139,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="304" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" ht="14.45" customHeight="1">
       <c r="A304" s="12"/>
       <c r="D304" t="s">
         <v>462</v>
@@ -6153,7 +6151,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="305" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" ht="14.45" customHeight="1">
       <c r="A305" s="12"/>
       <c r="D305" t="s">
         <v>463</v>
@@ -6165,7 +6163,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="306" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" ht="14.45" customHeight="1">
       <c r="A306" s="12"/>
       <c r="D306" t="s">
         <v>464</v>
@@ -6177,7 +6175,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="307" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" ht="14.45" customHeight="1">
       <c r="A307" s="12"/>
       <c r="D307" t="s">
         <v>465</v>
@@ -6189,7 +6187,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="308" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" ht="14.45" customHeight="1">
       <c r="A308" s="12"/>
       <c r="D308" t="s">
         <v>466</v>
@@ -6201,7 +6199,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="309" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" ht="14.45" customHeight="1">
       <c r="A309" s="12"/>
       <c r="D309" t="s">
         <v>467</v>
@@ -6213,7 +6211,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="312" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6" ht="14.45" customHeight="1">
       <c r="A312" s="12" t="s">
         <v>490</v>
       </c>
@@ -6230,7 +6228,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="313" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" ht="14.45" customHeight="1">
       <c r="A313" s="12"/>
       <c r="D313" t="s">
         <v>155</v>
@@ -6242,7 +6240,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="314" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" ht="14.45" customHeight="1">
       <c r="A314" s="12"/>
       <c r="D314" t="s">
         <v>158</v>
@@ -6254,7 +6252,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="315" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" ht="14.45" customHeight="1">
       <c r="A315" s="12"/>
       <c r="D315" t="s">
         <v>159</v>
@@ -6266,7 +6264,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="316" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1">
       <c r="A316" s="12"/>
       <c r="D316" s="9" t="s">
         <v>489</v>
@@ -6278,7 +6276,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="317" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1">
       <c r="A317" s="12"/>
       <c r="D317" s="9" t="s">
         <v>491</v>
@@ -6290,13 +6288,13 @@
         <v>502</v>
       </c>
     </row>
-    <row r="318" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1">
       <c r="A318" s="3"/>
     </row>
-    <row r="319" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" s="9" customFormat="1">
       <c r="A319" s="2"/>
     </row>
-    <row r="321" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6" ht="14.45" customHeight="1">
       <c r="A321" s="12" t="s">
         <v>348</v>
       </c>
@@ -6313,7 +6311,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="322" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6" ht="14.45" customHeight="1">
       <c r="A322" s="12"/>
       <c r="B322" t="s">
         <v>53</v>
@@ -6328,7 +6326,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="323" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6" ht="14.45" customHeight="1">
       <c r="A323" s="12"/>
       <c r="B323" t="s">
         <v>55</v>
@@ -6343,7 +6341,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="324" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:6" ht="14.45" customHeight="1">
       <c r="A324" s="12"/>
       <c r="B324" t="s">
         <v>58</v>
@@ -6358,7 +6356,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="325" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" ht="14.45" customHeight="1">
       <c r="A325" s="12"/>
       <c r="D325" t="s">
         <v>492</v>
@@ -6370,7 +6368,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="326" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:6" ht="14.45" customHeight="1">
       <c r="A326" s="12"/>
       <c r="B326" t="s">
         <v>59</v>
@@ -6385,7 +6383,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="327" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:6" ht="14.45" customHeight="1">
       <c r="A327" s="12"/>
       <c r="B327" t="s">
         <v>61</v>
@@ -6400,7 +6398,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="328" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:6" ht="14.45" customHeight="1">
       <c r="A328" s="12"/>
       <c r="B328" t="s">
         <v>63</v>
@@ -6415,7 +6413,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="329" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:6" ht="14.45" customHeight="1">
       <c r="A329" s="12"/>
       <c r="B329" t="s">
         <v>64</v>
@@ -6430,7 +6428,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="330" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6" ht="14.45" customHeight="1">
       <c r="A330" s="12"/>
       <c r="D330" t="s">
         <v>493</v>
@@ -6442,7 +6440,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="331" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:6" ht="14.45" customHeight="1">
       <c r="A331" s="12"/>
       <c r="D331" t="s">
         <v>494</v>
@@ -6454,7 +6452,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="332" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:6" ht="14.45" customHeight="1">
       <c r="A332" s="12"/>
       <c r="D332" t="s">
         <v>495</v>
@@ -6466,7 +6464,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="335" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:6" ht="21">
       <c r="A335" s="4" t="s">
         <v>120</v>
       </c>
@@ -6483,7 +6481,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="338" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:6" ht="14.45" customHeight="1">
       <c r="A338" s="12" t="s">
         <v>127</v>
       </c>
@@ -6497,7 +6495,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="339" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:6" ht="14.45" customHeight="1">
       <c r="A339" s="12"/>
       <c r="B339" t="s">
         <v>116</v>
@@ -6509,7 +6507,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="340" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:6" ht="14.45" customHeight="1">
       <c r="A340" s="12"/>
       <c r="B340" t="s">
         <v>118</v>
@@ -6521,7 +6519,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="341" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:6" ht="14.45" customHeight="1">
       <c r="A341" s="12"/>
       <c r="B341" t="s">
         <v>128</v>
@@ -6533,7 +6531,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="342" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:6" ht="14.45" customHeight="1">
       <c r="A342" s="12"/>
       <c r="B342" t="s">
         <v>121</v>
@@ -6545,10 +6543,10 @@
         <v>230</v>
       </c>
     </row>
-    <row r="343" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:6" ht="14.45" customHeight="1">
       <c r="A343" s="3"/>
     </row>
-    <row r="344" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:6" ht="14.45" customHeight="1">
       <c r="A344" s="3"/>
     </row>
   </sheetData>
@@ -6576,24 +6574,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rewrite refresh_item_list to better handle short vs long name lookups. Update documentation on player.inventory et al.
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variables.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
@@ -2094,9 +2094,6 @@
     <t>player.case</t>
   </si>
   <si>
-    <t>Table keyed to the full english names of equipment pieces. Value is the number of items with that name in inventory.</t>
-  </si>
-  <si>
     <t>//gs validate &lt;filter&gt;</t>
   </si>
   <si>
@@ -2107,13 +2104,16 @@
   </si>
   <si>
     <t>Returns true or false based on whether or not your pet is in the middle of an action (for pets, between midcast and aftercast.)</t>
+  </si>
+  <si>
+    <t>Table keyed with the name of equipment pieces.  Keys for both short name and long name exist, if applicable.  Value is a table containing containing item id, count, short name (shortname), and optionally long name (longname).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2288,7 +2288,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2323,7 +2322,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2499,14 +2497,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
@@ -2515,7 +2513,7 @@
     <col min="6" max="6" width="202.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="26.25">
       <c r="B1" s="6" t="s">
         <v>497</v>
       </c>
@@ -2530,7 +2528,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="14.45" customHeight="1">
       <c r="A3" s="13" t="s">
         <v>615</v>
       </c>
@@ -2544,7 +2542,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="14.45" customHeight="1">
       <c r="A4" s="13"/>
       <c r="D4" t="s">
         <v>616</v>
@@ -2556,7 +2554,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1">
       <c r="A5" s="13"/>
       <c r="B5" t="s">
         <v>177</v>
@@ -2571,7 +2569,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="13"/>
       <c r="B6" t="s">
         <v>178</v>
@@ -2586,7 +2584,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="13"/>
       <c r="B7" t="s">
         <v>179</v>
@@ -2601,7 +2599,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="13"/>
       <c r="D8" t="s">
         <v>181</v>
@@ -2613,7 +2611,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="13"/>
       <c r="D9" t="s">
         <v>180</v>
@@ -2625,7 +2623,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="13"/>
       <c r="D10" t="s">
         <v>508</v>
@@ -2637,7 +2635,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="13"/>
       <c r="D11" t="s">
         <v>623</v>
@@ -2649,7 +2647,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="13"/>
       <c r="D12" t="s">
         <v>185</v>
@@ -2661,7 +2659,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="13"/>
       <c r="D13" t="s">
         <v>198</v>
@@ -2673,7 +2671,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>119</v>
       </c>
@@ -2690,7 +2688,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="14.45" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" t="s">
         <v>510</v>
@@ -2705,7 +2703,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="14.45" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" t="s">
         <v>122</v>
@@ -2720,7 +2718,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="14.45" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" t="s">
         <v>121</v>
@@ -2732,7 +2730,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="3"/>
       <c r="B20" t="s">
         <v>123</v>
@@ -2747,7 +2745,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="14.45" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
         <v>117</v>
@@ -2762,7 +2760,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="14.45" customHeight="1">
       <c r="A22" s="3"/>
       <c r="D22" t="s">
         <v>610</v>
@@ -2774,19 +2772,19 @@
         <v>635</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="14.45" customHeight="1">
       <c r="A23" s="3"/>
       <c r="D23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E23" t="s">
         <v>500</v>
       </c>
       <c r="F23" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" t="s">
         <v>124</v>
@@ -2801,7 +2799,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" t="s">
         <v>125</v>
@@ -2816,7 +2814,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15" customHeight="1">
       <c r="A26" s="3"/>
       <c r="B26" t="s">
         <v>129</v>
@@ -2834,7 +2832,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" t="s">
         <v>130</v>
@@ -2849,7 +2847,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" t="s">
         <v>137</v>
@@ -2864,7 +2862,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15" customHeight="1">
       <c r="A29" s="3"/>
       <c r="B29" t="s">
         <v>0</v>
@@ -2879,7 +2877,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" t="s">
         <v>0</v>
@@ -2894,7 +2892,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" customHeight="1">
       <c r="A31" s="3"/>
       <c r="B31" t="s">
         <v>0</v>
@@ -2909,7 +2907,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15" customHeight="1">
       <c r="A32" s="3"/>
       <c r="B32" t="s">
         <v>0</v>
@@ -2924,7 +2922,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" t="s">
         <v>0</v>
@@ -2939,13 +2937,13 @@
         <v>631</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="14.45" customHeight="1">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="14.45" customHeight="1">
       <c r="A36" s="13" t="s">
         <v>141</v>
       </c>
@@ -2962,7 +2960,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="15" customHeight="1">
       <c r="A37" s="13"/>
       <c r="B37" t="s">
         <v>0</v>
@@ -2977,7 +2975,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="14.45" customHeight="1">
       <c r="A38" s="13"/>
       <c r="B38" t="s">
         <v>0</v>
@@ -2992,7 +2990,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="14.45" customHeight="1">
       <c r="A39" s="13"/>
       <c r="B39" t="s">
         <v>0</v>
@@ -3007,7 +3005,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="14.45" customHeight="1">
       <c r="A40" s="13"/>
       <c r="B40" t="s">
         <v>0</v>
@@ -3022,7 +3020,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="14.45" customHeight="1">
       <c r="A41" s="13"/>
       <c r="B41" t="s">
         <v>0</v>
@@ -3037,7 +3035,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="14.45" customHeight="1">
       <c r="A42" s="13"/>
       <c r="B42" t="s">
         <v>0</v>
@@ -3052,7 +3050,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="14.45" customHeight="1">
       <c r="A43" s="13"/>
       <c r="B43" t="s">
         <v>0</v>
@@ -3067,7 +3065,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="14.45" customHeight="1">
       <c r="A44" s="13"/>
       <c r="B44" t="s">
         <v>0</v>
@@ -3082,7 +3080,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="14.45" customHeight="1">
       <c r="A45" s="13"/>
       <c r="B45" t="s">
         <v>0</v>
@@ -3097,7 +3095,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="14.45" customHeight="1">
       <c r="A46" s="13"/>
       <c r="B46" t="s">
         <v>0</v>
@@ -3112,13 +3110,13 @@
         <v>176</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="14.45" customHeight="1">
       <c r="A47" s="8"/>
     </row>
-    <row r="48" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="14.45" customHeight="1">
       <c r="A48" s="8"/>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="15" customHeight="1">
       <c r="A49" s="12" t="s">
         <v>187</v>
       </c>
@@ -3129,7 +3127,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="15" customHeight="1">
       <c r="A50" s="12"/>
       <c r="D50" t="s">
         <v>190</v>
@@ -3138,7 +3136,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="15" customHeight="1">
       <c r="A51" s="12"/>
       <c r="D51" t="s">
         <v>192</v>
@@ -3147,7 +3145,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="15" customHeight="1">
       <c r="A52" s="12"/>
       <c r="D52" t="s">
         <v>193</v>
@@ -3156,7 +3154,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="15" customHeight="1">
       <c r="A53" s="12"/>
       <c r="D53" t="s">
         <v>196</v>
@@ -3165,7 +3163,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="15" customHeight="1">
       <c r="A54" s="12"/>
       <c r="B54" t="s">
         <v>226</v>
@@ -3177,7 +3175,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="15" customHeight="1">
       <c r="A55" s="12"/>
       <c r="B55" t="s">
         <v>229</v>
@@ -3189,7 +3187,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="15" customHeight="1">
       <c r="A56" s="12"/>
       <c r="B56" t="s">
         <v>228</v>
@@ -3201,7 +3199,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="15" customHeight="1">
       <c r="A57" s="12"/>
       <c r="B57" t="s">
         <v>227</v>
@@ -3213,19 +3211,19 @@
         <v>225</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="14.45" customHeight="1">
       <c r="A58" s="12"/>
       <c r="D58" t="s">
+        <v>692</v>
+      </c>
+      <c r="F58" t="s">
         <v>693</v>
       </c>
-      <c r="F58" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:6" ht="14.45" customHeight="1">
       <c r="A59" s="3"/>
     </row>
-    <row r="61" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="14.45" customHeight="1">
       <c r="A61" s="12" t="s">
         <v>1</v>
       </c>
@@ -3242,7 +3240,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="14.45" customHeight="1">
       <c r="A62" s="12"/>
       <c r="B62" t="s">
         <v>2</v>
@@ -3257,7 +3255,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="14.45" customHeight="1">
       <c r="A63" s="12"/>
       <c r="B63" t="s">
         <v>4</v>
@@ -3272,7 +3270,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="14.45" customHeight="1">
       <c r="A64" s="12"/>
       <c r="B64" t="s">
         <v>6</v>
@@ -3287,7 +3285,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="14.45" customHeight="1">
       <c r="A65" s="12"/>
       <c r="B65" t="s">
         <v>8</v>
@@ -3302,7 +3300,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="14.45" customHeight="1">
       <c r="A66" s="12"/>
       <c r="B66" t="s">
         <v>10</v>
@@ -3317,7 +3315,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="14.45" customHeight="1">
       <c r="A67" s="12"/>
       <c r="B67" t="s">
         <v>12</v>
@@ -3332,7 +3330,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="14.45" customHeight="1">
       <c r="A68" s="12"/>
       <c r="B68" t="s">
         <v>14</v>
@@ -3347,7 +3345,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="14.45" customHeight="1">
       <c r="A69" s="12"/>
       <c r="B69" t="s">
         <v>16</v>
@@ -3362,7 +3360,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="14.45" customHeight="1">
       <c r="A70" s="12"/>
       <c r="B70" t="s">
         <v>18</v>
@@ -3377,7 +3375,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="14.45" customHeight="1">
       <c r="A71" s="12"/>
       <c r="D71" t="s">
         <v>245</v>
@@ -3389,7 +3387,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="14.45" customHeight="1">
       <c r="A72" s="12"/>
       <c r="D72" t="s">
         <v>246</v>
@@ -3401,7 +3399,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="14.45" customHeight="1">
       <c r="A73" s="12"/>
       <c r="D73" t="s">
         <v>247</v>
@@ -3413,13 +3411,13 @@
         <v>249</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="14.45" customHeight="1">
       <c r="A74" s="3"/>
     </row>
-    <row r="75" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="14.45" customHeight="1">
       <c r="A75" s="3"/>
     </row>
-    <row r="76" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="14.45" customHeight="1">
       <c r="A76" s="12" t="s">
         <v>609</v>
       </c>
@@ -3436,7 +3434,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="14.45" customHeight="1">
       <c r="A77" s="12"/>
       <c r="B77" t="s">
         <v>74</v>
@@ -3451,7 +3449,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="14.45" customHeight="1">
       <c r="A78" s="12"/>
       <c r="B78" t="s">
         <v>76</v>
@@ -3466,7 +3464,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="15" customHeight="1">
       <c r="A79" s="12"/>
       <c r="B79" t="s">
         <v>78</v>
@@ -3481,7 +3479,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="15" customHeight="1">
       <c r="A80" s="12"/>
       <c r="B80" t="s">
         <v>80</v>
@@ -3496,7 +3494,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="15" customHeight="1">
       <c r="A81" s="12"/>
       <c r="B81" t="s">
         <v>82</v>
@@ -3511,7 +3509,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="14.25" customHeight="1">
       <c r="A82" s="12"/>
       <c r="D82" t="s">
         <v>592</v>
@@ -3523,7 +3521,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="14.45" customHeight="1">
       <c r="A83" s="12"/>
       <c r="D83" t="s">
         <v>575</v>
@@ -3535,7 +3533,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="14.45" customHeight="1">
       <c r="A84" s="12"/>
       <c r="D84" t="s">
         <v>576</v>
@@ -3547,7 +3545,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="14.45" customHeight="1">
       <c r="A85" s="12"/>
       <c r="D85" t="s">
         <v>577</v>
@@ -3559,7 +3557,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="14.45" customHeight="1">
       <c r="A86" s="12"/>
       <c r="D86" t="s">
         <v>578</v>
@@ -3571,7 +3569,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="14.45" customHeight="1">
       <c r="A87" s="12"/>
       <c r="D87" t="s">
         <v>579</v>
@@ -3583,7 +3581,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="14.45" customHeight="1">
       <c r="A88" s="12"/>
       <c r="D88" t="s">
         <v>580</v>
@@ -3595,7 +3593,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="14.45" customHeight="1">
       <c r="A89" s="12"/>
       <c r="D89" t="s">
         <v>581</v>
@@ -3607,7 +3605,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="14.45" customHeight="1">
       <c r="A90" s="12"/>
       <c r="D90" t="s">
         <v>582</v>
@@ -3619,7 +3617,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="14.45" customHeight="1">
       <c r="A91" s="12"/>
       <c r="D91" t="s">
         <v>583</v>
@@ -3631,7 +3629,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="14.45" customHeight="1">
       <c r="A92" s="12"/>
       <c r="D92" t="s">
         <v>584</v>
@@ -3643,7 +3641,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="14.45" customHeight="1">
       <c r="A93" s="12"/>
       <c r="D93" t="s">
         <v>585</v>
@@ -3655,7 +3653,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="14.45" customHeight="1">
       <c r="A94" s="12"/>
       <c r="D94" t="s">
         <v>586</v>
@@ -3667,7 +3665,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="14.45" customHeight="1">
       <c r="A95" s="12"/>
       <c r="D95" t="s">
         <v>587</v>
@@ -3679,7 +3677,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="14.45" customHeight="1">
       <c r="A96" s="12"/>
       <c r="D96" t="s">
         <v>588</v>
@@ -3691,7 +3689,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="14.45" customHeight="1">
       <c r="A97" s="12"/>
       <c r="D97" t="s">
         <v>589</v>
@@ -3703,7 +3701,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="14.45" customHeight="1">
       <c r="A98" s="12"/>
       <c r="D98" t="s">
         <v>590</v>
@@ -3715,7 +3713,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="14.45" customHeight="1">
       <c r="A99" s="12"/>
       <c r="D99" t="s">
         <v>591</v>
@@ -3727,7 +3725,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="14.45" customHeight="1">
       <c r="A102" s="12" t="s">
         <v>345</v>
       </c>
@@ -3744,7 +3742,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="14.45" customHeight="1">
       <c r="A103" s="12"/>
       <c r="D103" t="s">
         <v>636</v>
@@ -3756,7 +3754,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="14.45" customHeight="1">
       <c r="A104" s="12"/>
       <c r="B104" t="s">
         <v>22</v>
@@ -3771,7 +3769,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="14.45" customHeight="1">
       <c r="A105" s="12"/>
       <c r="B105" t="s">
         <v>26</v>
@@ -3786,7 +3784,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="14.45" customHeight="1">
       <c r="A106" s="12"/>
       <c r="B106" t="s">
         <v>28</v>
@@ -3801,7 +3799,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="14.45" customHeight="1">
       <c r="A107" s="12"/>
       <c r="B107" t="s">
         <v>30</v>
@@ -3816,7 +3814,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="14.45" customHeight="1">
       <c r="A108" s="12"/>
       <c r="B108" t="s">
         <v>32</v>
@@ -3831,7 +3829,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="14.45" customHeight="1">
       <c r="A109" s="12"/>
       <c r="B109" t="s">
         <v>33</v>
@@ -3846,7 +3844,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="14.45" customHeight="1">
       <c r="A110" s="12"/>
       <c r="B110" t="s">
         <v>36</v>
@@ -3861,7 +3859,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="14.45" customHeight="1">
       <c r="A111" s="12"/>
       <c r="B111" t="s">
         <v>38</v>
@@ -3876,7 +3874,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="14.45" customHeight="1">
       <c r="A112" s="12"/>
       <c r="D112" t="s">
         <v>326</v>
@@ -3888,7 +3886,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="14.45" customHeight="1">
       <c r="A113" s="12"/>
       <c r="B113" t="s">
         <v>40</v>
@@ -3903,7 +3901,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="14.45" customHeight="1">
       <c r="A114" s="12"/>
       <c r="D114" t="s">
         <v>328</v>
@@ -3915,7 +3913,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="14.45" customHeight="1">
       <c r="A115" s="12"/>
       <c r="B115" t="s">
         <v>41</v>
@@ -3930,7 +3928,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="14.45" customHeight="1">
       <c r="A116" s="12"/>
       <c r="D116" t="s">
         <v>330</v>
@@ -3942,7 +3940,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="14.45" customHeight="1">
       <c r="A117" s="12"/>
       <c r="B117" t="s">
         <v>42</v>
@@ -3957,7 +3955,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="14.45" customHeight="1">
       <c r="A118" s="12"/>
       <c r="D118" t="s">
         <v>331</v>
@@ -3969,7 +3967,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="14.45" customHeight="1">
       <c r="A119" s="12"/>
       <c r="B119" t="s">
         <v>43</v>
@@ -3984,7 +3982,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="14.45" customHeight="1">
       <c r="A120" s="12"/>
       <c r="B120" t="s">
         <v>49</v>
@@ -3999,7 +3997,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" ht="14.45" customHeight="1">
       <c r="A121" s="12"/>
       <c r="B121" t="s">
         <v>51</v>
@@ -4014,7 +4012,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" ht="14.45" customHeight="1">
       <c r="A122" s="12"/>
       <c r="D122" t="s">
         <v>318</v>
@@ -4026,7 +4024,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" ht="14.45" customHeight="1">
       <c r="A123" s="12"/>
       <c r="D123" t="s">
         <v>320</v>
@@ -4038,7 +4036,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" ht="14.45" customHeight="1">
       <c r="A124" s="12"/>
       <c r="D124" t="s">
         <v>322</v>
@@ -4050,7 +4048,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" ht="14.45" customHeight="1">
       <c r="A125" s="12"/>
       <c r="D125" t="s">
         <v>324</v>
@@ -4062,7 +4060,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="14.45" customHeight="1">
       <c r="A126" s="12"/>
       <c r="D126" t="s">
         <v>325</v>
@@ -4074,7 +4072,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="14.45" customHeight="1">
       <c r="A127" s="12"/>
       <c r="D127" t="s">
         <v>336</v>
@@ -4086,7 +4084,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" ht="14.45" customHeight="1">
       <c r="A128" s="12"/>
       <c r="D128" t="s">
         <v>338</v>
@@ -4098,7 +4096,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="14.45" customHeight="1">
       <c r="A129" s="12"/>
       <c r="D129" t="s">
         <v>339</v>
@@ -4110,7 +4108,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" ht="14.45" customHeight="1">
       <c r="A130" s="12"/>
       <c r="D130" t="s">
         <v>342</v>
@@ -4122,7 +4120,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" ht="14.45" customHeight="1">
       <c r="A131" s="12"/>
       <c r="D131" t="s">
         <v>379</v>
@@ -4134,7 +4132,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" ht="14.45" customHeight="1">
       <c r="A132" s="12"/>
       <c r="D132" t="s">
         <v>380</v>
@@ -4146,7 +4144,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" ht="14.45" customHeight="1">
       <c r="A133" s="12"/>
       <c r="D133" t="s">
         <v>381</v>
@@ -4158,7 +4156,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" ht="14.45" customHeight="1">
       <c r="A134" s="12"/>
       <c r="D134" t="s">
         <v>426</v>
@@ -4170,7 +4168,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" ht="14.45" customHeight="1">
       <c r="A135" s="12"/>
       <c r="D135" t="s">
         <v>513</v>
@@ -4182,7 +4180,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" ht="14.45" customHeight="1">
       <c r="A136" s="12"/>
       <c r="D136" t="s">
         <v>382</v>
@@ -4194,7 +4192,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" ht="14.45" customHeight="1">
       <c r="A137" s="12"/>
       <c r="D137" t="s">
         <v>383</v>
@@ -4206,7 +4204,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" ht="14.45" customHeight="1">
       <c r="A138" s="12"/>
       <c r="D138" t="s">
         <v>384</v>
@@ -4218,7 +4216,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" ht="14.45" customHeight="1">
       <c r="A139" s="12"/>
       <c r="D139" t="s">
         <v>385</v>
@@ -4230,7 +4228,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" ht="14.45" customHeight="1">
       <c r="A140" s="12"/>
       <c r="D140" t="s">
         <v>386</v>
@@ -4242,7 +4240,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" ht="14.45" customHeight="1">
       <c r="A141" s="12"/>
       <c r="D141" t="s">
         <v>387</v>
@@ -4254,7 +4252,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" ht="14.45" customHeight="1">
       <c r="A142" s="12"/>
       <c r="D142" t="s">
         <v>688</v>
@@ -4263,10 +4261,10 @@
         <v>140</v>
       </c>
       <c r="F142" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" ht="14.45" customHeight="1">
       <c r="A143" s="12"/>
       <c r="D143" t="s">
         <v>689</v>
@@ -4275,10 +4273,10 @@
         <v>140</v>
       </c>
       <c r="F143" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" ht="14.45" customHeight="1">
       <c r="A144" s="12"/>
       <c r="D144" t="s">
         <v>690</v>
@@ -4287,10 +4285,10 @@
         <v>140</v>
       </c>
       <c r="F144" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" ht="14.45" customHeight="1">
       <c r="A145" s="12"/>
       <c r="D145" t="s">
         <v>691</v>
@@ -4299,16 +4297,16 @@
         <v>140</v>
       </c>
       <c r="F145" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="14.45" customHeight="1">
       <c r="A146" s="7"/>
     </row>
-    <row r="147" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" ht="14.45" customHeight="1">
       <c r="A147" s="7"/>
     </row>
-    <row r="148" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" ht="14.45" customHeight="1">
       <c r="A148" s="12" t="s">
         <v>344</v>
       </c>
@@ -4325,7 +4323,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" ht="14.45" customHeight="1">
       <c r="A149" s="12"/>
       <c r="B149" t="s">
         <v>95</v>
@@ -4340,7 +4338,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" ht="14.45" customHeight="1">
       <c r="A150" s="12"/>
       <c r="B150" t="s">
         <v>96</v>
@@ -4355,7 +4353,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" ht="14.45" customHeight="1">
       <c r="A151" s="12"/>
       <c r="B151" t="s">
         <v>97</v>
@@ -4370,7 +4368,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" ht="14.45" customHeight="1">
       <c r="A152" s="12"/>
       <c r="B152" t="s">
         <v>278</v>
@@ -4385,7 +4383,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" ht="14.45" customHeight="1">
       <c r="A153" s="12"/>
       <c r="B153" t="s">
         <v>279</v>
@@ -4400,7 +4398,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" ht="14.45" customHeight="1">
       <c r="A154" s="12"/>
       <c r="B154" t="s">
         <v>280</v>
@@ -4415,7 +4413,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" ht="14.45" customHeight="1">
       <c r="A155" s="12"/>
       <c r="B155" t="s">
         <v>281</v>
@@ -4430,7 +4428,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" ht="14.45" customHeight="1">
       <c r="A156" s="12"/>
       <c r="B156" t="s">
         <v>282</v>
@@ -4445,7 +4443,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" ht="14.45" customHeight="1">
       <c r="A157" s="12"/>
       <c r="B157" t="s">
         <v>283</v>
@@ -4460,7 +4458,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" ht="14.45" customHeight="1">
       <c r="A158" s="12"/>
       <c r="B158" t="s">
         <v>284</v>
@@ -4475,7 +4473,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" ht="14.45" customHeight="1">
       <c r="A159" s="12"/>
       <c r="B159" t="s">
         <v>285</v>
@@ -4490,7 +4488,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="14.45" customHeight="1">
       <c r="A160" s="12"/>
       <c r="B160" t="s">
         <v>286</v>
@@ -4505,7 +4503,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" ht="14.45" customHeight="1">
       <c r="A161" s="12"/>
       <c r="B161" t="s">
         <v>287</v>
@@ -4520,7 +4518,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" ht="14.45" customHeight="1">
       <c r="A162" s="12"/>
       <c r="B162" t="s">
         <v>288</v>
@@ -4535,7 +4533,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="14.45" customHeight="1">
       <c r="A163" s="12"/>
       <c r="B163" t="s">
         <v>289</v>
@@ -4550,13 +4548,13 @@
         <v>291</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" ht="14.45" customHeight="1">
       <c r="A164" s="3"/>
     </row>
-    <row r="165" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" ht="14.45" customHeight="1">
       <c r="A165" s="3"/>
     </row>
-    <row r="166" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" ht="14.45" customHeight="1">
       <c r="A166" s="12" t="s">
         <v>349</v>
       </c>
@@ -4573,7 +4571,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" ht="14.45" customHeight="1">
       <c r="A167" s="12"/>
       <c r="B167" t="s">
         <v>68</v>
@@ -4588,7 +4586,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" ht="14.45" customHeight="1">
       <c r="A168" s="12"/>
       <c r="B168" t="s">
         <v>69</v>
@@ -4603,7 +4601,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" ht="14.45" customHeight="1">
       <c r="A169" s="12"/>
       <c r="B169" t="s">
         <v>70</v>
@@ -4618,7 +4616,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" ht="14.45" customHeight="1">
       <c r="A170" s="12"/>
       <c r="B170" t="s">
         <v>71</v>
@@ -4633,7 +4631,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" ht="14.45" customHeight="1">
       <c r="A171" s="12"/>
       <c r="D171" t="s">
         <v>353</v>
@@ -4645,7 +4643,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" ht="14.45" customHeight="1">
       <c r="A172" s="12"/>
       <c r="D172" t="s">
         <v>360</v>
@@ -4657,7 +4655,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" ht="14.45" customHeight="1">
       <c r="A173" s="12"/>
       <c r="D173" t="s">
         <v>361</v>
@@ -4669,7 +4667,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" ht="14.45" customHeight="1">
       <c r="A174" s="12"/>
       <c r="D174" t="s">
         <v>352</v>
@@ -4681,7 +4679,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" ht="14.45" customHeight="1">
       <c r="A175" s="12"/>
       <c r="D175" t="s">
         <v>354</v>
@@ -4693,7 +4691,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="14.45" customHeight="1">
       <c r="A176" s="12"/>
       <c r="D176" t="s">
         <v>355</v>
@@ -4705,7 +4703,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" ht="14.45" customHeight="1">
       <c r="A177" s="12"/>
       <c r="D177" t="s">
         <v>425</v>
@@ -4717,7 +4715,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="14.45" customHeight="1">
       <c r="A178" s="12"/>
       <c r="D178" t="s">
         <v>574</v>
@@ -4729,7 +4727,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="14.45" customHeight="1">
       <c r="A179" s="12"/>
       <c r="D179" t="s">
         <v>515</v>
@@ -4741,7 +4739,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" ht="14.45" customHeight="1">
       <c r="A180" s="12"/>
       <c r="D180" t="s">
         <v>369</v>
@@ -4753,7 +4751,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" ht="14.45" customHeight="1">
       <c r="A181" s="12"/>
       <c r="D181" t="s">
         <v>370</v>
@@ -4765,7 +4763,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" ht="14.45" customHeight="1">
       <c r="A182" s="12"/>
       <c r="D182" t="s">
         <v>357</v>
@@ -4777,7 +4775,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" ht="14.45" customHeight="1">
       <c r="A183" s="12"/>
       <c r="D183" t="s">
         <v>358</v>
@@ -4789,7 +4787,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" ht="14.45" customHeight="1">
       <c r="A184" s="12"/>
       <c r="D184" t="s">
         <v>359</v>
@@ -4801,7 +4799,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" ht="14.45" customHeight="1">
       <c r="A185" s="12"/>
       <c r="D185" t="s">
         <v>351</v>
@@ -4813,7 +4811,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" ht="14.45" customHeight="1">
       <c r="A186" s="12"/>
       <c r="D186" t="s">
         <v>356</v>
@@ -4825,7 +4823,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" ht="14.45" customHeight="1">
       <c r="A187" s="12"/>
       <c r="D187" t="s">
         <v>367</v>
@@ -4837,7 +4835,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" ht="14.45" customHeight="1">
       <c r="A188" s="12"/>
       <c r="D188" t="s">
         <v>377</v>
@@ -4849,13 +4847,13 @@
         <v>378</v>
       </c>
     </row>
-    <row r="189" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" ht="14.45" customHeight="1">
       <c r="A189" s="10"/>
     </row>
-    <row r="190" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" ht="14.45" customHeight="1">
       <c r="A190" s="3"/>
     </row>
-    <row r="191" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" ht="21" customHeight="1">
       <c r="A191" s="12" t="s">
         <v>530</v>
       </c>
@@ -4869,7 +4867,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6">
       <c r="A192" s="12"/>
       <c r="D192" t="s">
         <v>551</v>
@@ -4881,7 +4879,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6">
       <c r="A193" s="12"/>
       <c r="D193" t="s">
         <v>552</v>
@@ -4893,7 +4891,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6">
       <c r="A194" s="12"/>
       <c r="D194" t="s">
         <v>553</v>
@@ -4905,7 +4903,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6">
       <c r="A195" s="12"/>
       <c r="D195" t="s">
         <v>554</v>
@@ -4917,7 +4915,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6">
       <c r="A196" s="12"/>
       <c r="D196" t="s">
         <v>555</v>
@@ -4929,7 +4927,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6">
       <c r="A197" s="12"/>
       <c r="D197" t="s">
         <v>556</v>
@@ -4941,7 +4939,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6">
       <c r="A198" s="12"/>
       <c r="D198" t="s">
         <v>557</v>
@@ -4953,7 +4951,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6">
       <c r="A199" s="12"/>
       <c r="D199" t="s">
         <v>558</v>
@@ -4965,7 +4963,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6">
       <c r="A200" s="12"/>
       <c r="D200" t="s">
         <v>559</v>
@@ -4977,7 +4975,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6">
       <c r="A201" s="12"/>
       <c r="D201" t="s">
         <v>560</v>
@@ -4989,7 +4987,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6">
       <c r="A202" s="12"/>
       <c r="D202" t="s">
         <v>561</v>
@@ -5001,7 +4999,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6">
       <c r="A203" s="12"/>
       <c r="D203" t="s">
         <v>562</v>
@@ -5013,7 +5011,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6">
       <c r="A204" s="12"/>
       <c r="D204" t="s">
         <v>563</v>
@@ -5025,7 +5023,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6">
       <c r="A205" s="12"/>
       <c r="D205" t="s">
         <v>564</v>
@@ -5037,7 +5035,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6">
       <c r="A206" s="12"/>
       <c r="D206" t="s">
         <v>565</v>
@@ -5049,7 +5047,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6">
       <c r="A207" s="12"/>
       <c r="D207" t="s">
         <v>566</v>
@@ -5061,7 +5059,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6">
       <c r="A208" s="12"/>
       <c r="D208" t="s">
         <v>567</v>
@@ -5073,7 +5071,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6">
       <c r="A209" s="12"/>
       <c r="D209" t="s">
         <v>568</v>
@@ -5085,7 +5083,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6">
       <c r="A210" s="12"/>
       <c r="D210" t="s">
         <v>569</v>
@@ -5097,7 +5095,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6">
       <c r="A211" s="12"/>
       <c r="D211" t="s">
         <v>570</v>
@@ -5109,7 +5107,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6">
       <c r="A212" s="12"/>
       <c r="D212" t="s">
         <v>571</v>
@@ -5121,7 +5119,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6">
       <c r="A213" s="12"/>
       <c r="D213" t="s">
         <v>572</v>
@@ -5133,13 +5131,13 @@
         <v>412</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6">
       <c r="A214" s="11"/>
     </row>
-    <row r="215" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" ht="14.45" customHeight="1">
       <c r="A215" s="3"/>
     </row>
-    <row r="216" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" ht="14.45" customHeight="1">
       <c r="A216" s="12" t="s">
         <v>350</v>
       </c>
@@ -5153,7 +5151,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="217" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" ht="14.45" customHeight="1">
       <c r="A217" s="12"/>
       <c r="D217" t="s">
         <v>90</v>
@@ -5165,7 +5163,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="218" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" ht="14.45" customHeight="1">
       <c r="A218" s="12"/>
       <c r="D218" t="s">
         <v>91</v>
@@ -5177,7 +5175,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="219" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" ht="14.45" customHeight="1">
       <c r="A219" s="12"/>
       <c r="D219" t="s">
         <v>92</v>
@@ -5189,7 +5187,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="220" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" ht="14.45" customHeight="1">
       <c r="A220" s="12"/>
       <c r="D220" t="s">
         <v>93</v>
@@ -5201,7 +5199,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="221" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" ht="14.45" customHeight="1">
       <c r="A221" s="12"/>
       <c r="D221" t="s">
         <v>393</v>
@@ -5213,7 +5211,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="222" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" ht="14.45" customHeight="1">
       <c r="A222" s="12"/>
       <c r="D222" t="s">
         <v>398</v>
@@ -5225,7 +5223,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="223" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" ht="14.45" customHeight="1">
       <c r="A223" s="12"/>
       <c r="D223" t="s">
         <v>399</v>
@@ -5237,7 +5235,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" ht="14.45" customHeight="1">
       <c r="A224" s="12"/>
       <c r="D224" t="s">
         <v>400</v>
@@ -5249,7 +5247,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="225" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" ht="14.45" customHeight="1">
       <c r="A225" s="12"/>
       <c r="D225" t="s">
         <v>401</v>
@@ -5261,7 +5259,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="226" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" ht="14.45" customHeight="1">
       <c r="A226" s="12"/>
       <c r="D226" t="s">
         <v>402</v>
@@ -5273,7 +5271,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="227" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" ht="14.45" customHeight="1">
       <c r="A227" s="12"/>
       <c r="D227" t="s">
         <v>424</v>
@@ -5285,7 +5283,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="228" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" ht="14.45" customHeight="1">
       <c r="A228" s="12"/>
       <c r="D228" t="s">
         <v>525</v>
@@ -5297,7 +5295,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="229" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" ht="14.45" customHeight="1">
       <c r="A229" s="12"/>
       <c r="D229" t="s">
         <v>516</v>
@@ -5309,7 +5307,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="230" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" ht="14.45" customHeight="1">
       <c r="A230" s="12"/>
       <c r="D230" t="s">
         <v>403</v>
@@ -5321,7 +5319,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" ht="14.45" customHeight="1">
       <c r="A231" s="12"/>
       <c r="D231" t="s">
         <v>404</v>
@@ -5333,7 +5331,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" ht="14.45" customHeight="1">
       <c r="A232" s="12"/>
       <c r="D232" t="s">
         <v>405</v>
@@ -5345,7 +5343,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="233" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" ht="14.45" customHeight="1">
       <c r="A233" s="12"/>
       <c r="D233" t="s">
         <v>406</v>
@@ -5357,7 +5355,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="234" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" ht="14.45" customHeight="1">
       <c r="A234" s="12"/>
       <c r="D234" t="s">
         <v>407</v>
@@ -5369,7 +5367,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="235" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" ht="14.45" customHeight="1">
       <c r="A235" s="12"/>
       <c r="D235" t="s">
         <v>408</v>
@@ -5381,7 +5379,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="236" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" ht="14.45" customHeight="1">
       <c r="A236" s="12"/>
       <c r="D236" t="s">
         <v>409</v>
@@ -5393,7 +5391,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="237" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" ht="14.45" customHeight="1">
       <c r="A237" s="12"/>
       <c r="D237" t="s">
         <v>410</v>
@@ -5405,7 +5403,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="238" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" ht="14.45" customHeight="1">
       <c r="A238" s="12"/>
       <c r="D238" t="s">
         <v>411</v>
@@ -5417,10 +5415,10 @@
         <v>412</v>
       </c>
     </row>
-    <row r="239" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" ht="14.45" customHeight="1">
       <c r="A239" s="3"/>
     </row>
-    <row r="241" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" ht="14.45" customHeight="1">
       <c r="A241" s="12" t="s">
         <v>346</v>
       </c>
@@ -5437,7 +5435,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="242" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" ht="14.45" customHeight="1">
       <c r="A242" s="12"/>
       <c r="B242" t="s">
         <v>100</v>
@@ -5452,7 +5450,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="243" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" ht="14.45" customHeight="1">
       <c r="A243" s="12"/>
       <c r="B243" t="s">
         <v>102</v>
@@ -5467,7 +5465,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="244" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" ht="14.45" customHeight="1">
       <c r="A244" s="12"/>
       <c r="B244" t="s">
         <v>104</v>
@@ -5482,7 +5480,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="245" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" ht="14.45" customHeight="1">
       <c r="A245" s="12"/>
       <c r="B245" t="s">
         <v>108</v>
@@ -5497,7 +5495,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="246" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" ht="14.45" customHeight="1">
       <c r="A246" s="12"/>
       <c r="B246" t="s">
         <v>106</v>
@@ -5509,7 +5507,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="247" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" ht="14.45" customHeight="1">
       <c r="A247" s="12"/>
       <c r="D247" t="s">
         <v>432</v>
@@ -5521,7 +5519,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="248" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" ht="14.45" customHeight="1">
       <c r="A248" s="12"/>
       <c r="D248" t="s">
         <v>433</v>
@@ -5533,7 +5531,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="249" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" ht="14.45" customHeight="1">
       <c r="A249" s="12"/>
       <c r="D249" t="s">
         <v>434</v>
@@ -5545,7 +5543,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="250" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" ht="14.45" customHeight="1">
       <c r="A250" s="12"/>
       <c r="D250" t="s">
         <v>519</v>
@@ -5557,7 +5555,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="251" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" ht="14.45" customHeight="1">
       <c r="A251" s="12"/>
       <c r="D251" t="s">
         <v>517</v>
@@ -5569,7 +5567,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="252" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" ht="14.45" customHeight="1">
       <c r="A252" s="12"/>
       <c r="D252" t="s">
         <v>435</v>
@@ -5581,7 +5579,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="253" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" ht="14.45" customHeight="1">
       <c r="A253" s="12"/>
       <c r="D253" t="s">
         <v>436</v>
@@ -5593,7 +5591,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="254" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" ht="14.45" customHeight="1">
       <c r="A254" s="12"/>
       <c r="D254" t="s">
         <v>437</v>
@@ -5605,7 +5603,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="255" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" ht="14.45" customHeight="1">
       <c r="A255" s="12"/>
       <c r="D255" t="s">
         <v>438</v>
@@ -5617,7 +5615,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="256" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" ht="14.45" customHeight="1">
       <c r="A256" s="12"/>
       <c r="D256" t="s">
         <v>439</v>
@@ -5629,7 +5627,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="257" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" ht="14.45" customHeight="1">
       <c r="A257" s="12"/>
       <c r="D257" t="s">
         <v>440</v>
@@ -5641,7 +5639,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="258" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6" ht="14.45" customHeight="1">
       <c r="A258" s="12"/>
       <c r="D258" t="s">
         <v>441</v>
@@ -5653,7 +5651,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="259" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" ht="14.45" customHeight="1">
       <c r="A259" s="12"/>
       <c r="D259" t="s">
         <v>442</v>
@@ -5665,7 +5663,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="260" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" ht="14.45" customHeight="1">
       <c r="A260" s="12"/>
       <c r="D260" t="s">
         <v>639</v>
@@ -5674,7 +5672,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="261" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" ht="14.45" customHeight="1">
       <c r="A261" s="12"/>
       <c r="D261" t="s">
         <v>660</v>
@@ -5683,7 +5681,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="262" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" ht="14.45" customHeight="1">
       <c r="A262" s="12"/>
       <c r="D262" t="s">
         <v>661</v>
@@ -5692,7 +5690,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="263" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6" ht="14.45" customHeight="1">
       <c r="A263" s="12"/>
       <c r="D263" t="s">
         <v>429</v>
@@ -5701,7 +5699,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="264" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6" ht="14.45" customHeight="1">
       <c r="A264" s="12"/>
       <c r="D264" t="s">
         <v>642</v>
@@ -5710,7 +5708,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6">
       <c r="A265" s="12"/>
       <c r="D265" t="s">
         <v>643</v>
@@ -5719,7 +5717,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6">
       <c r="A266" s="12"/>
       <c r="D266" t="s">
         <v>640</v>
@@ -5728,7 +5726,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6">
       <c r="A267" s="12"/>
       <c r="D267" t="s">
         <v>641</v>
@@ -5737,7 +5735,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6">
       <c r="A268" s="12"/>
       <c r="D268" t="s">
         <v>644</v>
@@ -5746,7 +5744,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6">
       <c r="A269" s="12"/>
       <c r="D269" t="s">
         <v>645</v>
@@ -5755,7 +5753,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6">
       <c r="A270" s="12"/>
       <c r="D270" t="s">
         <v>646</v>
@@ -5767,7 +5765,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6">
       <c r="A271" s="12"/>
       <c r="D271" t="s">
         <v>653</v>
@@ -5779,7 +5777,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6">
       <c r="A272" s="12"/>
       <c r="D272" t="s">
         <v>647</v>
@@ -5791,7 +5789,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6">
       <c r="A273" s="12"/>
       <c r="D273" t="s">
         <v>654</v>
@@ -5803,7 +5801,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6">
       <c r="A274" s="12"/>
       <c r="D274" t="s">
         <v>648</v>
@@ -5815,7 +5813,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6">
       <c r="A275" s="12"/>
       <c r="D275" t="s">
         <v>656</v>
@@ -5827,7 +5825,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6">
       <c r="A276" s="12"/>
       <c r="D276" t="s">
         <v>649</v>
@@ -5839,7 +5837,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6">
       <c r="A277" s="12"/>
       <c r="D277" t="s">
         <v>655</v>
@@ -5851,7 +5849,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6">
       <c r="A278" s="12"/>
       <c r="D278" t="s">
         <v>650</v>
@@ -5863,7 +5861,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6">
       <c r="A279" s="12"/>
       <c r="D279" t="s">
         <v>657</v>
@@ -5875,7 +5873,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6">
       <c r="A280" s="12"/>
       <c r="D280" t="s">
         <v>651</v>
@@ -5887,7 +5885,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6">
       <c r="A281" s="12"/>
       <c r="D281" t="s">
         <v>658</v>
@@ -5899,7 +5897,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6">
       <c r="A282" s="12"/>
       <c r="D282" t="s">
         <v>652</v>
@@ -5911,7 +5909,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6">
       <c r="A283" s="12"/>
       <c r="D283" t="s">
         <v>659</v>
@@ -5923,7 +5921,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6">
       <c r="A284" s="12"/>
       <c r="D284" t="s">
         <v>662</v>
@@ -5935,7 +5933,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6">
       <c r="A285" s="12"/>
       <c r="D285" t="s">
         <v>663</v>
@@ -5947,7 +5945,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6">
       <c r="A286" s="12"/>
       <c r="D286" t="s">
         <v>664</v>
@@ -5959,7 +5957,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6">
       <c r="A287" s="12"/>
       <c r="D287" t="s">
         <v>665</v>
@@ -5971,7 +5969,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6">
       <c r="A288" s="12"/>
       <c r="D288" t="s">
         <v>666</v>
@@ -5983,7 +5981,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6">
       <c r="A289" s="12"/>
       <c r="D289" t="s">
         <v>667</v>
@@ -5995,7 +5993,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="292" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" ht="14.45" customHeight="1">
       <c r="A292" s="12" t="s">
         <v>347</v>
       </c>
@@ -6012,7 +6010,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="293" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" ht="14.45" customHeight="1">
       <c r="A293" s="12"/>
       <c r="B293" t="s">
         <v>110</v>
@@ -6027,7 +6025,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="294" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" ht="14.45" customHeight="1">
       <c r="A294" s="12"/>
       <c r="B294" t="s">
         <v>111</v>
@@ -6042,7 +6040,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="295" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" ht="14.45" customHeight="1">
       <c r="A295" s="12"/>
       <c r="D295" t="s">
         <v>454</v>
@@ -6054,7 +6052,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="296" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" ht="14.45" customHeight="1">
       <c r="A296" s="12"/>
       <c r="D296" t="s">
         <v>455</v>
@@ -6066,7 +6064,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="297" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" ht="14.45" customHeight="1">
       <c r="A297" s="12"/>
       <c r="D297" t="s">
         <v>456</v>
@@ -6078,7 +6076,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="298" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" ht="14.45" customHeight="1">
       <c r="A298" s="12"/>
       <c r="D298" t="s">
         <v>457</v>
@@ -6090,7 +6088,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="299" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" ht="14.45" customHeight="1">
       <c r="A299" s="12"/>
       <c r="D299" t="s">
         <v>459</v>
@@ -6099,7 +6097,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="300" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" ht="14.45" customHeight="1">
       <c r="A300" s="12"/>
       <c r="D300" t="s">
         <v>458</v>
@@ -6111,7 +6109,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="301" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6" ht="14.45" customHeight="1">
       <c r="A301" s="12"/>
       <c r="D301" t="s">
         <v>524</v>
@@ -6123,7 +6121,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="302" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:6" ht="14.45" customHeight="1">
       <c r="A302" s="12"/>
       <c r="D302" t="s">
         <v>518</v>
@@ -6135,7 +6133,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="303" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6" ht="14.45" customHeight="1">
       <c r="A303" s="12"/>
       <c r="D303" t="s">
         <v>460</v>
@@ -6147,7 +6145,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="304" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" ht="14.45" customHeight="1">
       <c r="A304" s="12"/>
       <c r="D304" t="s">
         <v>461</v>
@@ -6159,7 +6157,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="305" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" ht="14.45" customHeight="1">
       <c r="A305" s="12"/>
       <c r="D305" t="s">
         <v>462</v>
@@ -6171,7 +6169,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="306" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" ht="14.45" customHeight="1">
       <c r="A306" s="12"/>
       <c r="D306" t="s">
         <v>463</v>
@@ -6183,7 +6181,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="307" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" ht="14.45" customHeight="1">
       <c r="A307" s="12"/>
       <c r="D307" t="s">
         <v>464</v>
@@ -6195,7 +6193,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="308" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" ht="14.45" customHeight="1">
       <c r="A308" s="12"/>
       <c r="D308" t="s">
         <v>465</v>
@@ -6207,7 +6205,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="309" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" ht="14.45" customHeight="1">
       <c r="A309" s="12"/>
       <c r="D309" t="s">
         <v>466</v>
@@ -6219,7 +6217,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="310" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" ht="14.45" customHeight="1">
       <c r="A310" s="12"/>
       <c r="D310" t="s">
         <v>467</v>
@@ -6231,7 +6229,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="313" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" ht="14.45" customHeight="1">
       <c r="A313" s="12" t="s">
         <v>490</v>
       </c>
@@ -6248,7 +6246,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="314" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" ht="14.45" customHeight="1">
       <c r="A314" s="12"/>
       <c r="D314" t="s">
         <v>155</v>
@@ -6260,7 +6258,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="315" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" ht="14.45" customHeight="1">
       <c r="A315" s="12"/>
       <c r="D315" t="s">
         <v>158</v>
@@ -6272,7 +6270,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="316" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" ht="14.45" customHeight="1">
       <c r="A316" s="12"/>
       <c r="D316" t="s">
         <v>159</v>
@@ -6284,7 +6282,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="317" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1">
       <c r="A317" s="12"/>
       <c r="D317" s="9" t="s">
         <v>489</v>
@@ -6296,7 +6294,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="318" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1">
       <c r="A318" s="12"/>
       <c r="D318" s="9" t="s">
         <v>491</v>
@@ -6308,13 +6306,13 @@
         <v>502</v>
       </c>
     </row>
-    <row r="319" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1">
       <c r="A319" s="3"/>
     </row>
-    <row r="320" spans="1:6" s="9" customFormat="1" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6" s="9" customFormat="1">
       <c r="A320" s="2"/>
     </row>
-    <row r="322" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6" ht="14.45" customHeight="1">
       <c r="A322" s="12" t="s">
         <v>348</v>
       </c>
@@ -6331,7 +6329,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="323" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6" ht="14.45" customHeight="1">
       <c r="A323" s="12"/>
       <c r="B323" t="s">
         <v>53</v>
@@ -6346,7 +6344,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="324" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:6" ht="14.45" customHeight="1">
       <c r="A324" s="12"/>
       <c r="B324" t="s">
         <v>55</v>
@@ -6361,7 +6359,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="325" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" ht="14.45" customHeight="1">
       <c r="A325" s="12"/>
       <c r="B325" t="s">
         <v>58</v>
@@ -6376,7 +6374,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="326" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:6" ht="14.45" customHeight="1">
       <c r="A326" s="12"/>
       <c r="D326" t="s">
         <v>492</v>
@@ -6388,7 +6386,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="327" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:6" ht="14.45" customHeight="1">
       <c r="A327" s="12"/>
       <c r="B327" t="s">
         <v>59</v>
@@ -6403,7 +6401,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="328" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:6" ht="14.45" customHeight="1">
       <c r="A328" s="12"/>
       <c r="B328" t="s">
         <v>61</v>
@@ -6418,7 +6416,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="329" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:6" ht="14.45" customHeight="1">
       <c r="A329" s="12"/>
       <c r="B329" t="s">
         <v>63</v>
@@ -6433,7 +6431,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="330" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6" ht="14.45" customHeight="1">
       <c r="A330" s="12"/>
       <c r="B330" t="s">
         <v>64</v>
@@ -6448,7 +6446,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="331" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:6" ht="14.45" customHeight="1">
       <c r="A331" s="12"/>
       <c r="D331" t="s">
         <v>493</v>
@@ -6460,7 +6458,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="332" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:6" ht="14.45" customHeight="1">
       <c r="A332" s="12"/>
       <c r="D332" t="s">
         <v>494</v>
@@ -6472,7 +6470,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="333" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:6" ht="14.45" customHeight="1">
       <c r="A333" s="12"/>
       <c r="D333" t="s">
         <v>495</v>
@@ -6484,7 +6482,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="336" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:6" ht="21">
       <c r="A336" s="4" t="s">
         <v>120</v>
       </c>
@@ -6501,7 +6499,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="339" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:6" ht="14.45" customHeight="1">
       <c r="A339" s="12" t="s">
         <v>127</v>
       </c>
@@ -6515,7 +6513,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="340" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:6" ht="14.45" customHeight="1">
       <c r="A340" s="12"/>
       <c r="B340" t="s">
         <v>116</v>
@@ -6527,7 +6525,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="341" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:6" ht="14.45" customHeight="1">
       <c r="A341" s="12"/>
       <c r="B341" t="s">
         <v>118</v>
@@ -6539,7 +6537,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="342" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:6" ht="14.45" customHeight="1">
       <c r="A342" s="12"/>
       <c r="B342" t="s">
         <v>128</v>
@@ -6551,7 +6549,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="343" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:6" ht="14.45" customHeight="1">
       <c r="A343" s="12"/>
       <c r="B343" t="s">
         <v>121</v>
@@ -6563,10 +6561,10 @@
         <v>230</v>
       </c>
     </row>
-    <row r="344" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:6" ht="14.45" customHeight="1">
       <c r="A344" s="3"/>
     </row>
-    <row r="345" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:6" ht="14.45" customHeight="1">
       <c r="A345" s="3"/>
     </row>
   </sheetData>
@@ -6593,24 +6591,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update documentation for validate.
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variables.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variables.xlsx
@@ -2094,12 +2094,6 @@
     <t>player.case</t>
   </si>
   <si>
-    <t>//gs validate &lt;filter&gt;</t>
-  </si>
-  <si>
-    <t>This command checks to see whether the equipment in "sets" also exists in your inventory. &lt;filter&gt; is an optional list of words that restricts the output to only those items that contain text from one of the filter's words.</t>
-  </si>
-  <si>
     <t>pet_midaction()</t>
   </si>
   <si>
@@ -2107,6 +2101,12 @@
   </si>
   <si>
     <t>Table keyed with the name of equipment pieces.  Keys for both short name and long name exist, if applicable.  Value is a table containing containing item id, count, short name (shortname), and optionally long name (longname).</t>
+  </si>
+  <si>
+    <t>//gs validate [sets|inv] [filter]</t>
+  </si>
+  <si>
+    <t>This command checks to see whether the equipment in "sets" also exists in your inventory (default), or if the equipment in your inventory exists in "sets" (if the "inv" parameter is used). [filter] is an optional list of words that restricts the output to only those items that contain text from one of the filter's words.</t>
   </si>
 </sst>
 </file>
@@ -2500,8 +2500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="D140" sqref="D140"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2775,13 +2775,13 @@
     <row r="23" spans="1:6" ht="14.45" customHeight="1">
       <c r="A23" s="3"/>
       <c r="D23" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="E23" t="s">
         <v>500</v>
       </c>
       <c r="F23" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1">
@@ -3214,10 +3214,10 @@
     <row r="58" spans="1:6" ht="14.45" customHeight="1">
       <c r="A58" s="12"/>
       <c r="D58" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="F58" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="14.45" customHeight="1">
@@ -4261,7 +4261,7 @@
         <v>140</v>
       </c>
       <c r="F142" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="14.45" customHeight="1">
@@ -4273,7 +4273,7 @@
         <v>140</v>
       </c>
       <c r="F143" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="14.45" customHeight="1">
@@ -4285,7 +4285,7 @@
         <v>140</v>
       </c>
       <c r="F144" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="14.45" customHeight="1">
@@ -4297,7 +4297,7 @@
         <v>140</v>
       </c>
       <c r="F145" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="14.45" customHeight="1">

</xml_diff>

<commit_message>
GearSwap - Documentation update
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variables.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2091,9 +2091,6 @@
     <t>Allows users to register events in Lua that will be called by LuaCore directly. See the doku wiki for more details about options here. I'd call this "Super Advanced Mode." Also, this presently causes crashes on reload. Don't use it.</t>
   </si>
   <si>
-    <t>Passes in the "pet" table for the pet being summoned or dismissed and a boolean second argument that is true when you gain a pet or false when you lose one.</t>
-  </si>
-  <si>
     <t>pretarget(spell)</t>
   </si>
   <si>
@@ -2113,6 +2110,9 @@
   </si>
   <si>
     <t>pet_change(pet,gain)</t>
+  </si>
+  <si>
+    <t>Passes in the "pet" table and a boolean indicating whether the pet is being summoned (true) or dismissed (false). Order is not guaranteed relative to aftercast for JAs like Release or Leave. Currently does not work for Charm.</t>
   </si>
 </sst>
 </file>
@@ -2200,10 +2200,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2508,20 +2508,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F346"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" customWidth="1"/>
-    <col min="4" max="4" width="40.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="202.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="202.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="25.9" x14ac:dyDescent="0.5">
       <c r="B1" s="6" t="s">
         <v>492</v>
       </c>
@@ -2536,8 +2536,8 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>609</v>
       </c>
       <c r="D3" t="s">
@@ -2550,10 +2550,10 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+    <row r="4" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
       <c r="D4" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E4" t="s">
         <v>495</v>
@@ -2562,13 +2562,13 @@
         <v>620</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
       <c r="B5" t="s">
         <v>177</v>
       </c>
       <c r="D5" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E5" t="s">
         <v>495</v>
@@ -2577,13 +2577,13 @@
         <v>621</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
       <c r="B6" t="s">
         <v>178</v>
       </c>
       <c r="D6" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E6" t="s">
         <v>495</v>
@@ -2592,13 +2592,13 @@
         <v>618</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
       <c r="B7" t="s">
         <v>179</v>
       </c>
       <c r="D7" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E7" t="s">
         <v>495</v>
@@ -2607,22 +2607,22 @@
         <v>619</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
       <c r="D8" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E8" t="s">
         <v>495</v>
       </c>
       <c r="F8" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
+        <v>698</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
       <c r="D9" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E9" t="s">
         <v>495</v>
@@ -2631,10 +2631,10 @@
         <v>610</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
       <c r="D10" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="E10" t="s">
         <v>495</v>
@@ -2643,8 +2643,8 @@
         <v>611</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
       <c r="D11" t="s">
         <v>502</v>
       </c>
@@ -2655,8 +2655,8 @@
         <v>503</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
       <c r="D12" t="s">
         <v>616</v>
       </c>
@@ -2667,8 +2667,8 @@
         <v>617</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
       <c r="D13" t="s">
         <v>180</v>
       </c>
@@ -2679,8 +2679,8 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
       <c r="D14" t="s">
         <v>193</v>
       </c>
@@ -2691,8 +2691,8 @@
         <v>612</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>119</v>
       </c>
       <c r="B17" t="s">
@@ -2708,8 +2708,8 @@
         <v>606</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
+    <row r="18" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
       <c r="B18" t="s">
         <v>504</v>
       </c>
@@ -2723,8 +2723,8 @@
         <v>506</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
+    <row r="19" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
       <c r="B19" t="s">
         <v>122</v>
       </c>
@@ -2738,8 +2738,8 @@
         <v>614</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
+    <row r="20" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
       <c r="B20" t="s">
         <v>121</v>
       </c>
@@ -2750,8 +2750,8 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
       <c r="B21" t="s">
         <v>123</v>
       </c>
@@ -2765,8 +2765,8 @@
         <v>613</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13"/>
+    <row r="22" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
       <c r="B22" t="s">
         <v>117</v>
       </c>
@@ -2780,8 +2780,8 @@
         <v>615</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
+    <row r="23" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
       <c r="B23" t="s">
         <v>0</v>
       </c>
@@ -2795,8 +2795,8 @@
         <v>628</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
+    <row r="24" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
       <c r="B24" t="s">
         <v>0</v>
       </c>
@@ -2810,8 +2810,8 @@
         <v>686</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
       <c r="B25" t="s">
         <v>124</v>
       </c>
@@ -2825,8 +2825,8 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
       <c r="B26" t="s">
         <v>125</v>
       </c>
@@ -2840,8 +2840,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
       <c r="B27" t="s">
         <v>129</v>
       </c>
@@ -2858,8 +2858,8 @@
         <v>607</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
       <c r="B28" t="s">
         <v>130</v>
       </c>
@@ -2873,8 +2873,8 @@
         <v>608</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
       <c r="B29" t="s">
         <v>137</v>
       </c>
@@ -2888,8 +2888,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
       <c r="B30" t="s">
         <v>0</v>
       </c>
@@ -2903,8 +2903,8 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
       <c r="B31" t="s">
         <v>0</v>
       </c>
@@ -2918,8 +2918,8 @@
         <v>164</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
       <c r="B32" t="s">
         <v>0</v>
       </c>
@@ -2933,8 +2933,8 @@
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="13"/>
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
       <c r="B33" t="s">
         <v>0</v>
       </c>
@@ -2948,8 +2948,8 @@
         <v>690</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="13"/>
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="12"/>
       <c r="B34" t="s">
         <v>0</v>
       </c>
@@ -2963,14 +2963,14 @@
         <v>624</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="12" t="s">
+    <row r="37" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
         <v>141</v>
       </c>
       <c r="B37" t="s">
@@ -2986,8 +2986,8 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="12"/>
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="13"/>
       <c r="B38" t="s">
         <v>0</v>
       </c>
@@ -3001,8 +3001,8 @@
         <v>171</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="12"/>
+    <row r="39" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
       <c r="B39" t="s">
         <v>0</v>
       </c>
@@ -3016,8 +3016,8 @@
         <v>496</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="12"/>
+    <row r="40" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
       <c r="B40" t="s">
         <v>0</v>
       </c>
@@ -3031,8 +3031,8 @@
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="12"/>
+    <row r="41" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
       <c r="B41" t="s">
         <v>0</v>
       </c>
@@ -3046,8 +3046,8 @@
         <v>622</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="12"/>
+    <row r="42" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
       <c r="B42" t="s">
         <v>0</v>
       </c>
@@ -3061,8 +3061,8 @@
         <v>499</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="12"/>
+    <row r="43" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
       <c r="B43" t="s">
         <v>0</v>
       </c>
@@ -3076,8 +3076,8 @@
         <v>501</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="12"/>
+    <row r="44" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
       <c r="B44" t="s">
         <v>0</v>
       </c>
@@ -3091,8 +3091,8 @@
         <v>173</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="12"/>
+    <row r="45" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
       <c r="B45" t="s">
         <v>0</v>
       </c>
@@ -3106,8 +3106,8 @@
         <v>174</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="12"/>
+    <row r="46" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
       <c r="B46" t="s">
         <v>0</v>
       </c>
@@ -3121,8 +3121,8 @@
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="12"/>
+    <row r="47" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
       <c r="B47" t="s">
         <v>0</v>
       </c>
@@ -3136,14 +3136,14 @@
         <v>176</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="8"/>
     </row>
-    <row r="49" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="8"/>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="13" t="s">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
         <v>182</v>
       </c>
       <c r="D50" t="s">
@@ -3153,8 +3153,8 @@
         <v>184</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="13"/>
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="12"/>
       <c r="D51" t="s">
         <v>185</v>
       </c>
@@ -3162,8 +3162,8 @@
         <v>186</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="13"/>
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="12"/>
       <c r="D52" t="s">
         <v>187</v>
       </c>
@@ -3171,8 +3171,8 @@
         <v>190</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="13"/>
+    <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="12"/>
       <c r="D53" t="s">
         <v>188</v>
       </c>
@@ -3180,8 +3180,8 @@
         <v>189</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="13"/>
+    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="12"/>
       <c r="D54" t="s">
         <v>191</v>
       </c>
@@ -3189,8 +3189,8 @@
         <v>192</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="13"/>
+    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="12"/>
       <c r="B55" t="s">
         <v>221</v>
       </c>
@@ -3201,8 +3201,8 @@
         <v>212</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="13"/>
+    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="12"/>
       <c r="B56" t="s">
         <v>224</v>
       </c>
@@ -3213,8 +3213,8 @@
         <v>213</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="13"/>
+    <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="12"/>
       <c r="B57" t="s">
         <v>223</v>
       </c>
@@ -3225,8 +3225,8 @@
         <v>211</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="13"/>
+    <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="12"/>
       <c r="B58" t="s">
         <v>222</v>
       </c>
@@ -3237,8 +3237,8 @@
         <v>220</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="13"/>
+    <row r="59" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="12"/>
       <c r="D59" t="s">
         <v>688</v>
       </c>
@@ -3246,11 +3246,11 @@
         <v>689</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
     </row>
-    <row r="62" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="13" t="s">
+    <row r="62" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B62" t="s">
@@ -3266,8 +3266,8 @@
         <v>147</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="13"/>
+    <row r="63" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="12"/>
       <c r="B63" t="s">
         <v>2</v>
       </c>
@@ -3281,8 +3281,8 @@
         <v>237</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="13"/>
+    <row r="64" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="12"/>
       <c r="B64" t="s">
         <v>4</v>
       </c>
@@ -3296,8 +3296,8 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="13"/>
+    <row r="65" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="12"/>
       <c r="B65" t="s">
         <v>6</v>
       </c>
@@ -3311,8 +3311,8 @@
         <v>235</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="13"/>
+    <row r="66" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="12"/>
       <c r="B66" t="s">
         <v>8</v>
       </c>
@@ -3326,8 +3326,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="13"/>
+    <row r="67" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="12"/>
       <c r="B67" t="s">
         <v>10</v>
       </c>
@@ -3341,8 +3341,8 @@
         <v>233</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="13"/>
+    <row r="68" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="12"/>
       <c r="B68" t="s">
         <v>12</v>
       </c>
@@ -3356,8 +3356,8 @@
         <v>234</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="13"/>
+    <row r="69" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="12"/>
       <c r="B69" t="s">
         <v>14</v>
       </c>
@@ -3371,8 +3371,8 @@
         <v>231</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="13"/>
+    <row r="70" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="12"/>
       <c r="B70" t="s">
         <v>16</v>
       </c>
@@ -3386,8 +3386,8 @@
         <v>230</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="13"/>
+    <row r="71" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="12"/>
       <c r="B71" t="s">
         <v>18</v>
       </c>
@@ -3401,8 +3401,8 @@
         <v>232</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="13"/>
+    <row r="72" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="12"/>
       <c r="D72" t="s">
         <v>240</v>
       </c>
@@ -3413,8 +3413,8 @@
         <v>245</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="13"/>
+    <row r="73" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="12"/>
       <c r="D73" t="s">
         <v>241</v>
       </c>
@@ -3425,8 +3425,8 @@
         <v>243</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="13"/>
+    <row r="74" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="12"/>
       <c r="D74" t="s">
         <v>242</v>
       </c>
@@ -3437,14 +3437,14 @@
         <v>244</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
     </row>
-    <row r="76" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
     </row>
-    <row r="77" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="13" t="s">
+    <row r="77" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="12" t="s">
         <v>603</v>
       </c>
       <c r="B77" t="s">
@@ -3460,8 +3460,8 @@
         <v>267</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="13"/>
+    <row r="78" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="12"/>
       <c r="B78" t="s">
         <v>74</v>
       </c>
@@ -3475,8 +3475,8 @@
         <v>268</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="13"/>
+    <row r="79" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="12"/>
       <c r="B79" t="s">
         <v>76</v>
       </c>
@@ -3490,8 +3490,8 @@
         <v>238</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="13"/>
+    <row r="80" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="12"/>
       <c r="B80" t="s">
         <v>78</v>
       </c>
@@ -3505,8 +3505,8 @@
         <v>269</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="13"/>
+    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="12"/>
       <c r="B81" t="s">
         <v>80</v>
       </c>
@@ -3520,8 +3520,8 @@
         <v>270</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="13"/>
+    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="12"/>
       <c r="B82" t="s">
         <v>82</v>
       </c>
@@ -3535,8 +3535,8 @@
         <v>271</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="13"/>
+    <row r="83" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="12"/>
       <c r="D83" t="s">
         <v>586</v>
       </c>
@@ -3547,8 +3547,8 @@
         <v>587</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="13"/>
+    <row r="84" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="12"/>
       <c r="D84" t="s">
         <v>569</v>
       </c>
@@ -3559,8 +3559,8 @@
         <v>588</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="13"/>
+    <row r="85" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="12"/>
       <c r="D85" t="s">
         <v>570</v>
       </c>
@@ -3571,8 +3571,8 @@
         <v>589</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="13"/>
+    <row r="86" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="12"/>
       <c r="D86" t="s">
         <v>571</v>
       </c>
@@ -3583,8 +3583,8 @@
         <v>602</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="13"/>
+    <row r="87" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="12"/>
       <c r="D87" t="s">
         <v>572</v>
       </c>
@@ -3595,8 +3595,8 @@
         <v>357</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="13"/>
+    <row r="88" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="12"/>
       <c r="D88" t="s">
         <v>573</v>
       </c>
@@ -3607,8 +3607,8 @@
         <v>590</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="13"/>
+    <row r="89" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="12"/>
       <c r="D89" t="s">
         <v>574</v>
       </c>
@@ -3619,8 +3619,8 @@
         <v>591</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="13"/>
+    <row r="90" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="12"/>
       <c r="D90" t="s">
         <v>575</v>
       </c>
@@ -3631,8 +3631,8 @@
         <v>592</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="13"/>
+    <row r="91" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="12"/>
       <c r="D91" t="s">
         <v>576</v>
       </c>
@@ -3643,8 +3643,8 @@
         <v>508</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="13"/>
+    <row r="92" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="12"/>
       <c r="D92" t="s">
         <v>577</v>
       </c>
@@ -3655,8 +3655,8 @@
         <v>593</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="13"/>
+    <row r="93" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="12"/>
       <c r="D93" t="s">
         <v>578</v>
       </c>
@@ -3667,8 +3667,8 @@
         <v>594</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="13"/>
+    <row r="94" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="12"/>
       <c r="D94" t="s">
         <v>579</v>
       </c>
@@ -3679,8 +3679,8 @@
         <v>595</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="13"/>
+    <row r="95" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="12"/>
       <c r="D95" t="s">
         <v>580</v>
       </c>
@@ -3691,8 +3691,8 @@
         <v>596</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="13"/>
+    <row r="96" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="12"/>
       <c r="D96" t="s">
         <v>581</v>
       </c>
@@ -3703,8 +3703,8 @@
         <v>597</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="13"/>
+    <row r="97" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="12"/>
       <c r="D97" t="s">
         <v>582</v>
       </c>
@@ -3715,8 +3715,8 @@
         <v>598</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="13"/>
+    <row r="98" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="12"/>
       <c r="D98" t="s">
         <v>583</v>
       </c>
@@ -3727,8 +3727,8 @@
         <v>599</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="13"/>
+    <row r="99" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="12"/>
       <c r="D99" t="s">
         <v>584</v>
       </c>
@@ -3739,8 +3739,8 @@
         <v>600</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="13"/>
+    <row r="100" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="12"/>
       <c r="D100" t="s">
         <v>585</v>
       </c>
@@ -3751,8 +3751,8 @@
         <v>601</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="13" t="s">
+    <row r="103" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="12" t="s">
         <v>340</v>
       </c>
       <c r="B103" t="s">
@@ -3768,8 +3768,8 @@
         <v>260</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="13"/>
+    <row r="104" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="12"/>
       <c r="D104" t="s">
         <v>629</v>
       </c>
@@ -3780,8 +3780,8 @@
         <v>630</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="13"/>
+    <row r="105" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="12"/>
       <c r="B105" t="s">
         <v>22</v>
       </c>
@@ -3795,8 +3795,8 @@
         <v>261</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="13"/>
+    <row r="106" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="12"/>
       <c r="B106" t="s">
         <v>26</v>
       </c>
@@ -3810,8 +3810,8 @@
         <v>246</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="13"/>
+    <row r="107" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="12"/>
       <c r="B107" t="s">
         <v>28</v>
       </c>
@@ -3825,8 +3825,8 @@
         <v>247</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="13"/>
+    <row r="108" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="12"/>
       <c r="B108" t="s">
         <v>30</v>
       </c>
@@ -3840,8 +3840,8 @@
         <v>248</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="13"/>
+    <row r="109" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="12"/>
       <c r="B109" t="s">
         <v>32</v>
       </c>
@@ -3855,8 +3855,8 @@
         <v>249</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="13"/>
+    <row r="110" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="12"/>
       <c r="B110" t="s">
         <v>33</v>
       </c>
@@ -3870,8 +3870,8 @@
         <v>250</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="13"/>
+    <row r="111" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="12"/>
       <c r="B111" t="s">
         <v>36</v>
       </c>
@@ -3885,8 +3885,8 @@
         <v>251</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="13"/>
+    <row r="112" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="12"/>
       <c r="B112" t="s">
         <v>38</v>
       </c>
@@ -3900,8 +3900,8 @@
         <v>262</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="13"/>
+    <row r="113" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="12"/>
       <c r="D113" t="s">
         <v>321</v>
       </c>
@@ -3912,8 +3912,8 @@
         <v>322</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="13"/>
+    <row r="114" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="12"/>
       <c r="B114" t="s">
         <v>40</v>
       </c>
@@ -3927,8 +3927,8 @@
         <v>252</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="13"/>
+    <row r="115" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="12"/>
       <c r="D115" t="s">
         <v>323</v>
       </c>
@@ -3939,8 +3939,8 @@
         <v>324</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="13"/>
+    <row r="116" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="12"/>
       <c r="B116" t="s">
         <v>41</v>
       </c>
@@ -3954,8 +3954,8 @@
         <v>263</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="13"/>
+    <row r="117" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="12"/>
       <c r="D117" t="s">
         <v>325</v>
       </c>
@@ -3966,8 +3966,8 @@
         <v>327</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="13"/>
+    <row r="118" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="12"/>
       <c r="B118" t="s">
         <v>42</v>
       </c>
@@ -3981,8 +3981,8 @@
         <v>253</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="13"/>
+    <row r="119" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="12"/>
       <c r="D119" t="s">
         <v>326</v>
       </c>
@@ -3993,8 +3993,8 @@
         <v>328</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="13"/>
+    <row r="120" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="12"/>
       <c r="B120" t="s">
         <v>43</v>
       </c>
@@ -4008,8 +4008,8 @@
         <v>264</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="13"/>
+    <row r="121" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="12"/>
       <c r="B121" t="s">
         <v>49</v>
       </c>
@@ -4023,8 +4023,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="13"/>
+    <row r="122" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="12"/>
       <c r="B122" t="s">
         <v>51</v>
       </c>
@@ -4038,8 +4038,8 @@
         <v>254</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="13"/>
+    <row r="123" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="12"/>
       <c r="D123" t="s">
         <v>313</v>
       </c>
@@ -4050,8 +4050,8 @@
         <v>314</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="13"/>
+    <row r="124" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="12"/>
       <c r="D124" t="s">
         <v>315</v>
       </c>
@@ -4062,8 +4062,8 @@
         <v>316</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="13"/>
+    <row r="125" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="12"/>
       <c r="D125" t="s">
         <v>317</v>
       </c>
@@ -4074,8 +4074,8 @@
         <v>318</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="13"/>
+    <row r="126" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="12"/>
       <c r="D126" t="s">
         <v>319</v>
       </c>
@@ -4086,8 +4086,8 @@
         <v>329</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="13"/>
+    <row r="127" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="12"/>
       <c r="D127" t="s">
         <v>320</v>
       </c>
@@ -4098,8 +4098,8 @@
         <v>330</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="13"/>
+    <row r="128" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="12"/>
       <c r="D128" t="s">
         <v>331</v>
       </c>
@@ -4110,8 +4110,8 @@
         <v>332</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="13"/>
+    <row r="129" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="12"/>
       <c r="D129" t="s">
         <v>333</v>
       </c>
@@ -4122,8 +4122,8 @@
         <v>335</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="13"/>
+    <row r="130" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="12"/>
       <c r="D130" t="s">
         <v>334</v>
       </c>
@@ -4134,8 +4134,8 @@
         <v>336</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="13"/>
+    <row r="131" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="12"/>
       <c r="D131" t="s">
         <v>337</v>
       </c>
@@ -4146,8 +4146,8 @@
         <v>338</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="13"/>
+    <row r="132" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="12"/>
       <c r="D132" t="s">
         <v>374</v>
       </c>
@@ -4158,8 +4158,8 @@
         <v>392</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="13"/>
+    <row r="133" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="12"/>
       <c r="D133" t="s">
         <v>375</v>
       </c>
@@ -4170,8 +4170,8 @@
         <v>357</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="13"/>
+    <row r="134" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="12"/>
       <c r="D134" t="s">
         <v>376</v>
       </c>
@@ -4182,8 +4182,8 @@
         <v>422</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="13"/>
+    <row r="135" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="12"/>
       <c r="D135" t="s">
         <v>421</v>
       </c>
@@ -4194,8 +4194,8 @@
         <v>391</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="13"/>
+    <row r="136" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="12"/>
       <c r="D136" t="s">
         <v>507</v>
       </c>
@@ -4206,8 +4206,8 @@
         <v>508</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="13"/>
+    <row r="137" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="12"/>
       <c r="D137" t="s">
         <v>377</v>
       </c>
@@ -4218,8 +4218,8 @@
         <v>390</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="13"/>
+    <row r="138" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="12"/>
       <c r="D138" t="s">
         <v>378</v>
       </c>
@@ -4230,8 +4230,8 @@
         <v>389</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="13"/>
+    <row r="139" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="12"/>
       <c r="D139" t="s">
         <v>379</v>
       </c>
@@ -4242,8 +4242,8 @@
         <v>385</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="13"/>
+    <row r="140" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="12"/>
       <c r="D140" t="s">
         <v>380</v>
       </c>
@@ -4254,8 +4254,8 @@
         <v>386</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="13"/>
+    <row r="141" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="12"/>
       <c r="D141" t="s">
         <v>381</v>
       </c>
@@ -4266,8 +4266,8 @@
         <v>383</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="13"/>
+    <row r="142" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="12"/>
       <c r="D142" t="s">
         <v>382</v>
       </c>
@@ -4278,8 +4278,8 @@
         <v>371</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="13"/>
+    <row r="143" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="12"/>
       <c r="D143" t="s">
         <v>681</v>
       </c>
@@ -4290,8 +4290,8 @@
         <v>687</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="13"/>
+    <row r="144" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="12"/>
       <c r="D144" t="s">
         <v>682</v>
       </c>
@@ -4302,8 +4302,8 @@
         <v>687</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="13"/>
+    <row r="145" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="12"/>
       <c r="D145" t="s">
         <v>683</v>
       </c>
@@ -4314,8 +4314,8 @@
         <v>687</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="13"/>
+    <row r="146" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="12"/>
       <c r="D146" t="s">
         <v>684</v>
       </c>
@@ -4326,14 +4326,14 @@
         <v>687</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="7"/>
     </row>
-    <row r="148" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="7"/>
     </row>
-    <row r="149" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="13" t="s">
+    <row r="149" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="12" t="s">
         <v>339</v>
       </c>
       <c r="B149" t="s">
@@ -4349,8 +4349,8 @@
         <v>285</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="13"/>
+    <row r="150" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="12"/>
       <c r="B150" t="s">
         <v>95</v>
       </c>
@@ -4364,8 +4364,8 @@
         <v>300</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="13"/>
+    <row r="151" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="12"/>
       <c r="B151" t="s">
         <v>96</v>
       </c>
@@ -4379,8 +4379,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="13"/>
+    <row r="152" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="12"/>
       <c r="B152" t="s">
         <v>97</v>
       </c>
@@ -4394,8 +4394,8 @@
         <v>298</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="13"/>
+    <row r="153" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="12"/>
       <c r="B153" t="s">
         <v>273</v>
       </c>
@@ -4409,8 +4409,8 @@
         <v>297</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="13"/>
+    <row r="154" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="12"/>
       <c r="B154" t="s">
         <v>274</v>
       </c>
@@ -4424,8 +4424,8 @@
         <v>296</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="13"/>
+    <row r="155" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="12"/>
       <c r="B155" t="s">
         <v>275</v>
       </c>
@@ -4439,8 +4439,8 @@
         <v>295</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="13"/>
+    <row r="156" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="12"/>
       <c r="B156" t="s">
         <v>276</v>
       </c>
@@ -4454,8 +4454,8 @@
         <v>294</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="13"/>
+    <row r="157" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="12"/>
       <c r="B157" t="s">
         <v>277</v>
       </c>
@@ -4469,8 +4469,8 @@
         <v>293</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="13"/>
+    <row r="158" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="12"/>
       <c r="B158" t="s">
         <v>278</v>
       </c>
@@ -4484,8 +4484,8 @@
         <v>292</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="13"/>
+    <row r="159" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="12"/>
       <c r="B159" t="s">
         <v>279</v>
       </c>
@@ -4499,8 +4499,8 @@
         <v>291</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="13"/>
+    <row r="160" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="12"/>
       <c r="B160" t="s">
         <v>280</v>
       </c>
@@ -4514,8 +4514,8 @@
         <v>290</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="13"/>
+    <row r="161" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="12"/>
       <c r="B161" t="s">
         <v>281</v>
       </c>
@@ -4529,8 +4529,8 @@
         <v>289</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="13"/>
+    <row r="162" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="12"/>
       <c r="B162" t="s">
         <v>282</v>
       </c>
@@ -4544,8 +4544,8 @@
         <v>288</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="13"/>
+    <row r="163" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="12"/>
       <c r="B163" t="s">
         <v>283</v>
       </c>
@@ -4559,8 +4559,8 @@
         <v>287</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="13"/>
+    <row r="164" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="12"/>
       <c r="B164" t="s">
         <v>284</v>
       </c>
@@ -4574,14 +4574,14 @@
         <v>286</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3"/>
     </row>
-    <row r="166" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3"/>
     </row>
-    <row r="167" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="13" t="s">
+    <row r="167" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="12" t="s">
         <v>344</v>
       </c>
       <c r="B167" t="s">
@@ -4597,8 +4597,8 @@
         <v>255</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="13"/>
+    <row r="168" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="12"/>
       <c r="B168" t="s">
         <v>68</v>
       </c>
@@ -4612,8 +4612,8 @@
         <v>256</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="13"/>
+    <row r="169" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="12"/>
       <c r="B169" t="s">
         <v>69</v>
       </c>
@@ -4627,8 +4627,8 @@
         <v>265</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="13"/>
+    <row r="170" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="12"/>
       <c r="B170" t="s">
         <v>70</v>
       </c>
@@ -4642,8 +4642,8 @@
         <v>239</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="13"/>
+    <row r="171" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="12"/>
       <c r="B171" t="s">
         <v>71</v>
       </c>
@@ -4657,8 +4657,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="13"/>
+    <row r="172" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="12"/>
       <c r="D172" t="s">
         <v>348</v>
       </c>
@@ -4669,8 +4669,8 @@
         <v>361</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="13"/>
+    <row r="173" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="12"/>
       <c r="D173" t="s">
         <v>355</v>
       </c>
@@ -4681,8 +4681,8 @@
         <v>369</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="13"/>
+    <row r="174" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="12"/>
       <c r="D174" t="s">
         <v>356</v>
       </c>
@@ -4693,8 +4693,8 @@
         <v>370</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="13"/>
+    <row r="175" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="12"/>
       <c r="D175" t="s">
         <v>347</v>
       </c>
@@ -4705,8 +4705,8 @@
         <v>360</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="13"/>
+    <row r="176" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="12"/>
       <c r="D176" t="s">
         <v>349</v>
       </c>
@@ -4717,8 +4717,8 @@
         <v>357</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="13"/>
+    <row r="177" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="12"/>
       <c r="D177" t="s">
         <v>350</v>
       </c>
@@ -4729,8 +4729,8 @@
         <v>423</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="13"/>
+    <row r="178" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="12"/>
       <c r="D178" t="s">
         <v>420</v>
       </c>
@@ -4741,8 +4741,8 @@
         <v>358</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="13"/>
+    <row r="179" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="12"/>
       <c r="D179" t="s">
         <v>568</v>
       </c>
@@ -4753,8 +4753,8 @@
         <v>567</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="13"/>
+    <row r="180" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="12"/>
       <c r="D180" t="s">
         <v>509</v>
       </c>
@@ -4765,8 +4765,8 @@
         <v>508</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="13"/>
+    <row r="181" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="12"/>
       <c r="D181" t="s">
         <v>364</v>
       </c>
@@ -4777,8 +4777,8 @@
         <v>366</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A182" s="13"/>
+    <row r="182" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="12"/>
       <c r="D182" t="s">
         <v>365</v>
       </c>
@@ -4789,8 +4789,8 @@
         <v>367</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="13"/>
+    <row r="183" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="12"/>
       <c r="D183" t="s">
         <v>352</v>
       </c>
@@ -4801,8 +4801,8 @@
         <v>384</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A184" s="13"/>
+    <row r="184" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="12"/>
       <c r="D184" t="s">
         <v>353</v>
       </c>
@@ -4813,8 +4813,8 @@
         <v>368</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A185" s="13"/>
+    <row r="185" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="12"/>
       <c r="D185" t="s">
         <v>354</v>
       </c>
@@ -4825,8 +4825,8 @@
         <v>387</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A186" s="13"/>
+    <row r="186" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="12"/>
       <c r="D186" t="s">
         <v>346</v>
       </c>
@@ -4837,8 +4837,8 @@
         <v>371</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="13"/>
+    <row r="187" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="12"/>
       <c r="D187" t="s">
         <v>351</v>
       </c>
@@ -4849,8 +4849,8 @@
         <v>359</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="13"/>
+    <row r="188" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="12"/>
       <c r="D188" t="s">
         <v>362</v>
       </c>
@@ -4861,8 +4861,8 @@
         <v>363</v>
       </c>
     </row>
-    <row r="189" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="13"/>
+    <row r="189" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="12"/>
       <c r="D189" t="s">
         <v>372</v>
       </c>
@@ -4873,14 +4873,14 @@
         <v>373</v>
       </c>
     </row>
-    <row r="190" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="10"/>
     </row>
-    <row r="191" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3"/>
     </row>
-    <row r="192" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A192" s="13" t="s">
+    <row r="192" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="12" t="s">
         <v>524</v>
       </c>
       <c r="D192" t="s">
@@ -4893,8 +4893,8 @@
         <v>525</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A193" s="13"/>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" s="12"/>
       <c r="D193" t="s">
         <v>545</v>
       </c>
@@ -4905,8 +4905,8 @@
         <v>256</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A194" s="13"/>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" s="12"/>
       <c r="D194" t="s">
         <v>546</v>
       </c>
@@ -4917,8 +4917,8 @@
         <v>526</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A195" s="13"/>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" s="12"/>
       <c r="D195" t="s">
         <v>547</v>
       </c>
@@ -4929,8 +4929,8 @@
         <v>527</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A196" s="13"/>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" s="12"/>
       <c r="D196" t="s">
         <v>548</v>
       </c>
@@ -4941,8 +4941,8 @@
         <v>528</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A197" s="13"/>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" s="12"/>
       <c r="D197" t="s">
         <v>549</v>
       </c>
@@ -4953,8 +4953,8 @@
         <v>529</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A198" s="13"/>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" s="12"/>
       <c r="D198" t="s">
         <v>550</v>
       </c>
@@ -4965,8 +4965,8 @@
         <v>530</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A199" s="13"/>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199" s="12"/>
       <c r="D199" t="s">
         <v>551</v>
       </c>
@@ -4977,8 +4977,8 @@
         <v>531</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A200" s="13"/>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200" s="12"/>
       <c r="D200" t="s">
         <v>552</v>
       </c>
@@ -4989,8 +4989,8 @@
         <v>532</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A201" s="13"/>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201" s="12"/>
       <c r="D201" t="s">
         <v>553</v>
       </c>
@@ -5001,8 +5001,8 @@
         <v>357</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A202" s="13"/>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202" s="12"/>
       <c r="D202" t="s">
         <v>554</v>
       </c>
@@ -5013,8 +5013,8 @@
         <v>533</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A203" s="13"/>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203" s="12"/>
       <c r="D203" t="s">
         <v>555</v>
       </c>
@@ -5025,8 +5025,8 @@
         <v>534</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A204" s="13"/>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204" s="12"/>
       <c r="D204" t="s">
         <v>556</v>
       </c>
@@ -5037,8 +5037,8 @@
         <v>535</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A205" s="13"/>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205" s="12"/>
       <c r="D205" t="s">
         <v>557</v>
       </c>
@@ -5049,8 +5049,8 @@
         <v>508</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A206" s="13"/>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206" s="12"/>
       <c r="D206" t="s">
         <v>558</v>
       </c>
@@ -5061,8 +5061,8 @@
         <v>536</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A207" s="13"/>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207" s="12"/>
       <c r="D207" t="s">
         <v>559</v>
       </c>
@@ -5073,8 +5073,8 @@
         <v>537</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A208" s="13"/>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208" s="12"/>
       <c r="D208" t="s">
         <v>560</v>
       </c>
@@ -5085,8 +5085,8 @@
         <v>538</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A209" s="13"/>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209" s="12"/>
       <c r="D209" t="s">
         <v>561</v>
       </c>
@@ -5097,8 +5097,8 @@
         <v>539</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A210" s="13"/>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210" s="12"/>
       <c r="D210" t="s">
         <v>562</v>
       </c>
@@ -5109,8 +5109,8 @@
         <v>540</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A211" s="13"/>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211" s="12"/>
       <c r="D211" t="s">
         <v>563</v>
       </c>
@@ -5121,8 +5121,8 @@
         <v>541</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A212" s="13"/>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" s="12"/>
       <c r="D212" t="s">
         <v>564</v>
       </c>
@@ -5133,8 +5133,8 @@
         <v>542</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A213" s="13"/>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213" s="12"/>
       <c r="D213" t="s">
         <v>565</v>
       </c>
@@ -5145,8 +5145,8 @@
         <v>543</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A214" s="13"/>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214" s="12"/>
       <c r="D214" t="s">
         <v>566</v>
       </c>
@@ -5157,14 +5157,14 @@
         <v>407</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="11"/>
     </row>
-    <row r="216" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="3"/>
     </row>
-    <row r="217" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A217" s="13" t="s">
+    <row r="217" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A217" s="12" t="s">
         <v>345</v>
       </c>
       <c r="D217" t="s">
@@ -5177,8 +5177,8 @@
         <v>272</v>
       </c>
     </row>
-    <row r="218" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A218" s="13"/>
+    <row r="218" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A218" s="12"/>
       <c r="D218" t="s">
         <v>90</v>
       </c>
@@ -5189,8 +5189,8 @@
         <v>256</v>
       </c>
     </row>
-    <row r="219" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A219" s="13"/>
+    <row r="219" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A219" s="12"/>
       <c r="D219" t="s">
         <v>91</v>
       </c>
@@ -5201,8 +5201,8 @@
         <v>269</v>
       </c>
     </row>
-    <row r="220" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A220" s="13"/>
+    <row r="220" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="12"/>
       <c r="D220" t="s">
         <v>92</v>
       </c>
@@ -5213,8 +5213,8 @@
         <v>266</v>
       </c>
     </row>
-    <row r="221" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A221" s="13"/>
+    <row r="221" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A221" s="12"/>
       <c r="D221" t="s">
         <v>93</v>
       </c>
@@ -5225,8 +5225,8 @@
         <v>149</v>
       </c>
     </row>
-    <row r="222" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A222" s="13"/>
+    <row r="222" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A222" s="12"/>
       <c r="D222" t="s">
         <v>388</v>
       </c>
@@ -5237,8 +5237,8 @@
         <v>418</v>
       </c>
     </row>
-    <row r="223" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A223" s="13"/>
+    <row r="223" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="12"/>
       <c r="D223" t="s">
         <v>393</v>
       </c>
@@ -5249,8 +5249,8 @@
         <v>416</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A224" s="13"/>
+    <row r="224" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A224" s="12"/>
       <c r="D224" t="s">
         <v>394</v>
       </c>
@@ -5261,8 +5261,8 @@
         <v>417</v>
       </c>
     </row>
-    <row r="225" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="13"/>
+    <row r="225" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="12"/>
       <c r="D225" t="s">
         <v>395</v>
       </c>
@@ -5273,8 +5273,8 @@
         <v>523</v>
       </c>
     </row>
-    <row r="226" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A226" s="13"/>
+    <row r="226" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A226" s="12"/>
       <c r="D226" t="s">
         <v>396</v>
       </c>
@@ -5285,8 +5285,8 @@
         <v>357</v>
       </c>
     </row>
-    <row r="227" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A227" s="13"/>
+    <row r="227" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="12"/>
       <c r="D227" t="s">
         <v>397</v>
       </c>
@@ -5297,8 +5297,8 @@
         <v>521</v>
       </c>
     </row>
-    <row r="228" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A228" s="13"/>
+    <row r="228" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="12"/>
       <c r="D228" t="s">
         <v>419</v>
       </c>
@@ -5309,8 +5309,8 @@
         <v>522</v>
       </c>
     </row>
-    <row r="229" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A229" s="13"/>
+    <row r="229" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="12"/>
       <c r="D229" t="s">
         <v>519</v>
       </c>
@@ -5321,8 +5321,8 @@
         <v>520</v>
       </c>
     </row>
-    <row r="230" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A230" s="13"/>
+    <row r="230" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="12"/>
       <c r="D230" t="s">
         <v>510</v>
       </c>
@@ -5333,8 +5333,8 @@
         <v>508</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A231" s="13"/>
+    <row r="231" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="12"/>
       <c r="D231" t="s">
         <v>398</v>
       </c>
@@ -5345,8 +5345,8 @@
         <v>415</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A232" s="13"/>
+    <row r="232" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="12"/>
       <c r="D232" t="s">
         <v>399</v>
       </c>
@@ -5357,8 +5357,8 @@
         <v>414</v>
       </c>
     </row>
-    <row r="233" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A233" s="13"/>
+    <row r="233" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="12"/>
       <c r="D233" t="s">
         <v>400</v>
       </c>
@@ -5369,8 +5369,8 @@
         <v>413</v>
       </c>
     </row>
-    <row r="234" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="13"/>
+    <row r="234" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="12"/>
       <c r="D234" t="s">
         <v>401</v>
       </c>
@@ -5381,8 +5381,8 @@
         <v>412</v>
       </c>
     </row>
-    <row r="235" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A235" s="13"/>
+    <row r="235" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="12"/>
       <c r="D235" t="s">
         <v>402</v>
       </c>
@@ -5393,8 +5393,8 @@
         <v>411</v>
       </c>
     </row>
-    <row r="236" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A236" s="13"/>
+    <row r="236" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="12"/>
       <c r="D236" t="s">
         <v>403</v>
       </c>
@@ -5405,8 +5405,8 @@
         <v>410</v>
       </c>
     </row>
-    <row r="237" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A237" s="13"/>
+    <row r="237" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="12"/>
       <c r="D237" t="s">
         <v>404</v>
       </c>
@@ -5417,8 +5417,8 @@
         <v>409</v>
       </c>
     </row>
-    <row r="238" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A238" s="13"/>
+    <row r="238" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="12"/>
       <c r="D238" t="s">
         <v>405</v>
       </c>
@@ -5429,8 +5429,8 @@
         <v>408</v>
       </c>
     </row>
-    <row r="239" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A239" s="13"/>
+    <row r="239" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="12"/>
       <c r="D239" t="s">
         <v>406</v>
       </c>
@@ -5441,11 +5441,11 @@
         <v>407</v>
       </c>
     </row>
-    <row r="240" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="3"/>
     </row>
-    <row r="242" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A242" s="13" t="s">
+    <row r="242" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="12" t="s">
         <v>341</v>
       </c>
       <c r="B242" t="s">
@@ -5461,8 +5461,8 @@
         <v>448</v>
       </c>
     </row>
-    <row r="243" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A243" s="13"/>
+    <row r="243" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="12"/>
       <c r="B243" t="s">
         <v>100</v>
       </c>
@@ -5476,8 +5476,8 @@
         <v>151</v>
       </c>
     </row>
-    <row r="244" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A244" s="13"/>
+    <row r="244" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="12"/>
       <c r="B244" t="s">
         <v>102</v>
       </c>
@@ -5491,8 +5491,8 @@
         <v>153</v>
       </c>
     </row>
-    <row r="245" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A245" s="13"/>
+    <row r="245" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="12"/>
       <c r="B245" t="s">
         <v>104</v>
       </c>
@@ -5506,8 +5506,8 @@
         <v>425</v>
       </c>
     </row>
-    <row r="246" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A246" s="13"/>
+    <row r="246" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="12"/>
       <c r="B246" t="s">
         <v>108</v>
       </c>
@@ -5521,8 +5521,8 @@
         <v>426</v>
       </c>
     </row>
-    <row r="247" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A247" s="13"/>
+    <row r="247" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="12"/>
       <c r="B247" t="s">
         <v>106</v>
       </c>
@@ -5533,8 +5533,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="248" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A248" s="13"/>
+    <row r="248" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="12"/>
       <c r="D248" t="s">
         <v>427</v>
       </c>
@@ -5545,8 +5545,8 @@
         <v>447</v>
       </c>
     </row>
-    <row r="249" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A249" s="13"/>
+    <row r="249" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A249" s="12"/>
       <c r="D249" t="s">
         <v>428</v>
       </c>
@@ -5557,8 +5557,8 @@
         <v>357</v>
       </c>
     </row>
-    <row r="250" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A250" s="13"/>
+    <row r="250" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="12"/>
       <c r="D250" t="s">
         <v>429</v>
       </c>
@@ -5569,8 +5569,8 @@
         <v>446</v>
       </c>
     </row>
-    <row r="251" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A251" s="13"/>
+    <row r="251" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="12"/>
       <c r="D251" t="s">
         <v>513</v>
       </c>
@@ -5581,8 +5581,8 @@
         <v>514</v>
       </c>
     </row>
-    <row r="252" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A252" s="13"/>
+    <row r="252" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="12"/>
       <c r="D252" t="s">
         <v>511</v>
       </c>
@@ -5593,8 +5593,8 @@
         <v>515</v>
       </c>
     </row>
-    <row r="253" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A253" s="13"/>
+    <row r="253" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="12"/>
       <c r="D253" t="s">
         <v>430</v>
       </c>
@@ -5605,8 +5605,8 @@
         <v>445</v>
       </c>
     </row>
-    <row r="254" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A254" s="13"/>
+    <row r="254" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A254" s="12"/>
       <c r="D254" t="s">
         <v>431</v>
       </c>
@@ -5617,8 +5617,8 @@
         <v>444</v>
       </c>
     </row>
-    <row r="255" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A255" s="13"/>
+    <row r="255" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A255" s="12"/>
       <c r="D255" t="s">
         <v>432</v>
       </c>
@@ -5629,8 +5629,8 @@
         <v>443</v>
       </c>
     </row>
-    <row r="256" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A256" s="13"/>
+    <row r="256" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A256" s="12"/>
       <c r="D256" t="s">
         <v>433</v>
       </c>
@@ -5641,8 +5641,8 @@
         <v>442</v>
       </c>
     </row>
-    <row r="257" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A257" s="13"/>
+    <row r="257" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="12"/>
       <c r="D257" t="s">
         <v>434</v>
       </c>
@@ -5653,8 +5653,8 @@
         <v>441</v>
       </c>
     </row>
-    <row r="258" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A258" s="13"/>
+    <row r="258" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A258" s="12"/>
       <c r="D258" t="s">
         <v>435</v>
       </c>
@@ -5665,8 +5665,8 @@
         <v>440</v>
       </c>
     </row>
-    <row r="259" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A259" s="13"/>
+    <row r="259" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A259" s="12"/>
       <c r="D259" t="s">
         <v>436</v>
       </c>
@@ -5677,8 +5677,8 @@
         <v>439</v>
       </c>
     </row>
-    <row r="260" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A260" s="13"/>
+    <row r="260" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="12"/>
       <c r="D260" t="s">
         <v>437</v>
       </c>
@@ -5689,8 +5689,8 @@
         <v>438</v>
       </c>
     </row>
-    <row r="261" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A261" s="13"/>
+    <row r="261" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A261" s="12"/>
       <c r="D261" t="s">
         <v>632</v>
       </c>
@@ -5698,8 +5698,8 @@
         <v>631</v>
       </c>
     </row>
-    <row r="262" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A262" s="13"/>
+    <row r="262" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A262" s="12"/>
       <c r="D262" t="s">
         <v>653</v>
       </c>
@@ -5707,8 +5707,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="263" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A263" s="13"/>
+    <row r="263" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A263" s="12"/>
       <c r="D263" t="s">
         <v>654</v>
       </c>
@@ -5716,8 +5716,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="264" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A264" s="13"/>
+    <row r="264" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A264" s="12"/>
       <c r="D264" t="s">
         <v>424</v>
       </c>
@@ -5725,8 +5725,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="265" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A265" s="13"/>
+    <row r="265" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="12"/>
       <c r="D265" t="s">
         <v>635</v>
       </c>
@@ -5734,8 +5734,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A266" s="13"/>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266" s="12"/>
       <c r="D266" t="s">
         <v>636</v>
       </c>
@@ -5743,8 +5743,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A267" s="13"/>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267" s="12"/>
       <c r="D267" t="s">
         <v>633</v>
       </c>
@@ -5752,8 +5752,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A268" s="13"/>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268" s="12"/>
       <c r="D268" t="s">
         <v>634</v>
       </c>
@@ -5761,8 +5761,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A269" s="13"/>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269" s="12"/>
       <c r="D269" t="s">
         <v>637</v>
       </c>
@@ -5770,8 +5770,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A270" s="13"/>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270" s="12"/>
       <c r="D270" t="s">
         <v>638</v>
       </c>
@@ -5779,8 +5779,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A271" s="13"/>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271" s="12"/>
       <c r="D271" t="s">
         <v>639</v>
       </c>
@@ -5791,8 +5791,8 @@
         <v>680</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A272" s="13"/>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A272" s="12"/>
       <c r="D272" t="s">
         <v>646</v>
       </c>
@@ -5803,8 +5803,8 @@
         <v>674</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A273" s="13"/>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A273" s="12"/>
       <c r="D273" t="s">
         <v>640</v>
       </c>
@@ -5815,8 +5815,8 @@
         <v>679</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A274" s="13"/>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A274" s="12"/>
       <c r="D274" t="s">
         <v>647</v>
       </c>
@@ -5827,8 +5827,8 @@
         <v>673</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A275" s="13"/>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A275" s="12"/>
       <c r="D275" t="s">
         <v>641</v>
       </c>
@@ -5839,8 +5839,8 @@
         <v>677</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A276" s="13"/>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A276" s="12"/>
       <c r="D276" t="s">
         <v>649</v>
       </c>
@@ -5851,8 +5851,8 @@
         <v>675</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A277" s="13"/>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A277" s="12"/>
       <c r="D277" t="s">
         <v>642</v>
       </c>
@@ -5863,8 +5863,8 @@
         <v>678</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A278" s="13"/>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A278" s="12"/>
       <c r="D278" t="s">
         <v>648</v>
       </c>
@@ -5875,8 +5875,8 @@
         <v>672</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A279" s="13"/>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279" s="12"/>
       <c r="D279" t="s">
         <v>643</v>
       </c>
@@ -5887,8 +5887,8 @@
         <v>676</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A280" s="13"/>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A280" s="12"/>
       <c r="D280" t="s">
         <v>650</v>
       </c>
@@ -5899,8 +5899,8 @@
         <v>671</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A281" s="13"/>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A281" s="12"/>
       <c r="D281" t="s">
         <v>644</v>
       </c>
@@ -5911,8 +5911,8 @@
         <v>668</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A282" s="13"/>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A282" s="12"/>
       <c r="D282" t="s">
         <v>651</v>
       </c>
@@ -5923,8 +5923,8 @@
         <v>669</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A283" s="13"/>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A283" s="12"/>
       <c r="D283" t="s">
         <v>645</v>
       </c>
@@ -5935,8 +5935,8 @@
         <v>667</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A284" s="13"/>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A284" s="12"/>
       <c r="D284" t="s">
         <v>652</v>
       </c>
@@ -5947,8 +5947,8 @@
         <v>670</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A285" s="13"/>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A285" s="12"/>
       <c r="D285" t="s">
         <v>655</v>
       </c>
@@ -5959,8 +5959,8 @@
         <v>665</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A286" s="13"/>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A286" s="12"/>
       <c r="D286" t="s">
         <v>656</v>
       </c>
@@ -5971,8 +5971,8 @@
         <v>666</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A287" s="13"/>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A287" s="12"/>
       <c r="D287" t="s">
         <v>657</v>
       </c>
@@ -5983,8 +5983,8 @@
         <v>661</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A288" s="13"/>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A288" s="12"/>
       <c r="D288" t="s">
         <v>658</v>
       </c>
@@ -5995,8 +5995,8 @@
         <v>662</v>
       </c>
     </row>
-    <row r="289" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A289" s="13"/>
+    <row r="289" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A289" s="12"/>
       <c r="D289" t="s">
         <v>659</v>
       </c>
@@ -6007,8 +6007,8 @@
         <v>664</v>
       </c>
     </row>
-    <row r="290" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A290" s="13"/>
+    <row r="290" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A290" s="12"/>
       <c r="D290" t="s">
         <v>660</v>
       </c>
@@ -6019,8 +6019,8 @@
         <v>663</v>
       </c>
     </row>
-    <row r="293" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A293" s="13" t="s">
+    <row r="293" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A293" s="12" t="s">
         <v>342</v>
       </c>
       <c r="B293" t="s">
@@ -6036,8 +6036,8 @@
         <v>475</v>
       </c>
     </row>
-    <row r="294" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A294" s="13"/>
+    <row r="294" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A294" s="12"/>
       <c r="B294" t="s">
         <v>110</v>
       </c>
@@ -6051,8 +6051,8 @@
         <v>218</v>
       </c>
     </row>
-    <row r="295" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A295" s="13"/>
+    <row r="295" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A295" s="12"/>
       <c r="B295" t="s">
         <v>111</v>
       </c>
@@ -6066,8 +6066,8 @@
         <v>476</v>
       </c>
     </row>
-    <row r="296" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A296" s="13"/>
+    <row r="296" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A296" s="12"/>
       <c r="D296" t="s">
         <v>449</v>
       </c>
@@ -6078,8 +6078,8 @@
         <v>474</v>
       </c>
     </row>
-    <row r="297" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A297" s="13"/>
+    <row r="297" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A297" s="12"/>
       <c r="D297" t="s">
         <v>450</v>
       </c>
@@ -6090,8 +6090,8 @@
         <v>473</v>
       </c>
     </row>
-    <row r="298" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A298" s="13"/>
+    <row r="298" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A298" s="12"/>
       <c r="D298" t="s">
         <v>451</v>
       </c>
@@ -6102,8 +6102,8 @@
         <v>472</v>
       </c>
     </row>
-    <row r="299" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A299" s="13"/>
+    <row r="299" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A299" s="12"/>
       <c r="D299" t="s">
         <v>452</v>
       </c>
@@ -6114,8 +6114,8 @@
         <v>357</v>
       </c>
     </row>
-    <row r="300" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A300" s="13"/>
+    <row r="300" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="12"/>
       <c r="D300" t="s">
         <v>454</v>
       </c>
@@ -6123,8 +6123,8 @@
         <v>138</v>
       </c>
     </row>
-    <row r="301" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A301" s="13"/>
+    <row r="301" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A301" s="12"/>
       <c r="D301" t="s">
         <v>453</v>
       </c>
@@ -6135,8 +6135,8 @@
         <v>471</v>
       </c>
     </row>
-    <row r="302" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A302" s="13"/>
+    <row r="302" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A302" s="12"/>
       <c r="D302" t="s">
         <v>518</v>
       </c>
@@ -6147,8 +6147,8 @@
         <v>516</v>
       </c>
     </row>
-    <row r="303" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A303" s="13"/>
+    <row r="303" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A303" s="12"/>
       <c r="D303" t="s">
         <v>512</v>
       </c>
@@ -6159,8 +6159,8 @@
         <v>517</v>
       </c>
     </row>
-    <row r="304" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A304" s="13"/>
+    <row r="304" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A304" s="12"/>
       <c r="D304" t="s">
         <v>455</v>
       </c>
@@ -6171,8 +6171,8 @@
         <v>470</v>
       </c>
     </row>
-    <row r="305" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A305" s="13"/>
+    <row r="305" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A305" s="12"/>
       <c r="D305" t="s">
         <v>456</v>
       </c>
@@ -6183,8 +6183,8 @@
         <v>469</v>
       </c>
     </row>
-    <row r="306" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A306" s="13"/>
+    <row r="306" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A306" s="12"/>
       <c r="D306" t="s">
         <v>457</v>
       </c>
@@ -6195,8 +6195,8 @@
         <v>468</v>
       </c>
     </row>
-    <row r="307" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A307" s="13"/>
+    <row r="307" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A307" s="12"/>
       <c r="D307" t="s">
         <v>458</v>
       </c>
@@ -6207,8 +6207,8 @@
         <v>467</v>
       </c>
     </row>
-    <row r="308" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A308" s="13"/>
+    <row r="308" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A308" s="12"/>
       <c r="D308" t="s">
         <v>459</v>
       </c>
@@ -6219,8 +6219,8 @@
         <v>466</v>
       </c>
     </row>
-    <row r="309" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A309" s="13"/>
+    <row r="309" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A309" s="12"/>
       <c r="D309" t="s">
         <v>460</v>
       </c>
@@ -6231,8 +6231,8 @@
         <v>465</v>
       </c>
     </row>
-    <row r="310" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A310" s="13"/>
+    <row r="310" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A310" s="12"/>
       <c r="D310" t="s">
         <v>461</v>
       </c>
@@ -6243,8 +6243,8 @@
         <v>463</v>
       </c>
     </row>
-    <row r="311" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A311" s="13"/>
+    <row r="311" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A311" s="12"/>
       <c r="D311" t="s">
         <v>462</v>
       </c>
@@ -6255,8 +6255,8 @@
         <v>464</v>
       </c>
     </row>
-    <row r="314" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A314" s="13" t="s">
+    <row r="314" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A314" s="12" t="s">
         <v>485</v>
       </c>
       <c r="B314" t="s">
@@ -6272,8 +6272,8 @@
         <v>157</v>
       </c>
     </row>
-    <row r="315" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A315" s="13"/>
+    <row r="315" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A315" s="12"/>
       <c r="D315" t="s">
         <v>155</v>
       </c>
@@ -6284,8 +6284,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="316" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A316" s="13"/>
+    <row r="316" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A316" s="12"/>
       <c r="D316" t="s">
         <v>158</v>
       </c>
@@ -6296,8 +6296,8 @@
         <v>494</v>
       </c>
     </row>
-    <row r="317" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A317" s="13"/>
+    <row r="317" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A317" s="12"/>
       <c r="D317" t="s">
         <v>159</v>
       </c>
@@ -6308,8 +6308,8 @@
         <v>160</v>
       </c>
     </row>
-    <row r="318" spans="1:6" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A318" s="13"/>
+    <row r="318" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A318" s="12"/>
       <c r="D318" s="9" t="s">
         <v>484</v>
       </c>
@@ -6320,8 +6320,8 @@
         <v>497</v>
       </c>
     </row>
-    <row r="319" spans="1:6" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A319" s="13"/>
+    <row r="319" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A319" s="12"/>
       <c r="D319" s="9" t="s">
         <v>486</v>
       </c>
@@ -6332,14 +6332,14 @@
         <v>497</v>
       </c>
     </row>
-    <row r="320" spans="1:6" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A320" s="3"/>
     </row>
-    <row r="321" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A321" s="2"/>
     </row>
-    <row r="323" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A323" s="13" t="s">
+    <row r="323" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A323" s="12" t="s">
         <v>343</v>
       </c>
       <c r="B323" t="s">
@@ -6355,8 +6355,8 @@
         <v>483</v>
       </c>
     </row>
-    <row r="324" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A324" s="13"/>
+    <row r="324" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A324" s="12"/>
       <c r="B324" t="s">
         <v>53</v>
       </c>
@@ -6370,8 +6370,8 @@
         <v>491</v>
       </c>
     </row>
-    <row r="325" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A325" s="13"/>
+    <row r="325" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A325" s="12"/>
       <c r="B325" t="s">
         <v>55</v>
       </c>
@@ -6385,8 +6385,8 @@
         <v>482</v>
       </c>
     </row>
-    <row r="326" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A326" s="13"/>
+    <row r="326" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A326" s="12"/>
       <c r="B326" t="s">
         <v>58</v>
       </c>
@@ -6400,8 +6400,8 @@
         <v>481</v>
       </c>
     </row>
-    <row r="327" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A327" s="13"/>
+    <row r="327" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A327" s="12"/>
       <c r="D327" t="s">
         <v>487</v>
       </c>
@@ -6412,8 +6412,8 @@
         <v>226</v>
       </c>
     </row>
-    <row r="328" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A328" s="13"/>
+    <row r="328" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A328" s="12"/>
       <c r="B328" t="s">
         <v>59</v>
       </c>
@@ -6427,8 +6427,8 @@
         <v>480</v>
       </c>
     </row>
-    <row r="329" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A329" s="13"/>
+    <row r="329" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A329" s="12"/>
       <c r="B329" t="s">
         <v>61</v>
       </c>
@@ -6442,8 +6442,8 @@
         <v>227</v>
       </c>
     </row>
-    <row r="330" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A330" s="13"/>
+    <row r="330" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A330" s="12"/>
       <c r="B330" t="s">
         <v>63</v>
       </c>
@@ -6457,8 +6457,8 @@
         <v>479</v>
       </c>
     </row>
-    <row r="331" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A331" s="13"/>
+    <row r="331" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A331" s="12"/>
       <c r="B331" t="s">
         <v>64</v>
       </c>
@@ -6472,8 +6472,8 @@
         <v>478</v>
       </c>
     </row>
-    <row r="332" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A332" s="13"/>
+    <row r="332" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A332" s="12"/>
       <c r="D332" t="s">
         <v>488</v>
       </c>
@@ -6484,8 +6484,8 @@
         <v>228</v>
       </c>
     </row>
-    <row r="333" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A333" s="13"/>
+    <row r="333" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A333" s="12"/>
       <c r="D333" t="s">
         <v>489</v>
       </c>
@@ -6496,8 +6496,8 @@
         <v>477</v>
       </c>
     </row>
-    <row r="334" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A334" s="13"/>
+    <row r="334" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A334" s="12"/>
       <c r="D334" t="s">
         <v>490</v>
       </c>
@@ -6508,7 +6508,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="337" spans="1:6" ht="21" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A337" s="4" t="s">
         <v>120</v>
       </c>
@@ -6525,8 +6525,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="340" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A340" s="13" t="s">
+    <row r="340" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A340" s="12" t="s">
         <v>127</v>
       </c>
       <c r="B340" t="s">
@@ -6539,8 +6539,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="341" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A341" s="13"/>
+    <row r="341" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A341" s="12"/>
       <c r="B341" t="s">
         <v>116</v>
       </c>
@@ -6551,8 +6551,8 @@
         <v>167</v>
       </c>
     </row>
-    <row r="342" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A342" s="13"/>
+    <row r="342" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A342" s="12"/>
       <c r="B342" t="s">
         <v>118</v>
       </c>
@@ -6563,8 +6563,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="343" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A343" s="13"/>
+    <row r="343" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A343" s="12"/>
       <c r="B343" t="s">
         <v>128</v>
       </c>
@@ -6575,8 +6575,8 @@
         <v>169</v>
       </c>
     </row>
-    <row r="344" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A344" s="13"/>
+    <row r="344" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A344" s="12"/>
       <c r="B344" t="s">
         <v>121</v>
       </c>
@@ -6587,10 +6587,10 @@
         <v>225</v>
       </c>
     </row>
-    <row r="345" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A345" s="3"/>
     </row>
-    <row r="346" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A346" s="3"/>
     </row>
   </sheetData>
@@ -6623,7 +6623,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6635,7 +6635,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
GearSwap - Documentation update for pos_x/y/z
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variables.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variables.xlsx
@@ -1074,15 +1074,6 @@
     <t>player.target.index</t>
   </si>
   <si>
-    <t>player.target.x_pos</t>
-  </si>
-  <si>
-    <t>player.target.y_pos</t>
-  </si>
-  <si>
-    <t>player.target.z_pos</t>
-  </si>
-  <si>
     <t>player.target.tp</t>
   </si>
   <si>
@@ -1155,15 +1146,6 @@
     <t>player.speed_base</t>
   </si>
   <si>
-    <t>player.x_pos</t>
-  </si>
-  <si>
-    <t>player.y_pos</t>
-  </si>
-  <si>
-    <t>player.z_pos</t>
-  </si>
-  <si>
     <t>player.facing</t>
   </si>
   <si>
@@ -1218,15 +1200,6 @@
     <t>player.subtarget.speed_base</t>
   </si>
   <si>
-    <t>player.subtarget.x_pos</t>
-  </si>
-  <si>
-    <t>player.subtarget.y_pos</t>
-  </si>
-  <si>
-    <t>player.subtarget.z_pos</t>
-  </si>
-  <si>
     <t>player.subtarget.facing</t>
   </si>
   <si>
@@ -1314,15 +1287,6 @@
     <t>pet.speed_base</t>
   </si>
   <si>
-    <t>pet.x_pos</t>
-  </si>
-  <si>
-    <t>pet.y_pos</t>
-  </si>
-  <si>
-    <t>pet.z_pos</t>
-  </si>
-  <si>
     <t>pet.facing</t>
   </si>
   <si>
@@ -1389,15 +1353,6 @@
     <t>fellow.speed_base</t>
   </si>
   <si>
-    <t>fellow.x_pos</t>
-  </si>
-  <si>
-    <t>fellow.y_pos</t>
-  </si>
-  <si>
-    <t>fellow.z_pos</t>
-  </si>
-  <si>
     <t>fellow.facing</t>
   </si>
   <si>
@@ -1698,15 +1653,6 @@
     <t>player.last_subtarget.speed_base</t>
   </si>
   <si>
-    <t>player.last_subtarget.x_pos</t>
-  </si>
-  <si>
-    <t>player.last_subtarget.y_pos</t>
-  </si>
-  <si>
-    <t>player.last_subtarget.z_pos</t>
-  </si>
-  <si>
     <t>player.last_subtarget.facing</t>
   </si>
   <si>
@@ -1755,15 +1701,6 @@
     <t>spell.target.speed_base</t>
   </si>
   <si>
-    <t>spell.target.x_pos</t>
-  </si>
-  <si>
-    <t>spell.target.y_pos</t>
-  </si>
-  <si>
-    <t>spell.target.z_pos</t>
-  </si>
-  <si>
     <t>spell.target.facing</t>
   </si>
   <si>
@@ -2113,6 +2050,69 @@
   </si>
   <si>
     <t>Passes in the "pet" table and a boolean indicating whether the pet is being summoned (true) or dismissed (false). Order is not guaranteed relative to aftercast for JAs like Release or Leave. Currently does not work for Charm.</t>
+  </si>
+  <si>
+    <t>spell.target.x</t>
+  </si>
+  <si>
+    <t>spell.target.y</t>
+  </si>
+  <si>
+    <t>spell.target.z</t>
+  </si>
+  <si>
+    <t>player.x</t>
+  </si>
+  <si>
+    <t>player.y</t>
+  </si>
+  <si>
+    <t>player.z</t>
+  </si>
+  <si>
+    <t>player.target.x</t>
+  </si>
+  <si>
+    <t>player.target.y</t>
+  </si>
+  <si>
+    <t>player.target.z</t>
+  </si>
+  <si>
+    <t>player.last_subtarget.z</t>
+  </si>
+  <si>
+    <t>player.last_subtarget.y</t>
+  </si>
+  <si>
+    <t>player.last_subtarget.x</t>
+  </si>
+  <si>
+    <t>player.subtarget.y</t>
+  </si>
+  <si>
+    <t>player.subtarget.z</t>
+  </si>
+  <si>
+    <t>player.subtarget.x</t>
+  </si>
+  <si>
+    <t>pet.x</t>
+  </si>
+  <si>
+    <t>pet.y</t>
+  </si>
+  <si>
+    <t>pet.z</t>
+  </si>
+  <si>
+    <t>fellow.x</t>
+  </si>
+  <si>
+    <t>fellow.y</t>
+  </si>
+  <si>
+    <t>fellow.z</t>
   </si>
 </sst>
 </file>
@@ -2508,8 +2508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F346"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D144" sqref="D144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2523,11 +2523,11 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25.9" x14ac:dyDescent="0.5">
       <c r="B1" s="6" t="s">
-        <v>492</v>
+        <v>477</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6" t="s">
-        <v>493</v>
+        <v>478</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>257</v>
@@ -2538,13 +2538,13 @@
     </row>
     <row r="3" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>609</v>
+        <v>588</v>
       </c>
       <c r="D3" t="s">
         <v>194</v>
       </c>
       <c r="E3" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F3" t="s">
         <v>195</v>
@@ -2553,13 +2553,13 @@
     <row r="4" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="D4" t="s">
-        <v>691</v>
+        <v>670</v>
       </c>
       <c r="E4" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F4" t="s">
-        <v>620</v>
+        <v>599</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2568,13 +2568,13 @@
         <v>177</v>
       </c>
       <c r="D5" t="s">
-        <v>692</v>
+        <v>671</v>
       </c>
       <c r="E5" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F5" t="s">
-        <v>621</v>
+        <v>600</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2583,13 +2583,13 @@
         <v>178</v>
       </c>
       <c r="D6" t="s">
-        <v>693</v>
+        <v>672</v>
       </c>
       <c r="E6" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F6" t="s">
-        <v>618</v>
+        <v>597</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2598,73 +2598,73 @@
         <v>179</v>
       </c>
       <c r="D7" t="s">
-        <v>694</v>
+        <v>673</v>
       </c>
       <c r="E7" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F7" t="s">
-        <v>619</v>
+        <v>598</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="D8" t="s">
-        <v>697</v>
+        <v>676</v>
       </c>
       <c r="E8" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F8" t="s">
-        <v>698</v>
+        <v>677</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="D9" t="s">
-        <v>695</v>
+        <v>674</v>
       </c>
       <c r="E9" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F9" t="s">
-        <v>610</v>
+        <v>589</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="D10" t="s">
-        <v>696</v>
+        <v>675</v>
       </c>
       <c r="E10" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F10" t="s">
-        <v>611</v>
+        <v>590</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="D11" t="s">
-        <v>502</v>
+        <v>487</v>
       </c>
       <c r="E11" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F11" t="s">
-        <v>503</v>
+        <v>488</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="D12" t="s">
-        <v>616</v>
+        <v>595</v>
       </c>
       <c r="E12" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F12" t="s">
-        <v>617</v>
+        <v>596</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2673,7 +2673,7 @@
         <v>180</v>
       </c>
       <c r="E13" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F13" t="s">
         <v>181</v>
@@ -2685,10 +2685,10 @@
         <v>193</v>
       </c>
       <c r="E14" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F14" t="s">
-        <v>612</v>
+        <v>591</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2699,28 +2699,28 @@
         <v>196</v>
       </c>
       <c r="D17" t="s">
-        <v>605</v>
+        <v>584</v>
       </c>
       <c r="E17" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F17" t="s">
-        <v>606</v>
+        <v>585</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" t="s">
-        <v>504</v>
+        <v>489</v>
       </c>
       <c r="D18" t="s">
-        <v>505</v>
+        <v>490</v>
       </c>
       <c r="E18" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F18" t="s">
-        <v>506</v>
+        <v>491</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2732,10 +2732,10 @@
         <v>133</v>
       </c>
       <c r="E19" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F19" t="s">
-        <v>614</v>
+        <v>593</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2759,10 +2759,10 @@
         <v>161</v>
       </c>
       <c r="E21" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F21" t="s">
-        <v>613</v>
+        <v>592</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2774,10 +2774,10 @@
         <v>162</v>
       </c>
       <c r="E22" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F22" t="s">
-        <v>615</v>
+        <v>594</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2786,13 +2786,13 @@
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>604</v>
+        <v>583</v>
       </c>
       <c r="E23" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F23" t="s">
-        <v>628</v>
+        <v>607</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2801,13 +2801,13 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>685</v>
+        <v>664</v>
       </c>
       <c r="E24" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F24" t="s">
-        <v>686</v>
+        <v>665</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2819,7 +2819,7 @@
         <v>198</v>
       </c>
       <c r="E25" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F25" t="s">
         <v>200</v>
@@ -2834,7 +2834,7 @@
         <v>199</v>
       </c>
       <c r="E26" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F26" t="s">
         <v>201</v>
@@ -2852,10 +2852,10 @@
         <v>208</v>
       </c>
       <c r="E27" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F27" t="s">
-        <v>607</v>
+        <v>586</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2867,10 +2867,10 @@
         <v>132</v>
       </c>
       <c r="E28" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F28" t="s">
-        <v>608</v>
+        <v>587</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2882,7 +2882,7 @@
         <v>202</v>
       </c>
       <c r="E29" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F29" t="s">
         <v>203</v>
@@ -2897,7 +2897,7 @@
         <v>136</v>
       </c>
       <c r="E30" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F30" t="s">
         <v>163</v>
@@ -2912,7 +2912,7 @@
         <v>134</v>
       </c>
       <c r="E31" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F31" t="s">
         <v>164</v>
@@ -2927,7 +2927,7 @@
         <v>135</v>
       </c>
       <c r="E32" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F32" t="s">
         <v>165</v>
@@ -2942,10 +2942,10 @@
         <v>204</v>
       </c>
       <c r="E33" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F33" t="s">
-        <v>690</v>
+        <v>669</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2954,13 +2954,13 @@
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>623</v>
+        <v>602</v>
       </c>
       <c r="E34" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F34" t="s">
-        <v>624</v>
+        <v>603</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -3007,13 +3007,13 @@
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>625</v>
+        <v>604</v>
       </c>
       <c r="E39" t="s">
         <v>140</v>
       </c>
       <c r="F39" t="s">
-        <v>496</v>
+        <v>481</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3022,7 +3022,7 @@
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>626</v>
+        <v>605</v>
       </c>
       <c r="E40" t="s">
         <v>140</v>
@@ -3037,13 +3037,13 @@
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>627</v>
+        <v>606</v>
       </c>
       <c r="E41" t="s">
         <v>140</v>
       </c>
       <c r="F41" t="s">
-        <v>622</v>
+        <v>601</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3052,13 +3052,13 @@
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>498</v>
+        <v>483</v>
       </c>
       <c r="E42" t="s">
         <v>140</v>
       </c>
       <c r="F42" t="s">
-        <v>499</v>
+        <v>484</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3067,13 +3067,13 @@
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>500</v>
+        <v>485</v>
       </c>
       <c r="E43" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F43" t="s">
-        <v>501</v>
+        <v>486</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3085,7 +3085,7 @@
         <v>142</v>
       </c>
       <c r="E44" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F44" t="s">
         <v>173</v>
@@ -3100,7 +3100,7 @@
         <v>143</v>
       </c>
       <c r="E45" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F45" t="s">
         <v>174</v>
@@ -3115,7 +3115,7 @@
         <v>144</v>
       </c>
       <c r="E46" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F46" t="s">
         <v>175</v>
@@ -3130,16 +3130,16 @@
         <v>145</v>
       </c>
       <c r="E47" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="F47" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
     </row>
-    <row r="49" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3240,10 +3240,10 @@
     <row r="59" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
       <c r="D59" t="s">
-        <v>688</v>
+        <v>667</v>
       </c>
       <c r="F59" t="s">
-        <v>689</v>
+        <v>668</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3445,7 +3445,7 @@
     </row>
     <row r="77" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
-        <v>603</v>
+        <v>582</v>
       </c>
       <c r="B77" t="s">
         <v>72</v>
@@ -3538,217 +3538,217 @@
     <row r="83" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12"/>
       <c r="D83" t="s">
-        <v>586</v>
+        <v>565</v>
       </c>
       <c r="E83" t="s">
         <v>259</v>
       </c>
       <c r="F83" t="s">
-        <v>587</v>
+        <v>566</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12"/>
       <c r="D84" t="s">
-        <v>569</v>
+        <v>551</v>
       </c>
       <c r="E84" t="s">
         <v>258</v>
       </c>
       <c r="F84" t="s">
-        <v>588</v>
+        <v>567</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12"/>
       <c r="D85" t="s">
-        <v>570</v>
+        <v>552</v>
       </c>
       <c r="E85" t="s">
         <v>258</v>
       </c>
       <c r="F85" t="s">
-        <v>589</v>
+        <v>568</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12"/>
       <c r="D86" t="s">
-        <v>571</v>
+        <v>553</v>
       </c>
       <c r="E86" t="s">
         <v>258</v>
       </c>
       <c r="F86" t="s">
-        <v>602</v>
+        <v>581</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12"/>
       <c r="D87" t="s">
-        <v>572</v>
+        <v>554</v>
       </c>
       <c r="E87" t="s">
         <v>258</v>
       </c>
       <c r="F87" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12"/>
       <c r="D88" t="s">
-        <v>573</v>
+        <v>555</v>
       </c>
       <c r="E88" t="s">
         <v>138</v>
       </c>
       <c r="F88" t="s">
-        <v>590</v>
+        <v>569</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12"/>
       <c r="D89" t="s">
-        <v>574</v>
+        <v>556</v>
       </c>
       <c r="E89" t="s">
         <v>258</v>
       </c>
       <c r="F89" t="s">
-        <v>591</v>
+        <v>570</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12"/>
       <c r="D90" t="s">
-        <v>575</v>
+        <v>557</v>
       </c>
       <c r="E90" t="s">
         <v>138</v>
       </c>
       <c r="F90" t="s">
-        <v>592</v>
+        <v>571</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
       <c r="D91" t="s">
-        <v>576</v>
+        <v>558</v>
       </c>
       <c r="E91" t="s">
         <v>258</v>
       </c>
       <c r="F91" t="s">
-        <v>508</v>
+        <v>493</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
       <c r="D92" t="s">
-        <v>577</v>
+        <v>559</v>
       </c>
       <c r="E92" t="s">
         <v>258</v>
       </c>
       <c r="F92" t="s">
-        <v>593</v>
+        <v>572</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12"/>
       <c r="D93" t="s">
-        <v>578</v>
+        <v>560</v>
       </c>
       <c r="E93" t="s">
         <v>258</v>
       </c>
       <c r="F93" t="s">
-        <v>594</v>
+        <v>573</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12"/>
       <c r="D94" t="s">
-        <v>579</v>
+        <v>678</v>
       </c>
       <c r="E94" t="s">
         <v>258</v>
       </c>
       <c r="F94" t="s">
-        <v>595</v>
+        <v>574</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12"/>
       <c r="D95" t="s">
-        <v>580</v>
+        <v>679</v>
       </c>
       <c r="E95" t="s">
         <v>258</v>
       </c>
       <c r="F95" t="s">
-        <v>596</v>
+        <v>575</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12"/>
       <c r="D96" t="s">
-        <v>581</v>
+        <v>680</v>
       </c>
       <c r="E96" t="s">
         <v>258</v>
       </c>
       <c r="F96" t="s">
-        <v>597</v>
+        <v>576</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
       <c r="D97" t="s">
-        <v>582</v>
+        <v>561</v>
       </c>
       <c r="E97" t="s">
         <v>258</v>
       </c>
       <c r="F97" t="s">
-        <v>598</v>
+        <v>577</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
       <c r="D98" t="s">
-        <v>583</v>
+        <v>562</v>
       </c>
       <c r="E98" t="s">
         <v>258</v>
       </c>
       <c r="F98" t="s">
-        <v>599</v>
+        <v>578</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
       <c r="D99" t="s">
-        <v>584</v>
+        <v>563</v>
       </c>
       <c r="E99" t="s">
         <v>258</v>
       </c>
       <c r="F99" t="s">
-        <v>600</v>
+        <v>579</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12"/>
       <c r="D100" t="s">
-        <v>585</v>
+        <v>564</v>
       </c>
       <c r="E100" t="s">
         <v>258</v>
       </c>
       <c r="F100" t="s">
-        <v>601</v>
+        <v>580</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3771,13 +3771,13 @@
     <row r="104" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12"/>
       <c r="D104" t="s">
-        <v>629</v>
+        <v>608</v>
       </c>
       <c r="E104" t="s">
         <v>138</v>
       </c>
       <c r="F104" t="s">
-        <v>630</v>
+        <v>609</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4149,181 +4149,181 @@
     <row r="132" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="12"/>
       <c r="D132" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E132" t="s">
         <v>258</v>
       </c>
       <c r="F132" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
     </row>
     <row r="133" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="12"/>
       <c r="D133" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E133" t="s">
         <v>258</v>
       </c>
       <c r="F133" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="12"/>
       <c r="D134" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E134" t="s">
         <v>138</v>
       </c>
       <c r="F134" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="12"/>
       <c r="D135" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="E135" t="s">
         <v>258</v>
       </c>
       <c r="F135" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
     </row>
     <row r="136" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="12"/>
       <c r="D136" t="s">
-        <v>507</v>
+        <v>492</v>
       </c>
       <c r="E136" t="s">
         <v>258</v>
       </c>
       <c r="F136" t="s">
-        <v>508</v>
+        <v>493</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="12"/>
       <c r="D137" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E137" t="s">
         <v>258</v>
       </c>
       <c r="F137" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
     </row>
     <row r="138" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="12"/>
       <c r="D138" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E138" t="s">
         <v>258</v>
       </c>
       <c r="F138" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
     </row>
     <row r="139" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="12"/>
       <c r="D139" t="s">
+        <v>681</v>
+      </c>
+      <c r="E139" t="s">
+        <v>258</v>
+      </c>
+      <c r="F139" t="s">
         <v>379</v>
-      </c>
-      <c r="E139" t="s">
-        <v>258</v>
-      </c>
-      <c r="F139" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="140" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="12"/>
       <c r="D140" t="s">
+        <v>682</v>
+      </c>
+      <c r="E140" t="s">
+        <v>258</v>
+      </c>
+      <c r="F140" t="s">
         <v>380</v>
-      </c>
-      <c r="E140" t="s">
-        <v>258</v>
-      </c>
-      <c r="F140" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="141" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="12"/>
       <c r="D141" t="s">
-        <v>381</v>
+        <v>683</v>
       </c>
       <c r="E141" t="s">
         <v>258</v>
       </c>
       <c r="F141" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
     </row>
     <row r="142" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="12"/>
       <c r="D142" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="E142" t="s">
         <v>258</v>
       </c>
       <c r="F142" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="12"/>
       <c r="D143" t="s">
-        <v>681</v>
+        <v>660</v>
       </c>
       <c r="E143" t="s">
         <v>140</v>
       </c>
       <c r="F143" t="s">
-        <v>687</v>
+        <v>666</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="12"/>
       <c r="D144" t="s">
-        <v>682</v>
+        <v>661</v>
       </c>
       <c r="E144" t="s">
         <v>140</v>
       </c>
       <c r="F144" t="s">
-        <v>687</v>
+        <v>666</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="12"/>
       <c r="D145" t="s">
-        <v>683</v>
+        <v>662</v>
       </c>
       <c r="E145" t="s">
         <v>140</v>
       </c>
       <c r="F145" t="s">
-        <v>687</v>
+        <v>666</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="12"/>
       <c r="D146" t="s">
-        <v>684</v>
+        <v>663</v>
       </c>
       <c r="E146" t="s">
         <v>140</v>
       </c>
       <c r="F146" t="s">
-        <v>687</v>
+        <v>666</v>
       </c>
     </row>
     <row r="147" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4666,31 +4666,31 @@
         <v>259</v>
       </c>
       <c r="F172" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="12"/>
       <c r="D173" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="E173" t="s">
         <v>258</v>
       </c>
       <c r="F173" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="12"/>
       <c r="D174" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="E174" t="s">
         <v>258</v>
       </c>
       <c r="F174" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4702,7 +4702,7 @@
         <v>258</v>
       </c>
       <c r="F175" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="176" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4714,7 +4714,7 @@
         <v>258</v>
       </c>
       <c r="F176" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="177" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4726,103 +4726,103 @@
         <v>138</v>
       </c>
       <c r="F177" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="12"/>
       <c r="D178" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="E178" t="s">
         <v>258</v>
       </c>
       <c r="F178" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="12"/>
       <c r="D179" t="s">
-        <v>568</v>
+        <v>550</v>
       </c>
       <c r="E179" t="s">
         <v>138</v>
       </c>
       <c r="F179" t="s">
-        <v>567</v>
+        <v>549</v>
       </c>
     </row>
     <row r="180" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="12"/>
       <c r="D180" t="s">
-        <v>509</v>
+        <v>494</v>
       </c>
       <c r="E180" t="s">
         <v>258</v>
       </c>
       <c r="F180" t="s">
-        <v>508</v>
+        <v>493</v>
       </c>
     </row>
     <row r="181" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12"/>
       <c r="D181" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="E181" t="s">
         <v>258</v>
       </c>
       <c r="F181" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="182" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="12"/>
       <c r="D182" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E182" t="s">
         <v>258</v>
       </c>
       <c r="F182" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="183" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="12"/>
       <c r="D183" t="s">
-        <v>352</v>
+        <v>684</v>
       </c>
       <c r="E183" t="s">
         <v>258</v>
       </c>
       <c r="F183" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
     </row>
     <row r="184" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="12"/>
       <c r="D184" t="s">
-        <v>353</v>
+        <v>685</v>
       </c>
       <c r="E184" t="s">
         <v>258</v>
       </c>
       <c r="F184" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="12"/>
       <c r="D185" t="s">
-        <v>354</v>
+        <v>686</v>
       </c>
       <c r="E185" t="s">
         <v>258</v>
       </c>
       <c r="F185" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4834,7 +4834,7 @@
         <v>258</v>
       </c>
       <c r="F186" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4846,31 +4846,31 @@
         <v>258</v>
       </c>
       <c r="F187" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="188" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="12"/>
       <c r="D188" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="E188" t="s">
         <v>258</v>
       </c>
       <c r="F188" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="189" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="12"/>
       <c r="D189" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E189" t="s">
         <v>258</v>
       </c>
       <c r="F189" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="190" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4881,22 +4881,22 @@
     </row>
     <row r="192" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="12" t="s">
-        <v>524</v>
+        <v>509</v>
       </c>
       <c r="D192" t="s">
-        <v>544</v>
+        <v>529</v>
       </c>
       <c r="E192" t="s">
         <v>138</v>
       </c>
       <c r="F192" t="s">
-        <v>525</v>
+        <v>510</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="12"/>
       <c r="D193" t="s">
-        <v>545</v>
+        <v>530</v>
       </c>
       <c r="E193" t="s">
         <v>138</v>
@@ -4908,253 +4908,253 @@
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="12"/>
       <c r="D194" t="s">
-        <v>546</v>
+        <v>531</v>
       </c>
       <c r="E194" t="s">
         <v>258</v>
       </c>
       <c r="F194" t="s">
-        <v>526</v>
+        <v>511</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="12"/>
       <c r="D195" t="s">
-        <v>547</v>
+        <v>532</v>
       </c>
       <c r="E195" t="s">
         <v>258</v>
       </c>
       <c r="F195" t="s">
-        <v>527</v>
+        <v>512</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="12"/>
       <c r="D196" t="s">
-        <v>548</v>
+        <v>533</v>
       </c>
       <c r="E196" t="s">
         <v>259</v>
       </c>
       <c r="F196" t="s">
-        <v>528</v>
+        <v>513</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="12"/>
       <c r="D197" t="s">
-        <v>549</v>
+        <v>534</v>
       </c>
       <c r="E197" t="s">
         <v>259</v>
       </c>
       <c r="F197" t="s">
-        <v>529</v>
+        <v>514</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="12"/>
       <c r="D198" t="s">
-        <v>550</v>
+        <v>535</v>
       </c>
       <c r="E198" t="s">
         <v>258</v>
       </c>
       <c r="F198" t="s">
-        <v>530</v>
+        <v>515</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="12"/>
       <c r="D199" t="s">
-        <v>551</v>
+        <v>536</v>
       </c>
       <c r="E199" t="s">
         <v>258</v>
       </c>
       <c r="F199" t="s">
-        <v>531</v>
+        <v>516</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="12"/>
       <c r="D200" t="s">
-        <v>552</v>
+        <v>537</v>
       </c>
       <c r="E200" t="s">
         <v>258</v>
       </c>
       <c r="F200" t="s">
-        <v>532</v>
+        <v>517</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="12"/>
       <c r="D201" t="s">
-        <v>553</v>
+        <v>538</v>
       </c>
       <c r="E201" t="s">
         <v>258</v>
       </c>
       <c r="F201" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="12"/>
       <c r="D202" t="s">
-        <v>554</v>
+        <v>539</v>
       </c>
       <c r="E202" t="s">
         <v>138</v>
       </c>
       <c r="F202" t="s">
-        <v>533</v>
+        <v>518</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="12"/>
       <c r="D203" t="s">
-        <v>555</v>
+        <v>540</v>
       </c>
       <c r="E203" t="s">
         <v>258</v>
       </c>
       <c r="F203" t="s">
-        <v>534</v>
+        <v>519</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="12"/>
       <c r="D204" t="s">
-        <v>556</v>
+        <v>541</v>
       </c>
       <c r="E204" t="s">
         <v>138</v>
       </c>
       <c r="F204" t="s">
-        <v>535</v>
+        <v>520</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="12"/>
       <c r="D205" t="s">
-        <v>557</v>
+        <v>542</v>
       </c>
       <c r="E205" t="s">
         <v>258</v>
       </c>
       <c r="F205" t="s">
-        <v>508</v>
+        <v>493</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="12"/>
       <c r="D206" t="s">
-        <v>558</v>
+        <v>543</v>
       </c>
       <c r="E206" t="s">
         <v>258</v>
       </c>
       <c r="F206" t="s">
-        <v>536</v>
+        <v>521</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="12"/>
       <c r="D207" t="s">
-        <v>559</v>
+        <v>544</v>
       </c>
       <c r="E207" t="s">
         <v>258</v>
       </c>
       <c r="F207" t="s">
-        <v>537</v>
+        <v>522</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="12"/>
       <c r="D208" t="s">
-        <v>560</v>
+        <v>689</v>
       </c>
       <c r="E208" t="s">
         <v>258</v>
       </c>
       <c r="F208" t="s">
-        <v>538</v>
+        <v>523</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="12"/>
       <c r="D209" t="s">
-        <v>561</v>
+        <v>688</v>
       </c>
       <c r="E209" t="s">
         <v>258</v>
       </c>
       <c r="F209" t="s">
-        <v>539</v>
+        <v>524</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="12"/>
       <c r="D210" t="s">
-        <v>562</v>
+        <v>687</v>
       </c>
       <c r="E210" t="s">
         <v>258</v>
       </c>
       <c r="F210" t="s">
-        <v>540</v>
+        <v>525</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="12"/>
       <c r="D211" t="s">
-        <v>563</v>
+        <v>545</v>
       </c>
       <c r="E211" t="s">
         <v>258</v>
       </c>
       <c r="F211" t="s">
-        <v>541</v>
+        <v>526</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="12"/>
       <c r="D212" t="s">
-        <v>564</v>
+        <v>546</v>
       </c>
       <c r="E212" t="s">
         <v>258</v>
       </c>
       <c r="F212" t="s">
-        <v>542</v>
+        <v>527</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="12"/>
       <c r="D213" t="s">
-        <v>565</v>
+        <v>547</v>
       </c>
       <c r="E213" t="s">
         <v>258</v>
       </c>
       <c r="F213" t="s">
-        <v>543</v>
+        <v>528</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="12"/>
       <c r="D214" t="s">
-        <v>566</v>
+        <v>548</v>
       </c>
       <c r="E214" t="s">
         <v>258</v>
       </c>
       <c r="F214" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
@@ -5228,217 +5228,217 @@
     <row r="222" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="12"/>
       <c r="D222" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="E222" t="s">
         <v>259</v>
       </c>
       <c r="F222" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
     </row>
     <row r="223" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="12"/>
       <c r="D223" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="E223" t="s">
         <v>258</v>
       </c>
       <c r="F223" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
     </row>
     <row r="224" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="12"/>
       <c r="D224" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="E224" t="s">
         <v>258</v>
       </c>
       <c r="F224" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
     </row>
     <row r="225" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="12"/>
       <c r="D225" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="E225" t="s">
         <v>258</v>
       </c>
       <c r="F225" t="s">
-        <v>523</v>
+        <v>508</v>
       </c>
     </row>
     <row r="226" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="12"/>
       <c r="D226" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="E226" t="s">
         <v>258</v>
       </c>
       <c r="F226" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="227" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="12"/>
       <c r="D227" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="E227" t="s">
         <v>138</v>
       </c>
       <c r="F227" t="s">
-        <v>521</v>
+        <v>506</v>
       </c>
     </row>
     <row r="228" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="12"/>
       <c r="D228" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="E228" t="s">
         <v>258</v>
       </c>
       <c r="F228" t="s">
-        <v>522</v>
+        <v>507</v>
       </c>
     </row>
     <row r="229" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="12"/>
       <c r="D229" t="s">
-        <v>519</v>
+        <v>504</v>
       </c>
       <c r="E229" t="s">
         <v>138</v>
       </c>
       <c r="F229" t="s">
-        <v>520</v>
+        <v>505</v>
       </c>
     </row>
     <row r="230" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="12"/>
       <c r="D230" t="s">
-        <v>510</v>
+        <v>495</v>
       </c>
       <c r="E230" t="s">
         <v>258</v>
       </c>
       <c r="F230" t="s">
-        <v>508</v>
+        <v>493</v>
       </c>
     </row>
     <row r="231" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="12"/>
       <c r="D231" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="E231" t="s">
         <v>258</v>
       </c>
       <c r="F231" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
     </row>
     <row r="232" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="12"/>
       <c r="D232" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="E232" t="s">
         <v>258</v>
       </c>
       <c r="F232" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
     </row>
     <row r="233" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="12"/>
       <c r="D233" t="s">
-        <v>400</v>
+        <v>692</v>
       </c>
       <c r="E233" t="s">
         <v>258</v>
       </c>
       <c r="F233" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
     </row>
     <row r="234" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="12"/>
       <c r="D234" t="s">
-        <v>401</v>
+        <v>690</v>
       </c>
       <c r="E234" t="s">
         <v>258</v>
       </c>
       <c r="F234" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
     </row>
     <row r="235" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="12"/>
       <c r="D235" t="s">
+        <v>691</v>
+      </c>
+      <c r="E235" t="s">
+        <v>258</v>
+      </c>
+      <c r="F235" t="s">
         <v>402</v>
-      </c>
-      <c r="E235" t="s">
-        <v>258</v>
-      </c>
-      <c r="F235" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="236" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="12"/>
       <c r="D236" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="E236" t="s">
         <v>258</v>
       </c>
       <c r="F236" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
     </row>
     <row r="237" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="12"/>
       <c r="D237" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="E237" t="s">
         <v>258</v>
       </c>
       <c r="F237" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
     </row>
     <row r="238" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="12"/>
       <c r="D238" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="E238" t="s">
         <v>258</v>
       </c>
       <c r="F238" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
     </row>
     <row r="239" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="12"/>
       <c r="D239" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="E239" t="s">
         <v>258</v>
       </c>
       <c r="F239" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
     </row>
     <row r="240" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5458,7 +5458,7 @@
         <v>138</v>
       </c>
       <c r="F242" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
     </row>
     <row r="243" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5503,7 +5503,7 @@
         <v>258</v>
       </c>
       <c r="F245" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
     </row>
     <row r="246" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5518,7 +5518,7 @@
         <v>258</v>
       </c>
       <c r="F246" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
     </row>
     <row r="247" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5536,172 +5536,172 @@
     <row r="248" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="12"/>
       <c r="D248" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="E248" t="s">
         <v>258</v>
       </c>
       <c r="F248" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
     </row>
     <row r="249" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="12"/>
       <c r="D249" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="E249" t="s">
         <v>258</v>
       </c>
       <c r="F249" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="250" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="12"/>
       <c r="D250" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="E250" t="s">
         <v>258</v>
       </c>
       <c r="F250" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
     </row>
     <row r="251" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="12"/>
       <c r="D251" t="s">
-        <v>513</v>
+        <v>498</v>
       </c>
       <c r="E251" t="s">
         <v>138</v>
       </c>
       <c r="F251" t="s">
-        <v>514</v>
+        <v>499</v>
       </c>
     </row>
     <row r="252" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="12"/>
       <c r="D252" t="s">
-        <v>511</v>
+        <v>496</v>
       </c>
       <c r="E252" t="s">
         <v>258</v>
       </c>
       <c r="F252" t="s">
-        <v>515</v>
+        <v>500</v>
       </c>
     </row>
     <row r="253" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="12"/>
       <c r="D253" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="E253" t="s">
         <v>258</v>
       </c>
       <c r="F253" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
     </row>
     <row r="254" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="12"/>
       <c r="D254" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="E254" t="s">
         <v>258</v>
       </c>
       <c r="F254" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
     </row>
     <row r="255" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="12"/>
       <c r="D255" t="s">
-        <v>432</v>
+        <v>693</v>
       </c>
       <c r="E255" t="s">
         <v>258</v>
       </c>
       <c r="F255" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
     </row>
     <row r="256" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="12"/>
       <c r="D256" t="s">
-        <v>433</v>
+        <v>694</v>
       </c>
       <c r="E256" t="s">
         <v>258</v>
       </c>
       <c r="F256" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
     </row>
     <row r="257" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="12"/>
       <c r="D257" t="s">
-        <v>434</v>
+        <v>695</v>
       </c>
       <c r="E257" t="s">
         <v>258</v>
       </c>
       <c r="F257" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
     </row>
     <row r="258" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="12"/>
       <c r="D258" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="E258" t="s">
         <v>258</v>
       </c>
       <c r="F258" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="259" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="12"/>
       <c r="D259" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="E259" t="s">
         <v>258</v>
       </c>
       <c r="F259" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
     </row>
     <row r="260" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="12"/>
       <c r="D260" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="E260" t="s">
         <v>258</v>
       </c>
       <c r="F260" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
     </row>
     <row r="261" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="12"/>
       <c r="D261" t="s">
-        <v>632</v>
+        <v>611</v>
       </c>
       <c r="F261" t="s">
-        <v>631</v>
+        <v>610</v>
       </c>
     </row>
     <row r="262" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="12"/>
       <c r="D262" t="s">
-        <v>653</v>
+        <v>632</v>
       </c>
       <c r="E262" t="s">
         <v>258</v>
@@ -5710,7 +5710,7 @@
     <row r="263" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="12"/>
       <c r="D263" t="s">
-        <v>654</v>
+        <v>633</v>
       </c>
       <c r="E263" t="s">
         <v>258</v>
@@ -5719,7 +5719,7 @@
     <row r="264" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="12"/>
       <c r="D264" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="E264" t="s">
         <v>258</v>
@@ -5728,7 +5728,7 @@
     <row r="265" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="12"/>
       <c r="D265" t="s">
-        <v>635</v>
+        <v>614</v>
       </c>
       <c r="E265" t="s">
         <v>258</v>
@@ -5737,7 +5737,7 @@
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="12"/>
       <c r="D266" t="s">
-        <v>636</v>
+        <v>615</v>
       </c>
       <c r="E266" t="s">
         <v>258</v>
@@ -5746,7 +5746,7 @@
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="12"/>
       <c r="D267" t="s">
-        <v>633</v>
+        <v>612</v>
       </c>
       <c r="E267" t="s">
         <v>258</v>
@@ -5755,7 +5755,7 @@
     <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="12"/>
       <c r="D268" t="s">
-        <v>634</v>
+        <v>613</v>
       </c>
       <c r="E268" t="s">
         <v>258</v>
@@ -5764,7 +5764,7 @@
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" s="12"/>
       <c r="D269" t="s">
-        <v>637</v>
+        <v>616</v>
       </c>
       <c r="E269" t="s">
         <v>258</v>
@@ -5773,7 +5773,7 @@
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="12"/>
       <c r="D270" t="s">
-        <v>638</v>
+        <v>617</v>
       </c>
       <c r="E270" t="s">
         <v>258</v>
@@ -5782,241 +5782,241 @@
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="12"/>
       <c r="D271" t="s">
-        <v>639</v>
+        <v>618</v>
       </c>
       <c r="E271" t="s">
         <v>258</v>
       </c>
       <c r="F271" t="s">
-        <v>680</v>
+        <v>659</v>
       </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="12"/>
       <c r="D272" t="s">
-        <v>646</v>
+        <v>625</v>
       </c>
       <c r="E272" t="s">
         <v>258</v>
       </c>
       <c r="F272" t="s">
-        <v>674</v>
+        <v>653</v>
       </c>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="12"/>
       <c r="D273" t="s">
-        <v>640</v>
+        <v>619</v>
       </c>
       <c r="E273" t="s">
         <v>258</v>
       </c>
       <c r="F273" t="s">
-        <v>679</v>
+        <v>658</v>
       </c>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="12"/>
       <c r="D274" t="s">
-        <v>647</v>
+        <v>626</v>
       </c>
       <c r="E274" t="s">
         <v>258</v>
       </c>
       <c r="F274" t="s">
-        <v>673</v>
+        <v>652</v>
       </c>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" s="12"/>
       <c r="D275" t="s">
-        <v>641</v>
+        <v>620</v>
       </c>
       <c r="E275" t="s">
         <v>258</v>
       </c>
       <c r="F275" t="s">
-        <v>677</v>
+        <v>656</v>
       </c>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="12"/>
       <c r="D276" t="s">
-        <v>649</v>
+        <v>628</v>
       </c>
       <c r="E276" t="s">
         <v>258</v>
       </c>
       <c r="F276" t="s">
-        <v>675</v>
+        <v>654</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="12"/>
       <c r="D277" t="s">
-        <v>642</v>
+        <v>621</v>
       </c>
       <c r="E277" t="s">
         <v>258</v>
       </c>
       <c r="F277" t="s">
-        <v>678</v>
+        <v>657</v>
       </c>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" s="12"/>
       <c r="D278" t="s">
-        <v>648</v>
+        <v>627</v>
       </c>
       <c r="E278" t="s">
         <v>258</v>
       </c>
       <c r="F278" t="s">
-        <v>672</v>
+        <v>651</v>
       </c>
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" s="12"/>
       <c r="D279" t="s">
-        <v>643</v>
+        <v>622</v>
       </c>
       <c r="E279" t="s">
         <v>258</v>
       </c>
       <c r="F279" t="s">
-        <v>676</v>
+        <v>655</v>
       </c>
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" s="12"/>
       <c r="D280" t="s">
+        <v>629</v>
+      </c>
+      <c r="E280" t="s">
+        <v>258</v>
+      </c>
+      <c r="F280" t="s">
         <v>650</v>
-      </c>
-      <c r="E280" t="s">
-        <v>258</v>
-      </c>
-      <c r="F280" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" s="12"/>
       <c r="D281" t="s">
-        <v>644</v>
+        <v>623</v>
       </c>
       <c r="E281" t="s">
         <v>258</v>
       </c>
       <c r="F281" t="s">
-        <v>668</v>
+        <v>647</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" s="12"/>
       <c r="D282" t="s">
-        <v>651</v>
+        <v>630</v>
       </c>
       <c r="E282" t="s">
         <v>258</v>
       </c>
       <c r="F282" t="s">
-        <v>669</v>
+        <v>648</v>
       </c>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" s="12"/>
       <c r="D283" t="s">
-        <v>645</v>
+        <v>624</v>
       </c>
       <c r="E283" t="s">
         <v>258</v>
       </c>
       <c r="F283" t="s">
-        <v>667</v>
+        <v>646</v>
       </c>
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="12"/>
       <c r="D284" t="s">
-        <v>652</v>
+        <v>631</v>
       </c>
       <c r="E284" t="s">
         <v>258</v>
       </c>
       <c r="F284" t="s">
-        <v>670</v>
+        <v>649</v>
       </c>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="12"/>
       <c r="D285" t="s">
-        <v>655</v>
+        <v>634</v>
       </c>
       <c r="E285" t="s">
         <v>138</v>
       </c>
       <c r="F285" t="s">
-        <v>665</v>
+        <v>644</v>
       </c>
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" s="12"/>
       <c r="D286" t="s">
-        <v>656</v>
+        <v>635</v>
       </c>
       <c r="E286" t="s">
         <v>138</v>
       </c>
       <c r="F286" t="s">
-        <v>666</v>
+        <v>645</v>
       </c>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="12"/>
       <c r="D287" t="s">
-        <v>657</v>
+        <v>636</v>
       </c>
       <c r="E287" t="s">
         <v>140</v>
       </c>
       <c r="F287" t="s">
-        <v>661</v>
+        <v>640</v>
       </c>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="12"/>
       <c r="D288" t="s">
-        <v>658</v>
+        <v>637</v>
       </c>
       <c r="E288" t="s">
         <v>140</v>
       </c>
       <c r="F288" t="s">
-        <v>662</v>
+        <v>641</v>
       </c>
     </row>
     <row r="289" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289" s="12"/>
       <c r="D289" t="s">
-        <v>659</v>
+        <v>638</v>
       </c>
       <c r="E289" t="s">
         <v>140</v>
       </c>
       <c r="F289" t="s">
-        <v>664</v>
+        <v>643</v>
       </c>
     </row>
     <row r="290" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290" s="12"/>
       <c r="D290" t="s">
-        <v>660</v>
+        <v>639</v>
       </c>
       <c r="E290" t="s">
         <v>140</v>
       </c>
       <c r="F290" t="s">
-        <v>663</v>
+        <v>642</v>
       </c>
     </row>
     <row r="293" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6033,7 +6033,7 @@
         <v>138</v>
       </c>
       <c r="F293" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
     </row>
     <row r="294" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6063,61 +6063,61 @@
         <v>258</v>
       </c>
       <c r="F295" t="s">
-        <v>476</v>
+        <v>461</v>
       </c>
     </row>
     <row r="296" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A296" s="12"/>
       <c r="D296" t="s">
-        <v>449</v>
+        <v>437</v>
       </c>
       <c r="E296" t="s">
         <v>258</v>
       </c>
       <c r="F296" t="s">
-        <v>474</v>
+        <v>459</v>
       </c>
     </row>
     <row r="297" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A297" s="12"/>
       <c r="D297" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="E297" t="s">
         <v>258</v>
       </c>
       <c r="F297" t="s">
-        <v>473</v>
+        <v>458</v>
       </c>
     </row>
     <row r="298" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A298" s="12"/>
       <c r="D298" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
       <c r="E298" t="s">
         <v>258</v>
       </c>
       <c r="F298" t="s">
-        <v>472</v>
+        <v>457</v>
       </c>
     </row>
     <row r="299" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" s="12"/>
       <c r="D299" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="E299" t="s">
         <v>258</v>
       </c>
       <c r="F299" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="300" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A300" s="12"/>
       <c r="D300" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
       <c r="E300" t="s">
         <v>138</v>
@@ -6126,138 +6126,138 @@
     <row r="301" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A301" s="12"/>
       <c r="D301" t="s">
-        <v>453</v>
+        <v>441</v>
       </c>
       <c r="E301" t="s">
         <v>258</v>
       </c>
       <c r="F301" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
     </row>
     <row r="302" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="12"/>
       <c r="D302" t="s">
-        <v>518</v>
+        <v>503</v>
       </c>
       <c r="E302" t="s">
         <v>138</v>
       </c>
       <c r="F302" t="s">
-        <v>516</v>
+        <v>501</v>
       </c>
     </row>
     <row r="303" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="12"/>
       <c r="D303" t="s">
-        <v>512</v>
+        <v>497</v>
       </c>
       <c r="E303" t="s">
         <v>258</v>
       </c>
       <c r="F303" t="s">
-        <v>517</v>
+        <v>502</v>
       </c>
     </row>
     <row r="304" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="12"/>
       <c r="D304" t="s">
+        <v>443</v>
+      </c>
+      <c r="E304" t="s">
+        <v>258</v>
+      </c>
+      <c r="F304" t="s">
         <v>455</v>
-      </c>
-      <c r="E304" t="s">
-        <v>258</v>
-      </c>
-      <c r="F304" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="305" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A305" s="12"/>
       <c r="D305" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
       <c r="E305" t="s">
         <v>258</v>
       </c>
       <c r="F305" t="s">
-        <v>469</v>
+        <v>454</v>
       </c>
     </row>
     <row r="306" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A306" s="12"/>
       <c r="D306" t="s">
-        <v>457</v>
+        <v>696</v>
       </c>
       <c r="E306" t="s">
         <v>258</v>
       </c>
       <c r="F306" t="s">
-        <v>468</v>
+        <v>453</v>
       </c>
     </row>
     <row r="307" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A307" s="12"/>
       <c r="D307" t="s">
-        <v>458</v>
+        <v>697</v>
       </c>
       <c r="E307" t="s">
         <v>258</v>
       </c>
       <c r="F307" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
     </row>
     <row r="308" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A308" s="12"/>
       <c r="D308" t="s">
-        <v>459</v>
+        <v>698</v>
       </c>
       <c r="E308" t="s">
         <v>258</v>
       </c>
       <c r="F308" t="s">
-        <v>466</v>
+        <v>451</v>
       </c>
     </row>
     <row r="309" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A309" s="12"/>
       <c r="D309" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
       <c r="E309" t="s">
         <v>258</v>
       </c>
       <c r="F309" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
     </row>
     <row r="310" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A310" s="12"/>
       <c r="D310" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
       <c r="E310" t="s">
         <v>258</v>
       </c>
       <c r="F310" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
     </row>
     <row r="311" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A311" s="12"/>
       <c r="D311" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
       <c r="E311" t="s">
         <v>258</v>
       </c>
       <c r="F311" t="s">
-        <v>464</v>
+        <v>449</v>
       </c>
     </row>
     <row r="314" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A314" s="12" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="B314" t="s">
         <v>48</v>
@@ -6293,7 +6293,7 @@
         <v>140</v>
       </c>
       <c r="F316" t="s">
-        <v>494</v>
+        <v>479</v>
       </c>
     </row>
     <row r="317" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6311,25 +6311,25 @@
     <row r="318" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A318" s="12"/>
       <c r="D318" s="9" t="s">
-        <v>484</v>
+        <v>469</v>
       </c>
       <c r="E318" s="9" t="s">
         <v>140</v>
       </c>
       <c r="F318" s="9" t="s">
-        <v>497</v>
+        <v>482</v>
       </c>
     </row>
     <row r="319" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A319" s="12"/>
       <c r="D319" s="9" t="s">
-        <v>486</v>
+        <v>471</v>
       </c>
       <c r="E319" s="9" t="s">
         <v>140</v>
       </c>
       <c r="F319" s="9" t="s">
-        <v>497</v>
+        <v>482</v>
       </c>
     </row>
     <row r="320" spans="1:6" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6352,7 +6352,7 @@
         <v>138</v>
       </c>
       <c r="F323" t="s">
-        <v>483</v>
+        <v>468</v>
       </c>
     </row>
     <row r="324" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6367,7 +6367,7 @@
         <v>258</v>
       </c>
       <c r="F324" t="s">
-        <v>491</v>
+        <v>476</v>
       </c>
     </row>
     <row r="325" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6382,7 +6382,7 @@
         <v>138</v>
       </c>
       <c r="F325" t="s">
-        <v>482</v>
+        <v>467</v>
       </c>
     </row>
     <row r="326" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6397,13 +6397,13 @@
         <v>138</v>
       </c>
       <c r="F326" t="s">
-        <v>481</v>
+        <v>466</v>
       </c>
     </row>
     <row r="327" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A327" s="12"/>
       <c r="D327" t="s">
-        <v>487</v>
+        <v>472</v>
       </c>
       <c r="E327" t="s">
         <v>258</v>
@@ -6424,7 +6424,7 @@
         <v>138</v>
       </c>
       <c r="F328" t="s">
-        <v>480</v>
+        <v>465</v>
       </c>
     </row>
     <row r="329" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6454,7 +6454,7 @@
         <v>138</v>
       </c>
       <c r="F330" t="s">
-        <v>479</v>
+        <v>464</v>
       </c>
     </row>
     <row r="331" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6469,13 +6469,13 @@
         <v>258</v>
       </c>
       <c r="F331" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
     </row>
     <row r="332" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A332" s="12"/>
       <c r="D332" t="s">
-        <v>488</v>
+        <v>473</v>
       </c>
       <c r="E332" t="s">
         <v>138</v>
@@ -6487,19 +6487,19 @@
     <row r="333" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A333" s="12"/>
       <c r="D333" t="s">
-        <v>489</v>
+        <v>474</v>
       </c>
       <c r="E333" t="s">
         <v>258</v>
       </c>
       <c r="F333" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
     </row>
     <row r="334" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A334" s="12"/>
       <c r="D334" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
       <c r="E334" t="s">
         <v>259</v>

</xml_diff>

<commit_message>
GearSwap - Adding buff table to buff_change
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variables.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variables.xlsx
@@ -1686,9 +1686,6 @@
     <t>Changes the target to whatever value is passed. It can be a name or something like '&lt;t&gt;', but be aware that there will be no correction done on it. Valid only in pretarget.</t>
   </si>
   <si>
-    <t>buff_change(name,gain)</t>
-  </si>
-  <si>
     <t>S or set</t>
   </si>
   <si>
@@ -2097,9 +2094,6 @@
     <t>indi_change(indi_table,gain)</t>
   </si>
   <si>
-    <t>Passes the buff name and a boolean that indicates whether it was gained (true) or lost (false). Does not fire if your buff bar does not change. For instance, overwriting a March with another March will not trigger this event.</t>
-  </si>
-  <si>
     <t>Passes the indi effect table when an indi aura chanes and a boolean that indicates whether it was gained or lost.</t>
   </si>
   <si>
@@ -2365,6 +2359,12 @@
   </si>
   <si>
     <t>This function adds its argument function to the unhandled_comman event registry. It will be called (in the order that it is registered) when a command is passed in to gearswap (//gs ____) that gearswap doesn't know what to do with. If the argument function returns true, the command will be treated as handled and not passed on to further functions.</t>
+  </si>
+  <si>
+    <t>Passes the buff name and a boolean that indicates whether it was gained (true) or lost (false), as well as the resource table for the buff. Does not fire if your buff bar does not change. For instance, overwriting a March with another March will not trigger this event.</t>
+  </si>
+  <si>
+    <t>buff_change(name,gain,buff_table)</t>
   </si>
 </sst>
 </file>
@@ -2763,8 +2763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F391"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2808,13 +2808,13 @@
     <row r="4" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="D4" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E4" t="s">
         <v>450</v>
       </c>
       <c r="F4" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2823,13 +2823,13 @@
         <v>163</v>
       </c>
       <c r="D5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E5" t="s">
         <v>450</v>
       </c>
       <c r="F5" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2838,13 +2838,13 @@
         <v>164</v>
       </c>
       <c r="D6" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E6" t="s">
         <v>450</v>
       </c>
       <c r="F6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2853,13 +2853,13 @@
         <v>165</v>
       </c>
       <c r="D7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E7" t="s">
         <v>450</v>
       </c>
       <c r="F7" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2877,19 +2877,19 @@
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="D9" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="E9" t="s">
         <v>450</v>
       </c>
       <c r="F9" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="D10" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E10" t="s">
         <v>450</v>
@@ -2901,7 +2901,7 @@
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="D11" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="E11" t="s">
         <v>450</v>
@@ -2913,61 +2913,61 @@
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="D12" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E12" t="s">
         <v>450</v>
       </c>
       <c r="F12" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="D13" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E13" t="s">
         <v>450</v>
       </c>
       <c r="F13" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="D14" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E14" t="s">
         <v>450</v>
       </c>
       <c r="F14" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="D15" t="s">
-        <v>556</v>
+        <v>782</v>
       </c>
       <c r="E15" t="s">
         <v>450</v>
       </c>
       <c r="F15" t="s">
-        <v>693</v>
+        <v>781</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="D16" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E16" t="s">
         <v>450</v>
       </c>
       <c r="F16" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2979,24 +2979,24 @@
         <v>450</v>
       </c>
       <c r="F17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="D18" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="E18" t="s">
         <v>450</v>
       </c>
       <c r="F18" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="B21" t="s">
         <v>180</v>
@@ -3065,7 +3065,7 @@
         <v>450</v>
       </c>
       <c r="F25" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3080,7 +3080,7 @@
         <v>450</v>
       </c>
       <c r="F26" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3095,7 +3095,7 @@
         <v>450</v>
       </c>
       <c r="F27" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3104,13 +3104,13 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E28" t="s">
         <v>450</v>
       </c>
       <c r="F28" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3119,13 +3119,13 @@
         <v>119</v>
       </c>
       <c r="D29" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E29" t="s">
         <v>450</v>
       </c>
       <c r="F29" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3134,13 +3134,13 @@
         <v>120</v>
       </c>
       <c r="D30" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E30" t="s">
         <v>450</v>
       </c>
       <c r="F30" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3158,49 +3158,49 @@
         <v>450</v>
       </c>
       <c r="F31" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="C32" s="5"/>
       <c r="D32" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="E32" t="s">
         <v>450</v>
       </c>
       <c r="F32" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="E33" t="s">
         <v>450</v>
       </c>
       <c r="F33" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="C34" s="5"/>
       <c r="D34" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="E34" t="s">
         <v>450</v>
       </c>
       <c r="F34" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3215,7 +3215,7 @@
         <v>450</v>
       </c>
       <c r="F35" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3230,7 +3230,7 @@
         <v>450</v>
       </c>
       <c r="F36" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3239,13 +3239,13 @@
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E37" t="s">
         <v>450</v>
       </c>
       <c r="F37" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3275,7 +3275,7 @@
         <v>450</v>
       </c>
       <c r="F39" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3305,7 +3305,7 @@
         <v>450</v>
       </c>
       <c r="F41" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3314,13 +3314,13 @@
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E42" t="s">
         <v>450</v>
       </c>
       <c r="F42" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3329,13 +3329,13 @@
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="E43" t="s">
         <v>450</v>
       </c>
       <c r="F43" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3344,13 +3344,13 @@
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E44" t="s">
         <v>450</v>
       </c>
       <c r="F44" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3361,19 +3361,19 @@
     </row>
     <row r="47" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="B47" t="s">
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E47" t="s">
         <v>133</v>
       </c>
       <c r="F47" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3382,13 +3382,13 @@
         <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="E48" t="s">
         <v>135</v>
       </c>
       <c r="F48" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3397,13 +3397,13 @@
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="E49" t="s">
         <v>135</v>
       </c>
       <c r="F49" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3412,13 +3412,13 @@
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="E50" t="s">
         <v>135</v>
       </c>
       <c r="F50" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3427,13 +3427,13 @@
         <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="E51" t="s">
         <v>135</v>
       </c>
       <c r="F51" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3442,13 +3442,13 @@
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="E52" t="s">
         <v>135</v>
       </c>
       <c r="F52" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3459,19 +3459,19 @@
     </row>
     <row r="55" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="B55" t="s">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="E55" t="s">
         <v>135</v>
       </c>
       <c r="F55" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3486,7 +3486,7 @@
         <v>135</v>
       </c>
       <c r="F56" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3501,7 +3501,7 @@
         <v>135</v>
       </c>
       <c r="F57" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3510,13 +3510,13 @@
         <v>0</v>
       </c>
       <c r="D58" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E58" t="s">
         <v>135</v>
       </c>
       <c r="F58" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3525,13 +3525,13 @@
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E59" t="s">
         <v>135</v>
       </c>
       <c r="F59" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3540,13 +3540,13 @@
         <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E60" t="s">
         <v>135</v>
       </c>
       <c r="F60" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3570,13 +3570,13 @@
         <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="E62" t="s">
         <v>135</v>
       </c>
       <c r="F62" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3585,13 +3585,13 @@
         <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="E63" t="s">
         <v>135</v>
       </c>
       <c r="F63" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3600,13 +3600,13 @@
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E64" t="s">
         <v>135</v>
       </c>
       <c r="F64" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3615,13 +3615,13 @@
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="E65" t="s">
         <v>135</v>
       </c>
       <c r="F65" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3630,18 +3630,18 @@
         <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E66" t="s">
         <v>450</v>
       </c>
       <c r="F66" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="B69" t="s">
         <v>0</v>
@@ -3653,7 +3653,7 @@
         <v>450</v>
       </c>
       <c r="F69" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3668,7 +3668,7 @@
         <v>450</v>
       </c>
       <c r="F70" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3677,13 +3677,13 @@
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E71" t="s">
         <v>450</v>
       </c>
       <c r="F71" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3698,7 +3698,7 @@
         <v>450</v>
       </c>
       <c r="F72" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3713,7 +3713,7 @@
         <v>450</v>
       </c>
       <c r="F73" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3728,7 +3728,7 @@
         <v>450</v>
       </c>
       <c r="F74" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3737,13 +3737,13 @@
         <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="E75" t="s">
         <v>450</v>
       </c>
       <c r="F75" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3752,13 +3752,13 @@
         <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E76" t="s">
         <v>450</v>
       </c>
       <c r="F76" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3767,13 +3767,13 @@
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="E77" t="s">
         <v>450</v>
       </c>
       <c r="F77" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3782,13 +3782,13 @@
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="E78" t="s">
         <v>450</v>
       </c>
       <c r="F78" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3797,13 +3797,13 @@
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E79" t="s">
         <v>450</v>
       </c>
       <c r="F79" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3812,13 +3812,13 @@
         <v>0</v>
       </c>
       <c r="D80" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E80" t="s">
         <v>450</v>
       </c>
       <c r="F80" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3827,13 +3827,13 @@
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="E81" t="s">
         <v>450</v>
       </c>
       <c r="F81" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3842,13 +3842,13 @@
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="E82" t="s">
         <v>450</v>
       </c>
       <c r="F82" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3857,13 +3857,13 @@
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="E83" t="s">
         <v>450</v>
       </c>
       <c r="F83" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3872,13 +3872,13 @@
         <v>0</v>
       </c>
       <c r="D84" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E84" t="s">
         <v>450</v>
       </c>
       <c r="F84" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3928,13 +3928,13 @@
     <row r="91" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="13"/>
       <c r="B91" t="s">
+        <v>672</v>
+      </c>
+      <c r="D91" t="s">
         <v>673</v>
       </c>
-      <c r="D91" t="s">
+      <c r="F91" t="s">
         <v>674</v>
-      </c>
-      <c r="F91" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3955,7 +3955,7 @@
         <v>185</v>
       </c>
       <c r="F93" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3967,7 +3967,7 @@
         <v>189</v>
       </c>
       <c r="F94" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3979,7 +3979,7 @@
         <v>188</v>
       </c>
       <c r="F95" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3997,19 +3997,19 @@
     <row r="97" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="13"/>
       <c r="D97" t="s">
+        <v>617</v>
+      </c>
+      <c r="F97" t="s">
         <v>618</v>
-      </c>
-      <c r="F97" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="13"/>
       <c r="D98" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="F98" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4053,7 +4053,7 @@
         <v>4</v>
       </c>
       <c r="D103" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E103" t="s">
         <v>135</v>
@@ -4089,7 +4089,7 @@
         <v>133</v>
       </c>
       <c r="F105" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4098,7 +4098,7 @@
         <v>9</v>
       </c>
       <c r="D106" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="E106" t="s">
         <v>232</v>
@@ -4113,7 +4113,7 @@
         <v>10</v>
       </c>
       <c r="D107" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="E107" t="s">
         <v>232</v>
@@ -4140,13 +4140,13 @@
     <row r="109" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="13"/>
       <c r="D109" t="s">
+        <v>678</v>
+      </c>
+      <c r="E109" t="s">
+        <v>232</v>
+      </c>
+      <c r="F109" t="s">
         <v>679</v>
-      </c>
-      <c r="E109" t="s">
-        <v>232</v>
-      </c>
-      <c r="F109" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4167,13 +4167,13 @@
     <row r="111" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="13"/>
       <c r="D111" t="s">
+        <v>676</v>
+      </c>
+      <c r="E111" t="s">
+        <v>232</v>
+      </c>
+      <c r="F111" t="s">
         <v>677</v>
-      </c>
-      <c r="E111" t="s">
-        <v>232</v>
-      </c>
-      <c r="F111" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4182,7 +4182,7 @@
         <v>15</v>
       </c>
       <c r="D112" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E112" t="s">
         <v>232</v>
@@ -4230,13 +4230,13 @@
     <row r="116" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="13"/>
       <c r="D116" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="E116" t="s">
         <v>233</v>
       </c>
       <c r="F116" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4472,7 +4472,7 @@
     <row r="136" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="13"/>
       <c r="D136" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E136" t="s">
         <v>232</v>
@@ -4484,7 +4484,7 @@
     <row r="137" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="13"/>
       <c r="D137" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E137" t="s">
         <v>232</v>
@@ -4496,7 +4496,7 @@
     <row r="138" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="13"/>
       <c r="D138" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E138" t="s">
         <v>232</v>
@@ -4573,13 +4573,13 @@
     <row r="146" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="13"/>
       <c r="D146" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E146" t="s">
         <v>133</v>
       </c>
       <c r="F146" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="147" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4999,13 +4999,13 @@
     <row r="178" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="13"/>
       <c r="D178" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E178" t="s">
         <v>135</v>
       </c>
       <c r="F178" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5047,7 +5047,7 @@
     <row r="182" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="13"/>
       <c r="D182" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E182" t="s">
         <v>232</v>
@@ -5059,7 +5059,7 @@
     <row r="183" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="13"/>
       <c r="D183" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E183" t="s">
         <v>232</v>
@@ -5071,7 +5071,7 @@
     <row r="184" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="13"/>
       <c r="D184" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E184" t="s">
         <v>232</v>
@@ -5095,73 +5095,73 @@
     <row r="186" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="13"/>
       <c r="D186" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E186" t="s">
         <v>135</v>
       </c>
       <c r="F186" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="13"/>
       <c r="D187" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E187" t="s">
         <v>135</v>
       </c>
       <c r="F187" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="188" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="13"/>
       <c r="D188" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E188" t="s">
         <v>135</v>
       </c>
       <c r="F188" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="189" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="13"/>
       <c r="D189" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E189" t="s">
         <v>135</v>
       </c>
       <c r="F189" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="190" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="13"/>
       <c r="D190" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E190" t="s">
         <v>135</v>
       </c>
       <c r="F190" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="13"/>
       <c r="D191" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E191" t="s">
         <v>135</v>
       </c>
       <c r="F191" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="192" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5630,7 +5630,7 @@
     <row r="228" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="13"/>
       <c r="D228" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="E228" t="s">
         <v>232</v>
@@ -5642,7 +5642,7 @@
     <row r="229" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="13"/>
       <c r="D229" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E229" t="s">
         <v>232</v>
@@ -5654,7 +5654,7 @@
     <row r="230" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="13"/>
       <c r="D230" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="E230" t="s">
         <v>232</v>
@@ -5666,7 +5666,7 @@
     <row r="231" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="13"/>
       <c r="D231" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="E231" t="s">
         <v>232</v>
@@ -5914,7 +5914,7 @@
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" s="13"/>
       <c r="D253" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E253" t="s">
         <v>232</v>
@@ -5926,7 +5926,7 @@
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="13"/>
       <c r="D254" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E254" t="s">
         <v>232</v>
@@ -5938,7 +5938,7 @@
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="13"/>
       <c r="D255" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="E255" t="s">
         <v>232</v>
@@ -5950,7 +5950,7 @@
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="13"/>
       <c r="D256" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E256" t="s">
         <v>232</v>
@@ -6198,7 +6198,7 @@
     <row r="278" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A278" s="13"/>
       <c r="D278" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E278" t="s">
         <v>232</v>
@@ -6210,7 +6210,7 @@
     <row r="279" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A279" s="13"/>
       <c r="D279" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E279" t="s">
         <v>232</v>
@@ -6222,7 +6222,7 @@
     <row r="280" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A280" s="13"/>
       <c r="D280" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E280" t="s">
         <v>232</v>
@@ -6234,7 +6234,7 @@
     <row r="281" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="13"/>
       <c r="D281" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E281" t="s">
         <v>232</v>
@@ -6458,7 +6458,7 @@
     <row r="300" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A300" s="13"/>
       <c r="D300" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E300" t="s">
         <v>232</v>
@@ -6470,7 +6470,7 @@
     <row r="301" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A301" s="13"/>
       <c r="D301" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E301" t="s">
         <v>232</v>
@@ -6482,7 +6482,7 @@
     <row r="302" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="13"/>
       <c r="D302" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E302" t="s">
         <v>232</v>
@@ -6494,7 +6494,7 @@
     <row r="303" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="13"/>
       <c r="D303" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E303" t="s">
         <v>232</v>
@@ -6530,16 +6530,16 @@
     <row r="306" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A306" s="13"/>
       <c r="D306" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F306" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="307" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A307" s="13"/>
       <c r="D307" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E307" t="s">
         <v>232</v>
@@ -6548,7 +6548,7 @@
     <row r="308" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A308" s="13"/>
       <c r="D308" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E308" t="s">
         <v>232</v>
@@ -6566,7 +6566,7 @@
     <row r="310" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A310" s="13"/>
       <c r="D310" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E310" t="s">
         <v>232</v>
@@ -6575,7 +6575,7 @@
     <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" s="13"/>
       <c r="D311" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E311" t="s">
         <v>232</v>
@@ -6584,7 +6584,7 @@
     <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" s="13"/>
       <c r="D312" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E312" t="s">
         <v>232</v>
@@ -6593,7 +6593,7 @@
     <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313" s="13"/>
       <c r="D313" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E313" t="s">
         <v>232</v>
@@ -6602,7 +6602,7 @@
     <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314" s="13"/>
       <c r="D314" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E314" t="s">
         <v>232</v>
@@ -6611,7 +6611,7 @@
     <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315" s="13"/>
       <c r="D315" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E315" t="s">
         <v>232</v>
@@ -6620,241 +6620,241 @@
     <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" s="13"/>
       <c r="D316" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E316" t="s">
         <v>232</v>
       </c>
       <c r="F316" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" s="13"/>
       <c r="D317" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E317" t="s">
         <v>232</v>
       </c>
       <c r="F317" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" s="13"/>
       <c r="D318" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E318" t="s">
         <v>232</v>
       </c>
       <c r="F318" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A319" s="13"/>
       <c r="D319" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E319" t="s">
         <v>232</v>
       </c>
       <c r="F319" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320" s="13"/>
       <c r="D320" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E320" t="s">
         <v>232</v>
       </c>
       <c r="F320" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321" s="13"/>
       <c r="D321" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E321" t="s">
         <v>232</v>
       </c>
       <c r="F321" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A322" s="13"/>
       <c r="D322" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E322" t="s">
         <v>232</v>
       </c>
       <c r="F322" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A323" s="13"/>
       <c r="D323" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E323" t="s">
         <v>232</v>
       </c>
       <c r="F323" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A324" s="13"/>
       <c r="D324" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E324" t="s">
         <v>232</v>
       </c>
       <c r="F324" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="13"/>
       <c r="D325" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E325" t="s">
         <v>232</v>
       </c>
       <c r="F325" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A326" s="13"/>
       <c r="D326" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E326" t="s">
         <v>232</v>
       </c>
       <c r="F326" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A327" s="13"/>
       <c r="D327" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E327" t="s">
         <v>232</v>
       </c>
       <c r="F327" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A328" s="13"/>
       <c r="D328" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E328" t="s">
         <v>232</v>
       </c>
       <c r="F328" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A329" s="13"/>
       <c r="D329" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E329" t="s">
         <v>232</v>
       </c>
       <c r="F329" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A330" s="13"/>
       <c r="D330" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E330" t="s">
         <v>133</v>
       </c>
       <c r="F330" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A331" s="13"/>
       <c r="D331" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E331" t="s">
         <v>133</v>
       </c>
       <c r="F331" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A332" s="13"/>
       <c r="D332" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E332" t="s">
         <v>135</v>
       </c>
       <c r="F332" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A333" s="13"/>
       <c r="D333" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E333" t="s">
         <v>135</v>
       </c>
       <c r="F333" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="334" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A334" s="13"/>
       <c r="D334" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E334" t="s">
         <v>135</v>
       </c>
       <c r="F334" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="335" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A335" s="13"/>
       <c r="D335" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E335" t="s">
         <v>135</v>
       </c>
       <c r="F335" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="338" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -7024,7 +7024,7 @@
     <row r="351" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A351" s="13"/>
       <c r="D351" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E351" t="s">
         <v>232</v>
@@ -7036,7 +7036,7 @@
     <row r="352" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A352" s="13"/>
       <c r="D352" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="E352" t="s">
         <v>232</v>
@@ -7048,7 +7048,7 @@
     <row r="353" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A353" s="13"/>
       <c r="D353" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="E353" t="s">
         <v>232</v>
@@ -7060,7 +7060,7 @@
     <row r="354" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A354" s="13"/>
       <c r="D354" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E354" t="s">
         <v>232</v>
@@ -7343,7 +7343,7 @@
         <v>233</v>
       </c>
       <c r="F379" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="382" spans="1:6" ht="21" x14ac:dyDescent="0.35">
@@ -7433,13 +7433,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A101:A116"/>
-    <mergeCell ref="A3:A18"/>
-    <mergeCell ref="A69:A84"/>
-    <mergeCell ref="A55:A66"/>
-    <mergeCell ref="A87:A98"/>
-    <mergeCell ref="A47:A52"/>
-    <mergeCell ref="A21:A44"/>
     <mergeCell ref="A385:A389"/>
     <mergeCell ref="A359:A364"/>
     <mergeCell ref="A368:A379"/>
@@ -7451,6 +7444,13 @@
     <mergeCell ref="A194:A209"/>
     <mergeCell ref="A287:A335"/>
     <mergeCell ref="A145:A191"/>
+    <mergeCell ref="A101:A116"/>
+    <mergeCell ref="A3:A18"/>
+    <mergeCell ref="A69:A84"/>
+    <mergeCell ref="A55:A66"/>
+    <mergeCell ref="A87:A98"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="A21:A44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GearSwap - minor inconsistencies
</commit_message>
<xml_diff>
--- a/addons/GearSwap/beta_examples_and_information/Variables.xlsx
+++ b/addons/GearSwap/beta_examples_and_information/Variables.xlsx
@@ -2364,15 +2364,9 @@
     <t>file_unload(file_name)</t>
   </si>
   <si>
-    <t>buff</t>
-  </si>
-  <si>
     <t>player.buff_details</t>
   </si>
   <si>
-    <t>buff_id</t>
-  </si>
-  <si>
     <t>duration</t>
   </si>
   <si>
@@ -2407,6 +2401,12 @@
   </si>
   <si>
     <t>Passes the buff name and the associated player.buff_details table for the buff. Fires when a status effect is overwritten.</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -2805,8 +2805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F397"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A20"/>
+    <sheetView tabSelected="1" topLeftCell="A279" workbookViewId="0">
+      <selection activeCell="B290" sqref="B290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2991,31 +2991,31 @@
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="D15" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="E15" t="s">
         <v>450</v>
       </c>
       <c r="F15" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="D16" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="E16" t="s">
         <v>450</v>
       </c>
       <c r="F16" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="D17" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="E17" t="s">
         <v>450</v>
@@ -6350,28 +6350,28 @@
     </row>
     <row r="288" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A288" s="13" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B288" t="s">
-        <v>782</v>
+        <v>796</v>
       </c>
       <c r="E288" t="s">
         <v>133</v>
       </c>
       <c r="F288" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" s="13"/>
       <c r="B289" t="s">
-        <v>784</v>
+        <v>795</v>
       </c>
       <c r="E289" t="s">
         <v>232</v>
       </c>
       <c r="F289" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.25">
@@ -6383,31 +6383,31 @@
         <v>232</v>
       </c>
       <c r="F290" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" s="13"/>
       <c r="B291" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="E291" t="s">
         <v>135</v>
       </c>
       <c r="F291" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" s="13"/>
       <c r="B292" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="E292" t="s">
         <v>232</v>
       </c>
       <c r="F292" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="294" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -7558,11 +7558,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A103:A118"/>
-    <mergeCell ref="A71:A86"/>
-    <mergeCell ref="A57:A68"/>
-    <mergeCell ref="A89:A100"/>
-    <mergeCell ref="A49:A54"/>
     <mergeCell ref="A23:A46"/>
     <mergeCell ref="A3:A20"/>
     <mergeCell ref="A392:A396"/>
@@ -7577,6 +7572,11 @@
     <mergeCell ref="A294:A342"/>
     <mergeCell ref="A147:A193"/>
     <mergeCell ref="A288:A292"/>
+    <mergeCell ref="A103:A118"/>
+    <mergeCell ref="A71:A86"/>
+    <mergeCell ref="A57:A68"/>
+    <mergeCell ref="A89:A100"/>
+    <mergeCell ref="A49:A54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>